<commit_message>
Atualização de bases das ligas, do dia: 17-02-2024 às 11:11
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC212"/>
+  <dimension ref="A1:AC209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4876,7 +4876,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>5400048</v>
+        <v>5404699</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4888,73 +4888,73 @@
         <v>44982.125</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G50" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>3</v>
       </c>
-      <c r="I50">
-        <v>2</v>
-      </c>
       <c r="J50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K50">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="L50">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="M50">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="N50">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="O50">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P50">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="Q50">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R50">
-        <v>2.025</v>
+        <v>1.94</v>
       </c>
       <c r="S50">
-        <v>1.825</v>
+        <v>1.96</v>
       </c>
       <c r="T50">
         <v>2.75</v>
       </c>
       <c r="U50">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V50">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W50">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X50">
         <v>-1</v>
       </c>
       <c r="Y50">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z50">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA50">
-        <v>-0.5</v>
+        <v>0.96</v>
       </c>
       <c r="AB50">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC50">
         <v>-1</v>
@@ -4965,7 +4965,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>5404699</v>
+        <v>5400048</v>
       </c>
       <c r="C51" t="s">
         <v>28</v>
@@ -4977,73 +4977,73 @@
         <v>44982.125</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K51">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="L51">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="M51">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="N51">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="O51">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P51">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="Q51">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R51">
-        <v>1.94</v>
+        <v>2.025</v>
       </c>
       <c r="S51">
-        <v>1.96</v>
+        <v>1.825</v>
       </c>
       <c r="T51">
         <v>2.75</v>
       </c>
       <c r="U51">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V51">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W51">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X51">
         <v>-1</v>
       </c>
       <c r="Y51">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z51">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA51">
-        <v>0.96</v>
+        <v>-0.5</v>
       </c>
       <c r="AB51">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC51">
         <v>-1</v>
@@ -5499,7 +5499,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5404706</v>
+        <v>5404704</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5511,58 +5511,58 @@
         <v>44989.125</v>
       </c>
       <c r="F57" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>42</v>
       </c>
       <c r="K57">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="L57">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M57">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="N57">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="O57">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P57">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q57">
         <v>-0.25</v>
       </c>
       <c r="R57">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S57">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T57">
         <v>2.75</v>
       </c>
       <c r="U57">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V57">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W57">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="X57">
         <v>-1</v>
@@ -5571,16 +5571,16 @@
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0.8500000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AA57">
         <v>-1</v>
       </c>
       <c r="AB57">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AC57">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5588,7 +5588,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5404704</v>
+        <v>5404706</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5600,58 +5600,58 @@
         <v>44989.125</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="s">
         <v>42</v>
       </c>
       <c r="K58">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L58">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M58">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="N58">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O58">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P58">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q58">
         <v>-0.25</v>
       </c>
       <c r="R58">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S58">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T58">
         <v>2.75</v>
       </c>
       <c r="U58">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V58">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W58">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="X58">
         <v>-1</v>
@@ -5660,16 +5660,16 @@
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA58">
         <v>-1</v>
       </c>
       <c r="AB58">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AC58">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97">
+        <v>1.75</v>
+      </c>
+      <c r="L97">
+        <v>3.8</v>
+      </c>
+      <c r="M97">
         <v>4</v>
       </c>
-      <c r="J97" t="s">
-        <v>41</v>
-      </c>
-      <c r="K97">
-        <v>2.3</v>
-      </c>
-      <c r="L97">
-        <v>3.75</v>
-      </c>
-      <c r="M97">
-        <v>2.75</v>
-      </c>
       <c r="N97">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q97">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R97">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S97">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T97">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U97">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V97">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W97">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X97">
         <v>-1</v>
       </c>
       <c r="Y97">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z97">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA97">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB97">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K98">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L98">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M98">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N98">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q98">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R98">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S98">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T98">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U98">
+        <v>2</v>
+      </c>
+      <c r="V98">
         <v>1.85</v>
       </c>
-      <c r="V98">
-        <v>2</v>
-      </c>
       <c r="W98">
+        <v>-1</v>
+      </c>
+      <c r="X98">
+        <v>-1</v>
+      </c>
+      <c r="Y98">
+        <v>1.4</v>
+      </c>
+      <c r="Z98">
+        <v>-1</v>
+      </c>
+      <c r="AA98">
+        <v>0.8</v>
+      </c>
+      <c r="AB98">
         <v>1</v>
-      </c>
-      <c r="X98">
-        <v>-1</v>
-      </c>
-      <c r="Y98">
-        <v>-1</v>
-      </c>
-      <c r="Z98">
-        <v>1.025</v>
-      </c>
-      <c r="AA98">
-        <v>-1</v>
-      </c>
-      <c r="AB98">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -18938,7 +18938,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>7127372</v>
+        <v>7127370</v>
       </c>
       <c r="C208" t="s">
         <v>28</v>
@@ -18947,49 +18947,49 @@
         <v>28</v>
       </c>
       <c r="E208" s="2">
-        <v>45339.16666666666</v>
+        <v>45340.125</v>
       </c>
       <c r="F208" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G208" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K208">
-        <v>1.727</v>
+        <v>2.4</v>
       </c>
       <c r="L208">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M208">
-        <v>4.2</v>
+        <v>2.625</v>
       </c>
       <c r="N208">
-        <v>1.65</v>
+        <v>2.3</v>
       </c>
       <c r="O208">
-        <v>4.333</v>
+        <v>3.8</v>
       </c>
       <c r="P208">
-        <v>4.75</v>
+        <v>2.875</v>
       </c>
       <c r="Q208">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R208">
-        <v>2.06</v>
+        <v>2.05</v>
       </c>
       <c r="S208">
-        <v>1.84</v>
+        <v>1.85</v>
       </c>
       <c r="T208">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U208">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V208">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="W208">
         <v>0</v>
@@ -19012,7 +19012,7 @@
         <v>207</v>
       </c>
       <c r="B209">
-        <v>7126788</v>
+        <v>7127374</v>
       </c>
       <c r="C209" t="s">
         <v>28</v>
@@ -19021,49 +19021,49 @@
         <v>28</v>
       </c>
       <c r="E209" s="2">
-        <v>45339.23958333334</v>
+        <v>45340.125</v>
       </c>
       <c r="F209" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G209" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K209">
-        <v>2.625</v>
+        <v>1.909</v>
       </c>
       <c r="L209">
         <v>3.75</v>
       </c>
       <c r="M209">
-        <v>2.375</v>
+        <v>3.6</v>
       </c>
       <c r="N209">
-        <v>3.1</v>
+        <v>1.85</v>
       </c>
       <c r="O209">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P209">
-        <v>2.15</v>
+        <v>3.75</v>
       </c>
       <c r="Q209">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R209">
-        <v>1.97</v>
+        <v>1.9</v>
       </c>
       <c r="S209">
-        <v>1.93</v>
+        <v>2</v>
       </c>
       <c r="T209">
         <v>3</v>
       </c>
       <c r="U209">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V209">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W209">
         <v>0</v>
@@ -19078,228 +19078,6 @@
         <v>0</v>
       </c>
       <c r="AA209">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:27">
-      <c r="A210" s="1">
-        <v>208</v>
-      </c>
-      <c r="B210">
-        <v>7127373</v>
-      </c>
-      <c r="C210" t="s">
-        <v>28</v>
-      </c>
-      <c r="D210" t="s">
-        <v>28</v>
-      </c>
-      <c r="E210" s="2">
-        <v>45339.32291666666</v>
-      </c>
-      <c r="F210" t="s">
-        <v>34</v>
-      </c>
-      <c r="G210" t="s">
-        <v>39</v>
-      </c>
-      <c r="K210">
-        <v>2.4</v>
-      </c>
-      <c r="L210">
-        <v>4</v>
-      </c>
-      <c r="M210">
-        <v>2.5</v>
-      </c>
-      <c r="N210">
-        <v>2.3</v>
-      </c>
-      <c r="O210">
-        <v>4.2</v>
-      </c>
-      <c r="P210">
-        <v>2.625</v>
-      </c>
-      <c r="Q210">
-        <v>0</v>
-      </c>
-      <c r="R210">
-        <v>1.85</v>
-      </c>
-      <c r="S210">
-        <v>2.05</v>
-      </c>
-      <c r="T210">
-        <v>3.25</v>
-      </c>
-      <c r="U210">
-        <v>1.875</v>
-      </c>
-      <c r="V210">
-        <v>1.975</v>
-      </c>
-      <c r="W210">
-        <v>0</v>
-      </c>
-      <c r="X210">
-        <v>0</v>
-      </c>
-      <c r="Y210">
-        <v>0</v>
-      </c>
-      <c r="Z210">
-        <v>0</v>
-      </c>
-      <c r="AA210">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:27">
-      <c r="A211" s="1">
-        <v>209</v>
-      </c>
-      <c r="B211">
-        <v>7127370</v>
-      </c>
-      <c r="C211" t="s">
-        <v>28</v>
-      </c>
-      <c r="D211" t="s">
-        <v>28</v>
-      </c>
-      <c r="E211" s="2">
-        <v>45340.125</v>
-      </c>
-      <c r="F211" t="s">
-        <v>38</v>
-      </c>
-      <c r="G211" t="s">
-        <v>31</v>
-      </c>
-      <c r="K211">
-        <v>2.4</v>
-      </c>
-      <c r="L211">
-        <v>3.75</v>
-      </c>
-      <c r="M211">
-        <v>2.625</v>
-      </c>
-      <c r="N211">
-        <v>2.3</v>
-      </c>
-      <c r="O211">
-        <v>3.8</v>
-      </c>
-      <c r="P211">
-        <v>2.875</v>
-      </c>
-      <c r="Q211">
-        <v>-0.25</v>
-      </c>
-      <c r="R211">
-        <v>2.08</v>
-      </c>
-      <c r="S211">
-        <v>1.82</v>
-      </c>
-      <c r="T211">
-        <v>3</v>
-      </c>
-      <c r="U211">
-        <v>1.9</v>
-      </c>
-      <c r="V211">
-        <v>1.95</v>
-      </c>
-      <c r="W211">
-        <v>0</v>
-      </c>
-      <c r="X211">
-        <v>0</v>
-      </c>
-      <c r="Y211">
-        <v>0</v>
-      </c>
-      <c r="Z211">
-        <v>0</v>
-      </c>
-      <c r="AA211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:27">
-      <c r="A212" s="1">
-        <v>210</v>
-      </c>
-      <c r="B212">
-        <v>7127374</v>
-      </c>
-      <c r="C212" t="s">
-        <v>28</v>
-      </c>
-      <c r="D212" t="s">
-        <v>28</v>
-      </c>
-      <c r="E212" s="2">
-        <v>45340.125</v>
-      </c>
-      <c r="F212" t="s">
-        <v>36</v>
-      </c>
-      <c r="G212" t="s">
-        <v>30</v>
-      </c>
-      <c r="K212">
-        <v>1.909</v>
-      </c>
-      <c r="L212">
-        <v>3.75</v>
-      </c>
-      <c r="M212">
-        <v>3.6</v>
-      </c>
-      <c r="N212">
-        <v>1.85</v>
-      </c>
-      <c r="O212">
-        <v>4</v>
-      </c>
-      <c r="P212">
-        <v>3.75</v>
-      </c>
-      <c r="Q212">
-        <v>-0.5</v>
-      </c>
-      <c r="R212">
-        <v>1.91</v>
-      </c>
-      <c r="S212">
-        <v>1.99</v>
-      </c>
-      <c r="T212">
-        <v>3</v>
-      </c>
-      <c r="U212">
-        <v>1.95</v>
-      </c>
-      <c r="V212">
-        <v>1.9</v>
-      </c>
-      <c r="W212">
-        <v>0</v>
-      </c>
-      <c r="X212">
-        <v>0</v>
-      </c>
-      <c r="Y212">
-        <v>0</v>
-      </c>
-      <c r="Z212">
-        <v>0</v>
-      </c>
-      <c r="AA212">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 17-02-2024 às 22:47
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC209"/>
+  <dimension ref="A1:AC210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G97" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H97">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K97">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L97">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M97">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N97">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q97">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R97">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S97">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T97">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U97">
+        <v>2</v>
+      </c>
+      <c r="V97">
         <v>1.85</v>
       </c>
-      <c r="V97">
-        <v>2</v>
-      </c>
       <c r="W97">
+        <v>-1</v>
+      </c>
+      <c r="X97">
+        <v>-1</v>
+      </c>
+      <c r="Y97">
+        <v>1.4</v>
+      </c>
+      <c r="Z97">
+        <v>-1</v>
+      </c>
+      <c r="AA97">
+        <v>0.8</v>
+      </c>
+      <c r="AB97">
         <v>1</v>
-      </c>
-      <c r="X97">
-        <v>-1</v>
-      </c>
-      <c r="Y97">
-        <v>-1</v>
-      </c>
-      <c r="Z97">
-        <v>1.025</v>
-      </c>
-      <c r="AA97">
-        <v>-1</v>
-      </c>
-      <c r="AB97">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G98" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="J98" t="s">
+        <v>42</v>
+      </c>
+      <c r="K98">
+        <v>1.75</v>
+      </c>
+      <c r="L98">
+        <v>3.8</v>
+      </c>
+      <c r="M98">
         <v>4</v>
       </c>
-      <c r="J98" t="s">
-        <v>41</v>
-      </c>
-      <c r="K98">
-        <v>2.3</v>
-      </c>
-      <c r="L98">
-        <v>3.75</v>
-      </c>
-      <c r="M98">
-        <v>2.75</v>
-      </c>
       <c r="N98">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q98">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R98">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S98">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T98">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U98">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V98">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W98">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X98">
         <v>-1</v>
       </c>
       <c r="Y98">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA98">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB98">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -18977,19 +18977,19 @@
         <v>-0.25</v>
       </c>
       <c r="R208">
-        <v>2.05</v>
+        <v>2.02</v>
       </c>
       <c r="S208">
-        <v>1.85</v>
+        <v>1.88</v>
       </c>
       <c r="T208">
         <v>3</v>
       </c>
       <c r="U208">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V208">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W208">
         <v>0</v>
@@ -19051,19 +19051,19 @@
         <v>-0.5</v>
       </c>
       <c r="R209">
-        <v>1.9</v>
+        <v>1.87</v>
       </c>
       <c r="S209">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="T209">
         <v>3</v>
       </c>
       <c r="U209">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V209">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W209">
         <v>0</v>
@@ -19078,6 +19078,80 @@
         <v>0</v>
       </c>
       <c r="AA209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:27">
+      <c r="A210" s="1">
+        <v>208</v>
+      </c>
+      <c r="B210">
+        <v>7661946</v>
+      </c>
+      <c r="C210" t="s">
+        <v>28</v>
+      </c>
+      <c r="D210" t="s">
+        <v>28</v>
+      </c>
+      <c r="E210" s="2">
+        <v>45342.20833333334</v>
+      </c>
+      <c r="F210" t="s">
+        <v>33</v>
+      </c>
+      <c r="G210" t="s">
+        <v>40</v>
+      </c>
+      <c r="K210">
+        <v>1.45</v>
+      </c>
+      <c r="L210">
+        <v>4.75</v>
+      </c>
+      <c r="M210">
+        <v>6.5</v>
+      </c>
+      <c r="N210">
+        <v>1.45</v>
+      </c>
+      <c r="O210">
+        <v>4.75</v>
+      </c>
+      <c r="P210">
+        <v>6.5</v>
+      </c>
+      <c r="Q210">
+        <v>-1.25</v>
+      </c>
+      <c r="R210">
+        <v>2</v>
+      </c>
+      <c r="S210">
+        <v>1.9</v>
+      </c>
+      <c r="T210">
+        <v>3</v>
+      </c>
+      <c r="U210">
+        <v>1.875</v>
+      </c>
+      <c r="V210">
+        <v>1.975</v>
+      </c>
+      <c r="W210">
+        <v>0</v>
+      </c>
+      <c r="X210">
+        <v>0</v>
+      </c>
+      <c r="Y210">
+        <v>0</v>
+      </c>
+      <c r="Z210">
+        <v>0</v>
+      </c>
+      <c r="AA210">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 18-02-2024 às 22:54
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC210"/>
+  <dimension ref="A1:AC219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3274,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>5400043</v>
+        <v>5400042</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -3286,58 +3286,58 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>42</v>
       </c>
       <c r="K32">
-        <v>2.15</v>
+        <v>1.533</v>
       </c>
       <c r="L32">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M32">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="N32">
-        <v>2.2</v>
+        <v>1.333</v>
       </c>
       <c r="O32">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="P32">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="Q32">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R32">
+        <v>1.85</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>3.25</v>
+      </c>
+      <c r="U32">
+        <v>1.875</v>
+      </c>
+      <c r="V32">
         <v>1.975</v>
       </c>
-      <c r="S32">
-        <v>1.875</v>
-      </c>
-      <c r="T32">
-        <v>3</v>
-      </c>
-      <c r="U32">
-        <v>1.95</v>
-      </c>
-      <c r="V32">
-        <v>1.9</v>
-      </c>
       <c r="W32">
-        <v>1.2</v>
+        <v>0.333</v>
       </c>
       <c r="X32">
         <v>-1</v>
@@ -3346,13 +3346,13 @@
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC32">
         <v>-1</v>
@@ -3363,7 +3363,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5400042</v>
+        <v>5400043</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -3375,58 +3375,58 @@
         <v>44961.125</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" t="s">
         <v>42</v>
       </c>
       <c r="K33">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="L33">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M33">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N33">
-        <v>1.333</v>
+        <v>2.2</v>
       </c>
       <c r="O33">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P33">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="Q33">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R33">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S33">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T33">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U33">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V33">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W33">
-        <v>0.333</v>
+        <v>1.2</v>
       </c>
       <c r="X33">
         <v>-1</v>
@@ -3435,13 +3435,13 @@
         <v>-1</v>
       </c>
       <c r="Z33">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA33">
         <v>-1</v>
       </c>
       <c r="AB33">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC33">
         <v>-1</v>
@@ -6478,7 +6478,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5404714</v>
+        <v>5404713</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6490,76 +6490,76 @@
         <v>45003.125</v>
       </c>
       <c r="F68" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G68" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K68">
         <v>2.25</v>
       </c>
       <c r="L68">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M68">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="N68">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O68">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P68">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q68">
         <v>-0.25</v>
       </c>
       <c r="R68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T68">
         <v>2.75</v>
       </c>
       <c r="U68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W68">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X68">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y68">
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA68">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB68">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC68">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6567,7 +6567,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>5404713</v>
+        <v>5404714</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6579,76 +6579,76 @@
         <v>45003.125</v>
       </c>
       <c r="F69" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G69" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K69">
         <v>2.25</v>
       </c>
       <c r="L69">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M69">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N69">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="O69">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P69">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T69">
         <v>2.75</v>
       </c>
       <c r="U69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W69">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X69">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA69">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB69">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC69">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -9237,7 +9237,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5404735</v>
+        <v>5400064</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -9249,40 +9249,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G99" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H99">
+        <v>2</v>
+      </c>
+      <c r="I99">
         <v>0</v>
       </c>
-      <c r="I99">
-        <v>1</v>
-      </c>
       <c r="J99" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K99">
-        <v>3.6</v>
+        <v>1.65</v>
       </c>
       <c r="L99">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M99">
-        <v>1.909</v>
+        <v>4.5</v>
       </c>
       <c r="N99">
-        <v>4</v>
+        <v>1.533</v>
       </c>
       <c r="O99">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="P99">
-        <v>1.833</v>
+        <v>5.5</v>
       </c>
       <c r="Q99">
-        <v>0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R99">
         <v>2.025</v>
@@ -9291,34 +9291,34 @@
         <v>1.825</v>
       </c>
       <c r="T99">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U99">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V99">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W99">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="X99">
         <v>-1</v>
       </c>
       <c r="Y99">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Z99">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA99">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB99">
         <v>-1</v>
       </c>
       <c r="AC99">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:29">
@@ -9326,7 +9326,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>5400064</v>
+        <v>5404735</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -9338,40 +9338,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F100" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G100" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K100">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L100">
+        <v>3.75</v>
+      </c>
+      <c r="M100">
+        <v>1.909</v>
+      </c>
+      <c r="N100">
         <v>4</v>
       </c>
-      <c r="M100">
-        <v>4.5</v>
-      </c>
-      <c r="N100">
-        <v>1.533</v>
-      </c>
       <c r="O100">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="P100">
-        <v>5.5</v>
+        <v>1.833</v>
       </c>
       <c r="Q100">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R100">
         <v>2.025</v>
@@ -9380,34 +9380,34 @@
         <v>1.825</v>
       </c>
       <c r="T100">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="U100">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V100">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W100">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X100">
         <v>-1</v>
       </c>
       <c r="Y100">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Z100">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA100">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB100">
         <v>-1</v>
       </c>
       <c r="AC100">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="101" spans="1:29">
@@ -18938,7 +18938,7 @@
         <v>206</v>
       </c>
       <c r="B208">
-        <v>7127370</v>
+        <v>7127372</v>
       </c>
       <c r="C208" t="s">
         <v>28</v>
@@ -18947,72 +18947,87 @@
         <v>28</v>
       </c>
       <c r="E208" s="2">
-        <v>45340.125</v>
+        <v>45339.16666666666</v>
       </c>
       <c r="F208" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G208" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H208">
+        <v>2</v>
+      </c>
+      <c r="I208">
+        <v>1</v>
+      </c>
+      <c r="J208" t="s">
+        <v>42</v>
       </c>
       <c r="K208">
-        <v>2.4</v>
+        <v>1.727</v>
       </c>
       <c r="L208">
+        <v>4</v>
+      </c>
+      <c r="M208">
+        <v>4.2</v>
+      </c>
+      <c r="N208">
+        <v>1.55</v>
+      </c>
+      <c r="O208">
+        <v>5</v>
+      </c>
+      <c r="P208">
+        <v>5</v>
+      </c>
+      <c r="Q208">
+        <v>-1</v>
+      </c>
+      <c r="R208">
+        <v>1.85</v>
+      </c>
+      <c r="S208">
+        <v>2</v>
+      </c>
+      <c r="T208">
         <v>3.75</v>
       </c>
-      <c r="M208">
-        <v>2.625</v>
-      </c>
-      <c r="N208">
-        <v>2.3</v>
-      </c>
-      <c r="O208">
-        <v>3.8</v>
-      </c>
-      <c r="P208">
-        <v>2.875</v>
-      </c>
-      <c r="Q208">
-        <v>-0.25</v>
-      </c>
-      <c r="R208">
-        <v>2.02</v>
-      </c>
-      <c r="S208">
-        <v>1.88</v>
-      </c>
-      <c r="T208">
-        <v>3</v>
-      </c>
       <c r="U208">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V208">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W208">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="X208">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y208">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z208">
         <v>0</v>
       </c>
       <c r="AA208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:27">
+        <v>-0</v>
+      </c>
+      <c r="AB208">
+        <v>-1</v>
+      </c>
+      <c r="AC208">
+        <v>0.9750000000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:29">
       <c r="A209" s="1">
         <v>207</v>
       </c>
       <c r="B209">
-        <v>7127374</v>
+        <v>7126788</v>
       </c>
       <c r="C209" t="s">
         <v>28</v>
@@ -19021,137 +19036,863 @@
         <v>28</v>
       </c>
       <c r="E209" s="2">
-        <v>45340.125</v>
+        <v>45339.23958333334</v>
       </c>
       <c r="F209" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G209" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209">
+        <v>0</v>
+      </c>
+      <c r="J209" t="s">
+        <v>43</v>
       </c>
       <c r="K209">
-        <v>1.909</v>
+        <v>2.625</v>
       </c>
       <c r="L209">
         <v>3.75</v>
       </c>
       <c r="M209">
-        <v>3.6</v>
+        <v>2.375</v>
       </c>
       <c r="N209">
+        <v>2.9</v>
+      </c>
+      <c r="O209">
+        <v>3.8</v>
+      </c>
+      <c r="P209">
+        <v>2.25</v>
+      </c>
+      <c r="Q209">
+        <v>0.25</v>
+      </c>
+      <c r="R209">
+        <v>1.88</v>
+      </c>
+      <c r="S209">
+        <v>2.02</v>
+      </c>
+      <c r="T209">
+        <v>2.75</v>
+      </c>
+      <c r="U209">
         <v>1.85</v>
       </c>
-      <c r="O209">
-        <v>4</v>
-      </c>
-      <c r="P209">
-        <v>3.75</v>
-      </c>
-      <c r="Q209">
+      <c r="V209">
+        <v>2</v>
+      </c>
+      <c r="W209">
+        <v>-1</v>
+      </c>
+      <c r="X209">
+        <v>2.8</v>
+      </c>
+      <c r="Y209">
+        <v>-1</v>
+      </c>
+      <c r="Z209">
+        <v>0.4399999999999999</v>
+      </c>
+      <c r="AA209">
         <v>-0.5</v>
       </c>
-      <c r="R209">
-        <v>1.87</v>
-      </c>
-      <c r="S209">
-        <v>2.03</v>
-      </c>
-      <c r="T209">
-        <v>3</v>
-      </c>
-      <c r="U209">
-        <v>1.95</v>
-      </c>
-      <c r="V209">
-        <v>1.9</v>
-      </c>
-      <c r="W209">
-        <v>0</v>
-      </c>
-      <c r="X209">
-        <v>0</v>
-      </c>
-      <c r="Y209">
-        <v>0</v>
-      </c>
-      <c r="Z209">
-        <v>0</v>
-      </c>
-      <c r="AA209">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="210" spans="1:27">
+      <c r="AB209">
+        <v>-1</v>
+      </c>
+      <c r="AC209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:29">
       <c r="A210" s="1">
         <v>208</v>
       </c>
       <c r="B210">
+        <v>7127373</v>
+      </c>
+      <c r="C210" t="s">
+        <v>28</v>
+      </c>
+      <c r="D210" t="s">
+        <v>28</v>
+      </c>
+      <c r="E210" s="2">
+        <v>45339.32291666666</v>
+      </c>
+      <c r="F210" t="s">
+        <v>34</v>
+      </c>
+      <c r="G210" t="s">
+        <v>39</v>
+      </c>
+      <c r="H210">
+        <v>3</v>
+      </c>
+      <c r="I210">
+        <v>2</v>
+      </c>
+      <c r="J210" t="s">
+        <v>42</v>
+      </c>
+      <c r="K210">
+        <v>2.4</v>
+      </c>
+      <c r="L210">
+        <v>4</v>
+      </c>
+      <c r="M210">
+        <v>2.5</v>
+      </c>
+      <c r="N210">
+        <v>2.4</v>
+      </c>
+      <c r="O210">
+        <v>4.2</v>
+      </c>
+      <c r="P210">
+        <v>2.5</v>
+      </c>
+      <c r="Q210">
+        <v>0</v>
+      </c>
+      <c r="R210">
+        <v>1.925</v>
+      </c>
+      <c r="S210">
+        <v>1.925</v>
+      </c>
+      <c r="T210">
+        <v>3.25</v>
+      </c>
+      <c r="U210">
+        <v>1.95</v>
+      </c>
+      <c r="V210">
+        <v>1.9</v>
+      </c>
+      <c r="W210">
+        <v>1.4</v>
+      </c>
+      <c r="X210">
+        <v>-1</v>
+      </c>
+      <c r="Y210">
+        <v>-1</v>
+      </c>
+      <c r="Z210">
+        <v>0.925</v>
+      </c>
+      <c r="AA210">
+        <v>-1</v>
+      </c>
+      <c r="AB210">
+        <v>0.95</v>
+      </c>
+      <c r="AC210">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:29">
+      <c r="A211" s="1">
+        <v>209</v>
+      </c>
+      <c r="B211">
+        <v>7127374</v>
+      </c>
+      <c r="C211" t="s">
+        <v>28</v>
+      </c>
+      <c r="D211" t="s">
+        <v>28</v>
+      </c>
+      <c r="E211" s="2">
+        <v>45340.125</v>
+      </c>
+      <c r="F211" t="s">
+        <v>36</v>
+      </c>
+      <c r="G211" t="s">
+        <v>30</v>
+      </c>
+      <c r="H211">
+        <v>1</v>
+      </c>
+      <c r="I211">
+        <v>0</v>
+      </c>
+      <c r="J211" t="s">
+        <v>42</v>
+      </c>
+      <c r="K211">
+        <v>1.909</v>
+      </c>
+      <c r="L211">
+        <v>3.75</v>
+      </c>
+      <c r="M211">
+        <v>3.6</v>
+      </c>
+      <c r="N211">
+        <v>2.15</v>
+      </c>
+      <c r="O211">
+        <v>3.6</v>
+      </c>
+      <c r="P211">
+        <v>3.25</v>
+      </c>
+      <c r="Q211">
+        <v>-0.25</v>
+      </c>
+      <c r="R211">
+        <v>1.86</v>
+      </c>
+      <c r="S211">
+        <v>2.04</v>
+      </c>
+      <c r="T211">
+        <v>2.75</v>
+      </c>
+      <c r="U211">
+        <v>1.975</v>
+      </c>
+      <c r="V211">
+        <v>1.875</v>
+      </c>
+      <c r="W211">
+        <v>1.15</v>
+      </c>
+      <c r="X211">
+        <v>-1</v>
+      </c>
+      <c r="Y211">
+        <v>-1</v>
+      </c>
+      <c r="Z211">
+        <v>0.8600000000000001</v>
+      </c>
+      <c r="AA211">
+        <v>-1</v>
+      </c>
+      <c r="AB211">
+        <v>-1</v>
+      </c>
+      <c r="AC211">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="212" spans="1:29">
+      <c r="A212" s="1">
+        <v>210</v>
+      </c>
+      <c r="B212">
+        <v>7127370</v>
+      </c>
+      <c r="C212" t="s">
+        <v>28</v>
+      </c>
+      <c r="D212" t="s">
+        <v>28</v>
+      </c>
+      <c r="E212" s="2">
+        <v>45340.125</v>
+      </c>
+      <c r="F212" t="s">
+        <v>38</v>
+      </c>
+      <c r="G212" t="s">
+        <v>31</v>
+      </c>
+      <c r="H212">
+        <v>1</v>
+      </c>
+      <c r="I212">
+        <v>2</v>
+      </c>
+      <c r="J212" t="s">
+        <v>41</v>
+      </c>
+      <c r="K212">
+        <v>2.4</v>
+      </c>
+      <c r="L212">
+        <v>3.75</v>
+      </c>
+      <c r="M212">
+        <v>2.625</v>
+      </c>
+      <c r="N212">
+        <v>2.375</v>
+      </c>
+      <c r="O212">
+        <v>3.8</v>
+      </c>
+      <c r="P212">
+        <v>2.75</v>
+      </c>
+      <c r="Q212">
+        <v>0</v>
+      </c>
+      <c r="R212">
+        <v>1.8</v>
+      </c>
+      <c r="S212">
+        <v>2.05</v>
+      </c>
+      <c r="T212">
+        <v>3</v>
+      </c>
+      <c r="U212">
+        <v>1.9</v>
+      </c>
+      <c r="V212">
+        <v>1.95</v>
+      </c>
+      <c r="W212">
+        <v>-1</v>
+      </c>
+      <c r="X212">
+        <v>-1</v>
+      </c>
+      <c r="Y212">
+        <v>1.75</v>
+      </c>
+      <c r="Z212">
+        <v>-1</v>
+      </c>
+      <c r="AA212">
+        <v>1.05</v>
+      </c>
+      <c r="AB212">
+        <v>0</v>
+      </c>
+      <c r="AC212">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:29">
+      <c r="A213" s="1">
+        <v>211</v>
+      </c>
+      <c r="B213">
         <v>7661946</v>
       </c>
-      <c r="C210" t="s">
-        <v>28</v>
-      </c>
-      <c r="D210" t="s">
-        <v>28</v>
-      </c>
-      <c r="E210" s="2">
+      <c r="C213" t="s">
+        <v>28</v>
+      </c>
+      <c r="D213" t="s">
+        <v>28</v>
+      </c>
+      <c r="E213" s="2">
         <v>45342.20833333334</v>
       </c>
-      <c r="F210" t="s">
+      <c r="F213" t="s">
         <v>33</v>
       </c>
-      <c r="G210" t="s">
+      <c r="G213" t="s">
         <v>40</v>
       </c>
-      <c r="K210">
+      <c r="K213">
         <v>1.45</v>
       </c>
-      <c r="L210">
+      <c r="L213">
         <v>4.75</v>
       </c>
-      <c r="M210">
+      <c r="M213">
         <v>6.5</v>
       </c>
-      <c r="N210">
-        <v>1.45</v>
-      </c>
-      <c r="O210">
-        <v>4.75</v>
-      </c>
-      <c r="P210">
-        <v>6.5</v>
-      </c>
-      <c r="Q210">
-        <v>-1.25</v>
-      </c>
-      <c r="R210">
-        <v>2</v>
-      </c>
-      <c r="S210">
+      <c r="N213">
+        <v>1.533</v>
+      </c>
+      <c r="O213">
+        <v>4.333</v>
+      </c>
+      <c r="P213">
+        <v>5.75</v>
+      </c>
+      <c r="Q213">
+        <v>-1</v>
+      </c>
+      <c r="R213">
+        <v>1.92</v>
+      </c>
+      <c r="S213">
+        <v>1.98</v>
+      </c>
+      <c r="T213">
+        <v>3</v>
+      </c>
+      <c r="U213">
         <v>1.9</v>
       </c>
-      <c r="T210">
+      <c r="V213">
+        <v>1.95</v>
+      </c>
+      <c r="W213">
+        <v>0</v>
+      </c>
+      <c r="X213">
+        <v>0</v>
+      </c>
+      <c r="Y213">
+        <v>0</v>
+      </c>
+      <c r="Z213">
+        <v>0</v>
+      </c>
+      <c r="AA213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:29">
+      <c r="A214" s="1">
+        <v>212</v>
+      </c>
+      <c r="B214">
+        <v>7127375</v>
+      </c>
+      <c r="C214" t="s">
+        <v>28</v>
+      </c>
+      <c r="D214" t="s">
+        <v>28</v>
+      </c>
+      <c r="E214" s="2">
+        <v>45345.23958333334</v>
+      </c>
+      <c r="F214" t="s">
+        <v>39</v>
+      </c>
+      <c r="G214" t="s">
+        <v>40</v>
+      </c>
+      <c r="K214">
+        <v>2</v>
+      </c>
+      <c r="L214">
+        <v>3.75</v>
+      </c>
+      <c r="M214">
+        <v>3.2</v>
+      </c>
+      <c r="N214">
+        <v>1.909</v>
+      </c>
+      <c r="O214">
+        <v>3.75</v>
+      </c>
+      <c r="P214">
+        <v>3.4</v>
+      </c>
+      <c r="Q214">
+        <v>-0.5</v>
+      </c>
+      <c r="R214">
+        <v>1.99</v>
+      </c>
+      <c r="S214">
+        <v>1.91</v>
+      </c>
+      <c r="T214">
         <v>3</v>
       </c>
-      <c r="U210">
-        <v>1.875</v>
-      </c>
-      <c r="V210">
-        <v>1.975</v>
-      </c>
-      <c r="W210">
+      <c r="U214">
+        <v>1.9</v>
+      </c>
+      <c r="V214">
+        <v>1.95</v>
+      </c>
+      <c r="W214">
         <v>0</v>
       </c>
-      <c r="X210">
+      <c r="X214">
         <v>0</v>
       </c>
-      <c r="Y210">
+      <c r="Y214">
         <v>0</v>
       </c>
-      <c r="Z210">
+      <c r="Z214">
         <v>0</v>
       </c>
-      <c r="AA210">
+      <c r="AA214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:29">
+      <c r="A215" s="1">
+        <v>213</v>
+      </c>
+      <c r="B215">
+        <v>7126789</v>
+      </c>
+      <c r="C215" t="s">
+        <v>28</v>
+      </c>
+      <c r="D215" t="s">
+        <v>28</v>
+      </c>
+      <c r="E215" s="2">
+        <v>45346.14583333334</v>
+      </c>
+      <c r="F215" t="s">
+        <v>35</v>
+      </c>
+      <c r="G215" t="s">
+        <v>37</v>
+      </c>
+      <c r="K215">
+        <v>1.833</v>
+      </c>
+      <c r="L215">
+        <v>4</v>
+      </c>
+      <c r="M215">
+        <v>3.6</v>
+      </c>
+      <c r="N215">
+        <v>1.833</v>
+      </c>
+      <c r="O215">
+        <v>4</v>
+      </c>
+      <c r="P215">
+        <v>3.6</v>
+      </c>
+      <c r="Q215">
+        <v>-0.5</v>
+      </c>
+      <c r="R215">
+        <v>1.89</v>
+      </c>
+      <c r="S215">
+        <v>2.01</v>
+      </c>
+      <c r="T215">
+        <v>3.25</v>
+      </c>
+      <c r="U215">
+        <v>1.825</v>
+      </c>
+      <c r="V215">
+        <v>2.025</v>
+      </c>
+      <c r="W215">
+        <v>0</v>
+      </c>
+      <c r="X215">
+        <v>0</v>
+      </c>
+      <c r="Y215">
+        <v>0</v>
+      </c>
+      <c r="Z215">
+        <v>0</v>
+      </c>
+      <c r="AA215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:29">
+      <c r="A216" s="1">
+        <v>214</v>
+      </c>
+      <c r="B216">
+        <v>7127376</v>
+      </c>
+      <c r="C216" t="s">
+        <v>28</v>
+      </c>
+      <c r="D216" t="s">
+        <v>28</v>
+      </c>
+      <c r="E216" s="2">
+        <v>45346.16666666666</v>
+      </c>
+      <c r="F216" t="s">
+        <v>29</v>
+      </c>
+      <c r="G216" t="s">
+        <v>38</v>
+      </c>
+      <c r="K216">
+        <v>2.375</v>
+      </c>
+      <c r="L216">
+        <v>3.6</v>
+      </c>
+      <c r="M216">
+        <v>2.7</v>
+      </c>
+      <c r="N216">
+        <v>2.15</v>
+      </c>
+      <c r="O216">
+        <v>3.8</v>
+      </c>
+      <c r="P216">
+        <v>3</v>
+      </c>
+      <c r="Q216">
+        <v>-0.25</v>
+      </c>
+      <c r="R216">
+        <v>1.88</v>
+      </c>
+      <c r="S216">
+        <v>2.02</v>
+      </c>
+      <c r="T216">
+        <v>3.25</v>
+      </c>
+      <c r="U216">
+        <v>2</v>
+      </c>
+      <c r="V216">
+        <v>1.85</v>
+      </c>
+      <c r="W216">
+        <v>0</v>
+      </c>
+      <c r="X216">
+        <v>0</v>
+      </c>
+      <c r="Y216">
+        <v>0</v>
+      </c>
+      <c r="Z216">
+        <v>0</v>
+      </c>
+      <c r="AA216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:29">
+      <c r="A217" s="1">
+        <v>215</v>
+      </c>
+      <c r="B217">
+        <v>7127377</v>
+      </c>
+      <c r="C217" t="s">
+        <v>28</v>
+      </c>
+      <c r="D217" t="s">
+        <v>28</v>
+      </c>
+      <c r="E217" s="2">
+        <v>45346.23958333334</v>
+      </c>
+      <c r="F217" t="s">
+        <v>32</v>
+      </c>
+      <c r="G217" t="s">
+        <v>30</v>
+      </c>
+      <c r="K217">
+        <v>2.8</v>
+      </c>
+      <c r="L217">
+        <v>3.6</v>
+      </c>
+      <c r="M217">
+        <v>2.25</v>
+      </c>
+      <c r="N217">
+        <v>2.375</v>
+      </c>
+      <c r="O217">
+        <v>3.75</v>
+      </c>
+      <c r="P217">
+        <v>2.55</v>
+      </c>
+      <c r="Q217">
+        <v>0</v>
+      </c>
+      <c r="R217">
+        <v>1.82</v>
+      </c>
+      <c r="S217">
+        <v>2.08</v>
+      </c>
+      <c r="T217">
+        <v>3.25</v>
+      </c>
+      <c r="U217">
+        <v>1.925</v>
+      </c>
+      <c r="V217">
+        <v>1.925</v>
+      </c>
+      <c r="W217">
+        <v>0</v>
+      </c>
+      <c r="X217">
+        <v>0</v>
+      </c>
+      <c r="Y217">
+        <v>0</v>
+      </c>
+      <c r="Z217">
+        <v>0</v>
+      </c>
+      <c r="AA217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:29">
+      <c r="A218" s="1">
+        <v>216</v>
+      </c>
+      <c r="B218">
+        <v>7127378</v>
+      </c>
+      <c r="C218" t="s">
+        <v>28</v>
+      </c>
+      <c r="D218" t="s">
+        <v>28</v>
+      </c>
+      <c r="E218" s="2">
+        <v>45346.32291666666</v>
+      </c>
+      <c r="F218" t="s">
+        <v>34</v>
+      </c>
+      <c r="G218" t="s">
+        <v>31</v>
+      </c>
+      <c r="K218">
+        <v>2.6</v>
+      </c>
+      <c r="L218">
+        <v>3.5</v>
+      </c>
+      <c r="M218">
+        <v>2.5</v>
+      </c>
+      <c r="N218">
+        <v>2.7</v>
+      </c>
+      <c r="O218">
+        <v>3.5</v>
+      </c>
+      <c r="P218">
+        <v>2.5</v>
+      </c>
+      <c r="Q218">
+        <v>0</v>
+      </c>
+      <c r="R218">
+        <v>1.98</v>
+      </c>
+      <c r="S218">
+        <v>1.92</v>
+      </c>
+      <c r="T218">
+        <v>3</v>
+      </c>
+      <c r="U218">
+        <v>1.925</v>
+      </c>
+      <c r="V218">
+        <v>1.925</v>
+      </c>
+      <c r="W218">
+        <v>0</v>
+      </c>
+      <c r="X218">
+        <v>0</v>
+      </c>
+      <c r="Y218">
+        <v>0</v>
+      </c>
+      <c r="Z218">
+        <v>0</v>
+      </c>
+      <c r="AA218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:29">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219">
+        <v>7127379</v>
+      </c>
+      <c r="C219" t="s">
+        <v>28</v>
+      </c>
+      <c r="D219" t="s">
+        <v>28</v>
+      </c>
+      <c r="E219" s="2">
+        <v>45347.125</v>
+      </c>
+      <c r="F219" t="s">
+        <v>33</v>
+      </c>
+      <c r="G219" t="s">
+        <v>36</v>
+      </c>
+      <c r="K219">
+        <v>2</v>
+      </c>
+      <c r="L219">
+        <v>3.6</v>
+      </c>
+      <c r="M219">
+        <v>3.4</v>
+      </c>
+      <c r="N219">
+        <v>2.05</v>
+      </c>
+      <c r="O219">
+        <v>3.6</v>
+      </c>
+      <c r="P219">
+        <v>3.3</v>
+      </c>
+      <c r="Q219">
+        <v>-0.25</v>
+      </c>
+      <c r="R219">
+        <v>1.82</v>
+      </c>
+      <c r="S219">
+        <v>2.08</v>
+      </c>
+      <c r="T219">
+        <v>3</v>
+      </c>
+      <c r="U219">
+        <v>2</v>
+      </c>
+      <c r="V219">
+        <v>1.85</v>
+      </c>
+      <c r="W219">
+        <v>0</v>
+      </c>
+      <c r="X219">
+        <v>0</v>
+      </c>
+      <c r="Y219">
+        <v>0</v>
+      </c>
+      <c r="Z219">
+        <v>0</v>
+      </c>
+      <c r="AA219">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 19-02-2024 às 20:58
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -121,10 +121,10 @@
     <t>Perth Glory</t>
   </si>
   <si>
-    <t>Sydney FC</t>
+    <t>Central Coast Mariners</t>
   </si>
   <si>
-    <t>Central Coast Mariners</t>
+    <t>Sydney FC</t>
   </si>
   <si>
     <t>Melbourne City</t>
@@ -619,7 +619,7 @@
         <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5400034</v>
+        <v>5404672</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -1153,25 +1153,25 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
         <v>0</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
       <c r="J8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K8">
-        <v>1.95</v>
+        <v>2.15</v>
       </c>
       <c r="L8">
         <v>3.6</v>
       </c>
       <c r="M8">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="N8">
         <v>1.909</v>
@@ -1195,31 +1195,31 @@
         <v>3</v>
       </c>
       <c r="U8">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V8">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W8">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X8">
         <v>-1</v>
       </c>
       <c r="Y8">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z8">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA8">
+        <v>-1</v>
+      </c>
+      <c r="AB8">
         <v>0.925</v>
       </c>
-      <c r="AB8">
-        <v>-1</v>
-      </c>
       <c r="AC8">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1227,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5404672</v>
+        <v>5400034</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -1242,25 +1242,25 @@
         <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K9">
-        <v>2.15</v>
+        <v>1.95</v>
       </c>
       <c r="L9">
         <v>3.6</v>
       </c>
       <c r="M9">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="N9">
         <v>1.909</v>
@@ -1284,31 +1284,31 @@
         <v>3</v>
       </c>
       <c r="U9">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V9">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W9">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X9">
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z9">
+        <v>-1</v>
+      </c>
+      <c r="AA9">
         <v>0.925</v>
       </c>
-      <c r="AA9">
-        <v>-1</v>
-      </c>
       <c r="AB9">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC9">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -1598,7 +1598,7 @@
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1865,7 +1865,7 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -2221,7 +2221,7 @@
         <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2488,7 +2488,7 @@
         <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -2666,7 +2666,7 @@
         <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>44954.23958333334</v>
       </c>
       <c r="F29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G29" t="s">
         <v>30</v>
@@ -3274,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>5400042</v>
+        <v>5400043</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -3286,58 +3286,58 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" t="s">
         <v>42</v>
       </c>
       <c r="K32">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="L32">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M32">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N32">
-        <v>1.333</v>
+        <v>2.2</v>
       </c>
       <c r="O32">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P32">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="Q32">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R32">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S32">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T32">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U32">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V32">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W32">
-        <v>0.333</v>
+        <v>1.2</v>
       </c>
       <c r="X32">
         <v>-1</v>
@@ -3346,13 +3346,13 @@
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC32">
         <v>-1</v>
@@ -3363,7 +3363,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5400043</v>
+        <v>5400042</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -3375,58 +3375,58 @@
         <v>44961.125</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="s">
         <v>42</v>
       </c>
       <c r="K33">
-        <v>2.15</v>
+        <v>1.533</v>
       </c>
       <c r="L33">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M33">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="N33">
-        <v>2.2</v>
+        <v>1.333</v>
       </c>
       <c r="O33">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="P33">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="Q33">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R33">
+        <v>1.85</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
+      </c>
+      <c r="T33">
+        <v>3.25</v>
+      </c>
+      <c r="U33">
+        <v>1.875</v>
+      </c>
+      <c r="V33">
         <v>1.975</v>
       </c>
-      <c r="S33">
-        <v>1.875</v>
-      </c>
-      <c r="T33">
-        <v>3</v>
-      </c>
-      <c r="U33">
-        <v>1.95</v>
-      </c>
-      <c r="V33">
-        <v>1.9</v>
-      </c>
       <c r="W33">
-        <v>1.2</v>
+        <v>0.333</v>
       </c>
       <c r="X33">
         <v>-1</v>
@@ -3435,13 +3435,13 @@
         <v>-1</v>
       </c>
       <c r="Z33">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA33">
         <v>-1</v>
       </c>
       <c r="AB33">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC33">
         <v>-1</v>
@@ -3734,7 +3734,7 @@
         <v>39</v>
       </c>
       <c r="G37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -3912,7 +3912,7 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -4354,7 +4354,7 @@
         <v>44975.125</v>
       </c>
       <c r="F44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G44" t="s">
         <v>39</v>
@@ -4624,7 +4624,7 @@
         <v>34</v>
       </c>
       <c r="G47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -4799,7 +4799,7 @@
         <v>44981.23958333334</v>
       </c>
       <c r="F49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G49" t="s">
         <v>31</v>
@@ -4876,7 +4876,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>5404699</v>
+        <v>5400048</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4888,73 +4888,73 @@
         <v>44982.125</v>
       </c>
       <c r="F50" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G50" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J50" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K50">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="L50">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="M50">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="N50">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="O50">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P50">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="Q50">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R50">
-        <v>1.94</v>
+        <v>2.025</v>
       </c>
       <c r="S50">
-        <v>1.96</v>
+        <v>1.825</v>
       </c>
       <c r="T50">
         <v>2.75</v>
       </c>
       <c r="U50">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V50">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W50">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X50">
         <v>-1</v>
       </c>
       <c r="Y50">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z50">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA50">
-        <v>0.96</v>
+        <v>-0.5</v>
       </c>
       <c r="AB50">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC50">
         <v>-1</v>
@@ -4965,7 +4965,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>5400048</v>
+        <v>5404699</v>
       </c>
       <c r="C51" t="s">
         <v>28</v>
@@ -4977,73 +4977,73 @@
         <v>44982.125</v>
       </c>
       <c r="F51" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G51" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
         <v>3</v>
       </c>
-      <c r="I51">
-        <v>2</v>
-      </c>
       <c r="J51" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K51">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="L51">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="M51">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="N51">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="O51">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P51">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="Q51">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R51">
-        <v>2.025</v>
+        <v>1.94</v>
       </c>
       <c r="S51">
-        <v>1.825</v>
+        <v>1.96</v>
       </c>
       <c r="T51">
         <v>2.75</v>
       </c>
       <c r="U51">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V51">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W51">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X51">
         <v>-1</v>
       </c>
       <c r="Y51">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z51">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA51">
-        <v>-0.5</v>
+        <v>0.96</v>
       </c>
       <c r="AB51">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC51">
         <v>-1</v>
@@ -5514,7 +5514,7 @@
         <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H57">
         <v>2</v>
@@ -5689,7 +5689,7 @@
         <v>44989.23958333334</v>
       </c>
       <c r="F59" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G59" t="s">
         <v>33</v>
@@ -5956,7 +5956,7 @@
         <v>44996.125</v>
       </c>
       <c r="F62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G62" t="s">
         <v>38</v>
@@ -6137,7 +6137,7 @@
         <v>31</v>
       </c>
       <c r="G64" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -6478,7 +6478,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5404713</v>
+        <v>5404714</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6490,76 +6490,76 @@
         <v>45003.125</v>
       </c>
       <c r="F68" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G68" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K68">
         <v>2.25</v>
       </c>
       <c r="L68">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M68">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N68">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="O68">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P68">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q68">
         <v>-0.25</v>
       </c>
       <c r="R68">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S68">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T68">
         <v>2.75</v>
       </c>
       <c r="U68">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V68">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W68">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X68">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y68">
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA68">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB68">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC68">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6567,7 +6567,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>5404714</v>
+        <v>5404713</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6579,76 +6579,76 @@
         <v>45003.125</v>
       </c>
       <c r="F69" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G69" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K69">
         <v>2.25</v>
       </c>
       <c r="L69">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M69">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="N69">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O69">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P69">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S69">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T69">
         <v>2.75</v>
       </c>
       <c r="U69">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V69">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W69">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X69">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA69">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB69">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC69">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -6668,7 +6668,7 @@
         <v>45003.23958333334</v>
       </c>
       <c r="F70" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G70" t="s">
         <v>30</v>
@@ -6760,7 +6760,7 @@
         <v>33</v>
       </c>
       <c r="G71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H71">
         <v>2</v>
@@ -7113,7 +7113,7 @@
         <v>45017.125</v>
       </c>
       <c r="F75" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G75" t="s">
         <v>39</v>
@@ -7202,7 +7202,7 @@
         <v>45017.23958333334</v>
       </c>
       <c r="F76" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G76" t="s">
         <v>40</v>
@@ -7472,7 +7472,7 @@
         <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -7561,7 +7561,7 @@
         <v>32</v>
       </c>
       <c r="G80" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -8092,7 +8092,7 @@
         <v>45031.16666666666</v>
       </c>
       <c r="F86" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G86" t="s">
         <v>37</v>
@@ -8359,7 +8359,7 @@
         <v>45032.08333333334</v>
       </c>
       <c r="F89" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G89" t="s">
         <v>34</v>
@@ -8629,7 +8629,7 @@
         <v>29</v>
       </c>
       <c r="G92" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -8985,7 +8985,7 @@
         <v>39</v>
       </c>
       <c r="G96" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97">
+        <v>1.75</v>
+      </c>
+      <c r="L97">
+        <v>3.8</v>
+      </c>
+      <c r="M97">
         <v>4</v>
       </c>
-      <c r="J97" t="s">
-        <v>41</v>
-      </c>
-      <c r="K97">
-        <v>2.3</v>
-      </c>
-      <c r="L97">
-        <v>3.75</v>
-      </c>
-      <c r="M97">
-        <v>2.75</v>
-      </c>
       <c r="N97">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q97">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R97">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S97">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T97">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U97">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V97">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W97">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X97">
         <v>-1</v>
       </c>
       <c r="Y97">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z97">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA97">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB97">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K98">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L98">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M98">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N98">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q98">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R98">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S98">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T98">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U98">
+        <v>2</v>
+      </c>
+      <c r="V98">
         <v>1.85</v>
       </c>
-      <c r="V98">
-        <v>2</v>
-      </c>
       <c r="W98">
+        <v>-1</v>
+      </c>
+      <c r="X98">
+        <v>-1</v>
+      </c>
+      <c r="Y98">
+        <v>1.4</v>
+      </c>
+      <c r="Z98">
+        <v>-1</v>
+      </c>
+      <c r="AA98">
+        <v>0.8</v>
+      </c>
+      <c r="AB98">
         <v>1</v>
-      </c>
-      <c r="X98">
-        <v>-1</v>
-      </c>
-      <c r="Y98">
-        <v>-1</v>
-      </c>
-      <c r="Z98">
-        <v>1.025</v>
-      </c>
-      <c r="AA98">
-        <v>-1</v>
-      </c>
-      <c r="AB98">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -9249,7 +9249,7 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F99" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G99" t="s">
         <v>29</v>
@@ -9697,7 +9697,7 @@
         <v>30</v>
       </c>
       <c r="G104" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -9783,7 +9783,7 @@
         <v>45058.28125</v>
       </c>
       <c r="F105" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G105" t="s">
         <v>37</v>
@@ -9875,7 +9875,7 @@
         <v>32</v>
       </c>
       <c r="G106" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -9964,7 +9964,7 @@
         <v>37</v>
       </c>
       <c r="G107" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H107">
         <v>4</v>
@@ -10050,7 +10050,7 @@
         <v>45066.28125</v>
       </c>
       <c r="F108" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G108" t="s">
         <v>32</v>
@@ -10142,7 +10142,7 @@
         <v>37</v>
       </c>
       <c r="G109" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -10231,7 +10231,7 @@
         <v>32</v>
       </c>
       <c r="G110" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H110">
         <v>3</v>
@@ -10495,7 +10495,7 @@
         <v>45220.23958333334</v>
       </c>
       <c r="F113" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G113" t="s">
         <v>33</v>
@@ -10765,7 +10765,7 @@
         <v>39</v>
       </c>
       <c r="G116" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -11029,7 +11029,7 @@
         <v>45228.04166666666</v>
       </c>
       <c r="F119" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G119" t="s">
         <v>38</v>
@@ -11299,7 +11299,7 @@
         <v>37</v>
       </c>
       <c r="G122" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H122">
         <v>2</v>
@@ -11655,7 +11655,7 @@
         <v>34</v>
       </c>
       <c r="G126" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H126">
         <v>2</v>
@@ -12100,7 +12100,7 @@
         <v>32</v>
       </c>
       <c r="G131" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -12275,7 +12275,7 @@
         <v>45242.125</v>
       </c>
       <c r="F133" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G133" t="s">
         <v>39</v>
@@ -12542,7 +12542,7 @@
         <v>45255.23958333334</v>
       </c>
       <c r="F136" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G136" t="s">
         <v>30</v>
@@ -12987,7 +12987,7 @@
         <v>45262.23958333334</v>
       </c>
       <c r="F141" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G141" t="s">
         <v>34</v>
@@ -13076,7 +13076,7 @@
         <v>45263.04166666666</v>
       </c>
       <c r="F142" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G142" t="s">
         <v>33</v>
@@ -13343,7 +13343,7 @@
         <v>45268.23958333334</v>
       </c>
       <c r="F145" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G145" t="s">
         <v>40</v>
@@ -13610,7 +13610,7 @@
         <v>45269.23958333334</v>
       </c>
       <c r="F148" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G148" t="s">
         <v>38</v>
@@ -14147,7 +14147,7 @@
         <v>33</v>
       </c>
       <c r="G154" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H154">
         <v>3</v>
@@ -14236,7 +14236,7 @@
         <v>37</v>
       </c>
       <c r="G155" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H155">
         <v>3</v>
@@ -14414,7 +14414,7 @@
         <v>39</v>
       </c>
       <c r="G157" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -14678,7 +14678,7 @@
         <v>45283.14583333334</v>
       </c>
       <c r="F160" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G160" t="s">
         <v>40</v>
@@ -15034,7 +15034,7 @@
         <v>45289.23958333334</v>
       </c>
       <c r="F164" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G164" t="s">
         <v>31</v>
@@ -15301,7 +15301,7 @@
         <v>45291.20833333334</v>
       </c>
       <c r="F167" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G167" t="s">
         <v>34</v>
@@ -15660,7 +15660,7 @@
         <v>30</v>
       </c>
       <c r="G171" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H171">
         <v>0</v>
@@ -15749,7 +15749,7 @@
         <v>39</v>
       </c>
       <c r="G172" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H172">
         <v>1</v>
@@ -16280,7 +16280,7 @@
         <v>45304.13541666666</v>
       </c>
       <c r="F178" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G178" t="s">
         <v>33</v>
@@ -16369,7 +16369,7 @@
         <v>45304.25</v>
       </c>
       <c r="F179" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G179" t="s">
         <v>32</v>
@@ -16814,7 +16814,7 @@
         <v>45310.23958333334</v>
       </c>
       <c r="F184" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G184" t="s">
         <v>29</v>
@@ -16992,7 +16992,7 @@
         <v>45312.16666666666</v>
       </c>
       <c r="F186" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G186" t="s">
         <v>37</v>
@@ -17262,7 +17262,7 @@
         <v>33</v>
       </c>
       <c r="G189" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H189">
         <v>1</v>
@@ -17526,7 +17526,7 @@
         <v>45318.23958333334</v>
       </c>
       <c r="F192" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G192" t="s">
         <v>39</v>
@@ -17885,7 +17885,7 @@
         <v>40</v>
       </c>
       <c r="G196" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H196">
         <v>2</v>
@@ -18063,7 +18063,7 @@
         <v>32</v>
       </c>
       <c r="G198" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H198">
         <v>0</v>
@@ -18241,7 +18241,7 @@
         <v>31</v>
       </c>
       <c r="G200" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H200">
         <v>0</v>
@@ -18683,10 +18683,10 @@
         <v>45332.23958333334</v>
       </c>
       <c r="F205" t="s">
+        <v>35</v>
+      </c>
+      <c r="G205" t="s">
         <v>36</v>
-      </c>
-      <c r="G205" t="s">
-        <v>35</v>
       </c>
       <c r="H205">
         <v>1</v>
@@ -18950,7 +18950,7 @@
         <v>45339.16666666666</v>
       </c>
       <c r="F208" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G208" t="s">
         <v>32</v>
@@ -19217,7 +19217,7 @@
         <v>45340.125</v>
       </c>
       <c r="F211" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G211" t="s">
         <v>30</v>
@@ -19410,31 +19410,31 @@
         <v>6.5</v>
       </c>
       <c r="N213">
-        <v>1.533</v>
+        <v>1.5</v>
       </c>
       <c r="O213">
         <v>4.333</v>
       </c>
       <c r="P213">
-        <v>5.75</v>
+        <v>6.5</v>
       </c>
       <c r="Q213">
-        <v>-1</v>
+        <v>-1.25</v>
       </c>
       <c r="R213">
-        <v>1.92</v>
+        <v>2.08</v>
       </c>
       <c r="S213">
-        <v>1.98</v>
+        <v>1.82</v>
       </c>
       <c r="T213">
         <v>3</v>
       </c>
       <c r="U213">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="V213">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="W213">
         <v>0</v>
@@ -19487,7 +19487,7 @@
         <v>1.909</v>
       </c>
       <c r="O214">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="P214">
         <v>3.4</v>
@@ -19502,13 +19502,13 @@
         <v>1.91</v>
       </c>
       <c r="T214">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U214">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="V214">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="W214">
         <v>0</v>
@@ -19543,7 +19543,7 @@
         <v>45346.14583333334</v>
       </c>
       <c r="F215" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G215" t="s">
         <v>37</v>
@@ -19558,7 +19558,7 @@
         <v>3.6</v>
       </c>
       <c r="N215">
-        <v>1.833</v>
+        <v>1.8</v>
       </c>
       <c r="O215">
         <v>4</v>
@@ -19570,10 +19570,10 @@
         <v>-0.5</v>
       </c>
       <c r="R215">
-        <v>1.89</v>
+        <v>1.86</v>
       </c>
       <c r="S215">
-        <v>2.01</v>
+        <v>2.04</v>
       </c>
       <c r="T215">
         <v>3.25</v>
@@ -19605,7 +19605,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>7127376</v>
+        <v>7127377</v>
       </c>
       <c r="C216" t="s">
         <v>28</v>
@@ -19614,49 +19614,49 @@
         <v>28</v>
       </c>
       <c r="E216" s="2">
-        <v>45346.16666666666</v>
+        <v>45346.23958333334</v>
       </c>
       <c r="F216" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G216" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K216">
-        <v>2.375</v>
+        <v>2.8</v>
       </c>
       <c r="L216">
         <v>3.6</v>
       </c>
       <c r="M216">
-        <v>2.7</v>
+        <v>2.25</v>
       </c>
       <c r="N216">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O216">
         <v>3.8</v>
       </c>
       <c r="P216">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="Q216">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R216">
-        <v>1.88</v>
+        <v>1.85</v>
       </c>
       <c r="S216">
-        <v>2.02</v>
+        <v>2.05</v>
       </c>
       <c r="T216">
         <v>3.25</v>
       </c>
       <c r="U216">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V216">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W216">
         <v>0</v>
@@ -19679,7 +19679,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>7127377</v>
+        <v>7127378</v>
       </c>
       <c r="C217" t="s">
         <v>28</v>
@@ -19688,28 +19688,28 @@
         <v>28</v>
       </c>
       <c r="E217" s="2">
-        <v>45346.23958333334</v>
+        <v>45346.32291666666</v>
       </c>
       <c r="F217" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G217" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K217">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="L217">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M217">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="N217">
-        <v>2.375</v>
+        <v>2.6</v>
       </c>
       <c r="O217">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="P217">
         <v>2.55</v>
@@ -19718,19 +19718,19 @@
         <v>0</v>
       </c>
       <c r="R217">
-        <v>1.82</v>
+        <v>1.95</v>
       </c>
       <c r="S217">
-        <v>2.08</v>
+        <v>1.95</v>
       </c>
       <c r="T217">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U217">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V217">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W217">
         <v>0</v>
@@ -19753,7 +19753,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>7127378</v>
+        <v>7127376</v>
       </c>
       <c r="C218" t="s">
         <v>28</v>
@@ -19762,43 +19762,43 @@
         <v>28</v>
       </c>
       <c r="E218" s="2">
-        <v>45346.32291666666</v>
+        <v>45347.125</v>
       </c>
       <c r="F218" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G218" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K218">
-        <v>2.6</v>
+        <v>2.375</v>
       </c>
       <c r="L218">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M218">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="N218">
-        <v>2.7</v>
+        <v>2</v>
       </c>
       <c r="O218">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P218">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="Q218">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R218">
-        <v>1.98</v>
+        <v>2.06</v>
       </c>
       <c r="S218">
-        <v>1.92</v>
+        <v>1.84</v>
       </c>
       <c r="T218">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U218">
         <v>1.925</v>
@@ -19842,7 +19842,7 @@
         <v>33</v>
       </c>
       <c r="G219" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K219">
         <v>2</v>
@@ -19854,22 +19854,22 @@
         <v>3.4</v>
       </c>
       <c r="N219">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="O219">
         <v>3.6</v>
       </c>
       <c r="P219">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="Q219">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R219">
-        <v>1.82</v>
+        <v>2.01</v>
       </c>
       <c r="S219">
-        <v>2.08</v>
+        <v>1.89</v>
       </c>
       <c r="T219">
         <v>3</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 20-02-2024 às 23:00
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -121,10 +121,10 @@
     <t>Perth Glory</t>
   </si>
   <si>
-    <t>Central Coast Mariners</t>
+    <t>Sydney FC</t>
   </si>
   <si>
-    <t>Sydney FC</t>
+    <t>Central Coast Mariners</t>
   </si>
   <si>
     <t>Melbourne City</t>
@@ -619,7 +619,7 @@
         <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1138,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>5404672</v>
+        <v>5400034</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
@@ -1153,25 +1153,25 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8">
-        <v>2.15</v>
+        <v>1.95</v>
       </c>
       <c r="L8">
         <v>3.6</v>
       </c>
       <c r="M8">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="N8">
         <v>1.909</v>
@@ -1195,31 +1195,31 @@
         <v>3</v>
       </c>
       <c r="U8">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V8">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W8">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X8">
         <v>-1</v>
       </c>
       <c r="Y8">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="Z8">
+        <v>-1</v>
+      </c>
+      <c r="AA8">
         <v>0.925</v>
       </c>
-      <c r="AA8">
-        <v>-1</v>
-      </c>
       <c r="AB8">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC8">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1227,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5400034</v>
+        <v>5404672</v>
       </c>
       <c r="C9" t="s">
         <v>28</v>
@@ -1242,25 +1242,25 @@
         <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
       <c r="J9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K9">
-        <v>1.95</v>
+        <v>2.15</v>
       </c>
       <c r="L9">
         <v>3.6</v>
       </c>
       <c r="M9">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="N9">
         <v>1.909</v>
@@ -1284,31 +1284,31 @@
         <v>3</v>
       </c>
       <c r="U9">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V9">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W9">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X9">
         <v>-1</v>
       </c>
       <c r="Y9">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Z9">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA9">
+        <v>-1</v>
+      </c>
+      <c r="AB9">
         <v>0.925</v>
       </c>
-      <c r="AB9">
-        <v>-1</v>
-      </c>
       <c r="AC9">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -1598,7 +1598,7 @@
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1865,7 +1865,7 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H16">
         <v>2</v>
@@ -2221,7 +2221,7 @@
         <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2488,7 +2488,7 @@
         <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H23">
         <v>2</v>
@@ -2666,7 +2666,7 @@
         <v>33</v>
       </c>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -3019,7 +3019,7 @@
         <v>44954.23958333334</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
         <v>30</v>
@@ -3286,10 +3286,10 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" t="s">
         <v>36</v>
-      </c>
-      <c r="G32" t="s">
-        <v>35</v>
       </c>
       <c r="H32">
         <v>3</v>
@@ -3734,7 +3734,7 @@
         <v>39</v>
       </c>
       <c r="G37" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H37">
         <v>1</v>
@@ -3912,7 +3912,7 @@
         <v>30</v>
       </c>
       <c r="G39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -4354,7 +4354,7 @@
         <v>44975.125</v>
       </c>
       <c r="F44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G44" t="s">
         <v>39</v>
@@ -4624,7 +4624,7 @@
         <v>34</v>
       </c>
       <c r="G47" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -4799,7 +4799,7 @@
         <v>44981.23958333334</v>
       </c>
       <c r="F49" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G49" t="s">
         <v>31</v>
@@ -4891,7 +4891,7 @@
         <v>37</v>
       </c>
       <c r="G50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H50">
         <v>3</v>
@@ -5499,7 +5499,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5404704</v>
+        <v>5404706</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5511,58 +5511,58 @@
         <v>44989.125</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="s">
         <v>42</v>
       </c>
       <c r="K57">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L57">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M57">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="N57">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O57">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P57">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q57">
         <v>-0.25</v>
       </c>
       <c r="R57">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S57">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T57">
         <v>2.75</v>
       </c>
       <c r="U57">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V57">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W57">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="X57">
         <v>-1</v>
@@ -5571,16 +5571,16 @@
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0.875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA57">
         <v>-1</v>
       </c>
       <c r="AB57">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AC57">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5588,7 +5588,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5404706</v>
+        <v>5404704</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5600,58 +5600,58 @@
         <v>44989.125</v>
       </c>
       <c r="F58" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>42</v>
       </c>
       <c r="K58">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="L58">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M58">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="N58">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="O58">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P58">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q58">
         <v>-0.25</v>
       </c>
       <c r="R58">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S58">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T58">
         <v>2.75</v>
       </c>
       <c r="U58">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V58">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W58">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="X58">
         <v>-1</v>
@@ -5660,16 +5660,16 @@
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.8500000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AA58">
         <v>-1</v>
       </c>
       <c r="AB58">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AC58">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -5689,7 +5689,7 @@
         <v>44989.23958333334</v>
       </c>
       <c r="F59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G59" t="s">
         <v>33</v>
@@ -5956,7 +5956,7 @@
         <v>44996.125</v>
       </c>
       <c r="F62" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G62" t="s">
         <v>38</v>
@@ -6137,7 +6137,7 @@
         <v>31</v>
       </c>
       <c r="G64" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H64">
         <v>1</v>
@@ -6668,7 +6668,7 @@
         <v>45003.23958333334</v>
       </c>
       <c r="F70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G70" t="s">
         <v>30</v>
@@ -6760,7 +6760,7 @@
         <v>33</v>
       </c>
       <c r="G71" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H71">
         <v>2</v>
@@ -7113,7 +7113,7 @@
         <v>45017.125</v>
       </c>
       <c r="F75" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G75" t="s">
         <v>39</v>
@@ -7202,7 +7202,7 @@
         <v>45017.23958333334</v>
       </c>
       <c r="F76" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G76" t="s">
         <v>40</v>
@@ -7472,7 +7472,7 @@
         <v>40</v>
       </c>
       <c r="G79" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -7561,7 +7561,7 @@
         <v>32</v>
       </c>
       <c r="G80" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H80">
         <v>1</v>
@@ -8092,7 +8092,7 @@
         <v>45031.16666666666</v>
       </c>
       <c r="F86" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G86" t="s">
         <v>37</v>
@@ -8359,7 +8359,7 @@
         <v>45032.08333333334</v>
       </c>
       <c r="F89" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G89" t="s">
         <v>34</v>
@@ -8629,7 +8629,7 @@
         <v>29</v>
       </c>
       <c r="G92" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H92">
         <v>1</v>
@@ -8985,7 +8985,7 @@
         <v>39</v>
       </c>
       <c r="G96" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G97" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H97">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K97">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L97">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M97">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N97">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q97">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R97">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S97">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T97">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U97">
+        <v>2</v>
+      </c>
+      <c r="V97">
         <v>1.85</v>
       </c>
-      <c r="V97">
-        <v>2</v>
-      </c>
       <c r="W97">
+        <v>-1</v>
+      </c>
+      <c r="X97">
+        <v>-1</v>
+      </c>
+      <c r="Y97">
+        <v>1.4</v>
+      </c>
+      <c r="Z97">
+        <v>-1</v>
+      </c>
+      <c r="AA97">
+        <v>0.8</v>
+      </c>
+      <c r="AB97">
         <v>1</v>
-      </c>
-      <c r="X97">
-        <v>-1</v>
-      </c>
-      <c r="Y97">
-        <v>-1</v>
-      </c>
-      <c r="Z97">
-        <v>1.025</v>
-      </c>
-      <c r="AA97">
-        <v>-1</v>
-      </c>
-      <c r="AB97">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G98" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="J98" t="s">
+        <v>42</v>
+      </c>
+      <c r="K98">
+        <v>1.75</v>
+      </c>
+      <c r="L98">
+        <v>3.8</v>
+      </c>
+      <c r="M98">
         <v>4</v>
       </c>
-      <c r="J98" t="s">
-        <v>41</v>
-      </c>
-      <c r="K98">
-        <v>2.3</v>
-      </c>
-      <c r="L98">
-        <v>3.75</v>
-      </c>
-      <c r="M98">
-        <v>2.75</v>
-      </c>
       <c r="N98">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q98">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R98">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S98">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T98">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U98">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V98">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W98">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X98">
         <v>-1</v>
       </c>
       <c r="Y98">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA98">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB98">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -9237,7 +9237,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5400064</v>
+        <v>5404735</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -9249,40 +9249,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F99" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G99" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H99">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K99">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L99">
+        <v>3.75</v>
+      </c>
+      <c r="M99">
+        <v>1.909</v>
+      </c>
+      <c r="N99">
         <v>4</v>
       </c>
-      <c r="M99">
-        <v>4.5</v>
-      </c>
-      <c r="N99">
-        <v>1.533</v>
-      </c>
       <c r="O99">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="P99">
-        <v>5.5</v>
+        <v>1.833</v>
       </c>
       <c r="Q99">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R99">
         <v>2.025</v>
@@ -9291,34 +9291,34 @@
         <v>1.825</v>
       </c>
       <c r="T99">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="U99">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V99">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W99">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X99">
         <v>-1</v>
       </c>
       <c r="Y99">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Z99">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA99">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB99">
         <v>-1</v>
       </c>
       <c r="AC99">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="100" spans="1:29">
@@ -9326,7 +9326,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>5404735</v>
+        <v>5400064</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -9338,40 +9338,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F100" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G100" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H100">
+        <v>2</v>
+      </c>
+      <c r="I100">
         <v>0</v>
       </c>
-      <c r="I100">
-        <v>1</v>
-      </c>
       <c r="J100" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K100">
-        <v>3.6</v>
+        <v>1.65</v>
       </c>
       <c r="L100">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M100">
-        <v>1.909</v>
+        <v>4.5</v>
       </c>
       <c r="N100">
-        <v>4</v>
+        <v>1.533</v>
       </c>
       <c r="O100">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="P100">
-        <v>1.833</v>
+        <v>5.5</v>
       </c>
       <c r="Q100">
-        <v>0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R100">
         <v>2.025</v>
@@ -9380,34 +9380,34 @@
         <v>1.825</v>
       </c>
       <c r="T100">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U100">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V100">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W100">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="X100">
         <v>-1</v>
       </c>
       <c r="Y100">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Z100">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA100">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB100">
         <v>-1</v>
       </c>
       <c r="AC100">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="101" spans="1:29">
@@ -9697,7 +9697,7 @@
         <v>30</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -9783,7 +9783,7 @@
         <v>45058.28125</v>
       </c>
       <c r="F105" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G105" t="s">
         <v>37</v>
@@ -9875,7 +9875,7 @@
         <v>32</v>
       </c>
       <c r="G106" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -9964,7 +9964,7 @@
         <v>37</v>
       </c>
       <c r="G107" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H107">
         <v>4</v>
@@ -10050,7 +10050,7 @@
         <v>45066.28125</v>
       </c>
       <c r="F108" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G108" t="s">
         <v>32</v>
@@ -10142,7 +10142,7 @@
         <v>37</v>
       </c>
       <c r="G109" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -10231,7 +10231,7 @@
         <v>32</v>
       </c>
       <c r="G110" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H110">
         <v>3</v>
@@ -10495,7 +10495,7 @@
         <v>45220.23958333334</v>
       </c>
       <c r="F113" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G113" t="s">
         <v>33</v>
@@ -10765,7 +10765,7 @@
         <v>39</v>
       </c>
       <c r="G116" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H116">
         <v>3</v>
@@ -11029,7 +11029,7 @@
         <v>45228.04166666666</v>
       </c>
       <c r="F119" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G119" t="s">
         <v>38</v>
@@ -11299,7 +11299,7 @@
         <v>37</v>
       </c>
       <c r="G122" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H122">
         <v>2</v>
@@ -11655,7 +11655,7 @@
         <v>34</v>
       </c>
       <c r="G126" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H126">
         <v>2</v>
@@ -12100,7 +12100,7 @@
         <v>32</v>
       </c>
       <c r="G131" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H131">
         <v>1</v>
@@ -12275,7 +12275,7 @@
         <v>45242.125</v>
       </c>
       <c r="F133" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G133" t="s">
         <v>39</v>
@@ -12542,7 +12542,7 @@
         <v>45255.23958333334</v>
       </c>
       <c r="F136" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G136" t="s">
         <v>30</v>
@@ -12987,7 +12987,7 @@
         <v>45262.23958333334</v>
       </c>
       <c r="F141" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G141" t="s">
         <v>34</v>
@@ -13076,7 +13076,7 @@
         <v>45263.04166666666</v>
       </c>
       <c r="F142" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G142" t="s">
         <v>33</v>
@@ -13343,7 +13343,7 @@
         <v>45268.23958333334</v>
       </c>
       <c r="F145" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G145" t="s">
         <v>40</v>
@@ -13610,7 +13610,7 @@
         <v>45269.23958333334</v>
       </c>
       <c r="F148" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G148" t="s">
         <v>38</v>
@@ -14147,7 +14147,7 @@
         <v>33</v>
       </c>
       <c r="G154" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H154">
         <v>3</v>
@@ -14236,7 +14236,7 @@
         <v>37</v>
       </c>
       <c r="G155" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H155">
         <v>3</v>
@@ -14414,7 +14414,7 @@
         <v>39</v>
       </c>
       <c r="G157" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -14678,7 +14678,7 @@
         <v>45283.14583333334</v>
       </c>
       <c r="F160" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G160" t="s">
         <v>40</v>
@@ -15034,7 +15034,7 @@
         <v>45289.23958333334</v>
       </c>
       <c r="F164" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G164" t="s">
         <v>31</v>
@@ -15301,7 +15301,7 @@
         <v>45291.20833333334</v>
       </c>
       <c r="F167" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G167" t="s">
         <v>34</v>
@@ -15660,7 +15660,7 @@
         <v>30</v>
       </c>
       <c r="G171" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H171">
         <v>0</v>
@@ -15749,7 +15749,7 @@
         <v>39</v>
       </c>
       <c r="G172" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H172">
         <v>1</v>
@@ -16280,7 +16280,7 @@
         <v>45304.13541666666</v>
       </c>
       <c r="F178" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G178" t="s">
         <v>33</v>
@@ -16369,7 +16369,7 @@
         <v>45304.25</v>
       </c>
       <c r="F179" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G179" t="s">
         <v>32</v>
@@ -16814,7 +16814,7 @@
         <v>45310.23958333334</v>
       </c>
       <c r="F184" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G184" t="s">
         <v>29</v>
@@ -16992,7 +16992,7 @@
         <v>45312.16666666666</v>
       </c>
       <c r="F186" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G186" t="s">
         <v>37</v>
@@ -17262,7 +17262,7 @@
         <v>33</v>
       </c>
       <c r="G189" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H189">
         <v>1</v>
@@ -17526,7 +17526,7 @@
         <v>45318.23958333334</v>
       </c>
       <c r="F192" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G192" t="s">
         <v>39</v>
@@ -17885,7 +17885,7 @@
         <v>40</v>
       </c>
       <c r="G196" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H196">
         <v>2</v>
@@ -18063,7 +18063,7 @@
         <v>32</v>
       </c>
       <c r="G198" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H198">
         <v>0</v>
@@ -18241,7 +18241,7 @@
         <v>31</v>
       </c>
       <c r="G200" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H200">
         <v>0</v>
@@ -18683,10 +18683,10 @@
         <v>45332.23958333334</v>
       </c>
       <c r="F205" t="s">
+        <v>36</v>
+      </c>
+      <c r="G205" t="s">
         <v>35</v>
-      </c>
-      <c r="G205" t="s">
-        <v>36</v>
       </c>
       <c r="H205">
         <v>1</v>
@@ -18950,7 +18950,7 @@
         <v>45339.16666666666</v>
       </c>
       <c r="F208" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G208" t="s">
         <v>32</v>
@@ -19205,7 +19205,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C211" t="s">
         <v>28</v>
@@ -19217,76 +19217,76 @@
         <v>45340.125</v>
       </c>
       <c r="F211" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G211" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H211">
         <v>1</v>
       </c>
       <c r="I211">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J211" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K211">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L211">
         <v>3.75</v>
       </c>
       <c r="M211">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N211">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O211">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P211">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q211">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R211">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S211">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T211">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U211">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V211">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W211">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X211">
         <v>-1</v>
       </c>
       <c r="Y211">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z211">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA211">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB211">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC211">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="212" spans="1:29">
@@ -19294,7 +19294,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C212" t="s">
         <v>28</v>
@@ -19306,76 +19306,76 @@
         <v>45340.125</v>
       </c>
       <c r="F212" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G212" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H212">
         <v>1</v>
       </c>
       <c r="I212">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J212" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K212">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L212">
         <v>3.75</v>
       </c>
       <c r="M212">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N212">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O212">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P212">
+        <v>3.25</v>
+      </c>
+      <c r="Q212">
+        <v>-0.25</v>
+      </c>
+      <c r="R212">
+        <v>1.86</v>
+      </c>
+      <c r="S212">
+        <v>2.04</v>
+      </c>
+      <c r="T212">
         <v>2.75</v>
       </c>
-      <c r="Q212">
-        <v>0</v>
-      </c>
-      <c r="R212">
-        <v>1.8</v>
-      </c>
-      <c r="S212">
-        <v>2.05</v>
-      </c>
-      <c r="T212">
-        <v>3</v>
-      </c>
       <c r="U212">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V212">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W212">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X212">
         <v>-1</v>
       </c>
       <c r="Y212">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z212">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA212">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB212">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC212">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="213" spans="1:29">
@@ -19400,6 +19400,15 @@
       <c r="G213" t="s">
         <v>40</v>
       </c>
+      <c r="H213">
+        <v>2</v>
+      </c>
+      <c r="I213">
+        <v>1</v>
+      </c>
+      <c r="J213" t="s">
+        <v>42</v>
+      </c>
       <c r="K213">
         <v>1.45</v>
       </c>
@@ -19410,10 +19419,10 @@
         <v>6.5</v>
       </c>
       <c r="N213">
-        <v>1.5</v>
+        <v>1.444</v>
       </c>
       <c r="O213">
-        <v>4.333</v>
+        <v>4.5</v>
       </c>
       <c r="P213">
         <v>6.5</v>
@@ -19422,34 +19431,40 @@
         <v>-1.25</v>
       </c>
       <c r="R213">
-        <v>2.08</v>
+        <v>1.97</v>
       </c>
       <c r="S213">
-        <v>1.82</v>
+        <v>1.93</v>
       </c>
       <c r="T213">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U213">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V213">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W213">
-        <v>0</v>
+        <v>0.444</v>
       </c>
       <c r="X213">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y213">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z213">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AA213">
-        <v>0</v>
+        <v>0.465</v>
+      </c>
+      <c r="AB213">
+        <v>-0.5</v>
+      </c>
+      <c r="AC213">
+        <v>0.4375</v>
       </c>
     </row>
     <row r="214" spans="1:29">
@@ -19484,22 +19499,22 @@
         <v>3.2</v>
       </c>
       <c r="N214">
-        <v>1.909</v>
+        <v>1.95</v>
       </c>
       <c r="O214">
         <v>3.8</v>
       </c>
       <c r="P214">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="Q214">
         <v>-0.5</v>
       </c>
       <c r="R214">
-        <v>1.99</v>
+        <v>2.04</v>
       </c>
       <c r="S214">
-        <v>1.91</v>
+        <v>1.86</v>
       </c>
       <c r="T214">
         <v>3.25</v>
@@ -19543,7 +19558,7 @@
         <v>45346.14583333334</v>
       </c>
       <c r="F215" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G215" t="s">
         <v>37</v>
@@ -19727,10 +19742,10 @@
         <v>3</v>
       </c>
       <c r="U217">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V217">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W217">
         <v>0</v>
@@ -19792,10 +19807,10 @@
         <v>-0.5</v>
       </c>
       <c r="R218">
-        <v>2.06</v>
+        <v>2.07</v>
       </c>
       <c r="S218">
-        <v>1.84</v>
+        <v>1.83</v>
       </c>
       <c r="T218">
         <v>3.25</v>
@@ -19842,7 +19857,7 @@
         <v>33</v>
       </c>
       <c r="G219" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K219">
         <v>2</v>
@@ -19866,19 +19881,19 @@
         <v>-0.5</v>
       </c>
       <c r="R219">
-        <v>2.01</v>
+        <v>1.98</v>
       </c>
       <c r="S219">
-        <v>1.89</v>
+        <v>1.92</v>
       </c>
       <c r="T219">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U219">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V219">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W219">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 21-02-2024 às 23:25
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -3274,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>5400043</v>
+        <v>5400042</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -3286,58 +3286,58 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>42</v>
       </c>
       <c r="K32">
-        <v>2.15</v>
+        <v>1.533</v>
       </c>
       <c r="L32">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M32">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="N32">
-        <v>2.2</v>
+        <v>1.333</v>
       </c>
       <c r="O32">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="P32">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="Q32">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R32">
+        <v>1.85</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>3.25</v>
+      </c>
+      <c r="U32">
+        <v>1.875</v>
+      </c>
+      <c r="V32">
         <v>1.975</v>
       </c>
-      <c r="S32">
-        <v>1.875</v>
-      </c>
-      <c r="T32">
-        <v>3</v>
-      </c>
-      <c r="U32">
-        <v>1.95</v>
-      </c>
-      <c r="V32">
-        <v>1.9</v>
-      </c>
       <c r="W32">
-        <v>1.2</v>
+        <v>0.333</v>
       </c>
       <c r="X32">
         <v>-1</v>
@@ -3346,13 +3346,13 @@
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC32">
         <v>-1</v>
@@ -3363,7 +3363,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5400042</v>
+        <v>5400043</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -3375,58 +3375,58 @@
         <v>44961.125</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" t="s">
         <v>42</v>
       </c>
       <c r="K33">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="L33">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M33">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N33">
-        <v>1.333</v>
+        <v>2.2</v>
       </c>
       <c r="O33">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P33">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="Q33">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R33">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S33">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T33">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U33">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V33">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W33">
-        <v>0.333</v>
+        <v>1.2</v>
       </c>
       <c r="X33">
         <v>-1</v>
@@ -3435,13 +3435,13 @@
         <v>-1</v>
       </c>
       <c r="Z33">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA33">
         <v>-1</v>
       </c>
       <c r="AB33">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC33">
         <v>-1</v>
@@ -4876,7 +4876,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>5400048</v>
+        <v>5404699</v>
       </c>
       <c r="C50" t="s">
         <v>28</v>
@@ -4888,73 +4888,73 @@
         <v>44982.125</v>
       </c>
       <c r="F50" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G50" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>3</v>
       </c>
-      <c r="I50">
-        <v>2</v>
-      </c>
       <c r="J50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K50">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="L50">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="M50">
-        <v>4</v>
+        <v>2.8</v>
       </c>
       <c r="N50">
-        <v>1.8</v>
+        <v>2.1</v>
       </c>
       <c r="O50">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P50">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="Q50">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R50">
-        <v>2.025</v>
+        <v>1.94</v>
       </c>
       <c r="S50">
-        <v>1.825</v>
+        <v>1.96</v>
       </c>
       <c r="T50">
         <v>2.75</v>
       </c>
       <c r="U50">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V50">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W50">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="X50">
         <v>-1</v>
       </c>
       <c r="Y50">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z50">
-        <v>0.5125</v>
+        <v>-1</v>
       </c>
       <c r="AA50">
-        <v>-0.5</v>
+        <v>0.96</v>
       </c>
       <c r="AB50">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC50">
         <v>-1</v>
@@ -4965,7 +4965,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>5404699</v>
+        <v>5400048</v>
       </c>
       <c r="C51" t="s">
         <v>28</v>
@@ -4977,73 +4977,73 @@
         <v>44982.125</v>
       </c>
       <c r="F51" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K51">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="L51">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="M51">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="N51">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="O51">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P51">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="Q51">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R51">
-        <v>1.94</v>
+        <v>2.025</v>
       </c>
       <c r="S51">
-        <v>1.96</v>
+        <v>1.825</v>
       </c>
       <c r="T51">
         <v>2.75</v>
       </c>
       <c r="U51">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V51">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W51">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="X51">
         <v>-1</v>
       </c>
       <c r="Y51">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z51">
-        <v>-1</v>
+        <v>0.5125</v>
       </c>
       <c r="AA51">
-        <v>0.96</v>
+        <v>-0.5</v>
       </c>
       <c r="AB51">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC51">
         <v>-1</v>
@@ -5499,7 +5499,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5404706</v>
+        <v>5404704</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5511,58 +5511,58 @@
         <v>44989.125</v>
       </c>
       <c r="F57" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G57" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>42</v>
       </c>
       <c r="K57">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="L57">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M57">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="N57">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="O57">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P57">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q57">
         <v>-0.25</v>
       </c>
       <c r="R57">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S57">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T57">
         <v>2.75</v>
       </c>
       <c r="U57">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V57">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W57">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="X57">
         <v>-1</v>
@@ -5571,16 +5571,16 @@
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0.8500000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AA57">
         <v>-1</v>
       </c>
       <c r="AB57">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AC57">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5588,7 +5588,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5404704</v>
+        <v>5404706</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5600,58 +5600,58 @@
         <v>44989.125</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J58" t="s">
         <v>42</v>
       </c>
       <c r="K58">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L58">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M58">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="N58">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O58">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P58">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q58">
         <v>-0.25</v>
       </c>
       <c r="R58">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S58">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T58">
         <v>2.75</v>
       </c>
       <c r="U58">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V58">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W58">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="X58">
         <v>-1</v>
@@ -5660,16 +5660,16 @@
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA58">
         <v>-1</v>
       </c>
       <c r="AB58">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AC58">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -6478,7 +6478,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5404714</v>
+        <v>5404713</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6490,76 +6490,76 @@
         <v>45003.125</v>
       </c>
       <c r="F68" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G68" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K68">
         <v>2.25</v>
       </c>
       <c r="L68">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M68">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="N68">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O68">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P68">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q68">
         <v>-0.25</v>
       </c>
       <c r="R68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T68">
         <v>2.75</v>
       </c>
       <c r="U68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W68">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X68">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y68">
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA68">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB68">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC68">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6567,7 +6567,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>5404713</v>
+        <v>5404714</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6579,76 +6579,76 @@
         <v>45003.125</v>
       </c>
       <c r="F69" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G69" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K69">
         <v>2.25</v>
       </c>
       <c r="L69">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M69">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N69">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="O69">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P69">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T69">
         <v>2.75</v>
       </c>
       <c r="U69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W69">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X69">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA69">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB69">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC69">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -16446,7 +16446,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C180" t="s">
         <v>28</v>
@@ -16458,73 +16458,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F180" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G180" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H180">
         <v>3</v>
       </c>
       <c r="I180">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J180" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K180">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L180">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M180">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N180">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O180">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P180">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q180">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R180">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S180">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T180">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U180">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V180">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W180">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X180">
         <v>-1</v>
       </c>
       <c r="Y180">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z180">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA180">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB180">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC180">
         <v>-1</v>
@@ -16535,7 +16535,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C181" t="s">
         <v>28</v>
@@ -16547,73 +16547,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F181" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G181" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H181">
         <v>3</v>
       </c>
       <c r="I181">
+        <v>2</v>
+      </c>
+      <c r="J181" t="s">
+        <v>42</v>
+      </c>
+      <c r="K181">
+        <v>1.909</v>
+      </c>
+      <c r="L181">
         <v>4</v>
       </c>
-      <c r="J181" t="s">
-        <v>41</v>
-      </c>
-      <c r="K181">
-        <v>2.45</v>
-      </c>
-      <c r="L181">
-        <v>3.75</v>
-      </c>
       <c r="M181">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N181">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O181">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P181">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q181">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R181">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S181">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T181">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U181">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V181">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W181">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X181">
         <v>-1</v>
       </c>
       <c r="Y181">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z181">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA181">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB181">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC181">
         <v>-1</v>
@@ -19499,31 +19499,31 @@
         <v>3.2</v>
       </c>
       <c r="N214">
-        <v>1.95</v>
+        <v>1.909</v>
       </c>
       <c r="O214">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P214">
-        <v>3.25</v>
+        <v>3.6</v>
       </c>
       <c r="Q214">
         <v>-0.5</v>
       </c>
       <c r="R214">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="S214">
-        <v>1.86</v>
+        <v>1.95</v>
       </c>
       <c r="T214">
         <v>3.25</v>
       </c>
       <c r="U214">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="V214">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="W214">
         <v>0</v>
@@ -19659,10 +19659,10 @@
         <v>0</v>
       </c>
       <c r="R216">
-        <v>1.85</v>
+        <v>1.83</v>
       </c>
       <c r="S216">
-        <v>2.05</v>
+        <v>2.07</v>
       </c>
       <c r="T216">
         <v>3.25</v>
@@ -19721,22 +19721,22 @@
         <v>2.5</v>
       </c>
       <c r="N217">
-        <v>2.6</v>
+        <v>2.55</v>
       </c>
       <c r="O217">
         <v>3.5</v>
       </c>
       <c r="P217">
-        <v>2.55</v>
+        <v>2.6</v>
       </c>
       <c r="Q217">
         <v>0</v>
       </c>
       <c r="R217">
-        <v>1.95</v>
+        <v>1.88</v>
       </c>
       <c r="S217">
-        <v>1.95</v>
+        <v>2.02</v>
       </c>
       <c r="T217">
         <v>3</v>
@@ -19798,19 +19798,19 @@
         <v>2</v>
       </c>
       <c r="O218">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P218">
         <v>3.2</v>
       </c>
       <c r="Q218">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R218">
+        <v>1.83</v>
+      </c>
+      <c r="S218">
         <v>2.07</v>
-      </c>
-      <c r="S218">
-        <v>1.83</v>
       </c>
       <c r="T218">
         <v>3.25</v>
@@ -19881,10 +19881,10 @@
         <v>-0.5</v>
       </c>
       <c r="R219">
-        <v>1.98</v>
+        <v>1.99</v>
       </c>
       <c r="S219">
-        <v>1.92</v>
+        <v>1.91</v>
       </c>
       <c r="T219">
         <v>2.75</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 23-02-2024 às 08:18
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC219"/>
+  <dimension ref="A1:AC218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6478,7 +6478,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5404713</v>
+        <v>5404714</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6490,76 +6490,76 @@
         <v>45003.125</v>
       </c>
       <c r="F68" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G68" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I68">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J68" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K68">
         <v>2.25</v>
       </c>
       <c r="L68">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M68">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N68">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="O68">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P68">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q68">
         <v>-0.25</v>
       </c>
       <c r="R68">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S68">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T68">
         <v>2.75</v>
       </c>
       <c r="U68">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V68">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W68">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X68">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y68">
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA68">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB68">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC68">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6567,7 +6567,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>5404714</v>
+        <v>5404713</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6579,76 +6579,76 @@
         <v>45003.125</v>
       </c>
       <c r="F69" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G69" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K69">
         <v>2.25</v>
       </c>
       <c r="L69">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M69">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="N69">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O69">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P69">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S69">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T69">
         <v>2.75</v>
       </c>
       <c r="U69">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V69">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W69">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X69">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA69">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB69">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC69">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -9237,7 +9237,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5404735</v>
+        <v>5400064</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -9249,40 +9249,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G99" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H99">
+        <v>2</v>
+      </c>
+      <c r="I99">
         <v>0</v>
       </c>
-      <c r="I99">
-        <v>1</v>
-      </c>
       <c r="J99" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K99">
-        <v>3.6</v>
+        <v>1.65</v>
       </c>
       <c r="L99">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M99">
-        <v>1.909</v>
+        <v>4.5</v>
       </c>
       <c r="N99">
-        <v>4</v>
+        <v>1.533</v>
       </c>
       <c r="O99">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="P99">
-        <v>1.833</v>
+        <v>5.5</v>
       </c>
       <c r="Q99">
-        <v>0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R99">
         <v>2.025</v>
@@ -9291,34 +9291,34 @@
         <v>1.825</v>
       </c>
       <c r="T99">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U99">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V99">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W99">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="X99">
         <v>-1</v>
       </c>
       <c r="Y99">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Z99">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA99">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB99">
         <v>-1</v>
       </c>
       <c r="AC99">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="100" spans="1:29">
@@ -9326,7 +9326,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>5400064</v>
+        <v>5404735</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -9338,40 +9338,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F100" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G100" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J100" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K100">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L100">
+        <v>3.75</v>
+      </c>
+      <c r="M100">
+        <v>1.909</v>
+      </c>
+      <c r="N100">
         <v>4</v>
       </c>
-      <c r="M100">
-        <v>4.5</v>
-      </c>
-      <c r="N100">
-        <v>1.533</v>
-      </c>
       <c r="O100">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="P100">
-        <v>5.5</v>
+        <v>1.833</v>
       </c>
       <c r="Q100">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R100">
         <v>2.025</v>
@@ -9380,34 +9380,34 @@
         <v>1.825</v>
       </c>
       <c r="T100">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="U100">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V100">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W100">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X100">
         <v>-1</v>
       </c>
       <c r="Y100">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Z100">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA100">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB100">
         <v>-1</v>
       </c>
       <c r="AC100">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="101" spans="1:29">
@@ -19472,7 +19472,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>7127375</v>
+        <v>7126789</v>
       </c>
       <c r="C214" t="s">
         <v>28</v>
@@ -19481,49 +19481,49 @@
         <v>28</v>
       </c>
       <c r="E214" s="2">
-        <v>45345.23958333334</v>
+        <v>45346.14583333334</v>
       </c>
       <c r="F214" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G214" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K214">
-        <v>2</v>
+        <v>1.833</v>
       </c>
       <c r="L214">
+        <v>4</v>
+      </c>
+      <c r="M214">
+        <v>3.6</v>
+      </c>
+      <c r="N214">
+        <v>1.833</v>
+      </c>
+      <c r="O214">
+        <v>4.2</v>
+      </c>
+      <c r="P214">
         <v>3.75</v>
-      </c>
-      <c r="M214">
-        <v>3.2</v>
-      </c>
-      <c r="N214">
-        <v>1.909</v>
-      </c>
-      <c r="O214">
-        <v>4</v>
-      </c>
-      <c r="P214">
-        <v>3.6</v>
       </c>
       <c r="Q214">
         <v>-0.5</v>
       </c>
       <c r="R214">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="S214">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T214">
         <v>3.25</v>
       </c>
       <c r="U214">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V214">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W214">
         <v>0</v>
@@ -19546,7 +19546,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>7126789</v>
+        <v>7127377</v>
       </c>
       <c r="C215" t="s">
         <v>28</v>
@@ -19555,49 +19555,49 @@
         <v>28</v>
       </c>
       <c r="E215" s="2">
-        <v>45346.14583333334</v>
+        <v>45346.23958333334</v>
       </c>
       <c r="F215" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G215" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="K215">
-        <v>1.833</v>
+        <v>2.8</v>
       </c>
       <c r="L215">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M215">
-        <v>3.6</v>
+        <v>2.25</v>
       </c>
       <c r="N215">
-        <v>1.8</v>
+        <v>2.4</v>
       </c>
       <c r="O215">
         <v>4</v>
       </c>
       <c r="P215">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="Q215">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R215">
-        <v>1.86</v>
+        <v>1.85</v>
       </c>
       <c r="S215">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T215">
         <v>3.25</v>
       </c>
       <c r="U215">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V215">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W215">
         <v>0</v>
@@ -19620,7 +19620,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>7127377</v>
+        <v>7127378</v>
       </c>
       <c r="C216" t="s">
         <v>28</v>
@@ -19629,43 +19629,43 @@
         <v>28</v>
       </c>
       <c r="E216" s="2">
-        <v>45346.23958333334</v>
+        <v>45346.32291666666</v>
       </c>
       <c r="F216" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G216" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K216">
-        <v>2.8</v>
+        <v>2.6</v>
       </c>
       <c r="L216">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M216">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="N216">
-        <v>2.3</v>
+        <v>2.375</v>
       </c>
       <c r="O216">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="P216">
-        <v>2.6</v>
+        <v>2.875</v>
       </c>
       <c r="Q216">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R216">
-        <v>1.83</v>
+        <v>2.08</v>
       </c>
       <c r="S216">
-        <v>2.07</v>
+        <v>1.82</v>
       </c>
       <c r="T216">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U216">
         <v>1.925</v>
@@ -19694,7 +19694,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>7127378</v>
+        <v>7127376</v>
       </c>
       <c r="C217" t="s">
         <v>28</v>
@@ -19703,49 +19703,49 @@
         <v>28</v>
       </c>
       <c r="E217" s="2">
-        <v>45346.32291666666</v>
+        <v>45347.125</v>
       </c>
       <c r="F217" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G217" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="K217">
-        <v>2.6</v>
+        <v>2.375</v>
       </c>
       <c r="L217">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M217">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="N217">
-        <v>2.55</v>
+        <v>1.95</v>
       </c>
       <c r="O217">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="P217">
-        <v>2.6</v>
+        <v>3.4</v>
       </c>
       <c r="Q217">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R217">
-        <v>1.88</v>
+        <v>2</v>
       </c>
       <c r="S217">
-        <v>2.02</v>
+        <v>1.9</v>
       </c>
       <c r="T217">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U217">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V217">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W217">
         <v>0</v>
@@ -19768,7 +19768,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C218" t="s">
         <v>28</v>
@@ -19780,46 +19780,46 @@
         <v>45347.125</v>
       </c>
       <c r="F218" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G218" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K218">
-        <v>2.375</v>
+        <v>2</v>
       </c>
       <c r="L218">
         <v>3.6</v>
       </c>
       <c r="M218">
-        <v>2.7</v>
+        <v>3.4</v>
       </c>
       <c r="N218">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="O218">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="P218">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="Q218">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R218">
-        <v>1.83</v>
+        <v>1.92</v>
       </c>
       <c r="S218">
-        <v>2.07</v>
+        <v>1.98</v>
       </c>
       <c r="T218">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U218">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V218">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W218">
         <v>0</v>
@@ -19834,80 +19834,6 @@
         <v>0</v>
       </c>
       <c r="AA218">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:29">
-      <c r="A219" s="1">
-        <v>217</v>
-      </c>
-      <c r="B219">
-        <v>7127379</v>
-      </c>
-      <c r="C219" t="s">
-        <v>28</v>
-      </c>
-      <c r="D219" t="s">
-        <v>28</v>
-      </c>
-      <c r="E219" s="2">
-        <v>45347.125</v>
-      </c>
-      <c r="F219" t="s">
-        <v>33</v>
-      </c>
-      <c r="G219" t="s">
-        <v>36</v>
-      </c>
-      <c r="K219">
-        <v>2</v>
-      </c>
-      <c r="L219">
-        <v>3.6</v>
-      </c>
-      <c r="M219">
-        <v>3.4</v>
-      </c>
-      <c r="N219">
-        <v>1.95</v>
-      </c>
-      <c r="O219">
-        <v>3.6</v>
-      </c>
-      <c r="P219">
-        <v>3.5</v>
-      </c>
-      <c r="Q219">
-        <v>-0.5</v>
-      </c>
-      <c r="R219">
-        <v>1.99</v>
-      </c>
-      <c r="S219">
-        <v>1.91</v>
-      </c>
-      <c r="T219">
-        <v>2.75</v>
-      </c>
-      <c r="U219">
-        <v>1.85</v>
-      </c>
-      <c r="V219">
-        <v>2</v>
-      </c>
-      <c r="W219">
-        <v>0</v>
-      </c>
-      <c r="X219">
-        <v>0</v>
-      </c>
-      <c r="Y219">
-        <v>0</v>
-      </c>
-      <c r="Z219">
-        <v>0</v>
-      </c>
-      <c r="AA219">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 23-02-2024 às 23:34
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC218"/>
+  <dimension ref="A1:AC220"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3274,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>5400042</v>
+        <v>5400043</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -3286,58 +3286,58 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H32">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" t="s">
         <v>42</v>
       </c>
       <c r="K32">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="L32">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M32">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N32">
-        <v>1.333</v>
+        <v>2.2</v>
       </c>
       <c r="O32">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P32">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="Q32">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R32">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S32">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T32">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U32">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V32">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W32">
-        <v>0.333</v>
+        <v>1.2</v>
       </c>
       <c r="X32">
         <v>-1</v>
@@ -3346,13 +3346,13 @@
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC32">
         <v>-1</v>
@@ -3363,7 +3363,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5400043</v>
+        <v>5400042</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -3375,58 +3375,58 @@
         <v>44961.125</v>
       </c>
       <c r="F33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H33">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" t="s">
         <v>42</v>
       </c>
       <c r="K33">
-        <v>2.15</v>
+        <v>1.533</v>
       </c>
       <c r="L33">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M33">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="N33">
-        <v>2.2</v>
+        <v>1.333</v>
       </c>
       <c r="O33">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="P33">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="Q33">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R33">
+        <v>1.85</v>
+      </c>
+      <c r="S33">
+        <v>2</v>
+      </c>
+      <c r="T33">
+        <v>3.25</v>
+      </c>
+      <c r="U33">
+        <v>1.875</v>
+      </c>
+      <c r="V33">
         <v>1.975</v>
       </c>
-      <c r="S33">
-        <v>1.875</v>
-      </c>
-      <c r="T33">
-        <v>3</v>
-      </c>
-      <c r="U33">
-        <v>1.95</v>
-      </c>
-      <c r="V33">
-        <v>1.9</v>
-      </c>
       <c r="W33">
-        <v>1.2</v>
+        <v>0.333</v>
       </c>
       <c r="X33">
         <v>-1</v>
@@ -3435,13 +3435,13 @@
         <v>-1</v>
       </c>
       <c r="Z33">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA33">
         <v>-1</v>
       </c>
       <c r="AB33">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC33">
         <v>-1</v>
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97">
+        <v>1.75</v>
+      </c>
+      <c r="L97">
+        <v>3.8</v>
+      </c>
+      <c r="M97">
         <v>4</v>
       </c>
-      <c r="J97" t="s">
-        <v>41</v>
-      </c>
-      <c r="K97">
-        <v>2.3</v>
-      </c>
-      <c r="L97">
-        <v>3.75</v>
-      </c>
-      <c r="M97">
-        <v>2.75</v>
-      </c>
       <c r="N97">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q97">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R97">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S97">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T97">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U97">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V97">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W97">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X97">
         <v>-1</v>
       </c>
       <c r="Y97">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z97">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA97">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB97">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K98">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L98">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M98">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N98">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q98">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R98">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S98">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T98">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U98">
+        <v>2</v>
+      </c>
+      <c r="V98">
         <v>1.85</v>
       </c>
-      <c r="V98">
-        <v>2</v>
-      </c>
       <c r="W98">
+        <v>-1</v>
+      </c>
+      <c r="X98">
+        <v>-1</v>
+      </c>
+      <c r="Y98">
+        <v>1.4</v>
+      </c>
+      <c r="Z98">
+        <v>-1</v>
+      </c>
+      <c r="AA98">
+        <v>0.8</v>
+      </c>
+      <c r="AB98">
         <v>1</v>
-      </c>
-      <c r="X98">
-        <v>-1</v>
-      </c>
-      <c r="Y98">
-        <v>-1</v>
-      </c>
-      <c r="Z98">
-        <v>1.025</v>
-      </c>
-      <c r="AA98">
-        <v>-1</v>
-      </c>
-      <c r="AB98">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -9237,7 +9237,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>5400064</v>
+        <v>5404735</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -9249,40 +9249,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F99" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G99" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H99">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J99" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K99">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L99">
+        <v>3.75</v>
+      </c>
+      <c r="M99">
+        <v>1.909</v>
+      </c>
+      <c r="N99">
         <v>4</v>
       </c>
-      <c r="M99">
-        <v>4.5</v>
-      </c>
-      <c r="N99">
-        <v>1.533</v>
-      </c>
       <c r="O99">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="P99">
-        <v>5.5</v>
+        <v>1.833</v>
       </c>
       <c r="Q99">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R99">
         <v>2.025</v>
@@ -9291,34 +9291,34 @@
         <v>1.825</v>
       </c>
       <c r="T99">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="U99">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V99">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W99">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X99">
         <v>-1</v>
       </c>
       <c r="Y99">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Z99">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AA99">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB99">
         <v>-1</v>
       </c>
       <c r="AC99">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="100" spans="1:29">
@@ -9326,7 +9326,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>5404735</v>
+        <v>5400064</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -9338,40 +9338,40 @@
         <v>45045.16666666666</v>
       </c>
       <c r="F100" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G100" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H100">
+        <v>2</v>
+      </c>
+      <c r="I100">
         <v>0</v>
       </c>
-      <c r="I100">
-        <v>1</v>
-      </c>
       <c r="J100" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K100">
-        <v>3.6</v>
+        <v>1.65</v>
       </c>
       <c r="L100">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M100">
-        <v>1.909</v>
+        <v>4.5</v>
       </c>
       <c r="N100">
-        <v>4</v>
+        <v>1.533</v>
       </c>
       <c r="O100">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="P100">
-        <v>1.833</v>
+        <v>5.5</v>
       </c>
       <c r="Q100">
-        <v>0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="R100">
         <v>2.025</v>
@@ -9380,34 +9380,34 @@
         <v>1.825</v>
       </c>
       <c r="T100">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U100">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V100">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W100">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="X100">
         <v>-1</v>
       </c>
       <c r="Y100">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Z100">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA100">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB100">
         <v>-1</v>
       </c>
       <c r="AC100">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="101" spans="1:29">
@@ -16446,7 +16446,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C180" t="s">
         <v>28</v>
@@ -16458,73 +16458,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F180" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G180" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H180">
         <v>3</v>
       </c>
       <c r="I180">
+        <v>2</v>
+      </c>
+      <c r="J180" t="s">
+        <v>42</v>
+      </c>
+      <c r="K180">
+        <v>1.909</v>
+      </c>
+      <c r="L180">
         <v>4</v>
       </c>
-      <c r="J180" t="s">
-        <v>41</v>
-      </c>
-      <c r="K180">
-        <v>2.45</v>
-      </c>
-      <c r="L180">
-        <v>3.75</v>
-      </c>
       <c r="M180">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N180">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O180">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P180">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q180">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R180">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S180">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T180">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U180">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V180">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W180">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X180">
         <v>-1</v>
       </c>
       <c r="Y180">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z180">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA180">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB180">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC180">
         <v>-1</v>
@@ -16535,7 +16535,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C181" t="s">
         <v>28</v>
@@ -16547,73 +16547,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F181" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G181" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H181">
         <v>3</v>
       </c>
       <c r="I181">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J181" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K181">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L181">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M181">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N181">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O181">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P181">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q181">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R181">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S181">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T181">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U181">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V181">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W181">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X181">
         <v>-1</v>
       </c>
       <c r="Y181">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z181">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA181">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB181">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC181">
         <v>-1</v>
@@ -19472,7 +19472,7 @@
         <v>212</v>
       </c>
       <c r="B214">
-        <v>7126789</v>
+        <v>7127375</v>
       </c>
       <c r="C214" t="s">
         <v>28</v>
@@ -19481,64 +19481,79 @@
         <v>28</v>
       </c>
       <c r="E214" s="2">
-        <v>45346.14583333334</v>
+        <v>45345.23958333334</v>
       </c>
       <c r="F214" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G214" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="H214">
+        <v>2</v>
+      </c>
+      <c r="I214">
+        <v>2</v>
+      </c>
+      <c r="J214" t="s">
+        <v>43</v>
       </c>
       <c r="K214">
-        <v>1.833</v>
+        <v>2</v>
       </c>
       <c r="L214">
+        <v>3.75</v>
+      </c>
+      <c r="M214">
+        <v>3.2</v>
+      </c>
+      <c r="N214">
+        <v>1.727</v>
+      </c>
+      <c r="O214">
+        <v>4.333</v>
+      </c>
+      <c r="P214">
         <v>4</v>
       </c>
-      <c r="M214">
-        <v>3.6</v>
-      </c>
-      <c r="N214">
-        <v>1.833</v>
-      </c>
-      <c r="O214">
-        <v>4.2</v>
-      </c>
-      <c r="P214">
-        <v>3.75</v>
-      </c>
       <c r="Q214">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R214">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S214">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="T214">
         <v>3.25</v>
       </c>
       <c r="U214">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V214">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="W214">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X214">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="Y214">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z214">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA214">
-        <v>0</v>
+        <v>0.925</v>
+      </c>
+      <c r="AB214">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AC214">
+        <v>-1</v>
       </c>
     </row>
     <row r="215" spans="1:29">
@@ -19546,7 +19561,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>7127377</v>
+        <v>7875268</v>
       </c>
       <c r="C215" t="s">
         <v>28</v>
@@ -19555,64 +19570,79 @@
         <v>28</v>
       </c>
       <c r="E215" s="2">
-        <v>45346.23958333334</v>
+        <v>45345.38194444445</v>
       </c>
       <c r="F215" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G215" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="H215">
+        <v>1</v>
+      </c>
+      <c r="I215">
+        <v>1</v>
+      </c>
+      <c r="J215" t="s">
+        <v>43</v>
       </c>
       <c r="K215">
-        <v>2.8</v>
+        <v>1.75</v>
       </c>
       <c r="L215">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M215">
-        <v>2.25</v>
+        <v>3.4</v>
       </c>
       <c r="N215">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="O215">
         <v>4</v>
       </c>
       <c r="P215">
-        <v>2.625</v>
+        <v>3.4</v>
       </c>
       <c r="Q215">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R215">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="S215">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="T215">
         <v>3.25</v>
       </c>
       <c r="U215">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V215">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W215">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X215">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y215">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z215">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA215">
-        <v>0</v>
+        <v>1.025</v>
+      </c>
+      <c r="AB215">
+        <v>-1</v>
+      </c>
+      <c r="AC215">
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="216" spans="1:29">
@@ -19620,7 +19650,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>7127378</v>
+        <v>7126789</v>
       </c>
       <c r="C216" t="s">
         <v>28</v>
@@ -19629,49 +19659,49 @@
         <v>28</v>
       </c>
       <c r="E216" s="2">
-        <v>45346.32291666666</v>
+        <v>45346.14583333334</v>
       </c>
       <c r="F216" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G216" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K216">
-        <v>2.6</v>
+        <v>1.833</v>
       </c>
       <c r="L216">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="M216">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="N216">
-        <v>2.375</v>
+        <v>1.833</v>
       </c>
       <c r="O216">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="P216">
-        <v>2.875</v>
+        <v>3.75</v>
       </c>
       <c r="Q216">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R216">
-        <v>2.08</v>
+        <v>1.86</v>
       </c>
       <c r="S216">
-        <v>1.82</v>
+        <v>2.04</v>
       </c>
       <c r="T216">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U216">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V216">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W216">
         <v>0</v>
@@ -19694,7 +19724,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>7127376</v>
+        <v>7127377</v>
       </c>
       <c r="C217" t="s">
         <v>28</v>
@@ -19703,49 +19733,49 @@
         <v>28</v>
       </c>
       <c r="E217" s="2">
-        <v>45347.125</v>
+        <v>45346.23958333334</v>
       </c>
       <c r="F217" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G217" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="K217">
-        <v>2.375</v>
+        <v>2.4</v>
       </c>
       <c r="L217">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M217">
-        <v>2.7</v>
+        <v>2.6</v>
       </c>
       <c r="N217">
-        <v>1.95</v>
+        <v>2.4</v>
       </c>
       <c r="O217">
         <v>4</v>
       </c>
       <c r="P217">
-        <v>3.4</v>
+        <v>2.6</v>
       </c>
       <c r="Q217">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R217">
-        <v>2</v>
+        <v>1.84</v>
       </c>
       <c r="S217">
-        <v>1.9</v>
+        <v>2.06</v>
       </c>
       <c r="T217">
         <v>3.25</v>
       </c>
       <c r="U217">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V217">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W217">
         <v>0</v>
@@ -19768,7 +19798,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>7127379</v>
+        <v>7127378</v>
       </c>
       <c r="C218" t="s">
         <v>28</v>
@@ -19777,49 +19807,49 @@
         <v>28</v>
       </c>
       <c r="E218" s="2">
-        <v>45347.125</v>
+        <v>45346.32291666666</v>
       </c>
       <c r="F218" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G218" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K218">
-        <v>2</v>
+        <v>2.375</v>
       </c>
       <c r="L218">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M218">
-        <v>3.4</v>
+        <v>2.875</v>
       </c>
       <c r="N218">
-        <v>1.95</v>
+        <v>2.375</v>
       </c>
       <c r="O218">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P218">
-        <v>3.8</v>
+        <v>2.875</v>
       </c>
       <c r="Q218">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R218">
-        <v>1.92</v>
+        <v>2.07</v>
       </c>
       <c r="S218">
-        <v>1.98</v>
+        <v>1.83</v>
       </c>
       <c r="T218">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U218">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V218">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W218">
         <v>0</v>
@@ -19834,6 +19864,154 @@
         <v>0</v>
       </c>
       <c r="AA218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:29">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219">
+        <v>7127376</v>
+      </c>
+      <c r="C219" t="s">
+        <v>28</v>
+      </c>
+      <c r="D219" t="s">
+        <v>28</v>
+      </c>
+      <c r="E219" s="2">
+        <v>45347.125</v>
+      </c>
+      <c r="F219" t="s">
+        <v>29</v>
+      </c>
+      <c r="G219" t="s">
+        <v>38</v>
+      </c>
+      <c r="K219">
+        <v>1.95</v>
+      </c>
+      <c r="L219">
+        <v>4</v>
+      </c>
+      <c r="M219">
+        <v>3.4</v>
+      </c>
+      <c r="N219">
+        <v>1.95</v>
+      </c>
+      <c r="O219">
+        <v>4</v>
+      </c>
+      <c r="P219">
+        <v>3.4</v>
+      </c>
+      <c r="Q219">
+        <v>-0.5</v>
+      </c>
+      <c r="R219">
+        <v>2</v>
+      </c>
+      <c r="S219">
+        <v>1.9</v>
+      </c>
+      <c r="T219">
+        <v>3.25</v>
+      </c>
+      <c r="U219">
+        <v>1.875</v>
+      </c>
+      <c r="V219">
+        <v>1.975</v>
+      </c>
+      <c r="W219">
+        <v>0</v>
+      </c>
+      <c r="X219">
+        <v>0</v>
+      </c>
+      <c r="Y219">
+        <v>0</v>
+      </c>
+      <c r="Z219">
+        <v>0</v>
+      </c>
+      <c r="AA219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:29">
+      <c r="A220" s="1">
+        <v>218</v>
+      </c>
+      <c r="B220">
+        <v>7127379</v>
+      </c>
+      <c r="C220" t="s">
+        <v>28</v>
+      </c>
+      <c r="D220" t="s">
+        <v>28</v>
+      </c>
+      <c r="E220" s="2">
+        <v>45347.125</v>
+      </c>
+      <c r="F220" t="s">
+        <v>33</v>
+      </c>
+      <c r="G220" t="s">
+        <v>36</v>
+      </c>
+      <c r="K220">
+        <v>1.95</v>
+      </c>
+      <c r="L220">
+        <v>3.6</v>
+      </c>
+      <c r="M220">
+        <v>3.8</v>
+      </c>
+      <c r="N220">
+        <v>1.95</v>
+      </c>
+      <c r="O220">
+        <v>3.6</v>
+      </c>
+      <c r="P220">
+        <v>3.8</v>
+      </c>
+      <c r="Q220">
+        <v>-0.5</v>
+      </c>
+      <c r="R220">
+        <v>1.98</v>
+      </c>
+      <c r="S220">
+        <v>1.92</v>
+      </c>
+      <c r="T220">
+        <v>2.75</v>
+      </c>
+      <c r="U220">
+        <v>1.95</v>
+      </c>
+      <c r="V220">
+        <v>1.9</v>
+      </c>
+      <c r="W220">
+        <v>0</v>
+      </c>
+      <c r="X220">
+        <v>0</v>
+      </c>
+      <c r="Y220">
+        <v>0</v>
+      </c>
+      <c r="Z220">
+        <v>0</v>
+      </c>
+      <c r="AA220">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 24-02-2024 às 12:40
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC220"/>
+  <dimension ref="A1:AC218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G97" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H97">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I97">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J97" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K97">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L97">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M97">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N97">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q97">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R97">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S97">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T97">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U97">
+        <v>2</v>
+      </c>
+      <c r="V97">
         <v>1.85</v>
       </c>
-      <c r="V97">
-        <v>2</v>
-      </c>
       <c r="W97">
+        <v>-1</v>
+      </c>
+      <c r="X97">
+        <v>-1</v>
+      </c>
+      <c r="Y97">
+        <v>1.4</v>
+      </c>
+      <c r="Z97">
+        <v>-1</v>
+      </c>
+      <c r="AA97">
+        <v>0.8</v>
+      </c>
+      <c r="AB97">
         <v>1</v>
-      </c>
-      <c r="X97">
-        <v>-1</v>
-      </c>
-      <c r="Y97">
-        <v>-1</v>
-      </c>
-      <c r="Z97">
-        <v>1.025</v>
-      </c>
-      <c r="AA97">
-        <v>-1</v>
-      </c>
-      <c r="AB97">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G98" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I98">
+        <v>2</v>
+      </c>
+      <c r="J98" t="s">
+        <v>42</v>
+      </c>
+      <c r="K98">
+        <v>1.75</v>
+      </c>
+      <c r="L98">
+        <v>3.8</v>
+      </c>
+      <c r="M98">
         <v>4</v>
       </c>
-      <c r="J98" t="s">
-        <v>41</v>
-      </c>
-      <c r="K98">
-        <v>2.3</v>
-      </c>
-      <c r="L98">
-        <v>3.75</v>
-      </c>
-      <c r="M98">
-        <v>2.75</v>
-      </c>
       <c r="N98">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q98">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R98">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S98">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T98">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U98">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V98">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W98">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X98">
         <v>-1</v>
       </c>
       <c r="Y98">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA98">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB98">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -16446,7 +16446,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C180" t="s">
         <v>28</v>
@@ -16458,73 +16458,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F180" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G180" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H180">
         <v>3</v>
       </c>
       <c r="I180">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J180" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K180">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L180">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M180">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N180">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O180">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P180">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q180">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R180">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S180">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T180">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U180">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V180">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W180">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X180">
         <v>-1</v>
       </c>
       <c r="Y180">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z180">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA180">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB180">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC180">
         <v>-1</v>
@@ -16535,7 +16535,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C181" t="s">
         <v>28</v>
@@ -16547,73 +16547,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F181" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G181" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H181">
         <v>3</v>
       </c>
       <c r="I181">
+        <v>2</v>
+      </c>
+      <c r="J181" t="s">
+        <v>42</v>
+      </c>
+      <c r="K181">
+        <v>1.909</v>
+      </c>
+      <c r="L181">
         <v>4</v>
       </c>
-      <c r="J181" t="s">
-        <v>41</v>
-      </c>
-      <c r="K181">
-        <v>2.45</v>
-      </c>
-      <c r="L181">
-        <v>3.75</v>
-      </c>
       <c r="M181">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N181">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O181">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P181">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q181">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R181">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S181">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T181">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U181">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V181">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W181">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X181">
         <v>-1</v>
       </c>
       <c r="Y181">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z181">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA181">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB181">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC181">
         <v>-1</v>
@@ -19650,7 +19650,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>7126789</v>
+        <v>7127376</v>
       </c>
       <c r="C216" t="s">
         <v>28</v>
@@ -19659,49 +19659,49 @@
         <v>28</v>
       </c>
       <c r="E216" s="2">
-        <v>45346.14583333334</v>
+        <v>45347.125</v>
       </c>
       <c r="F216" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G216" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K216">
-        <v>1.833</v>
+        <v>1.95</v>
       </c>
       <c r="L216">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="M216">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="N216">
-        <v>1.833</v>
+        <v>1.909</v>
       </c>
       <c r="O216">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="P216">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="Q216">
         <v>-0.5</v>
       </c>
       <c r="R216">
-        <v>1.86</v>
+        <v>1.95</v>
       </c>
       <c r="S216">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="T216">
         <v>3.25</v>
       </c>
       <c r="U216">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="V216">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="W216">
         <v>0</v>
@@ -19724,7 +19724,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>7127377</v>
+        <v>7127379</v>
       </c>
       <c r="C217" t="s">
         <v>28</v>
@@ -19733,49 +19733,49 @@
         <v>28</v>
       </c>
       <c r="E217" s="2">
-        <v>45346.23958333334</v>
+        <v>45347.125</v>
       </c>
       <c r="F217" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G217" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="K217">
-        <v>2.4</v>
+        <v>1.95</v>
       </c>
       <c r="L217">
+        <v>3.6</v>
+      </c>
+      <c r="M217">
+        <v>3.8</v>
+      </c>
+      <c r="N217">
+        <v>1.909</v>
+      </c>
+      <c r="O217">
+        <v>3.6</v>
+      </c>
+      <c r="P217">
         <v>4</v>
       </c>
-      <c r="M217">
-        <v>2.6</v>
-      </c>
-      <c r="N217">
-        <v>2.4</v>
-      </c>
-      <c r="O217">
-        <v>4</v>
-      </c>
-      <c r="P217">
-        <v>2.6</v>
-      </c>
       <c r="Q217">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R217">
-        <v>1.84</v>
+        <v>1.92</v>
       </c>
       <c r="S217">
-        <v>2.06</v>
+        <v>1.98</v>
       </c>
       <c r="T217">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U217">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V217">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W217">
         <v>0</v>
@@ -19798,7 +19798,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>7127378</v>
+        <v>7127380</v>
       </c>
       <c r="C218" t="s">
         <v>28</v>
@@ -19807,34 +19807,34 @@
         <v>28</v>
       </c>
       <c r="E218" s="2">
-        <v>45346.32291666666</v>
+        <v>45353.125</v>
       </c>
       <c r="F218" t="s">
+        <v>40</v>
+      </c>
+      <c r="G218" t="s">
         <v>34</v>
-      </c>
-      <c r="G218" t="s">
-        <v>31</v>
       </c>
       <c r="K218">
         <v>2.375</v>
       </c>
       <c r="L218">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M218">
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="N218">
-        <v>2.375</v>
+        <v>2</v>
       </c>
       <c r="O218">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P218">
-        <v>2.875</v>
+        <v>3.4</v>
       </c>
       <c r="Q218">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R218">
         <v>2.07</v>
@@ -19846,10 +19846,10 @@
         <v>3</v>
       </c>
       <c r="U218">
-        <v>1.975</v>
+        <v>1.8</v>
       </c>
       <c r="V218">
-        <v>1.875</v>
+        <v>2.05</v>
       </c>
       <c r="W218">
         <v>0</v>
@@ -19864,154 +19864,6 @@
         <v>0</v>
       </c>
       <c r="AA218">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="219" spans="1:29">
-      <c r="A219" s="1">
-        <v>217</v>
-      </c>
-      <c r="B219">
-        <v>7127376</v>
-      </c>
-      <c r="C219" t="s">
-        <v>28</v>
-      </c>
-      <c r="D219" t="s">
-        <v>28</v>
-      </c>
-      <c r="E219" s="2">
-        <v>45347.125</v>
-      </c>
-      <c r="F219" t="s">
-        <v>29</v>
-      </c>
-      <c r="G219" t="s">
-        <v>38</v>
-      </c>
-      <c r="K219">
-        <v>1.95</v>
-      </c>
-      <c r="L219">
-        <v>4</v>
-      </c>
-      <c r="M219">
-        <v>3.4</v>
-      </c>
-      <c r="N219">
-        <v>1.95</v>
-      </c>
-      <c r="O219">
-        <v>4</v>
-      </c>
-      <c r="P219">
-        <v>3.4</v>
-      </c>
-      <c r="Q219">
-        <v>-0.5</v>
-      </c>
-      <c r="R219">
-        <v>2</v>
-      </c>
-      <c r="S219">
-        <v>1.9</v>
-      </c>
-      <c r="T219">
-        <v>3.25</v>
-      </c>
-      <c r="U219">
-        <v>1.875</v>
-      </c>
-      <c r="V219">
-        <v>1.975</v>
-      </c>
-      <c r="W219">
-        <v>0</v>
-      </c>
-      <c r="X219">
-        <v>0</v>
-      </c>
-      <c r="Y219">
-        <v>0</v>
-      </c>
-      <c r="Z219">
-        <v>0</v>
-      </c>
-      <c r="AA219">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="220" spans="1:29">
-      <c r="A220" s="1">
-        <v>218</v>
-      </c>
-      <c r="B220">
-        <v>7127379</v>
-      </c>
-      <c r="C220" t="s">
-        <v>28</v>
-      </c>
-      <c r="D220" t="s">
-        <v>28</v>
-      </c>
-      <c r="E220" s="2">
-        <v>45347.125</v>
-      </c>
-      <c r="F220" t="s">
-        <v>33</v>
-      </c>
-      <c r="G220" t="s">
-        <v>36</v>
-      </c>
-      <c r="K220">
-        <v>1.95</v>
-      </c>
-      <c r="L220">
-        <v>3.6</v>
-      </c>
-      <c r="M220">
-        <v>3.8</v>
-      </c>
-      <c r="N220">
-        <v>1.95</v>
-      </c>
-      <c r="O220">
-        <v>3.6</v>
-      </c>
-      <c r="P220">
-        <v>3.8</v>
-      </c>
-      <c r="Q220">
-        <v>-0.5</v>
-      </c>
-      <c r="R220">
-        <v>1.98</v>
-      </c>
-      <c r="S220">
-        <v>1.92</v>
-      </c>
-      <c r="T220">
-        <v>2.75</v>
-      </c>
-      <c r="U220">
-        <v>1.95</v>
-      </c>
-      <c r="V220">
-        <v>1.9</v>
-      </c>
-      <c r="W220">
-        <v>0</v>
-      </c>
-      <c r="X220">
-        <v>0</v>
-      </c>
-      <c r="Y220">
-        <v>0</v>
-      </c>
-      <c r="Z220">
-        <v>0</v>
-      </c>
-      <c r="AA220">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 24-02-2024 às 21:58
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC218"/>
+  <dimension ref="A1:AC221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3274,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>5400043</v>
+        <v>5400042</v>
       </c>
       <c r="C32" t="s">
         <v>28</v>
@@ -3286,58 +3286,58 @@
         <v>44961.125</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" t="s">
         <v>42</v>
       </c>
       <c r="K32">
-        <v>2.15</v>
+        <v>1.533</v>
       </c>
       <c r="L32">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M32">
-        <v>3.4</v>
+        <v>6</v>
       </c>
       <c r="N32">
-        <v>2.2</v>
+        <v>1.333</v>
       </c>
       <c r="O32">
-        <v>3.75</v>
+        <v>5</v>
       </c>
       <c r="P32">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="Q32">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R32">
+        <v>1.85</v>
+      </c>
+      <c r="S32">
+        <v>2</v>
+      </c>
+      <c r="T32">
+        <v>3.25</v>
+      </c>
+      <c r="U32">
+        <v>1.875</v>
+      </c>
+      <c r="V32">
         <v>1.975</v>
       </c>
-      <c r="S32">
-        <v>1.875</v>
-      </c>
-      <c r="T32">
-        <v>3</v>
-      </c>
-      <c r="U32">
-        <v>1.95</v>
-      </c>
-      <c r="V32">
-        <v>1.9</v>
-      </c>
       <c r="W32">
-        <v>1.2</v>
+        <v>0.333</v>
       </c>
       <c r="X32">
         <v>-1</v>
@@ -3346,13 +3346,13 @@
         <v>-1</v>
       </c>
       <c r="Z32">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.95</v>
+        <v>0.875</v>
       </c>
       <c r="AC32">
         <v>-1</v>
@@ -3363,7 +3363,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>5400042</v>
+        <v>5400043</v>
       </c>
       <c r="C33" t="s">
         <v>28</v>
@@ -3375,58 +3375,58 @@
         <v>44961.125</v>
       </c>
       <c r="F33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H33">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" t="s">
         <v>42</v>
       </c>
       <c r="K33">
-        <v>1.533</v>
+        <v>2.15</v>
       </c>
       <c r="L33">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M33">
-        <v>6</v>
+        <v>3.4</v>
       </c>
       <c r="N33">
-        <v>1.333</v>
+        <v>2.2</v>
       </c>
       <c r="O33">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P33">
-        <v>9.5</v>
+        <v>3</v>
       </c>
       <c r="Q33">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R33">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S33">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T33">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U33">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V33">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W33">
-        <v>0.333</v>
+        <v>1.2</v>
       </c>
       <c r="X33">
         <v>-1</v>
@@ -3435,13 +3435,13 @@
         <v>-1</v>
       </c>
       <c r="Z33">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA33">
         <v>-1</v>
       </c>
       <c r="AB33">
-        <v>0.875</v>
+        <v>0.95</v>
       </c>
       <c r="AC33">
         <v>-1</v>
@@ -5499,7 +5499,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>5404704</v>
+        <v>5404706</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5511,58 +5511,58 @@
         <v>44989.125</v>
       </c>
       <c r="F57" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G57" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H57">
         <v>2</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J57" t="s">
         <v>42</v>
       </c>
       <c r="K57">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L57">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M57">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="N57">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="O57">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P57">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="Q57">
         <v>-0.25</v>
       </c>
       <c r="R57">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S57">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="T57">
         <v>2.75</v>
       </c>
       <c r="U57">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V57">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W57">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="X57">
         <v>-1</v>
@@ -5571,16 +5571,16 @@
         <v>-1</v>
       </c>
       <c r="Z57">
-        <v>0.875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA57">
         <v>-1</v>
       </c>
       <c r="AB57">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AC57">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5588,7 +5588,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>5404706</v>
+        <v>5404704</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5600,58 +5600,58 @@
         <v>44989.125</v>
       </c>
       <c r="F58" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G58" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H58">
         <v>2</v>
       </c>
       <c r="I58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="s">
         <v>42</v>
       </c>
       <c r="K58">
-        <v>2.1</v>
+        <v>2.4</v>
       </c>
       <c r="L58">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M58">
-        <v>3.2</v>
+        <v>2.6</v>
       </c>
       <c r="N58">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="O58">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P58">
-        <v>3.3</v>
+        <v>3.1</v>
       </c>
       <c r="Q58">
         <v>-0.25</v>
       </c>
       <c r="R58">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S58">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T58">
         <v>2.75</v>
       </c>
       <c r="U58">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V58">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W58">
-        <v>1.1</v>
+        <v>1.2</v>
       </c>
       <c r="X58">
         <v>-1</v>
@@ -5660,16 +5660,16 @@
         <v>-1</v>
       </c>
       <c r="Z58">
-        <v>0.8500000000000001</v>
+        <v>0.875</v>
       </c>
       <c r="AA58">
         <v>-1</v>
       </c>
       <c r="AB58">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AC58">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -6478,7 +6478,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>5404714</v>
+        <v>5404713</v>
       </c>
       <c r="C68" t="s">
         <v>28</v>
@@ -6490,76 +6490,76 @@
         <v>45003.125</v>
       </c>
       <c r="F68" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G68" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K68">
         <v>2.25</v>
       </c>
       <c r="L68">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="M68">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="N68">
-        <v>2.15</v>
+        <v>2.3</v>
       </c>
       <c r="O68">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P68">
-        <v>3.2</v>
+        <v>2.9</v>
       </c>
       <c r="Q68">
         <v>-0.25</v>
       </c>
       <c r="R68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T68">
         <v>2.75</v>
       </c>
       <c r="U68">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V68">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W68">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="X68">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y68">
         <v>-1</v>
       </c>
       <c r="Z68">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AA68">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB68">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC68">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="69" spans="1:29">
@@ -6567,7 +6567,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>5404713</v>
+        <v>5404714</v>
       </c>
       <c r="C69" t="s">
         <v>28</v>
@@ -6579,76 +6579,76 @@
         <v>45003.125</v>
       </c>
       <c r="F69" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G69" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K69">
         <v>2.25</v>
       </c>
       <c r="L69">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="M69">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="N69">
-        <v>2.3</v>
+        <v>2.15</v>
       </c>
       <c r="O69">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P69">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="Q69">
         <v>-0.25</v>
       </c>
       <c r="R69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="S69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="T69">
         <v>2.75</v>
       </c>
       <c r="U69">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V69">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W69">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="X69">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y69">
         <v>-1</v>
       </c>
       <c r="Z69">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AA69">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB69">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC69">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="70" spans="1:29">
@@ -9059,7 +9059,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>5404732</v>
+        <v>5400063</v>
       </c>
       <c r="C97" t="s">
         <v>28</v>
@@ -9071,73 +9071,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F97" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G97" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I97">
+        <v>2</v>
+      </c>
+      <c r="J97" t="s">
+        <v>42</v>
+      </c>
+      <c r="K97">
+        <v>1.75</v>
+      </c>
+      <c r="L97">
+        <v>3.8</v>
+      </c>
+      <c r="M97">
         <v>4</v>
       </c>
-      <c r="J97" t="s">
-        <v>41</v>
-      </c>
-      <c r="K97">
-        <v>2.3</v>
-      </c>
-      <c r="L97">
-        <v>3.75</v>
-      </c>
-      <c r="M97">
-        <v>2.75</v>
-      </c>
       <c r="N97">
-        <v>2.625</v>
+        <v>2</v>
       </c>
       <c r="O97">
         <v>4</v>
       </c>
       <c r="P97">
-        <v>2.4</v>
+        <v>3.4</v>
       </c>
       <c r="Q97">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R97">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S97">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="T97">
-        <v>3.75</v>
+        <v>3</v>
       </c>
       <c r="U97">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V97">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W97">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="X97">
         <v>-1</v>
       </c>
       <c r="Y97">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z97">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AA97">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB97">
-        <v>1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC97">
         <v>-1</v>
@@ -9148,7 +9148,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>5400063</v>
+        <v>5404732</v>
       </c>
       <c r="C98" t="s">
         <v>28</v>
@@ -9160,73 +9160,73 @@
         <v>45044.28125</v>
       </c>
       <c r="F98" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H98">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J98" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K98">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="L98">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="M98">
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N98">
-        <v>2</v>
+        <v>2.625</v>
       </c>
       <c r="O98">
         <v>4</v>
       </c>
       <c r="P98">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="Q98">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="R98">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="S98">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="T98">
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="U98">
+        <v>2</v>
+      </c>
+      <c r="V98">
         <v>1.85</v>
       </c>
-      <c r="V98">
-        <v>2</v>
-      </c>
       <c r="W98">
+        <v>-1</v>
+      </c>
+      <c r="X98">
+        <v>-1</v>
+      </c>
+      <c r="Y98">
+        <v>1.4</v>
+      </c>
+      <c r="Z98">
+        <v>-1</v>
+      </c>
+      <c r="AA98">
+        <v>0.8</v>
+      </c>
+      <c r="AB98">
         <v>1</v>
-      </c>
-      <c r="X98">
-        <v>-1</v>
-      </c>
-      <c r="Y98">
-        <v>-1</v>
-      </c>
-      <c r="Z98">
-        <v>1.025</v>
-      </c>
-      <c r="AA98">
-        <v>-1</v>
-      </c>
-      <c r="AB98">
-        <v>0.8500000000000001</v>
       </c>
       <c r="AC98">
         <v>-1</v>
@@ -16446,7 +16446,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C180" t="s">
         <v>28</v>
@@ -16458,73 +16458,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F180" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G180" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H180">
         <v>3</v>
       </c>
       <c r="I180">
+        <v>2</v>
+      </c>
+      <c r="J180" t="s">
+        <v>42</v>
+      </c>
+      <c r="K180">
+        <v>1.909</v>
+      </c>
+      <c r="L180">
         <v>4</v>
       </c>
-      <c r="J180" t="s">
-        <v>41</v>
-      </c>
-      <c r="K180">
-        <v>2.45</v>
-      </c>
-      <c r="L180">
-        <v>3.75</v>
-      </c>
       <c r="M180">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N180">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O180">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P180">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q180">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R180">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S180">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T180">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U180">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V180">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W180">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X180">
         <v>-1</v>
       </c>
       <c r="Y180">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z180">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA180">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB180">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC180">
         <v>-1</v>
@@ -16535,7 +16535,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C181" t="s">
         <v>28</v>
@@ -16547,73 +16547,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F181" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G181" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H181">
         <v>3</v>
       </c>
       <c r="I181">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J181" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K181">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L181">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M181">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N181">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O181">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P181">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q181">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R181">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S181">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T181">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U181">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V181">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W181">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X181">
         <v>-1</v>
       </c>
       <c r="Y181">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z181">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA181">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB181">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC181">
         <v>-1</v>
@@ -19205,7 +19205,7 @@
         <v>209</v>
       </c>
       <c r="B211">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C211" t="s">
         <v>28</v>
@@ -19217,76 +19217,76 @@
         <v>45340.125</v>
       </c>
       <c r="F211" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G211" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H211">
         <v>1</v>
       </c>
       <c r="I211">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J211" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K211">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L211">
         <v>3.75</v>
       </c>
       <c r="M211">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N211">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O211">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P211">
+        <v>3.25</v>
+      </c>
+      <c r="Q211">
+        <v>-0.25</v>
+      </c>
+      <c r="R211">
+        <v>1.86</v>
+      </c>
+      <c r="S211">
+        <v>2.04</v>
+      </c>
+      <c r="T211">
         <v>2.75</v>
       </c>
-      <c r="Q211">
-        <v>0</v>
-      </c>
-      <c r="R211">
-        <v>1.8</v>
-      </c>
-      <c r="S211">
-        <v>2.05</v>
-      </c>
-      <c r="T211">
-        <v>3</v>
-      </c>
       <c r="U211">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V211">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W211">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X211">
         <v>-1</v>
       </c>
       <c r="Y211">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z211">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA211">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB211">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC211">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="212" spans="1:29">
@@ -19294,7 +19294,7 @@
         <v>210</v>
       </c>
       <c r="B212">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C212" t="s">
         <v>28</v>
@@ -19306,76 +19306,76 @@
         <v>45340.125</v>
       </c>
       <c r="F212" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G212" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H212">
         <v>1</v>
       </c>
       <c r="I212">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J212" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K212">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L212">
         <v>3.75</v>
       </c>
       <c r="M212">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N212">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O212">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P212">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q212">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R212">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S212">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T212">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U212">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V212">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W212">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X212">
         <v>-1</v>
       </c>
       <c r="Y212">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z212">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA212">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB212">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC212">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="213" spans="1:29">
@@ -19650,7 +19650,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>7127376</v>
+        <v>7126789</v>
       </c>
       <c r="C216" t="s">
         <v>28</v>
@@ -19659,64 +19659,79 @@
         <v>28</v>
       </c>
       <c r="E216" s="2">
-        <v>45347.125</v>
+        <v>45346.14583333334</v>
       </c>
       <c r="F216" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G216" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="H216">
+        <v>1</v>
+      </c>
+      <c r="I216">
+        <v>1</v>
+      </c>
+      <c r="J216" t="s">
+        <v>43</v>
       </c>
       <c r="K216">
-        <v>1.95</v>
+        <v>1.833</v>
       </c>
       <c r="L216">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="M216">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="N216">
-        <v>1.909</v>
+        <v>1.833</v>
       </c>
       <c r="O216">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="P216">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="Q216">
         <v>-0.5</v>
       </c>
       <c r="R216">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="S216">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="T216">
         <v>3.25</v>
       </c>
       <c r="U216">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="V216">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="W216">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X216">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="Y216">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z216">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA216">
-        <v>0</v>
+        <v>1.025</v>
+      </c>
+      <c r="AB216">
+        <v>-1</v>
+      </c>
+      <c r="AC216">
+        <v>1.025</v>
       </c>
     </row>
     <row r="217" spans="1:29">
@@ -19724,7 +19739,7 @@
         <v>215</v>
       </c>
       <c r="B217">
-        <v>7127379</v>
+        <v>7127377</v>
       </c>
       <c r="C217" t="s">
         <v>28</v>
@@ -19733,64 +19748,79 @@
         <v>28</v>
       </c>
       <c r="E217" s="2">
-        <v>45347.125</v>
+        <v>45346.23958333334</v>
       </c>
       <c r="F217" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G217" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="H217">
+        <v>1</v>
+      </c>
+      <c r="I217">
+        <v>2</v>
+      </c>
+      <c r="J217" t="s">
+        <v>41</v>
       </c>
       <c r="K217">
+        <v>2.4</v>
+      </c>
+      <c r="L217">
+        <v>4</v>
+      </c>
+      <c r="M217">
+        <v>2.6</v>
+      </c>
+      <c r="N217">
+        <v>2.45</v>
+      </c>
+      <c r="O217">
+        <v>4</v>
+      </c>
+      <c r="P217">
+        <v>2.55</v>
+      </c>
+      <c r="Q217">
+        <v>0</v>
+      </c>
+      <c r="R217">
+        <v>1.9</v>
+      </c>
+      <c r="S217">
         <v>1.95</v>
       </c>
-      <c r="L217">
-        <v>3.6</v>
-      </c>
-      <c r="M217">
-        <v>3.8</v>
-      </c>
-      <c r="N217">
-        <v>1.909</v>
-      </c>
-      <c r="O217">
-        <v>3.6</v>
-      </c>
-      <c r="P217">
-        <v>4</v>
-      </c>
-      <c r="Q217">
+      <c r="T217">
+        <v>3.25</v>
+      </c>
+      <c r="U217">
+        <v>2</v>
+      </c>
+      <c r="V217">
+        <v>1.85</v>
+      </c>
+      <c r="W217">
+        <v>-1</v>
+      </c>
+      <c r="X217">
+        <v>-1</v>
+      </c>
+      <c r="Y217">
+        <v>1.55</v>
+      </c>
+      <c r="Z217">
+        <v>-1</v>
+      </c>
+      <c r="AA217">
+        <v>0.95</v>
+      </c>
+      <c r="AB217">
         <v>-0.5</v>
       </c>
-      <c r="R217">
-        <v>1.92</v>
-      </c>
-      <c r="S217">
-        <v>1.98</v>
-      </c>
-      <c r="T217">
-        <v>2.75</v>
-      </c>
-      <c r="U217">
-        <v>1.925</v>
-      </c>
-      <c r="V217">
-        <v>1.925</v>
-      </c>
-      <c r="W217">
-        <v>0</v>
-      </c>
-      <c r="X217">
-        <v>0</v>
-      </c>
-      <c r="Y217">
-        <v>0</v>
-      </c>
-      <c r="Z217">
-        <v>0</v>
-      </c>
-      <c r="AA217">
-        <v>0</v>
+      <c r="AC217">
+        <v>0.425</v>
       </c>
     </row>
     <row r="218" spans="1:29">
@@ -19798,7 +19828,7 @@
         <v>216</v>
       </c>
       <c r="B218">
-        <v>7127380</v>
+        <v>7127378</v>
       </c>
       <c r="C218" t="s">
         <v>28</v>
@@ -19807,63 +19837,300 @@
         <v>28</v>
       </c>
       <c r="E218" s="2">
-        <v>45353.125</v>
+        <v>45346.32291666666</v>
       </c>
       <c r="F218" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G218" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="I218">
+        <v>0</v>
+      </c>
+      <c r="J218" t="s">
+        <v>43</v>
       </c>
       <c r="K218">
         <v>2.375</v>
       </c>
       <c r="L218">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M218">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="N218">
         <v>2</v>
       </c>
       <c r="O218">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P218">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="Q218">
         <v>-0.5</v>
       </c>
       <c r="R218">
+        <v>1.975</v>
+      </c>
+      <c r="S218">
+        <v>1.875</v>
+      </c>
+      <c r="T218">
+        <v>2.75</v>
+      </c>
+      <c r="U218">
+        <v>1.925</v>
+      </c>
+      <c r="V218">
+        <v>1.925</v>
+      </c>
+      <c r="W218">
+        <v>-1</v>
+      </c>
+      <c r="X218">
+        <v>2.4</v>
+      </c>
+      <c r="Y218">
+        <v>-1</v>
+      </c>
+      <c r="Z218">
+        <v>-1</v>
+      </c>
+      <c r="AA218">
+        <v>0.875</v>
+      </c>
+      <c r="AB218">
+        <v>-1</v>
+      </c>
+      <c r="AC218">
+        <v>0.925</v>
+      </c>
+    </row>
+    <row r="219" spans="1:29">
+      <c r="A219" s="1">
+        <v>217</v>
+      </c>
+      <c r="B219">
+        <v>7127376</v>
+      </c>
+      <c r="C219" t="s">
+        <v>28</v>
+      </c>
+      <c r="D219" t="s">
+        <v>28</v>
+      </c>
+      <c r="E219" s="2">
+        <v>45347.125</v>
+      </c>
+      <c r="F219" t="s">
+        <v>29</v>
+      </c>
+      <c r="G219" t="s">
+        <v>38</v>
+      </c>
+      <c r="K219">
+        <v>1.95</v>
+      </c>
+      <c r="L219">
+        <v>4</v>
+      </c>
+      <c r="M219">
+        <v>3.4</v>
+      </c>
+      <c r="N219">
+        <v>1.909</v>
+      </c>
+      <c r="O219">
+        <v>4</v>
+      </c>
+      <c r="P219">
+        <v>3.5</v>
+      </c>
+      <c r="Q219">
+        <v>-0.5</v>
+      </c>
+      <c r="R219">
+        <v>1.92</v>
+      </c>
+      <c r="S219">
+        <v>1.98</v>
+      </c>
+      <c r="T219">
+        <v>3.25</v>
+      </c>
+      <c r="U219">
+        <v>1.825</v>
+      </c>
+      <c r="V219">
+        <v>2.025</v>
+      </c>
+      <c r="W219">
+        <v>0</v>
+      </c>
+      <c r="X219">
+        <v>0</v>
+      </c>
+      <c r="Y219">
+        <v>0</v>
+      </c>
+      <c r="Z219">
+        <v>0</v>
+      </c>
+      <c r="AA219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:29">
+      <c r="A220" s="1">
+        <v>218</v>
+      </c>
+      <c r="B220">
+        <v>7127379</v>
+      </c>
+      <c r="C220" t="s">
+        <v>28</v>
+      </c>
+      <c r="D220" t="s">
+        <v>28</v>
+      </c>
+      <c r="E220" s="2">
+        <v>45347.125</v>
+      </c>
+      <c r="F220" t="s">
+        <v>33</v>
+      </c>
+      <c r="G220" t="s">
+        <v>36</v>
+      </c>
+      <c r="K220">
+        <v>1.95</v>
+      </c>
+      <c r="L220">
+        <v>3.6</v>
+      </c>
+      <c r="M220">
+        <v>3.8</v>
+      </c>
+      <c r="N220">
+        <v>1.909</v>
+      </c>
+      <c r="O220">
+        <v>3.6</v>
+      </c>
+      <c r="P220">
+        <v>4</v>
+      </c>
+      <c r="Q220">
+        <v>-0.5</v>
+      </c>
+      <c r="R220">
+        <v>1.92</v>
+      </c>
+      <c r="S220">
+        <v>1.98</v>
+      </c>
+      <c r="T220">
+        <v>2.75</v>
+      </c>
+      <c r="U220">
+        <v>1.925</v>
+      </c>
+      <c r="V220">
+        <v>1.925</v>
+      </c>
+      <c r="W220">
+        <v>0</v>
+      </c>
+      <c r="X220">
+        <v>0</v>
+      </c>
+      <c r="Y220">
+        <v>0</v>
+      </c>
+      <c r="Z220">
+        <v>0</v>
+      </c>
+      <c r="AA220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:29">
+      <c r="A221" s="1">
+        <v>219</v>
+      </c>
+      <c r="B221">
+        <v>7127380</v>
+      </c>
+      <c r="C221" t="s">
+        <v>28</v>
+      </c>
+      <c r="D221" t="s">
+        <v>28</v>
+      </c>
+      <c r="E221" s="2">
+        <v>45353.125</v>
+      </c>
+      <c r="F221" t="s">
+        <v>40</v>
+      </c>
+      <c r="G221" t="s">
+        <v>34</v>
+      </c>
+      <c r="K221">
+        <v>2.375</v>
+      </c>
+      <c r="L221">
+        <v>3.6</v>
+      </c>
+      <c r="M221">
+        <v>2.75</v>
+      </c>
+      <c r="N221">
+        <v>2</v>
+      </c>
+      <c r="O221">
+        <v>3.6</v>
+      </c>
+      <c r="P221">
+        <v>3.4</v>
+      </c>
+      <c r="Q221">
+        <v>-0.5</v>
+      </c>
+      <c r="R221">
         <v>2.07</v>
       </c>
-      <c r="S218">
+      <c r="S221">
         <v>1.83</v>
       </c>
-      <c r="T218">
+      <c r="T221">
         <v>3</v>
       </c>
-      <c r="U218">
+      <c r="U221">
         <v>1.8</v>
       </c>
-      <c r="V218">
+      <c r="V221">
         <v>2.05</v>
       </c>
-      <c r="W218">
+      <c r="W221">
         <v>0</v>
       </c>
-      <c r="X218">
+      <c r="X221">
         <v>0</v>
       </c>
-      <c r="Y218">
+      <c r="Y221">
         <v>0</v>
       </c>
-      <c r="Z218">
+      <c r="Z221">
         <v>0</v>
       </c>
-      <c r="AA218">
+      <c r="AA221">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 26-02-2024 às 22:04
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -10685,10 +10685,10 @@
         <v>-0.25</v>
       </c>
       <c r="R115">
-        <v>1.85</v>
+        <v>1.86</v>
       </c>
       <c r="S115">
-        <v>2.05</v>
+        <v>2.04</v>
       </c>
       <c r="T115">
         <v>3</v>
@@ -10747,31 +10747,31 @@
         <v>1.95</v>
       </c>
       <c r="N116">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="O116">
         <v>3.6</v>
       </c>
       <c r="P116">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="Q116">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R116">
-        <v>2.08</v>
+        <v>1.88</v>
       </c>
       <c r="S116">
-        <v>1.82</v>
+        <v>2.02</v>
       </c>
       <c r="T116">
         <v>3</v>
       </c>
       <c r="U116">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="V116">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W116">
         <v>0</v>
@@ -10833,19 +10833,19 @@
         <v>0</v>
       </c>
       <c r="R117">
-        <v>1.87</v>
+        <v>1.9</v>
       </c>
       <c r="S117">
-        <v>2.03</v>
+        <v>2</v>
       </c>
       <c r="T117">
         <v>3</v>
       </c>
       <c r="U117">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V117">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W117">
         <v>0</v>
@@ -10895,22 +10895,22 @@
         <v>3.5</v>
       </c>
       <c r="N118">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="O118">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P118">
-        <v>3.4</v>
+        <v>3.1</v>
       </c>
       <c r="Q118">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R118">
-        <v>2.07</v>
+        <v>1.97</v>
       </c>
       <c r="S118">
-        <v>1.83</v>
+        <v>1.93</v>
       </c>
       <c r="T118">
         <v>3.25</v>
@@ -10975,25 +10975,25 @@
         <v>3.6</v>
       </c>
       <c r="P119">
-        <v>2.25</v>
+        <v>2.2</v>
       </c>
       <c r="Q119">
         <v>0.25</v>
       </c>
       <c r="R119">
-        <v>1.88</v>
+        <v>1.92</v>
       </c>
       <c r="S119">
-        <v>2.02</v>
+        <v>1.98</v>
       </c>
       <c r="T119">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U119">
+        <v>2</v>
+      </c>
+      <c r="V119">
         <v>1.85</v>
-      </c>
-      <c r="V119">
-        <v>2</v>
       </c>
       <c r="W119">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 29-02-2024 às 07:50
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -10602,28 +10602,28 @@
         <v>2.9</v>
       </c>
       <c r="O114">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P114">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="Q114">
         <v>0.25</v>
       </c>
       <c r="R114">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="S114">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T114">
         <v>3.25</v>
       </c>
       <c r="U114">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V114">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W114">
         <v>0</v>
@@ -10673,7 +10673,7 @@
         <v>2.75</v>
       </c>
       <c r="N115">
-        <v>2.05</v>
+        <v>2.1</v>
       </c>
       <c r="O115">
         <v>3.6</v>
@@ -10685,10 +10685,10 @@
         <v>-0.25</v>
       </c>
       <c r="R115">
-        <v>1.86</v>
+        <v>1.84</v>
       </c>
       <c r="S115">
-        <v>2.04</v>
+        <v>2.06</v>
       </c>
       <c r="T115">
         <v>3</v>
@@ -10753,25 +10753,25 @@
         <v>3.6</v>
       </c>
       <c r="P116">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="Q116">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R116">
-        <v>1.88</v>
+        <v>2.07</v>
       </c>
       <c r="S116">
-        <v>2.02</v>
+        <v>1.83</v>
       </c>
       <c r="T116">
         <v>3</v>
       </c>
       <c r="U116">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V116">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="W116">
         <v>0</v>
@@ -10821,7 +10821,7 @@
         <v>2.7</v>
       </c>
       <c r="N117">
-        <v>2.5</v>
+        <v>2.6</v>
       </c>
       <c r="O117">
         <v>3.4</v>
@@ -10842,10 +10842,10 @@
         <v>3</v>
       </c>
       <c r="U117">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="V117">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="W117">
         <v>0</v>
@@ -10898,10 +10898,10 @@
         <v>2.2</v>
       </c>
       <c r="O118">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P118">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="Q118">
         <v>-0.25</v>
@@ -10969,31 +10969,31 @@
         <v>2.2</v>
       </c>
       <c r="N119">
-        <v>2.9</v>
+        <v>3.2</v>
       </c>
       <c r="O119">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P119">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="Q119">
         <v>0.25</v>
       </c>
       <c r="R119">
-        <v>1.92</v>
+        <v>2.06</v>
       </c>
       <c r="S119">
-        <v>1.98</v>
+        <v>1.84</v>
       </c>
       <c r="T119">
         <v>3</v>
       </c>
       <c r="U119">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="V119">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="W119">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 02-03-2024 às 08:34
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC119"/>
+  <dimension ref="A1:AC116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -10589,6 +10589,15 @@
       <c r="G114" t="s">
         <v>29</v>
       </c>
+      <c r="H114">
+        <v>2</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114" t="s">
+        <v>42</v>
+      </c>
       <c r="K114">
         <v>3</v>
       </c>
@@ -10605,40 +10614,46 @@
         <v>4</v>
       </c>
       <c r="P114">
-        <v>2.2</v>
+        <v>2.15</v>
       </c>
       <c r="Q114">
         <v>0.25</v>
       </c>
       <c r="R114">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="S114">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="T114">
         <v>3.25</v>
       </c>
       <c r="U114">
+        <v>1.975</v>
+      </c>
+      <c r="V114">
+        <v>1.875</v>
+      </c>
+      <c r="W114">
         <v>1.9</v>
       </c>
-      <c r="V114">
-        <v>1.95</v>
-      </c>
-      <c r="W114">
-        <v>0</v>
-      </c>
       <c r="X114">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y114">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z114">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="AA114">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB114">
+        <v>-1</v>
+      </c>
+      <c r="AC114">
+        <v>0.875</v>
       </c>
     </row>
     <row r="115" spans="1:29">
@@ -10646,7 +10661,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>7127380</v>
+        <v>7127383</v>
       </c>
       <c r="C115" t="s">
         <v>28</v>
@@ -10655,40 +10670,40 @@
         <v>28</v>
       </c>
       <c r="E115" s="2">
-        <v>45353.125</v>
+        <v>45354.04166666666</v>
       </c>
       <c r="F115" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G115" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K115">
-        <v>2.375</v>
+        <v>2</v>
       </c>
       <c r="L115">
         <v>3.6</v>
       </c>
       <c r="M115">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="N115">
         <v>2.1</v>
       </c>
       <c r="O115">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P115">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="Q115">
         <v>-0.25</v>
       </c>
       <c r="R115">
-        <v>1.84</v>
+        <v>1.88</v>
       </c>
       <c r="S115">
-        <v>2.06</v>
+        <v>2.02</v>
       </c>
       <c r="T115">
         <v>3</v>
@@ -10720,7 +10735,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>7127381</v>
+        <v>7127384</v>
       </c>
       <c r="C116" t="s">
         <v>28</v>
@@ -10729,28 +10744,28 @@
         <v>28</v>
       </c>
       <c r="E116" s="2">
-        <v>45353.16666666666</v>
+        <v>45354.125</v>
       </c>
       <c r="F116" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G116" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K116">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="L116">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="M116">
-        <v>1.95</v>
+        <v>2.2</v>
       </c>
       <c r="N116">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="O116">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P116">
         <v>2.1</v>
@@ -10786,228 +10801,6 @@
         <v>0</v>
       </c>
       <c r="AA116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:29">
-      <c r="A117" s="1">
-        <v>115</v>
-      </c>
-      <c r="B117">
-        <v>7127382</v>
-      </c>
-      <c r="C117" t="s">
-        <v>28</v>
-      </c>
-      <c r="D117" t="s">
-        <v>28</v>
-      </c>
-      <c r="E117" s="2">
-        <v>45353.23958333334</v>
-      </c>
-      <c r="F117" t="s">
-        <v>33</v>
-      </c>
-      <c r="G117" t="s">
-        <v>32</v>
-      </c>
-      <c r="K117">
-        <v>2.5</v>
-      </c>
-      <c r="L117">
-        <v>3.4</v>
-      </c>
-      <c r="M117">
-        <v>2.7</v>
-      </c>
-      <c r="N117">
-        <v>2.6</v>
-      </c>
-      <c r="O117">
-        <v>3.4</v>
-      </c>
-      <c r="P117">
-        <v>2.7</v>
-      </c>
-      <c r="Q117">
-        <v>0</v>
-      </c>
-      <c r="R117">
-        <v>1.9</v>
-      </c>
-      <c r="S117">
-        <v>2</v>
-      </c>
-      <c r="T117">
-        <v>3</v>
-      </c>
-      <c r="U117">
-        <v>1.85</v>
-      </c>
-      <c r="V117">
-        <v>2</v>
-      </c>
-      <c r="W117">
-        <v>0</v>
-      </c>
-      <c r="X117">
-        <v>0</v>
-      </c>
-      <c r="Y117">
-        <v>0</v>
-      </c>
-      <c r="Z117">
-        <v>0</v>
-      </c>
-      <c r="AA117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:29">
-      <c r="A118" s="1">
-        <v>116</v>
-      </c>
-      <c r="B118">
-        <v>7127383</v>
-      </c>
-      <c r="C118" t="s">
-        <v>28</v>
-      </c>
-      <c r="D118" t="s">
-        <v>28</v>
-      </c>
-      <c r="E118" s="2">
-        <v>45354.04166666666</v>
-      </c>
-      <c r="F118" t="s">
-        <v>36</v>
-      </c>
-      <c r="G118" t="s">
-        <v>30</v>
-      </c>
-      <c r="K118">
-        <v>2</v>
-      </c>
-      <c r="L118">
-        <v>3.6</v>
-      </c>
-      <c r="M118">
-        <v>3.5</v>
-      </c>
-      <c r="N118">
-        <v>2.2</v>
-      </c>
-      <c r="O118">
-        <v>3.75</v>
-      </c>
-      <c r="P118">
-        <v>3</v>
-      </c>
-      <c r="Q118">
-        <v>-0.25</v>
-      </c>
-      <c r="R118">
-        <v>1.97</v>
-      </c>
-      <c r="S118">
-        <v>1.93</v>
-      </c>
-      <c r="T118">
-        <v>3.25</v>
-      </c>
-      <c r="U118">
-        <v>2.025</v>
-      </c>
-      <c r="V118">
-        <v>1.825</v>
-      </c>
-      <c r="W118">
-        <v>0</v>
-      </c>
-      <c r="X118">
-        <v>0</v>
-      </c>
-      <c r="Y118">
-        <v>0</v>
-      </c>
-      <c r="Z118">
-        <v>0</v>
-      </c>
-      <c r="AA118">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="1:29">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119">
-        <v>7127384</v>
-      </c>
-      <c r="C119" t="s">
-        <v>28</v>
-      </c>
-      <c r="D119" t="s">
-        <v>28</v>
-      </c>
-      <c r="E119" s="2">
-        <v>45354.125</v>
-      </c>
-      <c r="F119" t="s">
-        <v>35</v>
-      </c>
-      <c r="G119" t="s">
-        <v>38</v>
-      </c>
-      <c r="K119">
-        <v>3</v>
-      </c>
-      <c r="L119">
-        <v>3.6</v>
-      </c>
-      <c r="M119">
-        <v>2.2</v>
-      </c>
-      <c r="N119">
-        <v>3.2</v>
-      </c>
-      <c r="O119">
-        <v>3.8</v>
-      </c>
-      <c r="P119">
-        <v>2.1</v>
-      </c>
-      <c r="Q119">
-        <v>0.25</v>
-      </c>
-      <c r="R119">
-        <v>2.06</v>
-      </c>
-      <c r="S119">
-        <v>1.84</v>
-      </c>
-      <c r="T119">
-        <v>3</v>
-      </c>
-      <c r="U119">
-        <v>2.05</v>
-      </c>
-      <c r="V119">
-        <v>1.8</v>
-      </c>
-      <c r="W119">
-        <v>0</v>
-      </c>
-      <c r="X119">
-        <v>0</v>
-      </c>
-      <c r="Y119">
-        <v>0</v>
-      </c>
-      <c r="Z119">
-        <v>0</v>
-      </c>
-      <c r="AA119">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 03-03-2024 às 00:35
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC116"/>
+  <dimension ref="A1:AC120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10661,7 +10661,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>7127383</v>
+        <v>7127380</v>
       </c>
       <c r="C115" t="s">
         <v>28</v>
@@ -10670,64 +10670,79 @@
         <v>28</v>
       </c>
       <c r="E115" s="2">
-        <v>45354.04166666666</v>
+        <v>45353.125</v>
       </c>
       <c r="F115" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G115" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="H115">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115" t="s">
+        <v>42</v>
       </c>
       <c r="K115">
-        <v>2</v>
+        <v>2.375</v>
       </c>
       <c r="L115">
         <v>3.6</v>
       </c>
       <c r="M115">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="N115">
-        <v>2.1</v>
+        <v>2.25</v>
       </c>
       <c r="O115">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P115">
-        <v>3.2</v>
+        <v>3</v>
       </c>
       <c r="Q115">
         <v>-0.25</v>
       </c>
       <c r="R115">
-        <v>1.88</v>
+        <v>2.025</v>
       </c>
       <c r="S115">
-        <v>2.02</v>
+        <v>1.825</v>
       </c>
       <c r="T115">
         <v>3</v>
       </c>
       <c r="U115">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="V115">
-        <v>2.025</v>
+        <v>2.05</v>
       </c>
       <c r="W115">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="X115">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y115">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z115">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AA115">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB115">
+        <v>-1</v>
+      </c>
+      <c r="AC115">
+        <v>1.05</v>
       </c>
     </row>
     <row r="116" spans="1:29">
@@ -10735,7 +10750,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>7127384</v>
+        <v>7127381</v>
       </c>
       <c r="C116" t="s">
         <v>28</v>
@@ -10744,63 +10759,389 @@
         <v>28</v>
       </c>
       <c r="E116" s="2">
-        <v>45354.125</v>
+        <v>45353.16666666666</v>
       </c>
       <c r="F116" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G116" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116" t="s">
+        <v>41</v>
       </c>
       <c r="K116">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="L116">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="M116">
-        <v>2.2</v>
+        <v>1.95</v>
       </c>
       <c r="N116">
-        <v>3.2</v>
+        <v>3.25</v>
       </c>
       <c r="O116">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="P116">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="Q116">
         <v>0.25</v>
       </c>
       <c r="R116">
-        <v>2.07</v>
+        <v>2.06</v>
       </c>
       <c r="S116">
-        <v>1.83</v>
+        <v>1.84</v>
       </c>
       <c r="T116">
+        <v>2.75</v>
+      </c>
+      <c r="U116">
+        <v>1.825</v>
+      </c>
+      <c r="V116">
+        <v>2.025</v>
+      </c>
+      <c r="W116">
+        <v>-1</v>
+      </c>
+      <c r="X116">
+        <v>-1</v>
+      </c>
+      <c r="Y116">
+        <v>1.05</v>
+      </c>
+      <c r="Z116">
+        <v>-1</v>
+      </c>
+      <c r="AA116">
+        <v>0.8400000000000001</v>
+      </c>
+      <c r="AB116">
+        <v>-1</v>
+      </c>
+      <c r="AC116">
+        <v>1.025</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29">
+      <c r="A117" s="1">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>7127382</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117" t="s">
+        <v>28</v>
+      </c>
+      <c r="E117" s="2">
+        <v>45353.23958333334</v>
+      </c>
+      <c r="F117" t="s">
+        <v>33</v>
+      </c>
+      <c r="G117" t="s">
+        <v>32</v>
+      </c>
+      <c r="H117">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>4</v>
+      </c>
+      <c r="J117" t="s">
+        <v>41</v>
+      </c>
+      <c r="K117">
+        <v>2.5</v>
+      </c>
+      <c r="L117">
+        <v>3.4</v>
+      </c>
+      <c r="M117">
+        <v>2.7</v>
+      </c>
+      <c r="N117">
+        <v>2.875</v>
+      </c>
+      <c r="O117">
+        <v>3.8</v>
+      </c>
+      <c r="P117">
+        <v>2.25</v>
+      </c>
+      <c r="Q117">
+        <v>0.25</v>
+      </c>
+      <c r="R117">
+        <v>1.85</v>
+      </c>
+      <c r="S117">
+        <v>2</v>
+      </c>
+      <c r="T117">
         <v>3</v>
       </c>
-      <c r="U116">
+      <c r="U117">
+        <v>1.825</v>
+      </c>
+      <c r="V117">
         <v>2.025</v>
       </c>
-      <c r="V116">
-        <v>1.825</v>
-      </c>
-      <c r="W116">
+      <c r="W117">
+        <v>-1</v>
+      </c>
+      <c r="X117">
+        <v>-1</v>
+      </c>
+      <c r="Y117">
+        <v>1.25</v>
+      </c>
+      <c r="Z117">
+        <v>-1</v>
+      </c>
+      <c r="AA117">
+        <v>1</v>
+      </c>
+      <c r="AB117">
+        <v>0.825</v>
+      </c>
+      <c r="AC117">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:29">
+      <c r="A118" s="1">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>7127383</v>
+      </c>
+      <c r="C118" t="s">
+        <v>28</v>
+      </c>
+      <c r="D118" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="2">
+        <v>45354.04166666666</v>
+      </c>
+      <c r="F118" t="s">
+        <v>36</v>
+      </c>
+      <c r="G118" t="s">
+        <v>30</v>
+      </c>
+      <c r="K118">
+        <v>2</v>
+      </c>
+      <c r="L118">
+        <v>3.6</v>
+      </c>
+      <c r="M118">
+        <v>3.5</v>
+      </c>
+      <c r="N118">
+        <v>1.909</v>
+      </c>
+      <c r="O118">
+        <v>3.8</v>
+      </c>
+      <c r="P118">
+        <v>3.75</v>
+      </c>
+      <c r="Q118">
+        <v>-0.5</v>
+      </c>
+      <c r="R118">
+        <v>1.91</v>
+      </c>
+      <c r="S118">
+        <v>1.99</v>
+      </c>
+      <c r="T118">
+        <v>3</v>
+      </c>
+      <c r="U118">
+        <v>1.95</v>
+      </c>
+      <c r="V118">
+        <v>1.9</v>
+      </c>
+      <c r="W118">
         <v>0</v>
       </c>
-      <c r="X116">
+      <c r="X118">
         <v>0</v>
       </c>
-      <c r="Y116">
+      <c r="Y118">
         <v>0</v>
       </c>
-      <c r="Z116">
+      <c r="Z118">
         <v>0</v>
       </c>
-      <c r="AA116">
+      <c r="AA118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29">
+      <c r="A119" s="1">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>7127384</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" t="s">
+        <v>28</v>
+      </c>
+      <c r="E119" s="2">
+        <v>45354.125</v>
+      </c>
+      <c r="F119" t="s">
+        <v>35</v>
+      </c>
+      <c r="G119" t="s">
+        <v>38</v>
+      </c>
+      <c r="K119">
+        <v>3</v>
+      </c>
+      <c r="L119">
+        <v>3.6</v>
+      </c>
+      <c r="M119">
+        <v>2.2</v>
+      </c>
+      <c r="N119">
+        <v>3.3</v>
+      </c>
+      <c r="O119">
+        <v>3.8</v>
+      </c>
+      <c r="P119">
+        <v>2.05</v>
+      </c>
+      <c r="Q119">
+        <v>0.5</v>
+      </c>
+      <c r="R119">
+        <v>1.85</v>
+      </c>
+      <c r="S119">
+        <v>2.05</v>
+      </c>
+      <c r="T119">
+        <v>3</v>
+      </c>
+      <c r="U119">
+        <v>2</v>
+      </c>
+      <c r="V119">
+        <v>1.85</v>
+      </c>
+      <c r="W119">
+        <v>0</v>
+      </c>
+      <c r="X119">
+        <v>0</v>
+      </c>
+      <c r="Y119">
+        <v>0</v>
+      </c>
+      <c r="Z119">
+        <v>0</v>
+      </c>
+      <c r="AA119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29">
+      <c r="A120" s="1">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>7127385</v>
+      </c>
+      <c r="C120" t="s">
+        <v>28</v>
+      </c>
+      <c r="D120" t="s">
+        <v>28</v>
+      </c>
+      <c r="E120" s="2">
+        <v>45359.23958333334</v>
+      </c>
+      <c r="F120" t="s">
+        <v>33</v>
+      </c>
+      <c r="G120" t="s">
+        <v>40</v>
+      </c>
+      <c r="K120">
+        <v>1.615</v>
+      </c>
+      <c r="L120">
+        <v>4.5</v>
+      </c>
+      <c r="M120">
+        <v>4.5</v>
+      </c>
+      <c r="N120">
+        <v>1.65</v>
+      </c>
+      <c r="O120">
+        <v>4.5</v>
+      </c>
+      <c r="P120">
+        <v>4.333</v>
+      </c>
+      <c r="Q120">
+        <v>-0.75</v>
+      </c>
+      <c r="R120">
+        <v>1.84</v>
+      </c>
+      <c r="S120">
+        <v>2.06</v>
+      </c>
+      <c r="T120">
+        <v>3</v>
+      </c>
+      <c r="U120">
+        <v>1.85</v>
+      </c>
+      <c r="V120">
+        <v>2</v>
+      </c>
+      <c r="W120">
+        <v>0</v>
+      </c>
+      <c r="X120">
+        <v>0</v>
+      </c>
+      <c r="Y120">
+        <v>0</v>
+      </c>
+      <c r="Z120">
+        <v>0</v>
+      </c>
+      <c r="AA120">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 07-03-2024 às 23:43
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC120"/>
+  <dimension ref="A1:AC125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -10945,6 +10945,15 @@
       <c r="G118" t="s">
         <v>30</v>
       </c>
+      <c r="H118">
+        <v>3</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+      <c r="J118" t="s">
+        <v>42</v>
+      </c>
       <c r="K118">
         <v>2</v>
       </c>
@@ -10955,46 +10964,52 @@
         <v>3.5</v>
       </c>
       <c r="N118">
-        <v>1.909</v>
+        <v>1.85</v>
       </c>
       <c r="O118">
         <v>3.8</v>
       </c>
       <c r="P118">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="Q118">
         <v>-0.5</v>
       </c>
       <c r="R118">
-        <v>1.91</v>
+        <v>1.85</v>
       </c>
       <c r="S118">
-        <v>1.99</v>
+        <v>2</v>
       </c>
       <c r="T118">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U118">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="V118">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="W118">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="X118">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y118">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z118">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA118">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB118">
+        <v>0.825</v>
+      </c>
+      <c r="AC118">
+        <v>-1</v>
       </c>
     </row>
     <row r="119" spans="1:29">
@@ -11019,6 +11034,15 @@
       <c r="G119" t="s">
         <v>38</v>
       </c>
+      <c r="H119">
+        <v>3</v>
+      </c>
+      <c r="I119">
+        <v>2</v>
+      </c>
+      <c r="J119" t="s">
+        <v>42</v>
+      </c>
       <c r="K119">
         <v>3</v>
       </c>
@@ -11029,22 +11053,22 @@
         <v>2.2</v>
       </c>
       <c r="N119">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="O119">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P119">
-        <v>2.05</v>
+        <v>1.909</v>
       </c>
       <c r="Q119">
         <v>0.5</v>
       </c>
       <c r="R119">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S119">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="T119">
         <v>3</v>
@@ -11056,19 +11080,25 @@
         <v>1.85</v>
       </c>
       <c r="W119">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="X119">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y119">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z119">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="AA119">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB119">
+        <v>1</v>
+      </c>
+      <c r="AC119">
+        <v>-1</v>
       </c>
     </row>
     <row r="120" spans="1:29">
@@ -11103,45 +11133,415 @@
         <v>4.5</v>
       </c>
       <c r="N120">
-        <v>1.65</v>
+        <v>1.666</v>
       </c>
       <c r="O120">
-        <v>4.5</v>
+        <v>4.333</v>
       </c>
       <c r="P120">
-        <v>4.333</v>
+        <v>4</v>
       </c>
       <c r="Q120">
         <v>-0.75</v>
       </c>
       <c r="R120">
-        <v>1.84</v>
+        <v>1.9</v>
       </c>
       <c r="S120">
-        <v>2.06</v>
+        <v>2</v>
       </c>
       <c r="T120">
+        <v>3.25</v>
+      </c>
+      <c r="U120">
+        <v>2</v>
+      </c>
+      <c r="V120">
+        <v>1.85</v>
+      </c>
+      <c r="W120">
+        <v>0</v>
+      </c>
+      <c r="X120">
+        <v>0</v>
+      </c>
+      <c r="Y120">
+        <v>0</v>
+      </c>
+      <c r="Z120">
+        <v>0</v>
+      </c>
+      <c r="AA120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29">
+      <c r="A121" s="1">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>7126791</v>
+      </c>
+      <c r="C121" t="s">
+        <v>28</v>
+      </c>
+      <c r="D121" t="s">
+        <v>28</v>
+      </c>
+      <c r="E121" s="2">
+        <v>45360.20833333334</v>
+      </c>
+      <c r="F121" t="s">
+        <v>29</v>
+      </c>
+      <c r="G121" t="s">
+        <v>36</v>
+      </c>
+      <c r="K121">
+        <v>2</v>
+      </c>
+      <c r="L121">
+        <v>3.5</v>
+      </c>
+      <c r="M121">
+        <v>3.6</v>
+      </c>
+      <c r="N121">
+        <v>1.909</v>
+      </c>
+      <c r="O121">
+        <v>3.8</v>
+      </c>
+      <c r="P121">
+        <v>3.75</v>
+      </c>
+      <c r="Q121">
+        <v>-0.5</v>
+      </c>
+      <c r="R121">
+        <v>1.95</v>
+      </c>
+      <c r="S121">
+        <v>1.95</v>
+      </c>
+      <c r="T121">
+        <v>2.75</v>
+      </c>
+      <c r="U121">
+        <v>1.825</v>
+      </c>
+      <c r="V121">
+        <v>2.025</v>
+      </c>
+      <c r="W121">
+        <v>0</v>
+      </c>
+      <c r="X121">
+        <v>0</v>
+      </c>
+      <c r="Y121">
+        <v>0</v>
+      </c>
+      <c r="Z121">
+        <v>0</v>
+      </c>
+      <c r="AA121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29">
+      <c r="A122" s="1">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>7127386</v>
+      </c>
+      <c r="C122" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" t="s">
+        <v>28</v>
+      </c>
+      <c r="E122" s="2">
+        <v>45360.26041666666</v>
+      </c>
+      <c r="F122" t="s">
+        <v>30</v>
+      </c>
+      <c r="G122" t="s">
+        <v>38</v>
+      </c>
+      <c r="K122">
+        <v>2.4</v>
+      </c>
+      <c r="L122">
+        <v>3.4</v>
+      </c>
+      <c r="M122">
+        <v>2.8</v>
+      </c>
+      <c r="N122">
         <v>3</v>
       </c>
-      <c r="U120">
+      <c r="O122">
+        <v>3.5</v>
+      </c>
+      <c r="P122">
+        <v>2.25</v>
+      </c>
+      <c r="Q122">
+        <v>0.25</v>
+      </c>
+      <c r="R122">
+        <v>1.92</v>
+      </c>
+      <c r="S122">
+        <v>1.98</v>
+      </c>
+      <c r="T122">
+        <v>3</v>
+      </c>
+      <c r="U122">
         <v>1.85</v>
       </c>
-      <c r="V120">
-        <v>2</v>
-      </c>
-      <c r="W120">
-        <v>0</v>
-      </c>
-      <c r="X120">
-        <v>0</v>
-      </c>
-      <c r="Y120">
-        <v>0</v>
-      </c>
-      <c r="Z120">
-        <v>0</v>
-      </c>
-      <c r="AA120">
+      <c r="V122">
+        <v>2</v>
+      </c>
+      <c r="W122">
+        <v>0</v>
+      </c>
+      <c r="X122">
+        <v>0</v>
+      </c>
+      <c r="Y122">
+        <v>0</v>
+      </c>
+      <c r="Z122">
+        <v>0</v>
+      </c>
+      <c r="AA122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:29">
+      <c r="A123" s="1">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>7127387</v>
+      </c>
+      <c r="C123" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="2">
+        <v>45360.32291666666</v>
+      </c>
+      <c r="F123" t="s">
+        <v>34</v>
+      </c>
+      <c r="G123" t="s">
+        <v>39</v>
+      </c>
+      <c r="K123">
+        <v>1.909</v>
+      </c>
+      <c r="L123">
+        <v>3.75</v>
+      </c>
+      <c r="M123">
+        <v>3.6</v>
+      </c>
+      <c r="N123">
+        <v>2.15</v>
+      </c>
+      <c r="O123">
+        <v>3.6</v>
+      </c>
+      <c r="P123">
+        <v>3</v>
+      </c>
+      <c r="Q123">
+        <v>-0.25</v>
+      </c>
+      <c r="R123">
+        <v>1.93</v>
+      </c>
+      <c r="S123">
+        <v>1.97</v>
+      </c>
+      <c r="T123">
+        <v>3.25</v>
+      </c>
+      <c r="U123">
+        <v>1.975</v>
+      </c>
+      <c r="V123">
+        <v>1.875</v>
+      </c>
+      <c r="W123">
+        <v>0</v>
+      </c>
+      <c r="X123">
+        <v>0</v>
+      </c>
+      <c r="Y123">
+        <v>0</v>
+      </c>
+      <c r="Z123">
+        <v>0</v>
+      </c>
+      <c r="AA123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29">
+      <c r="A124" s="1">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>7127388</v>
+      </c>
+      <c r="C124" t="s">
+        <v>28</v>
+      </c>
+      <c r="D124" t="s">
+        <v>28</v>
+      </c>
+      <c r="E124" s="2">
+        <v>45361.125</v>
+      </c>
+      <c r="F124" t="s">
+        <v>32</v>
+      </c>
+      <c r="G124" t="s">
+        <v>35</v>
+      </c>
+      <c r="K124">
+        <v>1.5</v>
+      </c>
+      <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.55</v>
+      </c>
+      <c r="O124">
+        <v>5</v>
+      </c>
+      <c r="P124">
+        <v>4.5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.9</v>
+      </c>
+      <c r="S124">
+        <v>2</v>
+      </c>
+      <c r="T124">
+        <v>3.5</v>
+      </c>
+      <c r="U124">
+        <v>1.975</v>
+      </c>
+      <c r="V124">
+        <v>1.875</v>
+      </c>
+      <c r="W124">
+        <v>0</v>
+      </c>
+      <c r="X124">
+        <v>0</v>
+      </c>
+      <c r="Y124">
+        <v>0</v>
+      </c>
+      <c r="Z124">
+        <v>0</v>
+      </c>
+      <c r="AA124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29">
+      <c r="A125" s="1">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>7128012</v>
+      </c>
+      <c r="C125" t="s">
+        <v>28</v>
+      </c>
+      <c r="D125" t="s">
+        <v>28</v>
+      </c>
+      <c r="E125" s="2">
+        <v>45361.125</v>
+      </c>
+      <c r="F125" t="s">
+        <v>31</v>
+      </c>
+      <c r="G125" t="s">
+        <v>37</v>
+      </c>
+      <c r="K125">
+        <v>2.4</v>
+      </c>
+      <c r="L125">
+        <v>3.5</v>
+      </c>
+      <c r="M125">
+        <v>2.75</v>
+      </c>
+      <c r="N125">
+        <v>3.1</v>
+      </c>
+      <c r="O125">
+        <v>3.5</v>
+      </c>
+      <c r="P125">
+        <v>2.2</v>
+      </c>
+      <c r="Q125">
+        <v>0.25</v>
+      </c>
+      <c r="R125">
+        <v>1.95</v>
+      </c>
+      <c r="S125">
+        <v>1.95</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>1.975</v>
+      </c>
+      <c r="V125">
+        <v>1.875</v>
+      </c>
+      <c r="W125">
+        <v>0</v>
+      </c>
+      <c r="X125">
+        <v>0</v>
+      </c>
+      <c r="Y125">
+        <v>0</v>
+      </c>
+      <c r="Z125">
+        <v>0</v>
+      </c>
+      <c r="AA125">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 09-03-2024 às 13:07
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC125"/>
+  <dimension ref="A1:AC127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -11123,6 +11123,15 @@
       <c r="G120" t="s">
         <v>40</v>
       </c>
+      <c r="H120">
+        <v>1</v>
+      </c>
+      <c r="I120">
+        <v>3</v>
+      </c>
+      <c r="J120" t="s">
+        <v>41</v>
+      </c>
       <c r="K120">
         <v>1.615</v>
       </c>
@@ -11133,10 +11142,10 @@
         <v>4.5</v>
       </c>
       <c r="N120">
-        <v>1.666</v>
+        <v>1.727</v>
       </c>
       <c r="O120">
-        <v>4.333</v>
+        <v>4.5</v>
       </c>
       <c r="P120">
         <v>4</v>
@@ -11145,34 +11154,40 @@
         <v>-0.75</v>
       </c>
       <c r="R120">
+        <v>1.95</v>
+      </c>
+      <c r="S120">
         <v>1.9</v>
-      </c>
-      <c r="S120">
-        <v>2</v>
       </c>
       <c r="T120">
         <v>3.25</v>
       </c>
       <c r="U120">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V120">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W120">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X120">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y120">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z120">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA120">
-        <v>0</v>
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AB120">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AC120">
+        <v>-1</v>
       </c>
     </row>
     <row r="121" spans="1:29">
@@ -11197,6 +11212,15 @@
       <c r="G121" t="s">
         <v>36</v>
       </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <v>0</v>
+      </c>
+      <c r="J121" t="s">
+        <v>42</v>
+      </c>
       <c r="K121">
         <v>2</v>
       </c>
@@ -11207,46 +11231,52 @@
         <v>3.6</v>
       </c>
       <c r="N121">
-        <v>1.909</v>
+        <v>2</v>
       </c>
       <c r="O121">
-        <v>3.8</v>
+        <v>3.75</v>
       </c>
       <c r="P121">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="Q121">
         <v>-0.5</v>
       </c>
       <c r="R121">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S121">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T121">
         <v>2.75</v>
       </c>
       <c r="U121">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V121">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X121">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y121">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z121">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AA121">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB121">
+        <v>-1</v>
+      </c>
+      <c r="AC121">
+        <v>0.875</v>
       </c>
     </row>
     <row r="122" spans="1:29">
@@ -11271,6 +11301,15 @@
       <c r="G122" t="s">
         <v>38</v>
       </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="I122">
+        <v>2</v>
+      </c>
+      <c r="J122" t="s">
+        <v>41</v>
+      </c>
       <c r="K122">
         <v>2.4</v>
       </c>
@@ -11281,46 +11320,52 @@
         <v>2.8</v>
       </c>
       <c r="N122">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O122">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P122">
-        <v>2.25</v>
+        <v>1.85</v>
       </c>
       <c r="Q122">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R122">
-        <v>1.92</v>
+        <v>2.01</v>
       </c>
       <c r="S122">
-        <v>1.98</v>
+        <v>1.89</v>
       </c>
       <c r="T122">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U122">
+        <v>2</v>
+      </c>
+      <c r="V122">
         <v>1.85</v>
       </c>
-      <c r="V122">
-        <v>2</v>
-      </c>
       <c r="W122">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X122">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y122">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z122">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA122">
-        <v>0</v>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="AB122">
+        <v>-0.5</v>
+      </c>
+      <c r="AC122">
+        <v>0.425</v>
       </c>
     </row>
     <row r="123" spans="1:29">
@@ -11328,7 +11373,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>7127387</v>
+        <v>7128012</v>
       </c>
       <c r="C123" t="s">
         <v>28</v>
@@ -11337,49 +11382,49 @@
         <v>28</v>
       </c>
       <c r="E123" s="2">
-        <v>45360.32291666666</v>
+        <v>45361.125</v>
       </c>
       <c r="F123" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G123" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K123">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L123">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="M123">
-        <v>3.6</v>
+        <v>2.75</v>
       </c>
       <c r="N123">
-        <v>2.15</v>
+        <v>3.1</v>
       </c>
       <c r="O123">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P123">
+        <v>2.25</v>
+      </c>
+      <c r="Q123">
+        <v>0.25</v>
+      </c>
+      <c r="R123">
+        <v>1.97</v>
+      </c>
+      <c r="S123">
+        <v>1.93</v>
+      </c>
+      <c r="T123">
         <v>3</v>
       </c>
-      <c r="Q123">
-        <v>-0.25</v>
-      </c>
-      <c r="R123">
-        <v>1.93</v>
-      </c>
-      <c r="S123">
-        <v>1.97</v>
-      </c>
-      <c r="T123">
-        <v>3.25</v>
-      </c>
       <c r="U123">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="V123">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="W123">
         <v>0</v>
@@ -11435,16 +11480,16 @@
         <v>5</v>
       </c>
       <c r="P124">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="Q124">
         <v>-1</v>
       </c>
       <c r="R124">
-        <v>1.9</v>
+        <v>1.92</v>
       </c>
       <c r="S124">
-        <v>2</v>
+        <v>1.98</v>
       </c>
       <c r="T124">
         <v>3.5</v>
@@ -11476,7 +11521,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7662592</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11485,49 +11530,49 @@
         <v>28</v>
       </c>
       <c r="E125" s="2">
-        <v>45361.125</v>
+        <v>45363.20833333334</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>2.1</v>
       </c>
       <c r="L125">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M125">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="N125">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="O125">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="P125">
-        <v>2.2</v>
+        <v>3.25</v>
       </c>
       <c r="Q125">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R125">
-        <v>1.95</v>
+        <v>1.84</v>
       </c>
       <c r="S125">
-        <v>1.95</v>
+        <v>2.06</v>
       </c>
       <c r="T125">
         <v>3</v>
       </c>
       <c r="U125">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V125">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W125">
         <v>0</v>
@@ -11542,6 +11587,154 @@
         <v>0</v>
       </c>
       <c r="AA125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29">
+      <c r="A126" s="1">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>7127392</v>
+      </c>
+      <c r="C126" t="s">
+        <v>28</v>
+      </c>
+      <c r="D126" t="s">
+        <v>28</v>
+      </c>
+      <c r="E126" s="2">
+        <v>45365.20833333334</v>
+      </c>
+      <c r="F126" t="s">
+        <v>40</v>
+      </c>
+      <c r="G126" t="s">
+        <v>38</v>
+      </c>
+      <c r="K126">
+        <v>4.5</v>
+      </c>
+      <c r="L126">
+        <v>3.5</v>
+      </c>
+      <c r="M126">
+        <v>1.8</v>
+      </c>
+      <c r="N126">
+        <v>4.2</v>
+      </c>
+      <c r="O126">
+        <v>3.5</v>
+      </c>
+      <c r="P126">
+        <v>1.909</v>
+      </c>
+      <c r="Q126">
+        <v>0.5</v>
+      </c>
+      <c r="R126">
+        <v>1.95</v>
+      </c>
+      <c r="S126">
+        <v>1.95</v>
+      </c>
+      <c r="T126">
+        <v>3</v>
+      </c>
+      <c r="U126">
+        <v>2.025</v>
+      </c>
+      <c r="V126">
+        <v>1.825</v>
+      </c>
+      <c r="W126">
+        <v>0</v>
+      </c>
+      <c r="X126">
+        <v>0</v>
+      </c>
+      <c r="Y126">
+        <v>0</v>
+      </c>
+      <c r="Z126">
+        <v>0</v>
+      </c>
+      <c r="AA126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:29">
+      <c r="A127" s="1">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>7127389</v>
+      </c>
+      <c r="C127" t="s">
+        <v>28</v>
+      </c>
+      <c r="D127" t="s">
+        <v>28</v>
+      </c>
+      <c r="E127" s="2">
+        <v>45366.23958333334</v>
+      </c>
+      <c r="F127" t="s">
+        <v>39</v>
+      </c>
+      <c r="G127" t="s">
+        <v>30</v>
+      </c>
+      <c r="K127">
+        <v>2.25</v>
+      </c>
+      <c r="L127">
+        <v>3.5</v>
+      </c>
+      <c r="M127">
+        <v>3</v>
+      </c>
+      <c r="N127">
+        <v>2.45</v>
+      </c>
+      <c r="O127">
+        <v>3.5</v>
+      </c>
+      <c r="P127">
+        <v>2.75</v>
+      </c>
+      <c r="Q127">
+        <v>0</v>
+      </c>
+      <c r="R127">
+        <v>1.83</v>
+      </c>
+      <c r="S127">
+        <v>2.07</v>
+      </c>
+      <c r="T127">
+        <v>3.25</v>
+      </c>
+      <c r="U127">
+        <v>1.85</v>
+      </c>
+      <c r="V127">
+        <v>2</v>
+      </c>
+      <c r="W127">
+        <v>0</v>
+      </c>
+      <c r="X127">
+        <v>0</v>
+      </c>
+      <c r="Y127">
+        <v>0</v>
+      </c>
+      <c r="Z127">
+        <v>0</v>
+      </c>
+      <c r="AA127">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 11-03-2024 às 22:32
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC127"/>
+  <dimension ref="A1:AC131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11373,7 +11373,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>7128012</v>
+        <v>7127387</v>
       </c>
       <c r="C123" t="s">
         <v>28</v>
@@ -11382,64 +11382,79 @@
         <v>28</v>
       </c>
       <c r="E123" s="2">
-        <v>45361.125</v>
+        <v>45360.32291666666</v>
       </c>
       <c r="F123" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G123" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="H123">
+        <v>2</v>
+      </c>
+      <c r="I123">
+        <v>2</v>
+      </c>
+      <c r="J123" t="s">
+        <v>43</v>
       </c>
       <c r="K123">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L123">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M123">
-        <v>2.75</v>
+        <v>3.6</v>
       </c>
       <c r="N123">
-        <v>3.1</v>
+        <v>2.2</v>
       </c>
       <c r="O123">
         <v>3.5</v>
       </c>
       <c r="P123">
-        <v>2.25</v>
+        <v>3.2</v>
       </c>
       <c r="Q123">
-        <v>0.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R123">
-        <v>1.97</v>
+        <v>1.98</v>
       </c>
       <c r="S123">
-        <v>1.93</v>
+        <v>1.92</v>
       </c>
       <c r="T123">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U123">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V123">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="W123">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X123">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y123">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z123">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AA123">
-        <v>0</v>
+        <v>0.46</v>
+      </c>
+      <c r="AB123">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AC123">
+        <v>-1</v>
       </c>
     </row>
     <row r="124" spans="1:29">
@@ -11447,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11459,61 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>3</v>
+      </c>
+      <c r="J124" t="s">
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.55</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>4.75</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
-        <v>1.92</v>
+        <v>2.025</v>
       </c>
       <c r="S124">
-        <v>1.98</v>
+        <v>1.825</v>
       </c>
       <c r="T124">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U124">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="V124">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="W124">
+        <v>-1</v>
+      </c>
+      <c r="X124">
+        <v>-1</v>
+      </c>
+      <c r="Y124">
+        <v>1.05</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
+        <v>0.825</v>
+      </c>
+      <c r="AB124">
         <v>0</v>
       </c>
-      <c r="X124">
-        <v>0</v>
-      </c>
-      <c r="Y124">
-        <v>0</v>
-      </c>
-      <c r="Z124">
-        <v>0</v>
-      </c>
-      <c r="AA124">
-        <v>0</v>
+      <c r="AC124">
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11521,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7662592</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11530,64 +11560,79 @@
         <v>28</v>
       </c>
       <c r="E125" s="2">
-        <v>45363.20833333334</v>
+        <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <v>1</v>
+      </c>
+      <c r="J125" t="s">
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M125">
-        <v>3.25</v>
+        <v>5</v>
       </c>
       <c r="N125">
-        <v>2.1</v>
+        <v>1.533</v>
       </c>
       <c r="O125">
-        <v>3.6</v>
+        <v>5.25</v>
       </c>
       <c r="P125">
-        <v>3.25</v>
+        <v>5</v>
       </c>
       <c r="Q125">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="R125">
-        <v>1.84</v>
+        <v>1.8</v>
       </c>
       <c r="S125">
-        <v>2.06</v>
+        <v>2.05</v>
       </c>
       <c r="T125">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U125">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X125">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA125">
-        <v>0</v>
+        <v>1.05</v>
+      </c>
+      <c r="AB125">
+        <v>-1</v>
+      </c>
+      <c r="AC125">
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -11595,7 +11640,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>7127392</v>
+        <v>7662592</v>
       </c>
       <c r="C126" t="s">
         <v>28</v>
@@ -11604,49 +11649,49 @@
         <v>28</v>
       </c>
       <c r="E126" s="2">
-        <v>45365.20833333334</v>
+        <v>45363.20833333334</v>
       </c>
       <c r="F126" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G126" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="K126">
-        <v>4.5</v>
+        <v>2.1</v>
       </c>
       <c r="L126">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M126">
-        <v>1.8</v>
+        <v>3.25</v>
       </c>
       <c r="N126">
-        <v>4.2</v>
+        <v>1.85</v>
       </c>
       <c r="O126">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P126">
-        <v>1.909</v>
+        <v>3.8</v>
       </c>
       <c r="Q126">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R126">
-        <v>1.95</v>
+        <v>1.88</v>
       </c>
       <c r="S126">
-        <v>1.95</v>
+        <v>2.02</v>
       </c>
       <c r="T126">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U126">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V126">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W126">
         <v>0</v>
@@ -11669,7 +11714,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>7127389</v>
+        <v>7127392</v>
       </c>
       <c r="C127" t="s">
         <v>28</v>
@@ -11678,49 +11723,49 @@
         <v>28</v>
       </c>
       <c r="E127" s="2">
-        <v>45366.23958333334</v>
+        <v>45365.20833333334</v>
       </c>
       <c r="F127" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G127" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="K127">
-        <v>2.25</v>
+        <v>4.5</v>
       </c>
       <c r="L127">
         <v>3.5</v>
       </c>
       <c r="M127">
+        <v>1.8</v>
+      </c>
+      <c r="N127">
+        <v>5</v>
+      </c>
+      <c r="O127">
+        <v>4</v>
+      </c>
+      <c r="P127">
+        <v>1.666</v>
+      </c>
+      <c r="Q127">
+        <v>0.75</v>
+      </c>
+      <c r="R127">
+        <v>2.03</v>
+      </c>
+      <c r="S127">
+        <v>1.87</v>
+      </c>
+      <c r="T127">
         <v>3</v>
       </c>
-      <c r="N127">
-        <v>2.45</v>
-      </c>
-      <c r="O127">
-        <v>3.5</v>
-      </c>
-      <c r="P127">
-        <v>2.75</v>
-      </c>
-      <c r="Q127">
-        <v>0</v>
-      </c>
-      <c r="R127">
-        <v>1.83</v>
-      </c>
-      <c r="S127">
-        <v>2.07</v>
-      </c>
-      <c r="T127">
-        <v>3.25</v>
-      </c>
       <c r="U127">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="V127">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W127">
         <v>0</v>
@@ -11735,6 +11780,302 @@
         <v>0</v>
       </c>
       <c r="AA127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:29">
+      <c r="A128" s="1">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>7127389</v>
+      </c>
+      <c r="C128" t="s">
+        <v>28</v>
+      </c>
+      <c r="D128" t="s">
+        <v>28</v>
+      </c>
+      <c r="E128" s="2">
+        <v>45366.23958333334</v>
+      </c>
+      <c r="F128" t="s">
+        <v>39</v>
+      </c>
+      <c r="G128" t="s">
+        <v>30</v>
+      </c>
+      <c r="K128">
+        <v>2.25</v>
+      </c>
+      <c r="L128">
+        <v>3.5</v>
+      </c>
+      <c r="M128">
+        <v>3</v>
+      </c>
+      <c r="N128">
+        <v>2.3</v>
+      </c>
+      <c r="O128">
+        <v>3.6</v>
+      </c>
+      <c r="P128">
+        <v>2.75</v>
+      </c>
+      <c r="Q128">
+        <v>-0.25</v>
+      </c>
+      <c r="R128">
+        <v>2.08</v>
+      </c>
+      <c r="S128">
+        <v>1.82</v>
+      </c>
+      <c r="T128">
+        <v>3.5</v>
+      </c>
+      <c r="U128">
+        <v>1.975</v>
+      </c>
+      <c r="V128">
+        <v>1.875</v>
+      </c>
+      <c r="W128">
+        <v>0</v>
+      </c>
+      <c r="X128">
+        <v>0</v>
+      </c>
+      <c r="Y128">
+        <v>0</v>
+      </c>
+      <c r="Z128">
+        <v>0</v>
+      </c>
+      <c r="AA128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:27">
+      <c r="A129" s="1">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>7127390</v>
+      </c>
+      <c r="C129" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" t="s">
+        <v>28</v>
+      </c>
+      <c r="E129" s="2">
+        <v>45367.0625</v>
+      </c>
+      <c r="F129" t="s">
+        <v>36</v>
+      </c>
+      <c r="G129" t="s">
+        <v>32</v>
+      </c>
+      <c r="K129">
+        <v>2.9</v>
+      </c>
+      <c r="L129">
+        <v>3.6</v>
+      </c>
+      <c r="M129">
+        <v>2.25</v>
+      </c>
+      <c r="N129">
+        <v>3.2</v>
+      </c>
+      <c r="O129">
+        <v>3.6</v>
+      </c>
+      <c r="P129">
+        <v>2.05</v>
+      </c>
+      <c r="Q129">
+        <v>0.25</v>
+      </c>
+      <c r="R129">
+        <v>2.02</v>
+      </c>
+      <c r="S129">
+        <v>1.88</v>
+      </c>
+      <c r="T129">
+        <v>3</v>
+      </c>
+      <c r="U129">
+        <v>2</v>
+      </c>
+      <c r="V129">
+        <v>1.85</v>
+      </c>
+      <c r="W129">
+        <v>0</v>
+      </c>
+      <c r="X129">
+        <v>0</v>
+      </c>
+      <c r="Y129">
+        <v>0</v>
+      </c>
+      <c r="Z129">
+        <v>0</v>
+      </c>
+      <c r="AA129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:27">
+      <c r="A130" s="1">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>7940069</v>
+      </c>
+      <c r="C130" t="s">
+        <v>28</v>
+      </c>
+      <c r="D130" t="s">
+        <v>28</v>
+      </c>
+      <c r="E130" s="2">
+        <v>45367.08333333334</v>
+      </c>
+      <c r="F130" t="s">
+        <v>35</v>
+      </c>
+      <c r="G130" t="s">
+        <v>31</v>
+      </c>
+      <c r="K130">
+        <v>2</v>
+      </c>
+      <c r="L130">
+        <v>3.8</v>
+      </c>
+      <c r="M130">
+        <v>3.25</v>
+      </c>
+      <c r="N130">
+        <v>1.85</v>
+      </c>
+      <c r="O130">
+        <v>4</v>
+      </c>
+      <c r="P130">
+        <v>3.5</v>
+      </c>
+      <c r="Q130">
+        <v>-0.5</v>
+      </c>
+      <c r="R130">
+        <v>1.89</v>
+      </c>
+      <c r="S130">
+        <v>2.01</v>
+      </c>
+      <c r="T130">
+        <v>3.5</v>
+      </c>
+      <c r="U130">
+        <v>2.025</v>
+      </c>
+      <c r="V130">
+        <v>1.825</v>
+      </c>
+      <c r="W130">
+        <v>0</v>
+      </c>
+      <c r="X130">
+        <v>0</v>
+      </c>
+      <c r="Y130">
+        <v>0</v>
+      </c>
+      <c r="Z130">
+        <v>0</v>
+      </c>
+      <c r="AA130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:27">
+      <c r="A131" s="1">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>7940070</v>
+      </c>
+      <c r="C131" t="s">
+        <v>28</v>
+      </c>
+      <c r="D131" t="s">
+        <v>28</v>
+      </c>
+      <c r="E131" s="2">
+        <v>45367.23958333334</v>
+      </c>
+      <c r="F131" t="s">
+        <v>34</v>
+      </c>
+      <c r="G131" t="s">
+        <v>33</v>
+      </c>
+      <c r="K131">
+        <v>2.75</v>
+      </c>
+      <c r="L131">
+        <v>3.5</v>
+      </c>
+      <c r="M131">
+        <v>2.375</v>
+      </c>
+      <c r="N131">
+        <v>2.8</v>
+      </c>
+      <c r="O131">
+        <v>3.5</v>
+      </c>
+      <c r="P131">
+        <v>2.3</v>
+      </c>
+      <c r="Q131">
+        <v>0.25</v>
+      </c>
+      <c r="R131">
+        <v>1.81</v>
+      </c>
+      <c r="S131">
+        <v>2.09</v>
+      </c>
+      <c r="T131">
+        <v>3</v>
+      </c>
+      <c r="U131">
+        <v>1.95</v>
+      </c>
+      <c r="V131">
+        <v>1.9</v>
+      </c>
+      <c r="W131">
+        <v>0</v>
+      </c>
+      <c r="X131">
+        <v>0</v>
+      </c>
+      <c r="Y131">
+        <v>0</v>
+      </c>
+      <c r="Z131">
+        <v>0</v>
+      </c>
+      <c r="AA131">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 17-03-2024 às 10:24
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -11657,6 +11657,15 @@
       <c r="G126" t="s">
         <v>33</v>
       </c>
+      <c r="H126">
+        <v>7</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+      <c r="J126" t="s">
+        <v>42</v>
+      </c>
       <c r="K126">
         <v>2.1</v>
       </c>
@@ -11670,7 +11679,7 @@
         <v>1.85</v>
       </c>
       <c r="O126">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P126">
         <v>3.8</v>
@@ -11679,34 +11688,40 @@
         <v>-0.5</v>
       </c>
       <c r="R126">
-        <v>1.88</v>
+        <v>1.9</v>
       </c>
       <c r="S126">
-        <v>2.02</v>
+        <v>2</v>
       </c>
       <c r="T126">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U126">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V126">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W126">
-        <v>0</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="X126">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y126">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z126">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA126">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB126">
+        <v>0.925</v>
+      </c>
+      <c r="AC126">
+        <v>-1</v>
       </c>
     </row>
     <row r="127" spans="1:29">
@@ -11731,6 +11746,15 @@
       <c r="G127" t="s">
         <v>38</v>
       </c>
+      <c r="H127">
+        <v>2</v>
+      </c>
+      <c r="I127">
+        <v>2</v>
+      </c>
+      <c r="J127" t="s">
+        <v>43</v>
+      </c>
       <c r="K127">
         <v>4.5</v>
       </c>
@@ -11741,22 +11765,22 @@
         <v>1.8</v>
       </c>
       <c r="N127">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="O127">
         <v>4</v>
       </c>
       <c r="P127">
-        <v>1.666</v>
+        <v>1.909</v>
       </c>
       <c r="Q127">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="R127">
-        <v>2.03</v>
+        <v>1.875</v>
       </c>
       <c r="S127">
-        <v>1.87</v>
+        <v>1.975</v>
       </c>
       <c r="T127">
         <v>3</v>
@@ -11768,19 +11792,25 @@
         <v>1.9</v>
       </c>
       <c r="W127">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X127">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y127">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z127">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="AA127">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB127">
+        <v>0.95</v>
+      </c>
+      <c r="AC127">
+        <v>-1</v>
       </c>
     </row>
     <row r="128" spans="1:29">
@@ -11805,6 +11835,15 @@
       <c r="G128" t="s">
         <v>30</v>
       </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128" t="s">
+        <v>41</v>
+      </c>
       <c r="K128">
         <v>2.25</v>
       </c>
@@ -11815,10 +11854,10 @@
         <v>3</v>
       </c>
       <c r="N128">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="O128">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="P128">
         <v>2.75</v>
@@ -11827,37 +11866,43 @@
         <v>-0.25</v>
       </c>
       <c r="R128">
-        <v>2.08</v>
+        <v>2</v>
       </c>
       <c r="S128">
-        <v>1.82</v>
+        <v>1.85</v>
       </c>
       <c r="T128">
         <v>3.5</v>
       </c>
       <c r="U128">
+        <v>1.875</v>
+      </c>
+      <c r="V128">
         <v>1.975</v>
       </c>
-      <c r="V128">
-        <v>1.875</v>
-      </c>
       <c r="W128">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X128">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y128">
-        <v>0</v>
+        <v>1.75</v>
       </c>
       <c r="Z128">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:27">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB128">
+        <v>-1</v>
+      </c>
+      <c r="AC128">
+        <v>0.9750000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:29">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -11879,6 +11924,15 @@
       <c r="G129" t="s">
         <v>32</v>
       </c>
+      <c r="H129">
+        <v>2</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+      <c r="J129" t="s">
+        <v>42</v>
+      </c>
       <c r="K129">
         <v>2.9</v>
       </c>
@@ -11889,49 +11943,55 @@
         <v>2.25</v>
       </c>
       <c r="N129">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="O129">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="P129">
-        <v>2.05</v>
+        <v>2.2</v>
       </c>
       <c r="Q129">
         <v>0.25</v>
       </c>
       <c r="R129">
-        <v>2.02</v>
+        <v>1.95</v>
       </c>
       <c r="S129">
-        <v>1.88</v>
+        <v>1.95</v>
       </c>
       <c r="T129">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U129">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V129">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W129">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="X129">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y129">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z129">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:27">
+        <v>-1</v>
+      </c>
+      <c r="AB129">
+        <v>0.4625</v>
+      </c>
+      <c r="AC129">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:29">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -11953,6 +12013,15 @@
       <c r="G130" t="s">
         <v>31</v>
       </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>2</v>
+      </c>
+      <c r="J130" t="s">
+        <v>41</v>
+      </c>
       <c r="K130">
         <v>2</v>
       </c>
@@ -11963,49 +12032,55 @@
         <v>3.25</v>
       </c>
       <c r="N130">
-        <v>1.85</v>
+        <v>1.833</v>
       </c>
       <c r="O130">
-        <v>4</v>
+        <v>4.333</v>
       </c>
       <c r="P130">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="Q130">
         <v>-0.5</v>
       </c>
       <c r="R130">
-        <v>1.89</v>
+        <v>1.825</v>
       </c>
       <c r="S130">
-        <v>2.01</v>
+        <v>2.025</v>
       </c>
       <c r="T130">
         <v>3.5</v>
       </c>
       <c r="U130">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V130">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W130">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X130">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y130">
-        <v>0</v>
+        <v>2.75</v>
       </c>
       <c r="Z130">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:27">
+        <v>1.025</v>
+      </c>
+      <c r="AB130">
+        <v>-1</v>
+      </c>
+      <c r="AC130">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="131" spans="1:29">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -12027,6 +12102,15 @@
       <c r="G131" t="s">
         <v>33</v>
       </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>2</v>
+      </c>
+      <c r="J131" t="s">
+        <v>41</v>
+      </c>
       <c r="K131">
         <v>2.75</v>
       </c>
@@ -12037,46 +12121,52 @@
         <v>2.375</v>
       </c>
       <c r="N131">
-        <v>2.8</v>
+        <v>2.55</v>
       </c>
       <c r="O131">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="P131">
-        <v>2.3</v>
+        <v>2.45</v>
       </c>
       <c r="Q131">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R131">
-        <v>1.81</v>
+        <v>2</v>
       </c>
       <c r="S131">
-        <v>2.09</v>
+        <v>1.85</v>
       </c>
       <c r="T131">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U131">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="V131">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W131">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X131">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y131">
-        <v>0</v>
+        <v>1.45</v>
       </c>
       <c r="Z131">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA131">
-        <v>0</v>
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB131">
+        <v>-0.5</v>
+      </c>
+      <c r="AC131">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 27-03-2024 às 20:23
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC131"/>
+  <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -12167,6 +12167,450 @@
       </c>
       <c r="AC131">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:29">
+      <c r="A132" s="1">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>7127395</v>
+      </c>
+      <c r="C132" t="s">
+        <v>28</v>
+      </c>
+      <c r="D132" t="s">
+        <v>28</v>
+      </c>
+      <c r="E132" s="2">
+        <v>45380.23958333334</v>
+      </c>
+      <c r="F132" t="s">
+        <v>30</v>
+      </c>
+      <c r="G132" t="s">
+        <v>40</v>
+      </c>
+      <c r="K132">
+        <v>1.666</v>
+      </c>
+      <c r="L132">
+        <v>4.2</v>
+      </c>
+      <c r="M132">
+        <v>4.333</v>
+      </c>
+      <c r="N132">
+        <v>1.85</v>
+      </c>
+      <c r="O132">
+        <v>4.5</v>
+      </c>
+      <c r="P132">
+        <v>3.4</v>
+      </c>
+      <c r="Q132">
+        <v>-0.5</v>
+      </c>
+      <c r="R132">
+        <v>1.89</v>
+      </c>
+      <c r="S132">
+        <v>2.01</v>
+      </c>
+      <c r="T132">
+        <v>3.5</v>
+      </c>
+      <c r="U132">
+        <v>2</v>
+      </c>
+      <c r="V132">
+        <v>1.85</v>
+      </c>
+      <c r="W132">
+        <v>0</v>
+      </c>
+      <c r="X132">
+        <v>0</v>
+      </c>
+      <c r="Y132">
+        <v>0</v>
+      </c>
+      <c r="Z132">
+        <v>0</v>
+      </c>
+      <c r="AA132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:29">
+      <c r="A133" s="1">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>7126793</v>
+      </c>
+      <c r="C133" t="s">
+        <v>28</v>
+      </c>
+      <c r="D133" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="2">
+        <v>45381.14583333334</v>
+      </c>
+      <c r="F133" t="s">
+        <v>29</v>
+      </c>
+      <c r="G133" t="s">
+        <v>39</v>
+      </c>
+      <c r="K133">
+        <v>1.571</v>
+      </c>
+      <c r="L133">
+        <v>4.333</v>
+      </c>
+      <c r="M133">
+        <v>5</v>
+      </c>
+      <c r="N133">
+        <v>1.533</v>
+      </c>
+      <c r="O133">
+        <v>4.75</v>
+      </c>
+      <c r="P133">
+        <v>5.25</v>
+      </c>
+      <c r="Q133">
+        <v>-1</v>
+      </c>
+      <c r="R133">
+        <v>1.9</v>
+      </c>
+      <c r="S133">
+        <v>2</v>
+      </c>
+      <c r="T133">
+        <v>3.25</v>
+      </c>
+      <c r="U133">
+        <v>1.875</v>
+      </c>
+      <c r="V133">
+        <v>1.975</v>
+      </c>
+      <c r="W133">
+        <v>0</v>
+      </c>
+      <c r="X133">
+        <v>0</v>
+      </c>
+      <c r="Y133">
+        <v>0</v>
+      </c>
+      <c r="Z133">
+        <v>0</v>
+      </c>
+      <c r="AA133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:29">
+      <c r="A134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>7127396</v>
+      </c>
+      <c r="C134" t="s">
+        <v>28</v>
+      </c>
+      <c r="D134" t="s">
+        <v>28</v>
+      </c>
+      <c r="E134" s="2">
+        <v>45381.23958333334</v>
+      </c>
+      <c r="F134" t="s">
+        <v>32</v>
+      </c>
+      <c r="G134" t="s">
+        <v>37</v>
+      </c>
+      <c r="K134">
+        <v>2.15</v>
+      </c>
+      <c r="L134">
+        <v>3.6</v>
+      </c>
+      <c r="M134">
+        <v>3.1</v>
+      </c>
+      <c r="N134">
+        <v>2.15</v>
+      </c>
+      <c r="O134">
+        <v>3.75</v>
+      </c>
+      <c r="P134">
+        <v>3.1</v>
+      </c>
+      <c r="Q134">
+        <v>-0.25</v>
+      </c>
+      <c r="R134">
+        <v>1.93</v>
+      </c>
+      <c r="S134">
+        <v>1.97</v>
+      </c>
+      <c r="T134">
+        <v>2.75</v>
+      </c>
+      <c r="U134">
+        <v>1.8</v>
+      </c>
+      <c r="V134">
+        <v>2.05</v>
+      </c>
+      <c r="W134">
+        <v>0</v>
+      </c>
+      <c r="X134">
+        <v>0</v>
+      </c>
+      <c r="Y134">
+        <v>0</v>
+      </c>
+      <c r="Z134">
+        <v>0</v>
+      </c>
+      <c r="AA134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:29">
+      <c r="A135" s="1">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>7127394</v>
+      </c>
+      <c r="C135" t="s">
+        <v>28</v>
+      </c>
+      <c r="D135" t="s">
+        <v>28</v>
+      </c>
+      <c r="E135" s="2">
+        <v>45381.875</v>
+      </c>
+      <c r="F135" t="s">
+        <v>36</v>
+      </c>
+      <c r="G135" t="s">
+        <v>35</v>
+      </c>
+      <c r="K135">
+        <v>1.8</v>
+      </c>
+      <c r="L135">
+        <v>3.8</v>
+      </c>
+      <c r="M135">
+        <v>4</v>
+      </c>
+      <c r="N135">
+        <v>2</v>
+      </c>
+      <c r="O135">
+        <v>3.6</v>
+      </c>
+      <c r="P135">
+        <v>3.6</v>
+      </c>
+      <c r="Q135">
+        <v>-0.5</v>
+      </c>
+      <c r="R135">
+        <v>2.06</v>
+      </c>
+      <c r="S135">
+        <v>1.84</v>
+      </c>
+      <c r="T135">
+        <v>3</v>
+      </c>
+      <c r="U135">
+        <v>1.925</v>
+      </c>
+      <c r="V135">
+        <v>1.925</v>
+      </c>
+      <c r="W135">
+        <v>0</v>
+      </c>
+      <c r="X135">
+        <v>0</v>
+      </c>
+      <c r="Y135">
+        <v>0</v>
+      </c>
+      <c r="Z135">
+        <v>0</v>
+      </c>
+      <c r="AA135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:29">
+      <c r="A136" s="1">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>7127397</v>
+      </c>
+      <c r="C136" t="s">
+        <v>28</v>
+      </c>
+      <c r="D136" t="s">
+        <v>28</v>
+      </c>
+      <c r="E136" s="2">
+        <v>45382.04166666666</v>
+      </c>
+      <c r="F136" t="s">
+        <v>38</v>
+      </c>
+      <c r="G136" t="s">
+        <v>34</v>
+      </c>
+      <c r="K136">
+        <v>1.4</v>
+      </c>
+      <c r="L136">
+        <v>5</v>
+      </c>
+      <c r="M136">
+        <v>6.5</v>
+      </c>
+      <c r="N136">
+        <v>1.4</v>
+      </c>
+      <c r="O136">
+        <v>5.5</v>
+      </c>
+      <c r="P136">
+        <v>6.5</v>
+      </c>
+      <c r="Q136">
+        <v>-1.25</v>
+      </c>
+      <c r="R136">
+        <v>1.91</v>
+      </c>
+      <c r="S136">
+        <v>1.99</v>
+      </c>
+      <c r="T136">
+        <v>3.25</v>
+      </c>
+      <c r="U136">
+        <v>1.925</v>
+      </c>
+      <c r="V136">
+        <v>1.925</v>
+      </c>
+      <c r="W136">
+        <v>0</v>
+      </c>
+      <c r="X136">
+        <v>0</v>
+      </c>
+      <c r="Y136">
+        <v>0</v>
+      </c>
+      <c r="Z136">
+        <v>0</v>
+      </c>
+      <c r="AA136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>7127398</v>
+      </c>
+      <c r="C137" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137" s="2">
+        <v>45383.04166666666</v>
+      </c>
+      <c r="F137" t="s">
+        <v>31</v>
+      </c>
+      <c r="G137" t="s">
+        <v>33</v>
+      </c>
+      <c r="K137">
+        <v>2.5</v>
+      </c>
+      <c r="L137">
+        <v>3.5</v>
+      </c>
+      <c r="M137">
+        <v>2.625</v>
+      </c>
+      <c r="N137">
+        <v>2.625</v>
+      </c>
+      <c r="O137">
+        <v>3.75</v>
+      </c>
+      <c r="P137">
+        <v>2.45</v>
+      </c>
+      <c r="Q137">
+        <v>0</v>
+      </c>
+      <c r="R137">
+        <v>2.03</v>
+      </c>
+      <c r="S137">
+        <v>1.87</v>
+      </c>
+      <c r="T137">
+        <v>3.25</v>
+      </c>
+      <c r="U137">
+        <v>1.95</v>
+      </c>
+      <c r="V137">
+        <v>1.9</v>
+      </c>
+      <c r="W137">
+        <v>0</v>
+      </c>
+      <c r="X137">
+        <v>0</v>
+      </c>
+      <c r="Y137">
+        <v>0</v>
+      </c>
+      <c r="Z137">
+        <v>0</v>
+      </c>
+      <c r="AA137">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 29-03-2024 às 13:24
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -12191,6 +12191,15 @@
       <c r="G132" t="s">
         <v>40</v>
       </c>
+      <c r="H132">
+        <v>4</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="J132" t="s">
+        <v>42</v>
+      </c>
       <c r="K132">
         <v>1.666</v>
       </c>
@@ -12201,46 +12210,52 @@
         <v>4.333</v>
       </c>
       <c r="N132">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="O132">
         <v>4.5</v>
       </c>
       <c r="P132">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="Q132">
         <v>-0.5</v>
       </c>
       <c r="R132">
-        <v>1.89</v>
+        <v>1.975</v>
       </c>
       <c r="S132">
-        <v>2.01</v>
+        <v>1.875</v>
       </c>
       <c r="T132">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="U132">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V132">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W132">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="X132">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y132">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z132">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA132">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB132">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AC132">
+        <v>-1</v>
       </c>
     </row>
     <row r="133" spans="1:29">
@@ -12287,10 +12302,10 @@
         <v>-1</v>
       </c>
       <c r="R133">
-        <v>1.9</v>
+        <v>1.89</v>
       </c>
       <c r="S133">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="T133">
         <v>3.25</v>
@@ -12361,19 +12376,19 @@
         <v>-0.25</v>
       </c>
       <c r="R134">
-        <v>1.93</v>
+        <v>1.95</v>
       </c>
       <c r="S134">
-        <v>1.97</v>
+        <v>1.95</v>
       </c>
       <c r="T134">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U134">
+        <v>2.05</v>
+      </c>
+      <c r="V134">
         <v>1.8</v>
-      </c>
-      <c r="V134">
-        <v>2.05</v>
       </c>
       <c r="W134">
         <v>0</v>
@@ -12423,31 +12438,31 @@
         <v>4</v>
       </c>
       <c r="N135">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="O135">
         <v>3.6</v>
       </c>
       <c r="P135">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="Q135">
         <v>-0.5</v>
       </c>
       <c r="R135">
-        <v>2.06</v>
+        <v>2.07</v>
       </c>
       <c r="S135">
-        <v>1.84</v>
+        <v>1.83</v>
       </c>
       <c r="T135">
         <v>3</v>
       </c>
       <c r="U135">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V135">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W135">
         <v>0</v>
@@ -12497,22 +12512,22 @@
         <v>6.5</v>
       </c>
       <c r="N136">
-        <v>1.4</v>
+        <v>1.444</v>
       </c>
       <c r="O136">
         <v>5.5</v>
       </c>
       <c r="P136">
-        <v>6.5</v>
+        <v>5.75</v>
       </c>
       <c r="Q136">
         <v>-1.25</v>
       </c>
       <c r="R136">
-        <v>1.91</v>
+        <v>1.92</v>
       </c>
       <c r="S136">
-        <v>1.99</v>
+        <v>1.98</v>
       </c>
       <c r="T136">
         <v>3.25</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 29-03-2024 às 17:05
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -12302,10 +12302,10 @@
         <v>-1</v>
       </c>
       <c r="R133">
-        <v>1.89</v>
+        <v>1.87</v>
       </c>
       <c r="S133">
-        <v>2.01</v>
+        <v>2.03</v>
       </c>
       <c r="T133">
         <v>3.25</v>
@@ -12364,22 +12364,22 @@
         <v>3.1</v>
       </c>
       <c r="N134">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="O134">
         <v>3.75</v>
       </c>
       <c r="P134">
-        <v>3.1</v>
+        <v>3</v>
       </c>
       <c r="Q134">
         <v>-0.25</v>
       </c>
       <c r="R134">
-        <v>1.95</v>
+        <v>1.93</v>
       </c>
       <c r="S134">
-        <v>1.95</v>
+        <v>1.97</v>
       </c>
       <c r="T134">
         <v>3</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 30-03-2024 às 19:32
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC137"/>
+  <dimension ref="A1:AC136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -12263,7 +12263,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>7126793</v>
+        <v>7127394</v>
       </c>
       <c r="C133" t="s">
         <v>28</v>
@@ -12272,49 +12272,49 @@
         <v>28</v>
       </c>
       <c r="E133" s="2">
-        <v>45381.14583333334</v>
+        <v>45381.875</v>
       </c>
       <c r="F133" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G133" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K133">
-        <v>1.571</v>
+        <v>1.8</v>
       </c>
       <c r="L133">
-        <v>4.333</v>
+        <v>3.8</v>
       </c>
       <c r="M133">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N133">
-        <v>1.533</v>
+        <v>2.2</v>
       </c>
       <c r="O133">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P133">
-        <v>5.25</v>
+        <v>3.2</v>
       </c>
       <c r="Q133">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R133">
-        <v>1.87</v>
+        <v>1.98</v>
       </c>
       <c r="S133">
-        <v>2.03</v>
+        <v>1.92</v>
       </c>
       <c r="T133">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U133">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="V133">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="W133">
         <v>0</v>
@@ -12337,7 +12337,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>7127396</v>
+        <v>7127397</v>
       </c>
       <c r="C134" t="s">
         <v>28</v>
@@ -12346,49 +12346,49 @@
         <v>28</v>
       </c>
       <c r="E134" s="2">
-        <v>45381.23958333334</v>
+        <v>45382.04166666666</v>
       </c>
       <c r="F134" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G134" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K134">
-        <v>2.15</v>
+        <v>1.4</v>
       </c>
       <c r="L134">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="M134">
-        <v>3.1</v>
+        <v>6.5</v>
       </c>
       <c r="N134">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="O134">
-        <v>3.75</v>
+        <v>5.5</v>
       </c>
       <c r="P134">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="Q134">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R134">
-        <v>1.93</v>
+        <v>2.05</v>
       </c>
       <c r="S134">
-        <v>1.97</v>
+        <v>1.85</v>
       </c>
       <c r="T134">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U134">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="V134">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="W134">
         <v>0</v>
@@ -12411,7 +12411,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>7127394</v>
+        <v>7127398</v>
       </c>
       <c r="C135" t="s">
         <v>28</v>
@@ -12420,49 +12420,49 @@
         <v>28</v>
       </c>
       <c r="E135" s="2">
-        <v>45381.875</v>
+        <v>45383.04166666666</v>
       </c>
       <c r="F135" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G135" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K135">
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="L135">
+        <v>3.5</v>
+      </c>
+      <c r="M135">
+        <v>2.625</v>
+      </c>
+      <c r="N135">
+        <v>2.9</v>
+      </c>
+      <c r="O135">
         <v>3.8</v>
       </c>
-      <c r="M135">
-        <v>4</v>
-      </c>
-      <c r="N135">
-        <v>2.05</v>
-      </c>
-      <c r="O135">
-        <v>3.6</v>
-      </c>
       <c r="P135">
-        <v>3.5</v>
+        <v>2.25</v>
       </c>
       <c r="Q135">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R135">
-        <v>2.07</v>
+        <v>1.84</v>
       </c>
       <c r="S135">
-        <v>1.83</v>
+        <v>2.06</v>
       </c>
       <c r="T135">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U135">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V135">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W135">
         <v>0</v>
@@ -12485,7 +12485,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>7127397</v>
+        <v>7898681</v>
       </c>
       <c r="C136" t="s">
         <v>28</v>
@@ -12494,49 +12494,49 @@
         <v>28</v>
       </c>
       <c r="E136" s="2">
-        <v>45382.04166666666</v>
+        <v>45384.20833333334</v>
       </c>
       <c r="F136" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G136" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="K136">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="L136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M136">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="N136">
-        <v>1.444</v>
+        <v>2.05</v>
       </c>
       <c r="O136">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="P136">
-        <v>5.75</v>
+        <v>3.1</v>
       </c>
       <c r="Q136">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R136">
-        <v>1.92</v>
+        <v>1.83</v>
       </c>
       <c r="S136">
-        <v>1.98</v>
+        <v>2.07</v>
       </c>
       <c r="T136">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U136">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V136">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W136">
         <v>0</v>
@@ -12551,80 +12551,6 @@
         <v>0</v>
       </c>
       <c r="AA136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:29">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137">
-        <v>7127398</v>
-      </c>
-      <c r="C137" t="s">
-        <v>28</v>
-      </c>
-      <c r="D137" t="s">
-        <v>28</v>
-      </c>
-      <c r="E137" s="2">
-        <v>45383.04166666666</v>
-      </c>
-      <c r="F137" t="s">
-        <v>31</v>
-      </c>
-      <c r="G137" t="s">
-        <v>33</v>
-      </c>
-      <c r="K137">
-        <v>2.5</v>
-      </c>
-      <c r="L137">
-        <v>3.5</v>
-      </c>
-      <c r="M137">
-        <v>2.625</v>
-      </c>
-      <c r="N137">
-        <v>2.625</v>
-      </c>
-      <c r="O137">
-        <v>3.75</v>
-      </c>
-      <c r="P137">
-        <v>2.45</v>
-      </c>
-      <c r="Q137">
-        <v>0</v>
-      </c>
-      <c r="R137">
-        <v>2.03</v>
-      </c>
-      <c r="S137">
-        <v>1.87</v>
-      </c>
-      <c r="T137">
-        <v>3.25</v>
-      </c>
-      <c r="U137">
-        <v>1.95</v>
-      </c>
-      <c r="V137">
-        <v>1.9</v>
-      </c>
-      <c r="W137">
-        <v>0</v>
-      </c>
-      <c r="X137">
-        <v>0</v>
-      </c>
-      <c r="Y137">
-        <v>0</v>
-      </c>
-      <c r="Z137">
-        <v>0</v>
-      </c>
-      <c r="AA137">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 31-03-2024 às 20:29
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC136"/>
+  <dimension ref="A1:AC137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -12263,7 +12263,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>7127394</v>
+        <v>7126793</v>
       </c>
       <c r="C133" t="s">
         <v>28</v>
@@ -12272,64 +12272,79 @@
         <v>28</v>
       </c>
       <c r="E133" s="2">
-        <v>45381.875</v>
+        <v>45381.14583333334</v>
       </c>
       <c r="F133" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="G133" t="s">
-        <v>35</v>
+        <v>39</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133" t="s">
+        <v>43</v>
       </c>
       <c r="K133">
-        <v>1.8</v>
+        <v>1.571</v>
       </c>
       <c r="L133">
-        <v>3.8</v>
+        <v>4.333</v>
       </c>
       <c r="M133">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N133">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="O133">
+        <v>5.25</v>
+      </c>
+      <c r="P133">
+        <v>6.5</v>
+      </c>
+      <c r="Q133">
+        <v>-1.25</v>
+      </c>
+      <c r="R133">
+        <v>1.825</v>
+      </c>
+      <c r="S133">
+        <v>2.025</v>
+      </c>
+      <c r="T133">
         <v>3.5</v>
       </c>
-      <c r="P133">
-        <v>3.2</v>
-      </c>
-      <c r="Q133">
-        <v>-0.25</v>
-      </c>
-      <c r="R133">
-        <v>1.98</v>
-      </c>
-      <c r="S133">
-        <v>1.92</v>
-      </c>
-      <c r="T133">
-        <v>2.75</v>
-      </c>
       <c r="U133">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V133">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W133">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X133">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="Y133">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z133">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA133">
-        <v>0</v>
+        <v>1.025</v>
+      </c>
+      <c r="AB133">
+        <v>-1</v>
+      </c>
+      <c r="AC133">
+        <v>0.875</v>
       </c>
     </row>
     <row r="134" spans="1:29">
@@ -12337,7 +12352,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>7127397</v>
+        <v>7127396</v>
       </c>
       <c r="C134" t="s">
         <v>28</v>
@@ -12346,64 +12361,79 @@
         <v>28</v>
       </c>
       <c r="E134" s="2">
-        <v>45382.04166666666</v>
+        <v>45381.23958333334</v>
       </c>
       <c r="F134" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G134" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="H134">
+        <v>2</v>
+      </c>
+      <c r="I134">
+        <v>0</v>
+      </c>
+      <c r="J134" t="s">
+        <v>42</v>
       </c>
       <c r="K134">
-        <v>1.4</v>
+        <v>2.15</v>
       </c>
       <c r="L134">
-        <v>5</v>
+        <v>3.6</v>
       </c>
       <c r="M134">
-        <v>6.5</v>
+        <v>3.1</v>
       </c>
       <c r="N134">
-        <v>1.4</v>
+        <v>2.3</v>
       </c>
       <c r="O134">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="P134">
-        <v>6.5</v>
+        <v>2.9</v>
       </c>
       <c r="Q134">
-        <v>-1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R134">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S134">
+        <v>1.825</v>
+      </c>
+      <c r="T134">
+        <v>2.75</v>
+      </c>
+      <c r="U134">
         <v>1.85</v>
       </c>
-      <c r="T134">
-        <v>3.25</v>
-      </c>
-      <c r="U134">
-        <v>1.875</v>
-      </c>
       <c r="V134">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W134">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="X134">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y134">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z134">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AA134">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB134">
+        <v>-1</v>
+      </c>
+      <c r="AC134">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:29">
@@ -12438,22 +12468,22 @@
         <v>2.625</v>
       </c>
       <c r="N135">
-        <v>2.9</v>
+        <v>2.625</v>
       </c>
       <c r="O135">
         <v>3.8</v>
       </c>
       <c r="P135">
-        <v>2.25</v>
+        <v>2.45</v>
       </c>
       <c r="Q135">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R135">
-        <v>1.84</v>
+        <v>2.02</v>
       </c>
       <c r="S135">
-        <v>2.06</v>
+        <v>1.88</v>
       </c>
       <c r="T135">
         <v>3.25</v>
@@ -12512,31 +12542,31 @@
         <v>3</v>
       </c>
       <c r="N136">
-        <v>2.05</v>
+        <v>2.15</v>
       </c>
       <c r="O136">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P136">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="Q136">
         <v>-0.25</v>
       </c>
       <c r="R136">
-        <v>1.83</v>
+        <v>1.95</v>
       </c>
       <c r="S136">
-        <v>2.07</v>
+        <v>1.95</v>
       </c>
       <c r="T136">
         <v>3</v>
       </c>
       <c r="U136">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="V136">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="W136">
         <v>0</v>
@@ -12551,6 +12581,80 @@
         <v>0</v>
       </c>
       <c r="AA136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:29">
+      <c r="A137" s="1">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>7661947</v>
+      </c>
+      <c r="C137" t="s">
+        <v>28</v>
+      </c>
+      <c r="D137" t="s">
+        <v>28</v>
+      </c>
+      <c r="E137" s="2">
+        <v>45385.32291666666</v>
+      </c>
+      <c r="F137" t="s">
+        <v>34</v>
+      </c>
+      <c r="G137" t="s">
+        <v>32</v>
+      </c>
+      <c r="K137">
+        <v>3.1</v>
+      </c>
+      <c r="L137">
+        <v>3.6</v>
+      </c>
+      <c r="M137">
+        <v>2.2</v>
+      </c>
+      <c r="N137">
+        <v>3.8</v>
+      </c>
+      <c r="O137">
+        <v>4.2</v>
+      </c>
+      <c r="P137">
+        <v>1.8</v>
+      </c>
+      <c r="Q137">
+        <v>0.5</v>
+      </c>
+      <c r="R137">
+        <v>2.04</v>
+      </c>
+      <c r="S137">
+        <v>1.86</v>
+      </c>
+      <c r="T137">
+        <v>3.25</v>
+      </c>
+      <c r="U137">
+        <v>1.875</v>
+      </c>
+      <c r="V137">
+        <v>1.975</v>
+      </c>
+      <c r="W137">
+        <v>0</v>
+      </c>
+      <c r="X137">
+        <v>0</v>
+      </c>
+      <c r="Y137">
+        <v>0</v>
+      </c>
+      <c r="Z137">
+        <v>0</v>
+      </c>
+      <c r="AA137">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 01-04-2024 às 22:23
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC137"/>
+  <dimension ref="A1:AC145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -12441,7 +12441,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>7127398</v>
+        <v>7127394</v>
       </c>
       <c r="C135" t="s">
         <v>28</v>
@@ -12450,64 +12450,79 @@
         <v>28</v>
       </c>
       <c r="E135" s="2">
-        <v>45383.04166666666</v>
+        <v>45381.875</v>
       </c>
       <c r="F135" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G135" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="I135">
+        <v>0</v>
+      </c>
+      <c r="J135" t="s">
+        <v>42</v>
       </c>
       <c r="K135">
-        <v>2.5</v>
+        <v>1.8</v>
       </c>
       <c r="L135">
+        <v>3.8</v>
+      </c>
+      <c r="M135">
+        <v>4</v>
+      </c>
+      <c r="N135">
+        <v>2.2</v>
+      </c>
+      <c r="O135">
         <v>3.5</v>
       </c>
-      <c r="M135">
-        <v>2.625</v>
-      </c>
-      <c r="N135">
-        <v>2.625</v>
-      </c>
-      <c r="O135">
-        <v>3.8</v>
-      </c>
       <c r="P135">
-        <v>2.45</v>
+        <v>3.2</v>
       </c>
       <c r="Q135">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R135">
-        <v>2.02</v>
+        <v>1.925</v>
       </c>
       <c r="S135">
-        <v>1.88</v>
+        <v>1.925</v>
       </c>
       <c r="T135">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U135">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V135">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W135">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="X135">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y135">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z135">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="AA135">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB135">
+        <v>-1</v>
+      </c>
+      <c r="AC135">
+        <v>1.025</v>
       </c>
     </row>
     <row r="136" spans="1:29">
@@ -12515,7 +12530,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>7898681</v>
+        <v>7127397</v>
       </c>
       <c r="C136" t="s">
         <v>28</v>
@@ -12524,64 +12539,79 @@
         <v>28</v>
       </c>
       <c r="E136" s="2">
-        <v>45384.20833333334</v>
+        <v>45382.04166666666</v>
       </c>
       <c r="F136" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G136" t="s">
-        <v>29</v>
+        <v>34</v>
+      </c>
+      <c r="H136">
+        <v>2</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+      <c r="J136" t="s">
+        <v>42</v>
       </c>
       <c r="K136">
-        <v>2.1</v>
+        <v>1.4</v>
       </c>
       <c r="L136">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M136">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="N136">
-        <v>2.15</v>
+        <v>1.363</v>
       </c>
       <c r="O136">
-        <v>3.8</v>
+        <v>6</v>
       </c>
       <c r="P136">
-        <v>2.9</v>
+        <v>7</v>
       </c>
       <c r="Q136">
-        <v>-0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R136">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="S136">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="T136">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U136">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V136">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W136">
-        <v>0</v>
+        <v>0.363</v>
       </c>
       <c r="X136">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y136">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z136">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA136">
-        <v>0</v>
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB136">
+        <v>-1</v>
+      </c>
+      <c r="AC136">
+        <v>0.925</v>
       </c>
     </row>
     <row r="137" spans="1:29">
@@ -12589,7 +12619,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>7661947</v>
+        <v>7127398</v>
       </c>
       <c r="C137" t="s">
         <v>28</v>
@@ -12598,63 +12628,670 @@
         <v>28</v>
       </c>
       <c r="E137" s="2">
-        <v>45385.32291666666</v>
+        <v>45383.04166666666</v>
       </c>
       <c r="F137" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G137" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>3</v>
+      </c>
+      <c r="J137" t="s">
+        <v>41</v>
       </c>
       <c r="K137">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="L137">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M137">
-        <v>2.2</v>
+        <v>2.625</v>
       </c>
       <c r="N137">
+        <v>2.6</v>
+      </c>
+      <c r="O137">
         <v>3.8</v>
       </c>
-      <c r="O137">
-        <v>4.2</v>
-      </c>
       <c r="P137">
-        <v>1.8</v>
+        <v>2.45</v>
       </c>
       <c r="Q137">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="R137">
-        <v>2.04</v>
+        <v>1.98</v>
       </c>
       <c r="S137">
-        <v>1.86</v>
+        <v>1.92</v>
       </c>
       <c r="T137">
         <v>3.25</v>
       </c>
       <c r="U137">
+        <v>1.9</v>
+      </c>
+      <c r="V137">
+        <v>1.95</v>
+      </c>
+      <c r="W137">
+        <v>-1</v>
+      </c>
+      <c r="X137">
+        <v>-1</v>
+      </c>
+      <c r="Y137">
+        <v>1.45</v>
+      </c>
+      <c r="Z137">
+        <v>-1</v>
+      </c>
+      <c r="AA137">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="AB137">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="AC137">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:29">
+      <c r="A138" s="1">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>7898681</v>
+      </c>
+      <c r="C138" t="s">
+        <v>28</v>
+      </c>
+      <c r="D138" t="s">
+        <v>28</v>
+      </c>
+      <c r="E138" s="2">
+        <v>45384.20833333334</v>
+      </c>
+      <c r="F138" t="s">
+        <v>37</v>
+      </c>
+      <c r="G138" t="s">
+        <v>29</v>
+      </c>
+      <c r="K138">
+        <v>2.1</v>
+      </c>
+      <c r="L138">
+        <v>4</v>
+      </c>
+      <c r="M138">
+        <v>3</v>
+      </c>
+      <c r="N138">
+        <v>2.2</v>
+      </c>
+      <c r="O138">
+        <v>3.8</v>
+      </c>
+      <c r="P138">
+        <v>3</v>
+      </c>
+      <c r="Q138">
+        <v>-0.25</v>
+      </c>
+      <c r="R138">
+        <v>1.95</v>
+      </c>
+      <c r="S138">
+        <v>1.95</v>
+      </c>
+      <c r="T138">
+        <v>3</v>
+      </c>
+      <c r="U138">
+        <v>2</v>
+      </c>
+      <c r="V138">
+        <v>1.85</v>
+      </c>
+      <c r="W138">
+        <v>0</v>
+      </c>
+      <c r="X138">
+        <v>0</v>
+      </c>
+      <c r="Y138">
+        <v>0</v>
+      </c>
+      <c r="Z138">
+        <v>0</v>
+      </c>
+      <c r="AA138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:29">
+      <c r="A139" s="1">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>7661947</v>
+      </c>
+      <c r="C139" t="s">
+        <v>28</v>
+      </c>
+      <c r="D139" t="s">
+        <v>28</v>
+      </c>
+      <c r="E139" s="2">
+        <v>45385.32291666666</v>
+      </c>
+      <c r="F139" t="s">
+        <v>34</v>
+      </c>
+      <c r="G139" t="s">
+        <v>32</v>
+      </c>
+      <c r="K139">
+        <v>3.1</v>
+      </c>
+      <c r="L139">
+        <v>3.6</v>
+      </c>
+      <c r="M139">
+        <v>2.2</v>
+      </c>
+      <c r="N139">
+        <v>3.8</v>
+      </c>
+      <c r="O139">
+        <v>4.2</v>
+      </c>
+      <c r="P139">
+        <v>1.8</v>
+      </c>
+      <c r="Q139">
+        <v>0.75</v>
+      </c>
+      <c r="R139">
+        <v>1.84</v>
+      </c>
+      <c r="S139">
+        <v>2.06</v>
+      </c>
+      <c r="T139">
+        <v>3.25</v>
+      </c>
+      <c r="U139">
         <v>1.875</v>
       </c>
-      <c r="V137">
+      <c r="V139">
         <v>1.975</v>
       </c>
-      <c r="W137">
-        <v>0</v>
-      </c>
-      <c r="X137">
-        <v>0</v>
-      </c>
-      <c r="Y137">
-        <v>0</v>
-      </c>
-      <c r="Z137">
-        <v>0</v>
-      </c>
-      <c r="AA137">
+      <c r="W139">
+        <v>0</v>
+      </c>
+      <c r="X139">
+        <v>0</v>
+      </c>
+      <c r="Y139">
+        <v>0</v>
+      </c>
+      <c r="Z139">
+        <v>0</v>
+      </c>
+      <c r="AA139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:29">
+      <c r="A140" s="1">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>7127399</v>
+      </c>
+      <c r="C140" t="s">
+        <v>28</v>
+      </c>
+      <c r="D140" t="s">
+        <v>28</v>
+      </c>
+      <c r="E140" s="2">
+        <v>45387.23958333334</v>
+      </c>
+      <c r="F140" t="s">
+        <v>33</v>
+      </c>
+      <c r="G140" t="s">
+        <v>35</v>
+      </c>
+      <c r="K140">
+        <v>2.1</v>
+      </c>
+      <c r="L140">
+        <v>3.75</v>
+      </c>
+      <c r="M140">
+        <v>3.1</v>
+      </c>
+      <c r="N140">
+        <v>2</v>
+      </c>
+      <c r="O140">
+        <v>4</v>
+      </c>
+      <c r="P140">
+        <v>3.2</v>
+      </c>
+      <c r="Q140">
+        <v>-0.5</v>
+      </c>
+      <c r="R140">
+        <v>2.03</v>
+      </c>
+      <c r="S140">
+        <v>1.87</v>
+      </c>
+      <c r="T140">
+        <v>3.25</v>
+      </c>
+      <c r="U140">
+        <v>2.025</v>
+      </c>
+      <c r="V140">
+        <v>1.825</v>
+      </c>
+      <c r="W140">
+        <v>0</v>
+      </c>
+      <c r="X140">
+        <v>0</v>
+      </c>
+      <c r="Y140">
+        <v>0</v>
+      </c>
+      <c r="Z140">
+        <v>0</v>
+      </c>
+      <c r="AA140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:29">
+      <c r="A141" s="1">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>8034339</v>
+      </c>
+      <c r="C141" t="s">
+        <v>28</v>
+      </c>
+      <c r="D141" t="s">
+        <v>28</v>
+      </c>
+      <c r="E141" s="2">
+        <v>45388.0625</v>
+      </c>
+      <c r="F141" t="s">
+        <v>40</v>
+      </c>
+      <c r="G141" t="s">
+        <v>31</v>
+      </c>
+      <c r="K141">
+        <v>2.6</v>
+      </c>
+      <c r="L141">
+        <v>3.5</v>
+      </c>
+      <c r="M141">
+        <v>2.55</v>
+      </c>
+      <c r="N141">
+        <v>2.1</v>
+      </c>
+      <c r="O141">
+        <v>3.75</v>
+      </c>
+      <c r="P141">
+        <v>3.1</v>
+      </c>
+      <c r="Q141">
+        <v>-0.25</v>
+      </c>
+      <c r="R141">
+        <v>1.85</v>
+      </c>
+      <c r="S141">
+        <v>2.05</v>
+      </c>
+      <c r="T141">
+        <v>3.25</v>
+      </c>
+      <c r="U141">
+        <v>1.925</v>
+      </c>
+      <c r="V141">
+        <v>1.925</v>
+      </c>
+      <c r="W141">
+        <v>0</v>
+      </c>
+      <c r="X141">
+        <v>0</v>
+      </c>
+      <c r="Y141">
+        <v>0</v>
+      </c>
+      <c r="Z141">
+        <v>0</v>
+      </c>
+      <c r="AA141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:29">
+      <c r="A142" s="1">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>8005739</v>
+      </c>
+      <c r="C142" t="s">
+        <v>28</v>
+      </c>
+      <c r="D142" t="s">
+        <v>28</v>
+      </c>
+      <c r="E142" s="2">
+        <v>45388.14583333334</v>
+      </c>
+      <c r="F142" t="s">
+        <v>37</v>
+      </c>
+      <c r="G142" t="s">
+        <v>36</v>
+      </c>
+      <c r="K142">
+        <v>1.8</v>
+      </c>
+      <c r="L142">
+        <v>3.6</v>
+      </c>
+      <c r="M142">
+        <v>4.333</v>
+      </c>
+      <c r="N142">
+        <v>1.727</v>
+      </c>
+      <c r="O142">
+        <v>3.6</v>
+      </c>
+      <c r="P142">
+        <v>4.75</v>
+      </c>
+      <c r="Q142">
+        <v>-0.75</v>
+      </c>
+      <c r="R142">
+        <v>1.99</v>
+      </c>
+      <c r="S142">
+        <v>1.91</v>
+      </c>
+      <c r="T142">
+        <v>2.75</v>
+      </c>
+      <c r="U142">
+        <v>2</v>
+      </c>
+      <c r="V142">
+        <v>1.85</v>
+      </c>
+      <c r="W142">
+        <v>0</v>
+      </c>
+      <c r="X142">
+        <v>0</v>
+      </c>
+      <c r="Y142">
+        <v>0</v>
+      </c>
+      <c r="Z142">
+        <v>0</v>
+      </c>
+      <c r="AA142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:29">
+      <c r="A143" s="1">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>7126794</v>
+      </c>
+      <c r="C143" t="s">
+        <v>28</v>
+      </c>
+      <c r="D143" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" s="2">
+        <v>45388.23958333334</v>
+      </c>
+      <c r="F143" t="s">
+        <v>38</v>
+      </c>
+      <c r="G143" t="s">
+        <v>29</v>
+      </c>
+      <c r="K143">
+        <v>1.833</v>
+      </c>
+      <c r="L143">
+        <v>3.5</v>
+      </c>
+      <c r="M143">
+        <v>4.5</v>
+      </c>
+      <c r="N143">
+        <v>2.15</v>
+      </c>
+      <c r="O143">
+        <v>3.75</v>
+      </c>
+      <c r="P143">
+        <v>3</v>
+      </c>
+      <c r="Q143">
+        <v>-0.25</v>
+      </c>
+      <c r="R143">
+        <v>1.95</v>
+      </c>
+      <c r="S143">
+        <v>1.95</v>
+      </c>
+      <c r="T143">
+        <v>2.75</v>
+      </c>
+      <c r="U143">
+        <v>1.8</v>
+      </c>
+      <c r="V143">
+        <v>2.05</v>
+      </c>
+      <c r="W143">
+        <v>0</v>
+      </c>
+      <c r="X143">
+        <v>0</v>
+      </c>
+      <c r="Y143">
+        <v>0</v>
+      </c>
+      <c r="Z143">
+        <v>0</v>
+      </c>
+      <c r="AA143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>7127403</v>
+      </c>
+      <c r="C144" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" s="2">
+        <v>45389.08333333334</v>
+      </c>
+      <c r="F144" t="s">
+        <v>39</v>
+      </c>
+      <c r="G144" t="s">
+        <v>32</v>
+      </c>
+      <c r="K144">
+        <v>3.6</v>
+      </c>
+      <c r="L144">
+        <v>3.6</v>
+      </c>
+      <c r="M144">
+        <v>1.952</v>
+      </c>
+      <c r="N144">
+        <v>4</v>
+      </c>
+      <c r="O144">
+        <v>3.75</v>
+      </c>
+      <c r="P144">
+        <v>1.85</v>
+      </c>
+      <c r="Q144">
+        <v>0.5</v>
+      </c>
+      <c r="R144">
+        <v>1.98</v>
+      </c>
+      <c r="S144">
+        <v>1.92</v>
+      </c>
+      <c r="T144">
+        <v>3</v>
+      </c>
+      <c r="U144">
+        <v>1.875</v>
+      </c>
+      <c r="V144">
+        <v>1.975</v>
+      </c>
+      <c r="W144">
+        <v>0</v>
+      </c>
+      <c r="X144">
+        <v>0</v>
+      </c>
+      <c r="Y144">
+        <v>0</v>
+      </c>
+      <c r="Z144">
+        <v>0</v>
+      </c>
+      <c r="AA144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>7127402</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="2">
+        <v>45389.16666666666</v>
+      </c>
+      <c r="F145" t="s">
+        <v>34</v>
+      </c>
+      <c r="G145" t="s">
+        <v>30</v>
+      </c>
+      <c r="K145">
+        <v>2.25</v>
+      </c>
+      <c r="L145">
+        <v>3.5</v>
+      </c>
+      <c r="M145">
+        <v>3</v>
+      </c>
+      <c r="N145">
+        <v>2.6</v>
+      </c>
+      <c r="O145">
+        <v>3.5</v>
+      </c>
+      <c r="P145">
+        <v>2.6</v>
+      </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
+      <c r="R145">
+        <v>1.95</v>
+      </c>
+      <c r="S145">
+        <v>1.95</v>
+      </c>
+      <c r="T145">
+        <v>3.25</v>
+      </c>
+      <c r="U145">
+        <v>1.925</v>
+      </c>
+      <c r="V145">
+        <v>1.925</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0</v>
+      </c>
+      <c r="Y145">
+        <v>0</v>
+      </c>
+      <c r="Z145">
+        <v>0</v>
+      </c>
+      <c r="AA145">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 02-04-2024 às 23:59
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -12725,6 +12725,15 @@
       <c r="G138" t="s">
         <v>29</v>
       </c>
+      <c r="H138">
+        <v>2</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+      <c r="J138" t="s">
+        <v>42</v>
+      </c>
       <c r="K138">
         <v>2.1</v>
       </c>
@@ -12735,46 +12744,52 @@
         <v>3</v>
       </c>
       <c r="N138">
-        <v>2.2</v>
+        <v>2.4</v>
       </c>
       <c r="O138">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P138">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="Q138">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R138">
-        <v>1.95</v>
+        <v>1.83</v>
       </c>
       <c r="S138">
-        <v>1.95</v>
+        <v>2.07</v>
       </c>
       <c r="T138">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U138">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V138">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W138">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="X138">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y138">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z138">
-        <v>0</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA138">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB138">
+        <v>0.5125</v>
+      </c>
+      <c r="AC138">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="139" spans="1:29">
@@ -12809,31 +12824,31 @@
         <v>2.2</v>
       </c>
       <c r="N139">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O139">
         <v>4.2</v>
       </c>
       <c r="P139">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="Q139">
         <v>0.75</v>
       </c>
       <c r="R139">
-        <v>1.84</v>
+        <v>1.87</v>
       </c>
       <c r="S139">
-        <v>2.06</v>
+        <v>2.03</v>
       </c>
       <c r="T139">
         <v>3.25</v>
       </c>
       <c r="U139">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="V139">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="W139">
         <v>0</v>
@@ -12904,10 +12919,10 @@
         <v>3.25</v>
       </c>
       <c r="U140">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V140">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W140">
         <v>0</v>
@@ -12957,10 +12972,10 @@
         <v>2.55</v>
       </c>
       <c r="N141">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="O141">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="P141">
         <v>3.1</v>
@@ -12969,19 +12984,19 @@
         <v>-0.25</v>
       </c>
       <c r="R141">
-        <v>1.85</v>
+        <v>1.86</v>
       </c>
       <c r="S141">
-        <v>2.05</v>
+        <v>2.04</v>
       </c>
       <c r="T141">
         <v>3.25</v>
       </c>
       <c r="U141">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V141">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W141">
         <v>0</v>
@@ -13031,31 +13046,31 @@
         <v>4.333</v>
       </c>
       <c r="N142">
-        <v>1.727</v>
+        <v>1.666</v>
       </c>
       <c r="O142">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P142">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="Q142">
         <v>-0.75</v>
       </c>
       <c r="R142">
-        <v>1.99</v>
+        <v>1.97</v>
       </c>
       <c r="S142">
-        <v>1.91</v>
+        <v>1.93</v>
       </c>
       <c r="T142">
         <v>2.75</v>
       </c>
       <c r="U142">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="V142">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="W142">
         <v>0</v>
@@ -13105,7 +13120,7 @@
         <v>4.5</v>
       </c>
       <c r="N143">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="O143">
         <v>3.75</v>
@@ -13117,19 +13132,19 @@
         <v>-0.25</v>
       </c>
       <c r="R143">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="S143">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="T143">
         <v>2.75</v>
       </c>
       <c r="U143">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V143">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W143">
         <v>0</v>
@@ -13191,10 +13206,10 @@
         <v>0.5</v>
       </c>
       <c r="R144">
-        <v>1.98</v>
+        <v>2</v>
       </c>
       <c r="S144">
-        <v>1.92</v>
+        <v>1.9</v>
       </c>
       <c r="T144">
         <v>3</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 06-04-2024 às 01:36
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC144"/>
+  <dimension ref="A1:AC145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -12797,7 +12797,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>7127399</v>
+        <v>7661947</v>
       </c>
       <c r="C139" t="s">
         <v>28</v>
@@ -12806,64 +12806,79 @@
         <v>28</v>
       </c>
       <c r="E139" s="2">
-        <v>45387.23958333334</v>
+        <v>45385.32291666666</v>
       </c>
       <c r="F139" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G139" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+      <c r="J139" t="s">
+        <v>43</v>
       </c>
       <c r="K139">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="L139">
+        <v>3.6</v>
+      </c>
+      <c r="M139">
+        <v>2.2</v>
+      </c>
+      <c r="N139">
+        <v>5</v>
+      </c>
+      <c r="O139">
+        <v>4.75</v>
+      </c>
+      <c r="P139">
+        <v>1.55</v>
+      </c>
+      <c r="Q139">
+        <v>1</v>
+      </c>
+      <c r="R139">
+        <v>1.975</v>
+      </c>
+      <c r="S139">
+        <v>1.875</v>
+      </c>
+      <c r="T139">
+        <v>3.5</v>
+      </c>
+      <c r="U139">
+        <v>1.925</v>
+      </c>
+      <c r="V139">
+        <v>1.925</v>
+      </c>
+      <c r="W139">
+        <v>-1</v>
+      </c>
+      <c r="X139">
         <v>3.75</v>
       </c>
-      <c r="M139">
-        <v>3.1</v>
-      </c>
-      <c r="N139">
-        <v>2.1</v>
-      </c>
-      <c r="O139">
-        <v>4</v>
-      </c>
-      <c r="P139">
-        <v>3.1</v>
-      </c>
-      <c r="Q139">
-        <v>-0.25</v>
-      </c>
-      <c r="R139">
-        <v>1.85</v>
-      </c>
-      <c r="S139">
-        <v>2.05</v>
-      </c>
-      <c r="T139">
-        <v>3.25</v>
-      </c>
-      <c r="U139">
-        <v>2</v>
-      </c>
-      <c r="V139">
-        <v>1.85</v>
-      </c>
-      <c r="W139">
-        <v>0</v>
-      </c>
-      <c r="X139">
-        <v>0</v>
-      </c>
       <c r="Y139">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z139">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA139">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB139">
+        <v>-1</v>
+      </c>
+      <c r="AC139">
+        <v>0.925</v>
       </c>
     </row>
     <row r="140" spans="1:29">
@@ -12871,7 +12886,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>8034339</v>
+        <v>7127399</v>
       </c>
       <c r="C140" t="s">
         <v>28</v>
@@ -12880,64 +12895,79 @@
         <v>28</v>
       </c>
       <c r="E140" s="2">
-        <v>45388.0625</v>
+        <v>45387.23958333334</v>
       </c>
       <c r="F140" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G140" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+      <c r="I140">
+        <v>2</v>
+      </c>
+      <c r="J140" t="s">
+        <v>41</v>
       </c>
       <c r="K140">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="L140">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M140">
-        <v>2.55</v>
+        <v>3.1</v>
       </c>
       <c r="N140">
-        <v>2.05</v>
+        <v>2.375</v>
       </c>
       <c r="O140">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P140">
-        <v>3.3</v>
+        <v>2.7</v>
       </c>
       <c r="Q140">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R140">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="S140">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="T140">
         <v>3.25</v>
       </c>
       <c r="U140">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V140">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W140">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X140">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y140">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="Z140">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA140">
-        <v>0</v>
+        <v>1.025</v>
+      </c>
+      <c r="AB140">
+        <v>-0.5</v>
+      </c>
+      <c r="AC140">
+        <v>0.425</v>
       </c>
     </row>
     <row r="141" spans="1:29">
@@ -12945,7 +12975,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>8005739</v>
+        <v>8034339</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -12954,49 +12984,49 @@
         <v>28</v>
       </c>
       <c r="E141" s="2">
-        <v>45388.14583333334</v>
+        <v>45388.0625</v>
       </c>
       <c r="F141" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G141" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="K141">
-        <v>1.8</v>
+        <v>2.6</v>
       </c>
       <c r="L141">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M141">
-        <v>4.333</v>
+        <v>2.55</v>
       </c>
       <c r="N141">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="O141">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="P141">
-        <v>4.5</v>
+        <v>3.25</v>
       </c>
       <c r="Q141">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R141">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="S141">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T141">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="U141">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V141">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W141">
         <v>0</v>
@@ -13019,7 +13049,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>7126794</v>
+        <v>8005739</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13028,49 +13058,49 @@
         <v>28</v>
       </c>
       <c r="E142" s="2">
-        <v>45388.23958333334</v>
+        <v>45388.14583333334</v>
       </c>
       <c r="F142" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G142" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K142">
-        <v>1.833</v>
+        <v>1.8</v>
       </c>
       <c r="L142">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M142">
-        <v>4.5</v>
+        <v>4.333</v>
       </c>
       <c r="N142">
-        <v>2.25</v>
+        <v>1.8</v>
       </c>
       <c r="O142">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P142">
-        <v>3.1</v>
+        <v>4.2</v>
       </c>
       <c r="Q142">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R142">
-        <v>1.98</v>
+        <v>2.05</v>
       </c>
       <c r="S142">
-        <v>1.92</v>
+        <v>1.85</v>
       </c>
       <c r="T142">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U142">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V142">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="W142">
         <v>0</v>
@@ -13093,7 +13123,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>7127403</v>
+        <v>7126794</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13102,49 +13132,49 @@
         <v>28</v>
       </c>
       <c r="E143" s="2">
-        <v>45389.08333333334</v>
+        <v>45388.23958333334</v>
       </c>
       <c r="F143" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G143" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K143">
-        <v>3.6</v>
+        <v>1.833</v>
       </c>
       <c r="L143">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M143">
-        <v>1.952</v>
+        <v>4.5</v>
       </c>
       <c r="N143">
-        <v>4.2</v>
+        <v>2.25</v>
       </c>
       <c r="O143">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="P143">
-        <v>1.8</v>
+        <v>3</v>
       </c>
       <c r="Q143">
-        <v>0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R143">
-        <v>1.89</v>
+        <v>1.99</v>
       </c>
       <c r="S143">
-        <v>2.01</v>
+        <v>1.91</v>
       </c>
       <c r="T143">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U143">
+        <v>1.95</v>
+      </c>
+      <c r="V143">
         <v>1.9</v>
-      </c>
-      <c r="V143">
-        <v>1.95</v>
       </c>
       <c r="W143">
         <v>0</v>
@@ -13167,7 +13197,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>7127402</v>
+        <v>7127403</v>
       </c>
       <c r="C144" t="s">
         <v>28</v>
@@ -13176,49 +13206,49 @@
         <v>28</v>
       </c>
       <c r="E144" s="2">
-        <v>45389.16666666666</v>
+        <v>45389.08333333334</v>
       </c>
       <c r="F144" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G144" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K144">
-        <v>2.25</v>
+        <v>3.6</v>
       </c>
       <c r="L144">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M144">
-        <v>3</v>
+        <v>1.952</v>
       </c>
       <c r="N144">
-        <v>2.8</v>
+        <v>4</v>
       </c>
       <c r="O144">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="P144">
-        <v>2.45</v>
+        <v>1.75</v>
       </c>
       <c r="Q144">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="R144">
-        <v>2.07</v>
+        <v>1.92</v>
       </c>
       <c r="S144">
-        <v>1.83</v>
+        <v>1.98</v>
       </c>
       <c r="T144">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="U144">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V144">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W144">
         <v>0</v>
@@ -13233,6 +13263,80 @@
         <v>0</v>
       </c>
       <c r="AA144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:27">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>7127402</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="2">
+        <v>45389.16666666666</v>
+      </c>
+      <c r="F145" t="s">
+        <v>34</v>
+      </c>
+      <c r="G145" t="s">
+        <v>30</v>
+      </c>
+      <c r="K145">
+        <v>2.25</v>
+      </c>
+      <c r="L145">
+        <v>3.5</v>
+      </c>
+      <c r="M145">
+        <v>3</v>
+      </c>
+      <c r="N145">
+        <v>2.7</v>
+      </c>
+      <c r="O145">
+        <v>3.75</v>
+      </c>
+      <c r="P145">
+        <v>2.4</v>
+      </c>
+      <c r="Q145">
+        <v>0</v>
+      </c>
+      <c r="R145">
+        <v>2.05</v>
+      </c>
+      <c r="S145">
+        <v>1.85</v>
+      </c>
+      <c r="T145">
+        <v>3.5</v>
+      </c>
+      <c r="U145">
+        <v>1.9</v>
+      </c>
+      <c r="V145">
+        <v>1.95</v>
+      </c>
+      <c r="W145">
+        <v>0</v>
+      </c>
+      <c r="X145">
+        <v>0</v>
+      </c>
+      <c r="Y145">
+        <v>0</v>
+      </c>
+      <c r="Z145">
+        <v>0</v>
+      </c>
+      <c r="AA145">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 06-04-2024 às 15:39
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC145"/>
+  <dimension ref="A1:AC143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -12975,7 +12975,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>8034339</v>
+        <v>7127403</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -12984,49 +12984,49 @@
         <v>28</v>
       </c>
       <c r="E141" s="2">
-        <v>45388.0625</v>
+        <v>45389.08333333334</v>
       </c>
       <c r="F141" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G141" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K141">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="L141">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M141">
-        <v>2.55</v>
+        <v>1.952</v>
       </c>
       <c r="N141">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O141">
         <v>4.2</v>
       </c>
       <c r="P141">
+        <v>1.75</v>
+      </c>
+      <c r="Q141">
+        <v>0.75</v>
+      </c>
+      <c r="R141">
+        <v>1.95</v>
+      </c>
+      <c r="S141">
+        <v>1.95</v>
+      </c>
+      <c r="T141">
         <v>3.25</v>
       </c>
-      <c r="Q141">
-        <v>-0.5</v>
-      </c>
-      <c r="R141">
-        <v>2</v>
-      </c>
-      <c r="S141">
-        <v>1.9</v>
-      </c>
-      <c r="T141">
-        <v>3.5</v>
-      </c>
       <c r="U141">
+        <v>1.875</v>
+      </c>
+      <c r="V141">
         <v>1.975</v>
-      </c>
-      <c r="V141">
-        <v>1.875</v>
       </c>
       <c r="W141">
         <v>0</v>
@@ -13049,7 +13049,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>8005739</v>
+        <v>7127402</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13058,49 +13058,49 @@
         <v>28</v>
       </c>
       <c r="E142" s="2">
-        <v>45388.14583333334</v>
+        <v>45389.16666666666</v>
       </c>
       <c r="F142" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G142" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K142">
-        <v>1.8</v>
+        <v>2.25</v>
       </c>
       <c r="L142">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M142">
-        <v>4.333</v>
+        <v>3</v>
       </c>
       <c r="N142">
-        <v>1.8</v>
+        <v>2.7</v>
       </c>
       <c r="O142">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="P142">
-        <v>4.2</v>
+        <v>2.4</v>
       </c>
       <c r="Q142">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R142">
-        <v>2.05</v>
+        <v>2.06</v>
       </c>
       <c r="S142">
-        <v>1.85</v>
+        <v>1.84</v>
       </c>
       <c r="T142">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="U142">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V142">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W142">
         <v>0</v>
@@ -13123,7 +13123,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>7126794</v>
+        <v>7127408</v>
       </c>
       <c r="C143" t="s">
         <v>28</v>
@@ -13132,49 +13132,49 @@
         <v>28</v>
       </c>
       <c r="E143" s="2">
-        <v>45388.23958333334</v>
+        <v>45395.10416666666</v>
       </c>
       <c r="F143" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G143" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="K143">
-        <v>1.833</v>
+        <v>3.5</v>
       </c>
       <c r="L143">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M143">
-        <v>4.5</v>
+        <v>1.909</v>
       </c>
       <c r="N143">
-        <v>2.25</v>
+        <v>3.4</v>
       </c>
       <c r="O143">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="P143">
-        <v>3</v>
+        <v>1.95</v>
       </c>
       <c r="Q143">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R143">
-        <v>1.99</v>
+        <v>1.88</v>
       </c>
       <c r="S143">
-        <v>1.91</v>
+        <v>2.02</v>
       </c>
       <c r="T143">
         <v>3</v>
       </c>
       <c r="U143">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V143">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="W143">
         <v>0</v>
@@ -13189,154 +13189,6 @@
         <v>0</v>
       </c>
       <c r="AA143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:29">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144">
-        <v>7127403</v>
-      </c>
-      <c r="C144" t="s">
-        <v>28</v>
-      </c>
-      <c r="D144" t="s">
-        <v>28</v>
-      </c>
-      <c r="E144" s="2">
-        <v>45389.08333333334</v>
-      </c>
-      <c r="F144" t="s">
-        <v>39</v>
-      </c>
-      <c r="G144" t="s">
-        <v>32</v>
-      </c>
-      <c r="K144">
-        <v>3.6</v>
-      </c>
-      <c r="L144">
-        <v>3.6</v>
-      </c>
-      <c r="M144">
-        <v>1.952</v>
-      </c>
-      <c r="N144">
-        <v>4</v>
-      </c>
-      <c r="O144">
-        <v>4.2</v>
-      </c>
-      <c r="P144">
-        <v>1.75</v>
-      </c>
-      <c r="Q144">
-        <v>0.75</v>
-      </c>
-      <c r="R144">
-        <v>1.92</v>
-      </c>
-      <c r="S144">
-        <v>1.98</v>
-      </c>
-      <c r="T144">
-        <v>3.25</v>
-      </c>
-      <c r="U144">
-        <v>1.875</v>
-      </c>
-      <c r="V144">
-        <v>1.975</v>
-      </c>
-      <c r="W144">
-        <v>0</v>
-      </c>
-      <c r="X144">
-        <v>0</v>
-      </c>
-      <c r="Y144">
-        <v>0</v>
-      </c>
-      <c r="Z144">
-        <v>0</v>
-      </c>
-      <c r="AA144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:27">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145">
-        <v>7127402</v>
-      </c>
-      <c r="C145" t="s">
-        <v>28</v>
-      </c>
-      <c r="D145" t="s">
-        <v>28</v>
-      </c>
-      <c r="E145" s="2">
-        <v>45389.16666666666</v>
-      </c>
-      <c r="F145" t="s">
-        <v>34</v>
-      </c>
-      <c r="G145" t="s">
-        <v>30</v>
-      </c>
-      <c r="K145">
-        <v>2.25</v>
-      </c>
-      <c r="L145">
-        <v>3.5</v>
-      </c>
-      <c r="M145">
-        <v>3</v>
-      </c>
-      <c r="N145">
-        <v>2.7</v>
-      </c>
-      <c r="O145">
-        <v>3.75</v>
-      </c>
-      <c r="P145">
-        <v>2.4</v>
-      </c>
-      <c r="Q145">
-        <v>0</v>
-      </c>
-      <c r="R145">
-        <v>2.05</v>
-      </c>
-      <c r="S145">
-        <v>1.85</v>
-      </c>
-      <c r="T145">
-        <v>3.5</v>
-      </c>
-      <c r="U145">
-        <v>1.9</v>
-      </c>
-      <c r="V145">
-        <v>1.95</v>
-      </c>
-      <c r="W145">
-        <v>0</v>
-      </c>
-      <c r="X145">
-        <v>0</v>
-      </c>
-      <c r="Y145">
-        <v>0</v>
-      </c>
-      <c r="Z145">
-        <v>0</v>
-      </c>
-      <c r="AA145">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 07-04-2024 às 22:30
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC143"/>
+  <dimension ref="A1:AC151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -12975,7 +12975,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>7127403</v>
+        <v>8034339</v>
       </c>
       <c r="C141" t="s">
         <v>28</v>
@@ -12984,64 +12984,79 @@
         <v>28</v>
       </c>
       <c r="E141" s="2">
-        <v>45389.08333333334</v>
+        <v>45388.0625</v>
       </c>
       <c r="F141" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G141" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="H141">
+        <v>4</v>
+      </c>
+      <c r="I141">
+        <v>2</v>
+      </c>
+      <c r="J141" t="s">
+        <v>42</v>
       </c>
       <c r="K141">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="L141">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M141">
-        <v>1.952</v>
+        <v>2.55</v>
       </c>
       <c r="N141">
-        <v>4</v>
+        <v>1.95</v>
       </c>
       <c r="O141">
         <v>4.2</v>
       </c>
       <c r="P141">
-        <v>1.75</v>
+        <v>3.3</v>
       </c>
       <c r="Q141">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R141">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="S141">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T141">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U141">
+        <v>1.975</v>
+      </c>
+      <c r="V141">
         <v>1.875</v>
       </c>
-      <c r="V141">
-        <v>1.975</v>
-      </c>
       <c r="W141">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="X141">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y141">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z141">
-        <v>0</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA141">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB141">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AC141">
+        <v>-1</v>
       </c>
     </row>
     <row r="142" spans="1:29">
@@ -13049,7 +13064,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>7127402</v>
+        <v>8005739</v>
       </c>
       <c r="C142" t="s">
         <v>28</v>
@@ -13058,43 +13073,52 @@
         <v>28</v>
       </c>
       <c r="E142" s="2">
-        <v>45389.16666666666</v>
+        <v>45388.14583333334</v>
       </c>
       <c r="F142" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G142" t="s">
-        <v>30</v>
+        <v>36</v>
+      </c>
+      <c r="H142">
+        <v>2</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142" t="s">
+        <v>42</v>
       </c>
       <c r="K142">
-        <v>2.25</v>
+        <v>1.8</v>
       </c>
       <c r="L142">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M142">
-        <v>3</v>
+        <v>4.333</v>
       </c>
       <c r="N142">
-        <v>2.7</v>
+        <v>1.8</v>
       </c>
       <c r="O142">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="P142">
-        <v>2.4</v>
+        <v>4.333</v>
       </c>
       <c r="Q142">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="R142">
-        <v>2.06</v>
+        <v>2.025</v>
       </c>
       <c r="S142">
-        <v>1.84</v>
+        <v>1.825</v>
       </c>
       <c r="T142">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="U142">
         <v>1.925</v>
@@ -13103,19 +13127,25 @@
         <v>1.925</v>
       </c>
       <c r="W142">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="X142">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y142">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z142">
-        <v>0</v>
+        <v>0.5125</v>
       </c>
       <c r="AA142">
-        <v>0</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AB142">
+        <v>0.925</v>
+      </c>
+      <c r="AC142">
+        <v>-1</v>
       </c>
     </row>
     <row r="143" spans="1:29">
@@ -13123,72 +13153,709 @@
         <v>141</v>
       </c>
       <c r="B143">
+        <v>7126794</v>
+      </c>
+      <c r="C143" t="s">
+        <v>28</v>
+      </c>
+      <c r="D143" t="s">
+        <v>28</v>
+      </c>
+      <c r="E143" s="2">
+        <v>45388.23958333334</v>
+      </c>
+      <c r="F143" t="s">
+        <v>38</v>
+      </c>
+      <c r="G143" t="s">
+        <v>29</v>
+      </c>
+      <c r="H143">
+        <v>2</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143" t="s">
+        <v>42</v>
+      </c>
+      <c r="K143">
+        <v>1.833</v>
+      </c>
+      <c r="L143">
+        <v>3.5</v>
+      </c>
+      <c r="M143">
+        <v>4.5</v>
+      </c>
+      <c r="N143">
+        <v>2.55</v>
+      </c>
+      <c r="O143">
+        <v>3.4</v>
+      </c>
+      <c r="P143">
+        <v>2.75</v>
+      </c>
+      <c r="Q143">
+        <v>0</v>
+      </c>
+      <c r="R143">
+        <v>1.85</v>
+      </c>
+      <c r="S143">
+        <v>2</v>
+      </c>
+      <c r="T143">
+        <v>2.75</v>
+      </c>
+      <c r="U143">
+        <v>1.925</v>
+      </c>
+      <c r="V143">
+        <v>1.925</v>
+      </c>
+      <c r="W143">
+        <v>1.55</v>
+      </c>
+      <c r="X143">
+        <v>-1</v>
+      </c>
+      <c r="Y143">
+        <v>-1</v>
+      </c>
+      <c r="Z143">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AA143">
+        <v>-1</v>
+      </c>
+      <c r="AB143">
+        <v>0.4625</v>
+      </c>
+      <c r="AC143">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29">
+      <c r="A144" s="1">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>7127403</v>
+      </c>
+      <c r="C144" t="s">
+        <v>28</v>
+      </c>
+      <c r="D144" t="s">
+        <v>28</v>
+      </c>
+      <c r="E144" s="2">
+        <v>45389.08333333334</v>
+      </c>
+      <c r="F144" t="s">
+        <v>39</v>
+      </c>
+      <c r="G144" t="s">
+        <v>32</v>
+      </c>
+      <c r="H144">
+        <v>3</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144" t="s">
+        <v>42</v>
+      </c>
+      <c r="K144">
+        <v>3.6</v>
+      </c>
+      <c r="L144">
+        <v>3.6</v>
+      </c>
+      <c r="M144">
+        <v>1.952</v>
+      </c>
+      <c r="N144">
+        <v>5</v>
+      </c>
+      <c r="O144">
+        <v>4.5</v>
+      </c>
+      <c r="P144">
+        <v>1.6</v>
+      </c>
+      <c r="Q144">
+        <v>1</v>
+      </c>
+      <c r="R144">
+        <v>1.875</v>
+      </c>
+      <c r="S144">
+        <v>1.975</v>
+      </c>
+      <c r="T144">
+        <v>3.25</v>
+      </c>
+      <c r="U144">
+        <v>1.875</v>
+      </c>
+      <c r="V144">
+        <v>1.975</v>
+      </c>
+      <c r="W144">
+        <v>4</v>
+      </c>
+      <c r="X144">
+        <v>-1</v>
+      </c>
+      <c r="Y144">
+        <v>-1</v>
+      </c>
+      <c r="Z144">
+        <v>0.875</v>
+      </c>
+      <c r="AA144">
+        <v>-1</v>
+      </c>
+      <c r="AB144">
+        <v>0.875</v>
+      </c>
+      <c r="AC144">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:29">
+      <c r="A145" s="1">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>7127402</v>
+      </c>
+      <c r="C145" t="s">
+        <v>28</v>
+      </c>
+      <c r="D145" t="s">
+        <v>28</v>
+      </c>
+      <c r="E145" s="2">
+        <v>45389.16666666666</v>
+      </c>
+      <c r="F145" t="s">
+        <v>34</v>
+      </c>
+      <c r="G145" t="s">
+        <v>30</v>
+      </c>
+      <c r="H145">
+        <v>2</v>
+      </c>
+      <c r="I145">
+        <v>4</v>
+      </c>
+      <c r="J145" t="s">
+        <v>41</v>
+      </c>
+      <c r="K145">
+        <v>2.25</v>
+      </c>
+      <c r="L145">
+        <v>3.5</v>
+      </c>
+      <c r="M145">
+        <v>3</v>
+      </c>
+      <c r="N145">
+        <v>3</v>
+      </c>
+      <c r="O145">
+        <v>3.8</v>
+      </c>
+      <c r="P145">
+        <v>2.2</v>
+      </c>
+      <c r="Q145">
+        <v>0.25</v>
+      </c>
+      <c r="R145">
+        <v>1.875</v>
+      </c>
+      <c r="S145">
+        <v>1.975</v>
+      </c>
+      <c r="T145">
+        <v>3.75</v>
+      </c>
+      <c r="U145">
+        <v>2</v>
+      </c>
+      <c r="V145">
+        <v>1.85</v>
+      </c>
+      <c r="W145">
+        <v>-1</v>
+      </c>
+      <c r="X145">
+        <v>-1</v>
+      </c>
+      <c r="Y145">
+        <v>1.2</v>
+      </c>
+      <c r="Z145">
+        <v>-1</v>
+      </c>
+      <c r="AA145">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB145">
+        <v>1</v>
+      </c>
+      <c r="AC145">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:29">
+      <c r="A146" s="1">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>7127404</v>
+      </c>
+      <c r="C146" t="s">
+        <v>28</v>
+      </c>
+      <c r="D146" t="s">
+        <v>28</v>
+      </c>
+      <c r="E146" s="2">
+        <v>45394.16666666666</v>
+      </c>
+      <c r="F146" t="s">
+        <v>36</v>
+      </c>
+      <c r="G146" t="s">
+        <v>38</v>
+      </c>
+      <c r="K146">
+        <v>3.1</v>
+      </c>
+      <c r="L146">
+        <v>3.4</v>
+      </c>
+      <c r="M146">
+        <v>2.25</v>
+      </c>
+      <c r="N146">
+        <v>3.4</v>
+      </c>
+      <c r="O146">
+        <v>3.5</v>
+      </c>
+      <c r="P146">
+        <v>2.1</v>
+      </c>
+      <c r="Q146">
+        <v>0.25</v>
+      </c>
+      <c r="R146">
+        <v>2.01</v>
+      </c>
+      <c r="S146">
+        <v>1.89</v>
+      </c>
+      <c r="T146">
+        <v>2.75</v>
+      </c>
+      <c r="U146">
+        <v>2</v>
+      </c>
+      <c r="V146">
+        <v>1.85</v>
+      </c>
+      <c r="W146">
+        <v>0</v>
+      </c>
+      <c r="X146">
+        <v>0</v>
+      </c>
+      <c r="Y146">
+        <v>0</v>
+      </c>
+      <c r="Z146">
+        <v>0</v>
+      </c>
+      <c r="AA146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:29">
+      <c r="A147" s="1">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>7127405</v>
+      </c>
+      <c r="C147" t="s">
+        <v>28</v>
+      </c>
+      <c r="D147" t="s">
+        <v>28</v>
+      </c>
+      <c r="E147" s="2">
+        <v>45394.28125</v>
+      </c>
+      <c r="F147" t="s">
+        <v>30</v>
+      </c>
+      <c r="G147" t="s">
+        <v>31</v>
+      </c>
+      <c r="K147">
+        <v>1.833</v>
+      </c>
+      <c r="L147">
+        <v>4</v>
+      </c>
+      <c r="M147">
+        <v>3.75</v>
+      </c>
+      <c r="N147">
+        <v>1.85</v>
+      </c>
+      <c r="O147">
+        <v>4</v>
+      </c>
+      <c r="P147">
+        <v>3.75</v>
+      </c>
+      <c r="Q147">
+        <v>-0.5</v>
+      </c>
+      <c r="R147">
+        <v>1.87</v>
+      </c>
+      <c r="S147">
+        <v>2.03</v>
+      </c>
+      <c r="T147">
+        <v>3.5</v>
+      </c>
+      <c r="U147">
+        <v>1.95</v>
+      </c>
+      <c r="V147">
+        <v>1.9</v>
+      </c>
+      <c r="W147">
+        <v>0</v>
+      </c>
+      <c r="X147">
+        <v>0</v>
+      </c>
+      <c r="Y147">
+        <v>0</v>
+      </c>
+      <c r="Z147">
+        <v>0</v>
+      </c>
+      <c r="AA147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:29">
+      <c r="A148" s="1">
+        <v>146</v>
+      </c>
+      <c r="B148">
         <v>7127408</v>
       </c>
-      <c r="C143" t="s">
-        <v>28</v>
-      </c>
-      <c r="D143" t="s">
-        <v>28</v>
-      </c>
-      <c r="E143" s="2">
+      <c r="C148" t="s">
+        <v>28</v>
+      </c>
+      <c r="D148" t="s">
+        <v>28</v>
+      </c>
+      <c r="E148" s="2">
         <v>45395.10416666666</v>
       </c>
-      <c r="F143" t="s">
+      <c r="F148" t="s">
         <v>40</v>
       </c>
-      <c r="G143" t="s">
+      <c r="G148" t="s">
         <v>37</v>
       </c>
-      <c r="K143">
+      <c r="K148">
         <v>3.5</v>
       </c>
-      <c r="L143">
+      <c r="L148">
         <v>3.8</v>
       </c>
-      <c r="M143">
+      <c r="M148">
         <v>1.909</v>
       </c>
-      <c r="N143">
+      <c r="N148">
         <v>3.4</v>
       </c>
-      <c r="O143">
+      <c r="O148">
         <v>3.8</v>
       </c>
-      <c r="P143">
+      <c r="P148">
         <v>1.95</v>
       </c>
-      <c r="Q143">
+      <c r="Q148">
         <v>0.5</v>
       </c>
-      <c r="R143">
-        <v>1.88</v>
-      </c>
-      <c r="S143">
-        <v>2.02</v>
-      </c>
-      <c r="T143">
+      <c r="R148">
+        <v>1.89</v>
+      </c>
+      <c r="S148">
+        <v>2.01</v>
+      </c>
+      <c r="T148">
         <v>3</v>
       </c>
-      <c r="U143">
+      <c r="U148">
         <v>1.975</v>
       </c>
-      <c r="V143">
+      <c r="V148">
         <v>1.875</v>
       </c>
-      <c r="W143">
+      <c r="W148">
         <v>0</v>
       </c>
-      <c r="X143">
+      <c r="X148">
         <v>0</v>
       </c>
-      <c r="Y143">
+      <c r="Y148">
         <v>0</v>
       </c>
-      <c r="Z143">
+      <c r="Z148">
         <v>0</v>
       </c>
-      <c r="AA143">
+      <c r="AA148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:29">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>7127407</v>
+      </c>
+      <c r="C149" t="s">
+        <v>28</v>
+      </c>
+      <c r="D149" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149" s="2">
+        <v>45395.1875</v>
+      </c>
+      <c r="F149" t="s">
+        <v>35</v>
+      </c>
+      <c r="G149" t="s">
+        <v>39</v>
+      </c>
+      <c r="K149">
+        <v>2.1</v>
+      </c>
+      <c r="L149">
+        <v>3.6</v>
+      </c>
+      <c r="M149">
+        <v>3.25</v>
+      </c>
+      <c r="N149">
+        <v>1.833</v>
+      </c>
+      <c r="O149">
+        <v>3.75</v>
+      </c>
+      <c r="P149">
+        <v>4</v>
+      </c>
+      <c r="Q149">
+        <v>-0.5</v>
+      </c>
+      <c r="R149">
+        <v>1.86</v>
+      </c>
+      <c r="S149">
+        <v>2.04</v>
+      </c>
+      <c r="T149">
+        <v>3.25</v>
+      </c>
+      <c r="U149">
+        <v>1.925</v>
+      </c>
+      <c r="V149">
+        <v>1.925</v>
+      </c>
+      <c r="W149">
+        <v>0</v>
+      </c>
+      <c r="X149">
+        <v>0</v>
+      </c>
+      <c r="Y149">
+        <v>0</v>
+      </c>
+      <c r="Z149">
+        <v>0</v>
+      </c>
+      <c r="AA149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:29">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>7127406</v>
+      </c>
+      <c r="C150" t="s">
+        <v>28</v>
+      </c>
+      <c r="D150" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150" s="2">
+        <v>45395.28125</v>
+      </c>
+      <c r="F150" t="s">
+        <v>32</v>
+      </c>
+      <c r="G150" t="s">
+        <v>33</v>
+      </c>
+      <c r="K150">
+        <v>1.833</v>
+      </c>
+      <c r="L150">
+        <v>4</v>
+      </c>
+      <c r="M150">
+        <v>3.75</v>
+      </c>
+      <c r="N150">
+        <v>1.615</v>
+      </c>
+      <c r="O150">
+        <v>4.333</v>
+      </c>
+      <c r="P150">
+        <v>4.5</v>
+      </c>
+      <c r="Q150">
+        <v>-0.75</v>
+      </c>
+      <c r="R150">
+        <v>1.85</v>
+      </c>
+      <c r="S150">
+        <v>2.05</v>
+      </c>
+      <c r="T150">
+        <v>3.25</v>
+      </c>
+      <c r="U150">
+        <v>1.925</v>
+      </c>
+      <c r="V150">
+        <v>1.925</v>
+      </c>
+      <c r="W150">
+        <v>0</v>
+      </c>
+      <c r="X150">
+        <v>0</v>
+      </c>
+      <c r="Y150">
+        <v>0</v>
+      </c>
+      <c r="Z150">
+        <v>0</v>
+      </c>
+      <c r="AA150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:29">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>7127409</v>
+      </c>
+      <c r="C151" t="s">
+        <v>28</v>
+      </c>
+      <c r="D151" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="2">
+        <v>45396.08333333334</v>
+      </c>
+      <c r="F151" t="s">
+        <v>29</v>
+      </c>
+      <c r="G151" t="s">
+        <v>34</v>
+      </c>
+      <c r="K151">
+        <v>1.571</v>
+      </c>
+      <c r="L151">
+        <v>4.5</v>
+      </c>
+      <c r="M151">
+        <v>4.75</v>
+      </c>
+      <c r="N151">
+        <v>1.444</v>
+      </c>
+      <c r="O151">
+        <v>5</v>
+      </c>
+      <c r="P151">
+        <v>6</v>
+      </c>
+      <c r="Q151">
+        <v>-1.25</v>
+      </c>
+      <c r="R151">
+        <v>1.91</v>
+      </c>
+      <c r="S151">
+        <v>1.99</v>
+      </c>
+      <c r="T151">
+        <v>3.5</v>
+      </c>
+      <c r="U151">
+        <v>2.025</v>
+      </c>
+      <c r="V151">
+        <v>1.825</v>
+      </c>
+      <c r="W151">
+        <v>0</v>
+      </c>
+      <c r="X151">
+        <v>0</v>
+      </c>
+      <c r="Y151">
+        <v>0</v>
+      </c>
+      <c r="Z151">
+        <v>0</v>
+      </c>
+      <c r="AA151">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 08-04-2024 às 21:28
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -13447,22 +13447,22 @@
         <v>2.25</v>
       </c>
       <c r="N146">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O146">
         <v>3.5</v>
       </c>
       <c r="P146">
-        <v>2.1</v>
+        <v>2.05</v>
       </c>
       <c r="Q146">
         <v>0.25</v>
       </c>
       <c r="R146">
-        <v>2.01</v>
+        <v>2.08</v>
       </c>
       <c r="S146">
-        <v>1.89</v>
+        <v>1.82</v>
       </c>
       <c r="T146">
         <v>2.75</v>
@@ -13521,31 +13521,31 @@
         <v>3.75</v>
       </c>
       <c r="N147">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="O147">
         <v>4</v>
       </c>
       <c r="P147">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="Q147">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R147">
+        <v>2.03</v>
+      </c>
+      <c r="S147">
         <v>1.87</v>
-      </c>
-      <c r="S147">
-        <v>2.03</v>
       </c>
       <c r="T147">
         <v>3.5</v>
       </c>
       <c r="U147">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V147">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W147">
         <v>0</v>
@@ -13669,31 +13669,31 @@
         <v>3.25</v>
       </c>
       <c r="N149">
-        <v>1.833</v>
+        <v>1.8</v>
       </c>
       <c r="O149">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="P149">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q149">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R149">
+        <v>2.04</v>
+      </c>
+      <c r="S149">
         <v>1.86</v>
-      </c>
-      <c r="S149">
-        <v>2.04</v>
       </c>
       <c r="T149">
         <v>3.25</v>
       </c>
       <c r="U149">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V149">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W149">
         <v>0</v>
@@ -13755,10 +13755,10 @@
         <v>-0.75</v>
       </c>
       <c r="R150">
-        <v>1.85</v>
+        <v>1.84</v>
       </c>
       <c r="S150">
-        <v>2.05</v>
+        <v>2.06</v>
       </c>
       <c r="T150">
         <v>3.25</v>
@@ -13817,31 +13817,31 @@
         <v>4.75</v>
       </c>
       <c r="N151">
-        <v>1.444</v>
+        <v>1.4</v>
       </c>
       <c r="O151">
         <v>5</v>
       </c>
       <c r="P151">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="Q151">
         <v>-1.25</v>
       </c>
       <c r="R151">
-        <v>1.91</v>
+        <v>1.87</v>
       </c>
       <c r="S151">
-        <v>1.99</v>
+        <v>2.03</v>
       </c>
       <c r="T151">
         <v>3.5</v>
       </c>
       <c r="U151">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V151">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W151">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 09-04-2024 às 22:40
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -13447,7 +13447,7 @@
         <v>2.25</v>
       </c>
       <c r="N146">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="O146">
         <v>3.5</v>
@@ -13456,13 +13456,13 @@
         <v>2.05</v>
       </c>
       <c r="Q146">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R146">
-        <v>2.08</v>
+        <v>1.83</v>
       </c>
       <c r="S146">
-        <v>1.82</v>
+        <v>2.07</v>
       </c>
       <c r="T146">
         <v>2.75</v>
@@ -13524,28 +13524,28 @@
         <v>1.8</v>
       </c>
       <c r="O147">
-        <v>4</v>
+        <v>4.333</v>
       </c>
       <c r="P147">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q147">
         <v>-0.75</v>
       </c>
       <c r="R147">
-        <v>2.03</v>
+        <v>2.05</v>
       </c>
       <c r="S147">
-        <v>1.87</v>
+        <v>1.85</v>
       </c>
       <c r="T147">
         <v>3.5</v>
       </c>
       <c r="U147">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V147">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W147">
         <v>0</v>
@@ -13681,10 +13681,10 @@
         <v>-0.75</v>
       </c>
       <c r="R149">
-        <v>2.04</v>
+        <v>2.01</v>
       </c>
       <c r="S149">
-        <v>1.86</v>
+        <v>1.89</v>
       </c>
       <c r="T149">
         <v>3.25</v>
@@ -13752,13 +13752,13 @@
         <v>4.5</v>
       </c>
       <c r="Q150">
-        <v>-0.75</v>
+        <v>-1</v>
       </c>
       <c r="R150">
-        <v>1.84</v>
+        <v>2.07</v>
       </c>
       <c r="S150">
-        <v>2.06</v>
+        <v>1.83</v>
       </c>
       <c r="T150">
         <v>3.25</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 11-04-2024 às 00:31
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -13459,10 +13459,10 @@
         <v>0.5</v>
       </c>
       <c r="R146">
-        <v>1.83</v>
+        <v>1.84</v>
       </c>
       <c r="S146">
-        <v>2.07</v>
+        <v>2.06</v>
       </c>
       <c r="T146">
         <v>2.75</v>
@@ -13521,31 +13521,31 @@
         <v>3.75</v>
       </c>
       <c r="N147">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="O147">
         <v>4.333</v>
       </c>
       <c r="P147">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q147">
         <v>-0.75</v>
       </c>
       <c r="R147">
-        <v>2.05</v>
+        <v>1.97</v>
       </c>
       <c r="S147">
-        <v>1.85</v>
+        <v>1.93</v>
       </c>
       <c r="T147">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="U147">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="V147">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W147">
         <v>0</v>
@@ -13595,7 +13595,7 @@
         <v>1.909</v>
       </c>
       <c r="N148">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="O148">
         <v>3.8</v>
@@ -13607,19 +13607,19 @@
         <v>0.5</v>
       </c>
       <c r="R148">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S148">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="T148">
         <v>3</v>
       </c>
       <c r="U148">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V148">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W148">
         <v>0</v>
@@ -13669,22 +13669,22 @@
         <v>3.25</v>
       </c>
       <c r="N149">
-        <v>1.8</v>
+        <v>1.727</v>
       </c>
       <c r="O149">
+        <v>4.333</v>
+      </c>
+      <c r="P149">
         <v>4.2</v>
-      </c>
-      <c r="P149">
-        <v>3.8</v>
       </c>
       <c r="Q149">
         <v>-0.75</v>
       </c>
       <c r="R149">
-        <v>2.01</v>
+        <v>1.9</v>
       </c>
       <c r="S149">
-        <v>1.89</v>
+        <v>2</v>
       </c>
       <c r="T149">
         <v>3.25</v>
@@ -13746,19 +13746,19 @@
         <v>1.615</v>
       </c>
       <c r="O150">
-        <v>4.333</v>
+        <v>4.5</v>
       </c>
       <c r="P150">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="Q150">
         <v>-1</v>
       </c>
       <c r="R150">
-        <v>2.07</v>
+        <v>2.06</v>
       </c>
       <c r="S150">
-        <v>1.83</v>
+        <v>1.84</v>
       </c>
       <c r="T150">
         <v>3.25</v>
@@ -13823,25 +13823,25 @@
         <v>5</v>
       </c>
       <c r="P151">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="Q151">
         <v>-1.25</v>
       </c>
       <c r="R151">
-        <v>1.87</v>
+        <v>1.88</v>
       </c>
       <c r="S151">
-        <v>2.03</v>
+        <v>2.02</v>
       </c>
       <c r="T151">
         <v>3.5</v>
       </c>
       <c r="U151">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V151">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W151">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 11-04-2024 às 23:56
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -13447,31 +13447,31 @@
         <v>2.25</v>
       </c>
       <c r="N146">
+        <v>3.3</v>
+      </c>
+      <c r="O146">
         <v>3.6</v>
       </c>
-      <c r="O146">
-        <v>3.5</v>
-      </c>
       <c r="P146">
-        <v>2.05</v>
+        <v>2.1</v>
       </c>
       <c r="Q146">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R146">
-        <v>1.84</v>
+        <v>2.02</v>
       </c>
       <c r="S146">
-        <v>2.06</v>
+        <v>1.88</v>
       </c>
       <c r="T146">
         <v>2.75</v>
       </c>
       <c r="U146">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V146">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="W146">
         <v>0</v>
@@ -13521,10 +13521,10 @@
         <v>3.75</v>
       </c>
       <c r="N147">
-        <v>1.75</v>
+        <v>1.7</v>
       </c>
       <c r="O147">
-        <v>4.333</v>
+        <v>4.5</v>
       </c>
       <c r="P147">
         <v>4</v>
@@ -13533,19 +13533,19 @@
         <v>-0.75</v>
       </c>
       <c r="R147">
-        <v>1.97</v>
+        <v>1.85</v>
       </c>
       <c r="S147">
-        <v>1.93</v>
+        <v>2.05</v>
       </c>
       <c r="T147">
         <v>3.75</v>
       </c>
       <c r="U147">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="V147">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="W147">
         <v>0</v>
@@ -13616,10 +13616,10 @@
         <v>3</v>
       </c>
       <c r="U148">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="V148">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="W148">
         <v>0</v>
@@ -13755,19 +13755,19 @@
         <v>-1</v>
       </c>
       <c r="R150">
-        <v>2.06</v>
+        <v>2.07</v>
       </c>
       <c r="S150">
-        <v>1.84</v>
+        <v>1.83</v>
       </c>
       <c r="T150">
         <v>3.25</v>
       </c>
       <c r="U150">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V150">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W150">
         <v>0</v>
@@ -13826,22 +13826,22 @@
         <v>7</v>
       </c>
       <c r="Q151">
-        <v>-1.25</v>
+        <v>-1.5</v>
       </c>
       <c r="R151">
-        <v>1.88</v>
+        <v>2.04</v>
       </c>
       <c r="S151">
-        <v>2.02</v>
+        <v>1.86</v>
       </c>
       <c r="T151">
         <v>3.5</v>
       </c>
       <c r="U151">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V151">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W151">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 12-04-2024 às 20:28
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC151"/>
+  <dimension ref="A1:AC149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -13420,7 +13420,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>7127404</v>
+        <v>7127408</v>
       </c>
       <c r="C146" t="s">
         <v>28</v>
@@ -13429,49 +13429,49 @@
         <v>28</v>
       </c>
       <c r="E146" s="2">
-        <v>45394.16666666666</v>
+        <v>45395.10416666666</v>
       </c>
       <c r="F146" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="G146" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K146">
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="L146">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M146">
-        <v>2.25</v>
+        <v>1.909</v>
       </c>
       <c r="N146">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="O146">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="P146">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="Q146">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R146">
-        <v>2.02</v>
+        <v>1.99</v>
       </c>
       <c r="S146">
-        <v>1.88</v>
+        <v>1.91</v>
       </c>
       <c r="T146">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U146">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V146">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="W146">
         <v>0</v>
@@ -13494,7 +13494,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>7127405</v>
+        <v>7127407</v>
       </c>
       <c r="C147" t="s">
         <v>28</v>
@@ -13503,49 +13503,49 @@
         <v>28</v>
       </c>
       <c r="E147" s="2">
-        <v>45394.28125</v>
+        <v>45395.1875</v>
       </c>
       <c r="F147" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G147" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K147">
-        <v>1.833</v>
+        <v>2.1</v>
       </c>
       <c r="L147">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M147">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="N147">
-        <v>1.7</v>
+        <v>1.727</v>
       </c>
       <c r="O147">
-        <v>4.5</v>
+        <v>4.333</v>
       </c>
       <c r="P147">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="Q147">
         <v>-0.75</v>
       </c>
       <c r="R147">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="S147">
-        <v>2.05</v>
+        <v>2.01</v>
       </c>
       <c r="T147">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="U147">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V147">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W147">
         <v>0</v>
@@ -13568,7 +13568,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>7127408</v>
+        <v>7127406</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
@@ -13577,49 +13577,49 @@
         <v>28</v>
       </c>
       <c r="E148" s="2">
-        <v>45395.10416666666</v>
+        <v>45395.28125</v>
       </c>
       <c r="F148" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G148" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K148">
+        <v>1.833</v>
+      </c>
+      <c r="L148">
+        <v>4</v>
+      </c>
+      <c r="M148">
+        <v>3.75</v>
+      </c>
+      <c r="N148">
+        <v>1.65</v>
+      </c>
+      <c r="O148">
+        <v>4.5</v>
+      </c>
+      <c r="P148">
+        <v>4.5</v>
+      </c>
+      <c r="Q148">
+        <v>-1</v>
+      </c>
+      <c r="R148">
+        <v>2.07</v>
+      </c>
+      <c r="S148">
+        <v>1.83</v>
+      </c>
+      <c r="T148">
         <v>3.5</v>
       </c>
-      <c r="L148">
-        <v>3.8</v>
-      </c>
-      <c r="M148">
-        <v>1.909</v>
-      </c>
-      <c r="N148">
-        <v>3.6</v>
-      </c>
-      <c r="O148">
-        <v>3.8</v>
-      </c>
-      <c r="P148">
-        <v>1.95</v>
-      </c>
-      <c r="Q148">
-        <v>0.5</v>
-      </c>
-      <c r="R148">
-        <v>1.9</v>
-      </c>
-      <c r="S148">
-        <v>2</v>
-      </c>
-      <c r="T148">
-        <v>3</v>
-      </c>
       <c r="U148">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="V148">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="W148">
         <v>0</v>
@@ -13642,7 +13642,7 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>7127407</v>
+        <v>7127409</v>
       </c>
       <c r="C149" t="s">
         <v>28</v>
@@ -13651,49 +13651,49 @@
         <v>28</v>
       </c>
       <c r="E149" s="2">
-        <v>45395.1875</v>
+        <v>45396.08333333334</v>
       </c>
       <c r="F149" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G149" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K149">
-        <v>2.1</v>
+        <v>1.571</v>
       </c>
       <c r="L149">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="M149">
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
       <c r="N149">
-        <v>1.727</v>
+        <v>1.4</v>
       </c>
       <c r="O149">
-        <v>4.333</v>
+        <v>5</v>
       </c>
       <c r="P149">
-        <v>4.2</v>
+        <v>7</v>
       </c>
       <c r="Q149">
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="R149">
-        <v>1.9</v>
+        <v>2.02</v>
       </c>
       <c r="S149">
-        <v>2</v>
+        <v>1.88</v>
       </c>
       <c r="T149">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U149">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V149">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W149">
         <v>0</v>
@@ -13708,154 +13708,6 @@
         <v>0</v>
       </c>
       <c r="AA149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:29">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150">
-        <v>7127406</v>
-      </c>
-      <c r="C150" t="s">
-        <v>28</v>
-      </c>
-      <c r="D150" t="s">
-        <v>28</v>
-      </c>
-      <c r="E150" s="2">
-        <v>45395.28125</v>
-      </c>
-      <c r="F150" t="s">
-        <v>32</v>
-      </c>
-      <c r="G150" t="s">
-        <v>33</v>
-      </c>
-      <c r="K150">
-        <v>1.833</v>
-      </c>
-      <c r="L150">
-        <v>4</v>
-      </c>
-      <c r="M150">
-        <v>3.75</v>
-      </c>
-      <c r="N150">
-        <v>1.615</v>
-      </c>
-      <c r="O150">
-        <v>4.5</v>
-      </c>
-      <c r="P150">
-        <v>4.75</v>
-      </c>
-      <c r="Q150">
-        <v>-1</v>
-      </c>
-      <c r="R150">
-        <v>2.07</v>
-      </c>
-      <c r="S150">
-        <v>1.83</v>
-      </c>
-      <c r="T150">
-        <v>3.25</v>
-      </c>
-      <c r="U150">
-        <v>1.9</v>
-      </c>
-      <c r="V150">
-        <v>1.95</v>
-      </c>
-      <c r="W150">
-        <v>0</v>
-      </c>
-      <c r="X150">
-        <v>0</v>
-      </c>
-      <c r="Y150">
-        <v>0</v>
-      </c>
-      <c r="Z150">
-        <v>0</v>
-      </c>
-      <c r="AA150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:29">
-      <c r="A151" s="1">
-        <v>149</v>
-      </c>
-      <c r="B151">
-        <v>7127409</v>
-      </c>
-      <c r="C151" t="s">
-        <v>28</v>
-      </c>
-      <c r="D151" t="s">
-        <v>28</v>
-      </c>
-      <c r="E151" s="2">
-        <v>45396.08333333334</v>
-      </c>
-      <c r="F151" t="s">
-        <v>29</v>
-      </c>
-      <c r="G151" t="s">
-        <v>34</v>
-      </c>
-      <c r="K151">
-        <v>1.571</v>
-      </c>
-      <c r="L151">
-        <v>4.5</v>
-      </c>
-      <c r="M151">
-        <v>4.75</v>
-      </c>
-      <c r="N151">
-        <v>1.4</v>
-      </c>
-      <c r="O151">
-        <v>5</v>
-      </c>
-      <c r="P151">
-        <v>7</v>
-      </c>
-      <c r="Q151">
-        <v>-1.5</v>
-      </c>
-      <c r="R151">
-        <v>2.04</v>
-      </c>
-      <c r="S151">
-        <v>1.86</v>
-      </c>
-      <c r="T151">
-        <v>3.5</v>
-      </c>
-      <c r="U151">
-        <v>1.95</v>
-      </c>
-      <c r="V151">
-        <v>1.9</v>
-      </c>
-      <c r="W151">
-        <v>0</v>
-      </c>
-      <c r="X151">
-        <v>0</v>
-      </c>
-      <c r="Y151">
-        <v>0</v>
-      </c>
-      <c r="Z151">
-        <v>0</v>
-      </c>
-      <c r="AA151">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 14-04-2024 às 15:12
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC149"/>
+  <dimension ref="A1:AC148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -13420,7 +13420,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>7127408</v>
+        <v>7127404</v>
       </c>
       <c r="C146" t="s">
         <v>28</v>
@@ -13429,64 +13429,79 @@
         <v>28</v>
       </c>
       <c r="E146" s="2">
-        <v>45395.10416666666</v>
+        <v>45394.16666666666</v>
       </c>
       <c r="F146" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G146" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146" t="s">
+        <v>42</v>
       </c>
       <c r="K146">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="L146">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M146">
-        <v>1.909</v>
+        <v>2.25</v>
       </c>
       <c r="N146">
-        <v>3.5</v>
+        <v>2.9</v>
       </c>
       <c r="O146">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P146">
-        <v>1.909</v>
+        <v>2.3</v>
       </c>
       <c r="Q146">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R146">
-        <v>1.99</v>
+        <v>1.86</v>
       </c>
       <c r="S146">
-        <v>1.91</v>
+        <v>2.04</v>
       </c>
       <c r="T146">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U146">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V146">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W146">
-        <v>0</v>
+        <v>1.9</v>
       </c>
       <c r="X146">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y146">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z146">
-        <v>0</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA146">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB146">
+        <v>-1</v>
+      </c>
+      <c r="AC146">
+        <v>0.925</v>
       </c>
     </row>
     <row r="147" spans="1:29">
@@ -13494,7 +13509,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>7127407</v>
+        <v>7127405</v>
       </c>
       <c r="C147" t="s">
         <v>28</v>
@@ -13503,64 +13518,79 @@
         <v>28</v>
       </c>
       <c r="E147" s="2">
-        <v>45395.1875</v>
+        <v>45394.28125</v>
       </c>
       <c r="F147" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G147" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+      <c r="I147">
+        <v>2</v>
+      </c>
+      <c r="J147" t="s">
+        <v>41</v>
       </c>
       <c r="K147">
-        <v>2.1</v>
+        <v>1.833</v>
       </c>
       <c r="L147">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M147">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="N147">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="O147">
-        <v>4.333</v>
+        <v>5.25</v>
       </c>
       <c r="P147">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="Q147">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="R147">
-        <v>1.89</v>
+        <v>2</v>
       </c>
       <c r="S147">
-        <v>2.01</v>
+        <v>1.85</v>
       </c>
       <c r="T147">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="U147">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V147">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W147">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X147">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y147">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z147">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA147">
-        <v>0</v>
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AB147">
+        <v>-1</v>
+      </c>
+      <c r="AC147">
+        <v>0.925</v>
       </c>
     </row>
     <row r="148" spans="1:29">
@@ -13568,7 +13598,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>7127406</v>
+        <v>7127409</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
@@ -13577,49 +13607,49 @@
         <v>28</v>
       </c>
       <c r="E148" s="2">
-        <v>45395.28125</v>
+        <v>45396.08333333334</v>
       </c>
       <c r="F148" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G148" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K148">
-        <v>1.833</v>
+        <v>1.571</v>
       </c>
       <c r="L148">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="M148">
-        <v>3.75</v>
+        <v>4.75</v>
       </c>
       <c r="N148">
-        <v>1.65</v>
+        <v>1.4</v>
       </c>
       <c r="O148">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="P148">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="Q148">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="R148">
-        <v>2.07</v>
+        <v>2.01</v>
       </c>
       <c r="S148">
-        <v>1.83</v>
+        <v>1.89</v>
       </c>
       <c r="T148">
         <v>3.5</v>
       </c>
       <c r="U148">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V148">
-        <v>1.85</v>
+        <v>2</v>
       </c>
       <c r="W148">
         <v>0</v>
@@ -13634,80 +13664,6 @@
         <v>0</v>
       </c>
       <c r="AA148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:29">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149">
-        <v>7127409</v>
-      </c>
-      <c r="C149" t="s">
-        <v>28</v>
-      </c>
-      <c r="D149" t="s">
-        <v>28</v>
-      </c>
-      <c r="E149" s="2">
-        <v>45396.08333333334</v>
-      </c>
-      <c r="F149" t="s">
-        <v>29</v>
-      </c>
-      <c r="G149" t="s">
-        <v>34</v>
-      </c>
-      <c r="K149">
-        <v>1.571</v>
-      </c>
-      <c r="L149">
-        <v>4.5</v>
-      </c>
-      <c r="M149">
-        <v>4.75</v>
-      </c>
-      <c r="N149">
-        <v>1.4</v>
-      </c>
-      <c r="O149">
-        <v>5</v>
-      </c>
-      <c r="P149">
-        <v>7</v>
-      </c>
-      <c r="Q149">
-        <v>-1.5</v>
-      </c>
-      <c r="R149">
-        <v>2.02</v>
-      </c>
-      <c r="S149">
-        <v>1.88</v>
-      </c>
-      <c r="T149">
-        <v>3.5</v>
-      </c>
-      <c r="U149">
-        <v>1.975</v>
-      </c>
-      <c r="V149">
-        <v>1.875</v>
-      </c>
-      <c r="W149">
-        <v>0</v>
-      </c>
-      <c r="X149">
-        <v>0</v>
-      </c>
-      <c r="Y149">
-        <v>0</v>
-      </c>
-      <c r="Z149">
-        <v>0</v>
-      </c>
-      <c r="AA149">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 14-04-2024 às 18:28
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC148"/>
+  <dimension ref="A1:AC155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -13598,7 +13598,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>7127409</v>
+        <v>7127408</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
@@ -13607,63 +13607,626 @@
         <v>28</v>
       </c>
       <c r="E148" s="2">
-        <v>45396.08333333334</v>
+        <v>45395.10416666666</v>
       </c>
       <c r="F148" t="s">
+        <v>40</v>
+      </c>
+      <c r="G148" t="s">
+        <v>37</v>
+      </c>
+      <c r="H148">
+        <v>0</v>
+      </c>
+      <c r="I148">
+        <v>2</v>
+      </c>
+      <c r="J148" t="s">
+        <v>41</v>
+      </c>
+      <c r="K148">
+        <v>3.5</v>
+      </c>
+      <c r="L148">
+        <v>3.8</v>
+      </c>
+      <c r="M148">
+        <v>1.909</v>
+      </c>
+      <c r="N148">
+        <v>3.5</v>
+      </c>
+      <c r="O148">
+        <v>4</v>
+      </c>
+      <c r="P148">
+        <v>1.95</v>
+      </c>
+      <c r="Q148">
+        <v>0.5</v>
+      </c>
+      <c r="R148">
+        <v>1.875</v>
+      </c>
+      <c r="S148">
+        <v>1.975</v>
+      </c>
+      <c r="T148">
+        <v>2.75</v>
+      </c>
+      <c r="U148">
+        <v>1.8</v>
+      </c>
+      <c r="V148">
+        <v>2.05</v>
+      </c>
+      <c r="W148">
+        <v>-1</v>
+      </c>
+      <c r="X148">
+        <v>-1</v>
+      </c>
+      <c r="Y148">
+        <v>0.95</v>
+      </c>
+      <c r="Z148">
+        <v>-1</v>
+      </c>
+      <c r="AA148">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB148">
+        <v>-1</v>
+      </c>
+      <c r="AC148">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="149" spans="1:29">
+      <c r="A149" s="1">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>7127407</v>
+      </c>
+      <c r="C149" t="s">
+        <v>28</v>
+      </c>
+      <c r="D149" t="s">
+        <v>28</v>
+      </c>
+      <c r="E149" s="2">
+        <v>45395.1875</v>
+      </c>
+      <c r="F149" t="s">
+        <v>35</v>
+      </c>
+      <c r="G149" t="s">
+        <v>39</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>2</v>
+      </c>
+      <c r="J149" t="s">
+        <v>41</v>
+      </c>
+      <c r="K149">
+        <v>2.1</v>
+      </c>
+      <c r="L149">
+        <v>3.6</v>
+      </c>
+      <c r="M149">
+        <v>3.25</v>
+      </c>
+      <c r="N149">
+        <v>1.75</v>
+      </c>
+      <c r="O149">
+        <v>4.333</v>
+      </c>
+      <c r="P149">
+        <v>4</v>
+      </c>
+      <c r="Q149">
+        <v>-0.75</v>
+      </c>
+      <c r="R149">
+        <v>1.925</v>
+      </c>
+      <c r="S149">
+        <v>1.925</v>
+      </c>
+      <c r="T149">
+        <v>3.5</v>
+      </c>
+      <c r="U149">
+        <v>2.025</v>
+      </c>
+      <c r="V149">
+        <v>1.825</v>
+      </c>
+      <c r="W149">
+        <v>-1</v>
+      </c>
+      <c r="X149">
+        <v>-1</v>
+      </c>
+      <c r="Y149">
+        <v>3</v>
+      </c>
+      <c r="Z149">
+        <v>-1</v>
+      </c>
+      <c r="AA149">
+        <v>0.925</v>
+      </c>
+      <c r="AB149">
+        <v>-1</v>
+      </c>
+      <c r="AC149">
+        <v>0.825</v>
+      </c>
+    </row>
+    <row r="150" spans="1:29">
+      <c r="A150" s="1">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>7127406</v>
+      </c>
+      <c r="C150" t="s">
+        <v>28</v>
+      </c>
+      <c r="D150" t="s">
+        <v>28</v>
+      </c>
+      <c r="E150" s="2">
+        <v>45395.28125</v>
+      </c>
+      <c r="F150" t="s">
+        <v>32</v>
+      </c>
+      <c r="G150" t="s">
+        <v>33</v>
+      </c>
+      <c r="H150">
+        <v>2</v>
+      </c>
+      <c r="I150">
+        <v>1</v>
+      </c>
+      <c r="J150" t="s">
+        <v>42</v>
+      </c>
+      <c r="K150">
+        <v>1.833</v>
+      </c>
+      <c r="L150">
+        <v>4</v>
+      </c>
+      <c r="M150">
+        <v>3.75</v>
+      </c>
+      <c r="N150">
+        <v>1.666</v>
+      </c>
+      <c r="O150">
+        <v>4.333</v>
+      </c>
+      <c r="P150">
+        <v>4.5</v>
+      </c>
+      <c r="Q150">
+        <v>-0.75</v>
+      </c>
+      <c r="R150">
+        <v>1.825</v>
+      </c>
+      <c r="S150">
+        <v>2.025</v>
+      </c>
+      <c r="T150">
+        <v>3.25</v>
+      </c>
+      <c r="U150">
+        <v>1.95</v>
+      </c>
+      <c r="V150">
+        <v>1.9</v>
+      </c>
+      <c r="W150">
+        <v>0.6659999999999999</v>
+      </c>
+      <c r="X150">
+        <v>-1</v>
+      </c>
+      <c r="Y150">
+        <v>-1</v>
+      </c>
+      <c r="Z150">
+        <v>0.4125</v>
+      </c>
+      <c r="AA150">
+        <v>-0.5</v>
+      </c>
+      <c r="AB150">
+        <v>-0.5</v>
+      </c>
+      <c r="AC150">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="151" spans="1:29">
+      <c r="A151" s="1">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>7702377</v>
+      </c>
+      <c r="C151" t="s">
+        <v>28</v>
+      </c>
+      <c r="D151" t="s">
+        <v>28</v>
+      </c>
+      <c r="E151" s="2">
+        <v>45398.25</v>
+      </c>
+      <c r="F151" t="s">
+        <v>40</v>
+      </c>
+      <c r="G151" t="s">
+        <v>30</v>
+      </c>
+      <c r="K151">
+        <v>2.4</v>
+      </c>
+      <c r="L151">
+        <v>3.75</v>
+      </c>
+      <c r="M151">
+        <v>2.5</v>
+      </c>
+      <c r="N151">
+        <v>2.5</v>
+      </c>
+      <c r="O151">
+        <v>3.75</v>
+      </c>
+      <c r="P151">
+        <v>2.5</v>
+      </c>
+      <c r="Q151">
+        <v>0</v>
+      </c>
+      <c r="R151">
+        <v>1.98</v>
+      </c>
+      <c r="S151">
+        <v>1.92</v>
+      </c>
+      <c r="T151">
+        <v>3.5</v>
+      </c>
+      <c r="U151">
+        <v>1.875</v>
+      </c>
+      <c r="V151">
+        <v>1.975</v>
+      </c>
+      <c r="W151">
+        <v>0</v>
+      </c>
+      <c r="X151">
+        <v>0</v>
+      </c>
+      <c r="Y151">
+        <v>0</v>
+      </c>
+      <c r="Z151">
+        <v>0</v>
+      </c>
+      <c r="AA151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:29">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>7127410</v>
+      </c>
+      <c r="C152" t="s">
+        <v>28</v>
+      </c>
+      <c r="D152" t="s">
+        <v>28</v>
+      </c>
+      <c r="E152" s="2">
+        <v>45401.28125</v>
+      </c>
+      <c r="F152" t="s">
+        <v>39</v>
+      </c>
+      <c r="G152" t="s">
+        <v>36</v>
+      </c>
+      <c r="K152">
+        <v>2.8</v>
+      </c>
+      <c r="L152">
+        <v>3.4</v>
+      </c>
+      <c r="M152">
+        <v>2.45</v>
+      </c>
+      <c r="N152">
+        <v>2.8</v>
+      </c>
+      <c r="O152">
+        <v>3.4</v>
+      </c>
+      <c r="P152">
+        <v>2.45</v>
+      </c>
+      <c r="Q152">
+        <v>0</v>
+      </c>
+      <c r="R152">
+        <v>2.04</v>
+      </c>
+      <c r="S152">
+        <v>1.86</v>
+      </c>
+      <c r="T152">
+        <v>2.75</v>
+      </c>
+      <c r="U152">
+        <v>1.825</v>
+      </c>
+      <c r="V152">
+        <v>2.025</v>
+      </c>
+      <c r="W152">
+        <v>0</v>
+      </c>
+      <c r="X152">
+        <v>0</v>
+      </c>
+      <c r="Y152">
+        <v>0</v>
+      </c>
+      <c r="Z152">
+        <v>0</v>
+      </c>
+      <c r="AA152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:29">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>8096897</v>
+      </c>
+      <c r="C153" t="s">
+        <v>28</v>
+      </c>
+      <c r="D153" t="s">
+        <v>28</v>
+      </c>
+      <c r="E153" s="2">
+        <v>45402.10416666666</v>
+      </c>
+      <c r="F153" t="s">
+        <v>33</v>
+      </c>
+      <c r="G153" t="s">
         <v>29</v>
       </c>
-      <c r="G148" t="s">
-        <v>34</v>
-      </c>
-      <c r="K148">
-        <v>1.571</v>
-      </c>
-      <c r="L148">
-        <v>4.5</v>
-      </c>
-      <c r="M148">
+      <c r="K153">
+        <v>3.25</v>
+      </c>
+      <c r="L153">
+        <v>3.8</v>
+      </c>
+      <c r="M153">
+        <v>2</v>
+      </c>
+      <c r="N153">
+        <v>3.25</v>
+      </c>
+      <c r="O153">
+        <v>3.8</v>
+      </c>
+      <c r="P153">
+        <v>2</v>
+      </c>
+      <c r="Q153">
+        <v>0.5</v>
+      </c>
+      <c r="R153">
+        <v>1.84</v>
+      </c>
+      <c r="S153">
+        <v>2.06</v>
+      </c>
+      <c r="T153">
+        <v>3</v>
+      </c>
+      <c r="U153">
+        <v>1.875</v>
+      </c>
+      <c r="V153">
+        <v>1.975</v>
+      </c>
+      <c r="W153">
+        <v>0</v>
+      </c>
+      <c r="X153">
+        <v>0</v>
+      </c>
+      <c r="Y153">
+        <v>0</v>
+      </c>
+      <c r="Z153">
+        <v>0</v>
+      </c>
+      <c r="AA153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:29">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>7127411</v>
+      </c>
+      <c r="C154" t="s">
+        <v>28</v>
+      </c>
+      <c r="D154" t="s">
+        <v>28</v>
+      </c>
+      <c r="E154" s="2">
+        <v>45402.1875</v>
+      </c>
+      <c r="F154" t="s">
+        <v>38</v>
+      </c>
+      <c r="G154" t="s">
+        <v>35</v>
+      </c>
+      <c r="K154">
+        <v>1.65</v>
+      </c>
+      <c r="L154">
+        <v>4</v>
+      </c>
+      <c r="M154">
         <v>4.75</v>
       </c>
-      <c r="N148">
-        <v>1.4</v>
-      </c>
-      <c r="O148">
-        <v>5</v>
-      </c>
-      <c r="P148">
-        <v>7</v>
-      </c>
-      <c r="Q148">
-        <v>-1.5</v>
-      </c>
-      <c r="R148">
-        <v>2.01</v>
-      </c>
-      <c r="S148">
-        <v>1.89</v>
-      </c>
-      <c r="T148">
+      <c r="N154">
+        <v>1.65</v>
+      </c>
+      <c r="O154">
+        <v>4</v>
+      </c>
+      <c r="P154">
+        <v>4.75</v>
+      </c>
+      <c r="Q154">
+        <v>-0.75</v>
+      </c>
+      <c r="R154">
+        <v>1.84</v>
+      </c>
+      <c r="S154">
+        <v>2.06</v>
+      </c>
+      <c r="T154">
+        <v>3</v>
+      </c>
+      <c r="U154">
+        <v>1.875</v>
+      </c>
+      <c r="V154">
+        <v>1.975</v>
+      </c>
+      <c r="W154">
+        <v>0</v>
+      </c>
+      <c r="X154">
+        <v>0</v>
+      </c>
+      <c r="Y154">
+        <v>0</v>
+      </c>
+      <c r="Z154">
+        <v>0</v>
+      </c>
+      <c r="AA154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:29">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>7127415</v>
+      </c>
+      <c r="C155" t="s">
+        <v>28</v>
+      </c>
+      <c r="D155" t="s">
+        <v>28</v>
+      </c>
+      <c r="E155" s="2">
+        <v>45402.28125</v>
+      </c>
+      <c r="F155" t="s">
+        <v>31</v>
+      </c>
+      <c r="G155" t="s">
+        <v>32</v>
+      </c>
+      <c r="K155">
+        <v>3.8</v>
+      </c>
+      <c r="L155">
+        <v>4.2</v>
+      </c>
+      <c r="M155">
+        <v>1.8</v>
+      </c>
+      <c r="N155">
+        <v>3.8</v>
+      </c>
+      <c r="O155">
+        <v>4.2</v>
+      </c>
+      <c r="P155">
+        <v>1.8</v>
+      </c>
+      <c r="Q155">
+        <v>0.75</v>
+      </c>
+      <c r="R155">
+        <v>1.92</v>
+      </c>
+      <c r="S155">
+        <v>1.98</v>
+      </c>
+      <c r="T155">
         <v>3.5</v>
       </c>
-      <c r="U148">
-        <v>1.85</v>
-      </c>
-      <c r="V148">
-        <v>2</v>
-      </c>
-      <c r="W148">
+      <c r="U155">
+        <v>1.925</v>
+      </c>
+      <c r="V155">
+        <v>1.925</v>
+      </c>
+      <c r="W155">
         <v>0</v>
       </c>
-      <c r="X148">
+      <c r="X155">
         <v>0</v>
       </c>
-      <c r="Y148">
+      <c r="Y155">
         <v>0</v>
       </c>
-      <c r="Z148">
+      <c r="Z155">
         <v>0</v>
       </c>
-      <c r="AA148">
+      <c r="AA155">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 15-04-2024 às 22:35
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC155"/>
+  <dimension ref="A1:AC156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -13865,7 +13865,7 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>7702377</v>
+        <v>7127409</v>
       </c>
       <c r="C151" t="s">
         <v>28</v>
@@ -13874,64 +13874,79 @@
         <v>28</v>
       </c>
       <c r="E151" s="2">
-        <v>45398.25</v>
+        <v>45396.08333333334</v>
       </c>
       <c r="F151" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G151" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="H151">
+        <v>8</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151" t="s">
+        <v>42</v>
       </c>
       <c r="K151">
-        <v>2.4</v>
+        <v>1.571</v>
       </c>
       <c r="L151">
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="M151">
-        <v>2.5</v>
+        <v>4.75</v>
       </c>
       <c r="N151">
-        <v>2.5</v>
+        <v>1.363</v>
       </c>
       <c r="O151">
-        <v>3.75</v>
+        <v>5.25</v>
       </c>
       <c r="P151">
-        <v>2.5</v>
+        <v>7.5</v>
       </c>
       <c r="Q151">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="R151">
-        <v>1.98</v>
+        <v>1.95</v>
       </c>
       <c r="S151">
-        <v>1.92</v>
+        <v>1.95</v>
       </c>
       <c r="T151">
         <v>3.5</v>
       </c>
       <c r="U151">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="V151">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W151">
-        <v>0</v>
+        <v>0.363</v>
       </c>
       <c r="X151">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y151">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z151">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AA151">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB151">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="AC151">
+        <v>-1</v>
       </c>
     </row>
     <row r="152" spans="1:29">
@@ -13939,7 +13954,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>7127410</v>
+        <v>7702377</v>
       </c>
       <c r="C152" t="s">
         <v>28</v>
@@ -13948,49 +13963,49 @@
         <v>28</v>
       </c>
       <c r="E152" s="2">
-        <v>45401.28125</v>
+        <v>45398.25</v>
       </c>
       <c r="F152" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G152" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="K152">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="L152">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="M152">
-        <v>2.45</v>
+        <v>2.5</v>
       </c>
       <c r="N152">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="O152">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="P152">
-        <v>2.45</v>
+        <v>2.4</v>
       </c>
       <c r="Q152">
         <v>0</v>
       </c>
       <c r="R152">
-        <v>2.04</v>
+        <v>1.99</v>
       </c>
       <c r="S152">
-        <v>1.86</v>
+        <v>1.91</v>
       </c>
       <c r="T152">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="U152">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V152">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W152">
         <v>0</v>
@@ -14013,7 +14028,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>8096897</v>
+        <v>7127410</v>
       </c>
       <c r="C153" t="s">
         <v>28</v>
@@ -14022,49 +14037,49 @@
         <v>28</v>
       </c>
       <c r="E153" s="2">
-        <v>45402.10416666666</v>
+        <v>45401.28125</v>
       </c>
       <c r="F153" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G153" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="K153">
-        <v>3.25</v>
+        <v>2.8</v>
       </c>
       <c r="L153">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M153">
-        <v>2</v>
+        <v>2.45</v>
       </c>
       <c r="N153">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="O153">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="P153">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="Q153">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R153">
-        <v>1.84</v>
+        <v>1.88</v>
       </c>
       <c r="S153">
-        <v>2.06</v>
+        <v>2.02</v>
       </c>
       <c r="T153">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U153">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="V153">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="W153">
         <v>0</v>
@@ -14087,7 +14102,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>7127411</v>
+        <v>8096897</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14096,34 +14111,34 @@
         <v>28</v>
       </c>
       <c r="E154" s="2">
-        <v>45402.1875</v>
+        <v>45402.10416666666</v>
       </c>
       <c r="F154" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G154" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K154">
-        <v>1.65</v>
+        <v>3.25</v>
       </c>
       <c r="L154">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="M154">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="N154">
-        <v>1.65</v>
+        <v>3.25</v>
       </c>
       <c r="O154">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P154">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="Q154">
-        <v>-0.75</v>
+        <v>0.5</v>
       </c>
       <c r="R154">
         <v>1.84</v>
@@ -14161,7 +14176,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>7127415</v>
+        <v>7127411</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -14170,49 +14185,49 @@
         <v>28</v>
       </c>
       <c r="E155" s="2">
-        <v>45402.28125</v>
+        <v>45402.1875</v>
       </c>
       <c r="F155" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G155" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K155">
-        <v>3.8</v>
+        <v>1.65</v>
       </c>
       <c r="L155">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="M155">
-        <v>1.8</v>
+        <v>4.75</v>
       </c>
       <c r="N155">
-        <v>3.8</v>
+        <v>1.65</v>
       </c>
       <c r="O155">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="P155">
-        <v>1.8</v>
+        <v>4.75</v>
       </c>
       <c r="Q155">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R155">
-        <v>1.92</v>
+        <v>1.84</v>
       </c>
       <c r="S155">
-        <v>1.98</v>
+        <v>2.06</v>
       </c>
       <c r="T155">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U155">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V155">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14227,6 +14242,80 @@
         <v>0</v>
       </c>
       <c r="AA155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:29">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>7127415</v>
+      </c>
+      <c r="C156" t="s">
+        <v>28</v>
+      </c>
+      <c r="D156" t="s">
+        <v>28</v>
+      </c>
+      <c r="E156" s="2">
+        <v>45402.28125</v>
+      </c>
+      <c r="F156" t="s">
+        <v>31</v>
+      </c>
+      <c r="G156" t="s">
+        <v>32</v>
+      </c>
+      <c r="K156">
+        <v>3.8</v>
+      </c>
+      <c r="L156">
+        <v>4.2</v>
+      </c>
+      <c r="M156">
+        <v>1.8</v>
+      </c>
+      <c r="N156">
+        <v>4.2</v>
+      </c>
+      <c r="O156">
+        <v>4.2</v>
+      </c>
+      <c r="P156">
+        <v>1.727</v>
+      </c>
+      <c r="Q156">
+        <v>0.75</v>
+      </c>
+      <c r="R156">
+        <v>1.95</v>
+      </c>
+      <c r="S156">
+        <v>1.95</v>
+      </c>
+      <c r="T156">
+        <v>3.5</v>
+      </c>
+      <c r="U156">
+        <v>1.925</v>
+      </c>
+      <c r="V156">
+        <v>1.925</v>
+      </c>
+      <c r="W156">
+        <v>0</v>
+      </c>
+      <c r="X156">
+        <v>0</v>
+      </c>
+      <c r="Y156">
+        <v>0</v>
+      </c>
+      <c r="Z156">
+        <v>0</v>
+      </c>
+      <c r="AA156">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 18-04-2024 às 00:36
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC156"/>
+  <dimension ref="A1:AC158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -13971,6 +13971,15 @@
       <c r="G152" t="s">
         <v>30</v>
       </c>
+      <c r="H152">
+        <v>3</v>
+      </c>
+      <c r="I152">
+        <v>3</v>
+      </c>
+      <c r="J152" t="s">
+        <v>43</v>
+      </c>
       <c r="K152">
         <v>2.4</v>
       </c>
@@ -13981,46 +13990,52 @@
         <v>2.5</v>
       </c>
       <c r="N152">
-        <v>2.5</v>
+        <v>2.625</v>
       </c>
       <c r="O152">
         <v>4.2</v>
       </c>
       <c r="P152">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="Q152">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R152">
-        <v>1.99</v>
+        <v>1.8</v>
       </c>
       <c r="S152">
-        <v>1.91</v>
+        <v>2.05</v>
       </c>
       <c r="T152">
         <v>3.5</v>
       </c>
       <c r="U152">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="V152">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="W152">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X152">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="Y152">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z152">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AA152">
-        <v>0</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AB152">
+        <v>0.925</v>
+      </c>
+      <c r="AC152">
+        <v>-1</v>
       </c>
     </row>
     <row r="153" spans="1:29">
@@ -14055,10 +14070,10 @@
         <v>2.45</v>
       </c>
       <c r="N153">
-        <v>3</v>
+        <v>2.9</v>
       </c>
       <c r="O153">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P153">
         <v>2.25</v>
@@ -14067,19 +14082,19 @@
         <v>0.25</v>
       </c>
       <c r="R153">
-        <v>1.88</v>
+        <v>1.86</v>
       </c>
       <c r="S153">
-        <v>2.02</v>
+        <v>2.04</v>
       </c>
       <c r="T153">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U153">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="V153">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="W153">
         <v>0</v>
@@ -14129,22 +14144,22 @@
         <v>2</v>
       </c>
       <c r="N154">
-        <v>3.25</v>
+        <v>3.2</v>
       </c>
       <c r="O154">
         <v>3.8</v>
       </c>
       <c r="P154">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="Q154">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R154">
-        <v>1.84</v>
+        <v>2.03</v>
       </c>
       <c r="S154">
-        <v>2.06</v>
+        <v>1.87</v>
       </c>
       <c r="T154">
         <v>3</v>
@@ -14206,7 +14221,7 @@
         <v>1.65</v>
       </c>
       <c r="O155">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="P155">
         <v>4.75</v>
@@ -14215,19 +14230,19 @@
         <v>-0.75</v>
       </c>
       <c r="R155">
-        <v>1.84</v>
+        <v>1.83</v>
       </c>
       <c r="S155">
-        <v>2.06</v>
+        <v>2.07</v>
       </c>
       <c r="T155">
         <v>3</v>
       </c>
       <c r="U155">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="V155">
-        <v>1.975</v>
+        <v>2.05</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14283,16 +14298,16 @@
         <v>4.2</v>
       </c>
       <c r="P156">
-        <v>1.727</v>
+        <v>1.7</v>
       </c>
       <c r="Q156">
         <v>0.75</v>
       </c>
       <c r="R156">
-        <v>1.95</v>
+        <v>1.98</v>
       </c>
       <c r="S156">
-        <v>1.95</v>
+        <v>1.92</v>
       </c>
       <c r="T156">
         <v>3.5</v>
@@ -14316,6 +14331,154 @@
         <v>0</v>
       </c>
       <c r="AA156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:29">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>7127413</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" t="s">
+        <v>28</v>
+      </c>
+      <c r="E157" s="2">
+        <v>45403.08333333334</v>
+      </c>
+      <c r="F157" t="s">
+        <v>37</v>
+      </c>
+      <c r="G157" t="s">
+        <v>30</v>
+      </c>
+      <c r="K157">
+        <v>1.75</v>
+      </c>
+      <c r="L157">
+        <v>4</v>
+      </c>
+      <c r="M157">
+        <v>4</v>
+      </c>
+      <c r="N157">
+        <v>1.8</v>
+      </c>
+      <c r="O157">
+        <v>4</v>
+      </c>
+      <c r="P157">
+        <v>3.8</v>
+      </c>
+      <c r="Q157">
+        <v>-0.75</v>
+      </c>
+      <c r="R157">
+        <v>2.06</v>
+      </c>
+      <c r="S157">
+        <v>1.84</v>
+      </c>
+      <c r="T157">
+        <v>3.25</v>
+      </c>
+      <c r="U157">
+        <v>1.925</v>
+      </c>
+      <c r="V157">
+        <v>1.925</v>
+      </c>
+      <c r="W157">
+        <v>0</v>
+      </c>
+      <c r="X157">
+        <v>0</v>
+      </c>
+      <c r="Y157">
+        <v>0</v>
+      </c>
+      <c r="Z157">
+        <v>0</v>
+      </c>
+      <c r="AA157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:29">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>7127414</v>
+      </c>
+      <c r="C158" t="s">
+        <v>28</v>
+      </c>
+      <c r="D158" t="s">
+        <v>28</v>
+      </c>
+      <c r="E158" s="2">
+        <v>45403.16666666666</v>
+      </c>
+      <c r="F158" t="s">
+        <v>34</v>
+      </c>
+      <c r="G158" t="s">
+        <v>40</v>
+      </c>
+      <c r="K158">
+        <v>2.4</v>
+      </c>
+      <c r="L158">
+        <v>3.6</v>
+      </c>
+      <c r="M158">
+        <v>2.625</v>
+      </c>
+      <c r="N158">
+        <v>2.375</v>
+      </c>
+      <c r="O158">
+        <v>3.6</v>
+      </c>
+      <c r="P158">
+        <v>2.625</v>
+      </c>
+      <c r="Q158">
+        <v>0</v>
+      </c>
+      <c r="R158">
+        <v>1.82</v>
+      </c>
+      <c r="S158">
+        <v>2.08</v>
+      </c>
+      <c r="T158">
+        <v>3.25</v>
+      </c>
+      <c r="U158">
+        <v>1.9</v>
+      </c>
+      <c r="V158">
+        <v>1.95</v>
+      </c>
+      <c r="W158">
+        <v>0</v>
+      </c>
+      <c r="X158">
+        <v>0</v>
+      </c>
+      <c r="Y158">
+        <v>0</v>
+      </c>
+      <c r="Z158">
+        <v>0</v>
+      </c>
+      <c r="AA158">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 19-04-2024 às 00:38
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC158"/>
+  <dimension ref="A1:AC157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC104">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P105">
+        <v>3.25</v>
+      </c>
+      <c r="Q105">
+        <v>-0.25</v>
+      </c>
+      <c r="R105">
+        <v>1.86</v>
+      </c>
+      <c r="S105">
+        <v>2.04</v>
+      </c>
+      <c r="T105">
         <v>2.75</v>
       </c>
-      <c r="Q105">
-        <v>0</v>
-      </c>
-      <c r="R105">
-        <v>1.8</v>
-      </c>
-      <c r="S105">
-        <v>2.05</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
       <c r="U105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -14070,31 +14070,31 @@
         <v>2.45</v>
       </c>
       <c r="N153">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="O153">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="P153">
-        <v>2.25</v>
+        <v>2.15</v>
       </c>
       <c r="Q153">
         <v>0.25</v>
       </c>
       <c r="R153">
-        <v>1.86</v>
+        <v>1.9</v>
       </c>
       <c r="S153">
-        <v>2.04</v>
+        <v>2</v>
       </c>
       <c r="T153">
         <v>3</v>
       </c>
       <c r="U153">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V153">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W153">
         <v>0</v>
@@ -14156,19 +14156,19 @@
         <v>0.25</v>
       </c>
       <c r="R154">
-        <v>2.03</v>
+        <v>2.04</v>
       </c>
       <c r="S154">
-        <v>1.87</v>
+        <v>1.86</v>
       </c>
       <c r="T154">
         <v>3</v>
       </c>
       <c r="U154">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="V154">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="W154">
         <v>0</v>
@@ -14239,10 +14239,10 @@
         <v>3</v>
       </c>
       <c r="U155">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V155">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14304,19 +14304,19 @@
         <v>0.75</v>
       </c>
       <c r="R156">
-        <v>1.98</v>
+        <v>2.02</v>
       </c>
       <c r="S156">
-        <v>1.92</v>
+        <v>1.88</v>
       </c>
       <c r="T156">
         <v>3.5</v>
       </c>
       <c r="U156">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V156">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W156">
         <v>0</v>
@@ -14339,7 +14339,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>7127413</v>
+        <v>7127414</v>
       </c>
       <c r="C157" t="s">
         <v>28</v>
@@ -14348,49 +14348,49 @@
         <v>28</v>
       </c>
       <c r="E157" s="2">
-        <v>45403.08333333334</v>
+        <v>45403.16666666666</v>
       </c>
       <c r="F157" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G157" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="K157">
-        <v>1.75</v>
+        <v>2.4</v>
       </c>
       <c r="L157">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M157">
-        <v>4</v>
+        <v>2.625</v>
       </c>
       <c r="N157">
-        <v>1.8</v>
+        <v>2.3</v>
       </c>
       <c r="O157">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="P157">
-        <v>3.8</v>
+        <v>2.6</v>
       </c>
       <c r="Q157">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="R157">
-        <v>2.06</v>
+        <v>1.83</v>
       </c>
       <c r="S157">
-        <v>1.84</v>
+        <v>2.07</v>
       </c>
       <c r="T157">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="U157">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V157">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W157">
         <v>0</v>
@@ -14405,80 +14405,6 @@
         <v>0</v>
       </c>
       <c r="AA157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:29">
-      <c r="A158" s="1">
-        <v>156</v>
-      </c>
-      <c r="B158">
-        <v>7127414</v>
-      </c>
-      <c r="C158" t="s">
-        <v>28</v>
-      </c>
-      <c r="D158" t="s">
-        <v>28</v>
-      </c>
-      <c r="E158" s="2">
-        <v>45403.16666666666</v>
-      </c>
-      <c r="F158" t="s">
-        <v>34</v>
-      </c>
-      <c r="G158" t="s">
-        <v>40</v>
-      </c>
-      <c r="K158">
-        <v>2.4</v>
-      </c>
-      <c r="L158">
-        <v>3.6</v>
-      </c>
-      <c r="M158">
-        <v>2.625</v>
-      </c>
-      <c r="N158">
-        <v>2.375</v>
-      </c>
-      <c r="O158">
-        <v>3.6</v>
-      </c>
-      <c r="P158">
-        <v>2.625</v>
-      </c>
-      <c r="Q158">
-        <v>0</v>
-      </c>
-      <c r="R158">
-        <v>1.82</v>
-      </c>
-      <c r="S158">
-        <v>2.08</v>
-      </c>
-      <c r="T158">
-        <v>3.25</v>
-      </c>
-      <c r="U158">
-        <v>1.9</v>
-      </c>
-      <c r="V158">
-        <v>1.95</v>
-      </c>
-      <c r="W158">
-        <v>0</v>
-      </c>
-      <c r="X158">
-        <v>0</v>
-      </c>
-      <c r="Y158">
-        <v>0</v>
-      </c>
-      <c r="Z158">
-        <v>0</v>
-      </c>
-      <c r="AA158">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 19-04-2024 às 21:40
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC157"/>
+  <dimension ref="A1:AC156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -14043,7 +14043,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>7127410</v>
+        <v>8096897</v>
       </c>
       <c r="C153" t="s">
         <v>28</v>
@@ -14052,49 +14052,49 @@
         <v>28</v>
       </c>
       <c r="E153" s="2">
-        <v>45401.28125</v>
+        <v>45402.10416666666</v>
       </c>
       <c r="F153" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G153" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="K153">
-        <v>2.8</v>
+        <v>3.25</v>
       </c>
       <c r="L153">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M153">
-        <v>2.45</v>
+        <v>2</v>
       </c>
       <c r="N153">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="O153">
         <v>4</v>
       </c>
       <c r="P153">
-        <v>2.15</v>
+        <v>2</v>
       </c>
       <c r="Q153">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R153">
-        <v>1.9</v>
+        <v>1.87</v>
       </c>
       <c r="S153">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="T153">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U153">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V153">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W153">
         <v>0</v>
@@ -14117,7 +14117,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>8096897</v>
+        <v>7127411</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14126,49 +14126,49 @@
         <v>28</v>
       </c>
       <c r="E154" s="2">
-        <v>45402.10416666666</v>
+        <v>45402.1875</v>
       </c>
       <c r="F154" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G154" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K154">
+        <v>1.65</v>
+      </c>
+      <c r="L154">
+        <v>4</v>
+      </c>
+      <c r="M154">
+        <v>4.75</v>
+      </c>
+      <c r="N154">
+        <v>1.6</v>
+      </c>
+      <c r="O154">
+        <v>4.333</v>
+      </c>
+      <c r="P154">
+        <v>5</v>
+      </c>
+      <c r="Q154">
+        <v>-1</v>
+      </c>
+      <c r="R154">
+        <v>2.05</v>
+      </c>
+      <c r="S154">
+        <v>1.85</v>
+      </c>
+      <c r="T154">
         <v>3.25</v>
       </c>
-      <c r="L154">
-        <v>3.8</v>
-      </c>
-      <c r="M154">
-        <v>2</v>
-      </c>
-      <c r="N154">
-        <v>3.2</v>
-      </c>
-      <c r="O154">
-        <v>3.8</v>
-      </c>
-      <c r="P154">
-        <v>2.1</v>
-      </c>
-      <c r="Q154">
-        <v>0.25</v>
-      </c>
-      <c r="R154">
-        <v>2.04</v>
-      </c>
-      <c r="S154">
-        <v>1.86</v>
-      </c>
-      <c r="T154">
-        <v>3</v>
-      </c>
       <c r="U154">
-        <v>1.825</v>
+        <v>2.05</v>
       </c>
       <c r="V154">
-        <v>2.025</v>
+        <v>1.8</v>
       </c>
       <c r="W154">
         <v>0</v>
@@ -14191,7 +14191,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>7127411</v>
+        <v>7127415</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -14200,49 +14200,49 @@
         <v>28</v>
       </c>
       <c r="E155" s="2">
-        <v>45402.1875</v>
+        <v>45402.28125</v>
       </c>
       <c r="F155" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G155" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K155">
-        <v>1.65</v>
+        <v>3.8</v>
       </c>
       <c r="L155">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="M155">
-        <v>4.75</v>
+        <v>1.8</v>
       </c>
       <c r="N155">
-        <v>1.65</v>
+        <v>4.333</v>
       </c>
       <c r="O155">
         <v>4.2</v>
       </c>
       <c r="P155">
-        <v>4.75</v>
+        <v>1.666</v>
       </c>
       <c r="Q155">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="R155">
-        <v>1.83</v>
+        <v>2.02</v>
       </c>
       <c r="S155">
-        <v>2.07</v>
+        <v>1.88</v>
       </c>
       <c r="T155">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U155">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V155">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14265,7 +14265,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>7127415</v>
+        <v>7127414</v>
       </c>
       <c r="C156" t="s">
         <v>28</v>
@@ -14274,49 +14274,49 @@
         <v>28</v>
       </c>
       <c r="E156" s="2">
-        <v>45402.28125</v>
+        <v>45403.16666666666</v>
       </c>
       <c r="F156" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G156" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="K156">
-        <v>3.8</v>
+        <v>2.4</v>
       </c>
       <c r="L156">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="M156">
-        <v>1.8</v>
+        <v>2.625</v>
       </c>
       <c r="N156">
-        <v>4.2</v>
+        <v>2.4</v>
       </c>
       <c r="O156">
-        <v>4.2</v>
+        <v>3.75</v>
       </c>
       <c r="P156">
-        <v>1.7</v>
+        <v>2.7</v>
       </c>
       <c r="Q156">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="R156">
-        <v>2.02</v>
+        <v>1.84</v>
       </c>
       <c r="S156">
-        <v>1.88</v>
+        <v>2.06</v>
       </c>
       <c r="T156">
         <v>3.5</v>
       </c>
       <c r="U156">
+        <v>1.975</v>
+      </c>
+      <c r="V156">
         <v>1.875</v>
-      </c>
-      <c r="V156">
-        <v>1.975</v>
       </c>
       <c r="W156">
         <v>0</v>
@@ -14331,80 +14331,6 @@
         <v>0</v>
       </c>
       <c r="AA156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:29">
-      <c r="A157" s="1">
-        <v>155</v>
-      </c>
-      <c r="B157">
-        <v>7127414</v>
-      </c>
-      <c r="C157" t="s">
-        <v>28</v>
-      </c>
-      <c r="D157" t="s">
-        <v>28</v>
-      </c>
-      <c r="E157" s="2">
-        <v>45403.16666666666</v>
-      </c>
-      <c r="F157" t="s">
-        <v>34</v>
-      </c>
-      <c r="G157" t="s">
-        <v>40</v>
-      </c>
-      <c r="K157">
-        <v>2.4</v>
-      </c>
-      <c r="L157">
-        <v>3.6</v>
-      </c>
-      <c r="M157">
-        <v>2.625</v>
-      </c>
-      <c r="N157">
-        <v>2.3</v>
-      </c>
-      <c r="O157">
-        <v>3.75</v>
-      </c>
-      <c r="P157">
-        <v>2.6</v>
-      </c>
-      <c r="Q157">
-        <v>0</v>
-      </c>
-      <c r="R157">
-        <v>1.83</v>
-      </c>
-      <c r="S157">
-        <v>2.07</v>
-      </c>
-      <c r="T157">
-        <v>3.5</v>
-      </c>
-      <c r="U157">
-        <v>1.95</v>
-      </c>
-      <c r="V157">
-        <v>1.9</v>
-      </c>
-      <c r="W157">
-        <v>0</v>
-      </c>
-      <c r="X157">
-        <v>0</v>
-      </c>
-      <c r="Y157">
-        <v>0</v>
-      </c>
-      <c r="Z157">
-        <v>0</v>
-      </c>
-      <c r="AA157">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 19-04-2024 às 23:27
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC156"/>
+  <dimension ref="A1:AC157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G73" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
+        <v>2</v>
+      </c>
+      <c r="J73" t="s">
+        <v>42</v>
+      </c>
+      <c r="K73">
+        <v>1.909</v>
+      </c>
+      <c r="L73">
         <v>4</v>
       </c>
-      <c r="J73" t="s">
-        <v>41</v>
-      </c>
-      <c r="K73">
-        <v>2.45</v>
-      </c>
-      <c r="L73">
-        <v>3.75</v>
-      </c>
       <c r="M73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J74" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G112" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
+        <v>4.2</v>
+      </c>
+      <c r="P113">
         <v>3.6</v>
-      </c>
-      <c r="P113">
-        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
+        <v>1.89</v>
+      </c>
+      <c r="S113">
+        <v>2.01</v>
+      </c>
+      <c r="T113">
+        <v>3.5</v>
+      </c>
+      <c r="U113">
+        <v>1.95</v>
+      </c>
+      <c r="V113">
         <v>1.9</v>
       </c>
-      <c r="S113">
-        <v>1.95</v>
-      </c>
-      <c r="T113">
-        <v>2.75</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
+        <v>1.01</v>
+      </c>
+      <c r="AB113">
         <v>0.95</v>
       </c>
-      <c r="AB113">
-        <v>-1</v>
-      </c>
       <c r="AC113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>1.533</v>
+      </c>
+      <c r="O124">
+        <v>5.25</v>
+      </c>
+      <c r="P124">
+        <v>5</v>
+      </c>
+      <c r="Q124">
+        <v>-1</v>
+      </c>
+      <c r="R124">
+        <v>1.8</v>
+      </c>
+      <c r="S124">
+        <v>2.05</v>
+      </c>
+      <c r="T124">
         <v>3.5</v>
       </c>
-      <c r="M124">
-        <v>2.75</v>
-      </c>
-      <c r="N124">
-        <v>3.4</v>
-      </c>
-      <c r="O124">
-        <v>3.75</v>
-      </c>
-      <c r="P124">
-        <v>2.05</v>
-      </c>
-      <c r="Q124">
-        <v>0.25</v>
-      </c>
-      <c r="R124">
-        <v>2.025</v>
-      </c>
-      <c r="S124">
-        <v>1.825</v>
-      </c>
-      <c r="T124">
-        <v>3</v>
-      </c>
       <c r="U124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
         <v>1.05</v>
       </c>
-      <c r="Z124">
-        <v>-1</v>
-      </c>
-      <c r="AA124">
-        <v>0.825</v>
-      </c>
       <c r="AB124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC124">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R125">
+        <v>2.025</v>
+      </c>
+      <c r="S125">
+        <v>1.825</v>
+      </c>
+      <c r="T125">
+        <v>3</v>
+      </c>
+      <c r="U125">
+        <v>2.05</v>
+      </c>
+      <c r="V125">
         <v>1.8</v>
       </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>3.5</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC125">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -14043,7 +14043,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>8096897</v>
+        <v>7127410</v>
       </c>
       <c r="C153" t="s">
         <v>28</v>
@@ -14052,64 +14052,79 @@
         <v>28</v>
       </c>
       <c r="E153" s="2">
-        <v>45402.10416666666</v>
+        <v>45401.28125</v>
       </c>
       <c r="F153" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G153" t="s">
-        <v>29</v>
+        <v>36</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+      <c r="I153">
+        <v>1</v>
+      </c>
+      <c r="J153" t="s">
+        <v>43</v>
       </c>
       <c r="K153">
-        <v>3.25</v>
+        <v>2.8</v>
       </c>
       <c r="L153">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M153">
-        <v>2</v>
+        <v>2.45</v>
       </c>
       <c r="N153">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="O153">
         <v>4</v>
       </c>
       <c r="P153">
-        <v>2</v>
+        <v>2.15</v>
       </c>
       <c r="Q153">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R153">
-        <v>1.87</v>
+        <v>1.925</v>
       </c>
       <c r="S153">
-        <v>2.03</v>
+        <v>1.925</v>
       </c>
       <c r="T153">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U153">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V153">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W153">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X153">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y153">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z153">
-        <v>0</v>
+        <v>0.4625</v>
       </c>
       <c r="AA153">
-        <v>0</v>
+        <v>-0.5</v>
+      </c>
+      <c r="AB153">
+        <v>-1</v>
+      </c>
+      <c r="AC153">
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="154" spans="1:29">
@@ -14117,7 +14132,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>7127411</v>
+        <v>8096897</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14126,49 +14141,49 @@
         <v>28</v>
       </c>
       <c r="E154" s="2">
-        <v>45402.1875</v>
+        <v>45402.10416666666</v>
       </c>
       <c r="F154" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G154" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K154">
-        <v>1.65</v>
+        <v>3.25</v>
       </c>
       <c r="L154">
+        <v>3.8</v>
+      </c>
+      <c r="M154">
+        <v>2</v>
+      </c>
+      <c r="N154">
+        <v>3.3</v>
+      </c>
+      <c r="O154">
         <v>4</v>
       </c>
-      <c r="M154">
-        <v>4.75</v>
-      </c>
-      <c r="N154">
-        <v>1.6</v>
-      </c>
-      <c r="O154">
-        <v>4.333</v>
-      </c>
       <c r="P154">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q154">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="R154">
-        <v>2.05</v>
+        <v>1.87</v>
       </c>
       <c r="S154">
-        <v>1.85</v>
+        <v>2.03</v>
       </c>
       <c r="T154">
         <v>3.25</v>
       </c>
       <c r="U154">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="V154">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="W154">
         <v>0</v>
@@ -14191,7 +14206,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>7127415</v>
+        <v>7127411</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -14200,49 +14215,49 @@
         <v>28</v>
       </c>
       <c r="E155" s="2">
-        <v>45402.28125</v>
+        <v>45402.1875</v>
       </c>
       <c r="F155" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G155" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K155">
-        <v>3.8</v>
+        <v>1.65</v>
       </c>
       <c r="L155">
-        <v>4.2</v>
+        <v>4</v>
       </c>
       <c r="M155">
+        <v>4.75</v>
+      </c>
+      <c r="N155">
+        <v>1.6</v>
+      </c>
+      <c r="O155">
+        <v>4.333</v>
+      </c>
+      <c r="P155">
+        <v>5</v>
+      </c>
+      <c r="Q155">
+        <v>-1</v>
+      </c>
+      <c r="R155">
+        <v>2.04</v>
+      </c>
+      <c r="S155">
+        <v>1.86</v>
+      </c>
+      <c r="T155">
+        <v>3.25</v>
+      </c>
+      <c r="U155">
+        <v>2.05</v>
+      </c>
+      <c r="V155">
         <v>1.8</v>
-      </c>
-      <c r="N155">
-        <v>4.333</v>
-      </c>
-      <c r="O155">
-        <v>4.2</v>
-      </c>
-      <c r="P155">
-        <v>1.666</v>
-      </c>
-      <c r="Q155">
-        <v>0.75</v>
-      </c>
-      <c r="R155">
-        <v>2.02</v>
-      </c>
-      <c r="S155">
-        <v>1.88</v>
-      </c>
-      <c r="T155">
-        <v>3.5</v>
-      </c>
-      <c r="U155">
-        <v>1.925</v>
-      </c>
-      <c r="V155">
-        <v>1.925</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14265,7 +14280,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>7127414</v>
+        <v>7127415</v>
       </c>
       <c r="C156" t="s">
         <v>28</v>
@@ -14274,49 +14289,49 @@
         <v>28</v>
       </c>
       <c r="E156" s="2">
-        <v>45403.16666666666</v>
+        <v>45402.28125</v>
       </c>
       <c r="F156" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G156" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="K156">
-        <v>2.4</v>
+        <v>3.8</v>
       </c>
       <c r="L156">
-        <v>3.6</v>
+        <v>4.2</v>
       </c>
       <c r="M156">
-        <v>2.625</v>
+        <v>1.8</v>
       </c>
       <c r="N156">
-        <v>2.4</v>
+        <v>4.333</v>
       </c>
       <c r="O156">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="P156">
-        <v>2.7</v>
+        <v>1.666</v>
       </c>
       <c r="Q156">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="R156">
-        <v>1.84</v>
+        <v>2.02</v>
       </c>
       <c r="S156">
-        <v>2.06</v>
+        <v>1.88</v>
       </c>
       <c r="T156">
         <v>3.5</v>
       </c>
       <c r="U156">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V156">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W156">
         <v>0</v>
@@ -14331,6 +14346,80 @@
         <v>0</v>
       </c>
       <c r="AA156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:29">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>7127414</v>
+      </c>
+      <c r="C157" t="s">
+        <v>28</v>
+      </c>
+      <c r="D157" t="s">
+        <v>28</v>
+      </c>
+      <c r="E157" s="2">
+        <v>45403.16666666666</v>
+      </c>
+      <c r="F157" t="s">
+        <v>34</v>
+      </c>
+      <c r="G157" t="s">
+        <v>40</v>
+      </c>
+      <c r="K157">
+        <v>2.4</v>
+      </c>
+      <c r="L157">
+        <v>3.6</v>
+      </c>
+      <c r="M157">
+        <v>2.625</v>
+      </c>
+      <c r="N157">
+        <v>2.4</v>
+      </c>
+      <c r="O157">
+        <v>3.75</v>
+      </c>
+      <c r="P157">
+        <v>2.7</v>
+      </c>
+      <c r="Q157">
+        <v>0</v>
+      </c>
+      <c r="R157">
+        <v>1.84</v>
+      </c>
+      <c r="S157">
+        <v>2.06</v>
+      </c>
+      <c r="T157">
+        <v>3.5</v>
+      </c>
+      <c r="U157">
+        <v>1.975</v>
+      </c>
+      <c r="V157">
+        <v>1.875</v>
+      </c>
+      <c r="W157">
+        <v>0</v>
+      </c>
+      <c r="X157">
+        <v>0</v>
+      </c>
+      <c r="Y157">
+        <v>0</v>
+      </c>
+      <c r="Z157">
+        <v>0</v>
+      </c>
+      <c r="AA157">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 21-04-2024 às 13:33
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC157"/>
+  <dimension ref="A1:AC159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6923,7 +6923,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>28</v>
@@ -6935,73 +6935,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H73">
         <v>3</v>
       </c>
       <c r="I73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="L73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="M73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="N73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="O73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="P73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="Q73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="S73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="T73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="X73">
         <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AC73">
         <v>-1</v>
@@ -7012,7 +7012,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>28</v>
@@ -7024,73 +7024,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="F74" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H74">
         <v>3</v>
       </c>
       <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74">
+        <v>1.909</v>
+      </c>
+      <c r="L74">
         <v>4</v>
       </c>
-      <c r="J74" t="s">
-        <v>41</v>
-      </c>
-      <c r="K74">
-        <v>2.45</v>
-      </c>
-      <c r="L74">
-        <v>3.75</v>
-      </c>
       <c r="M74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="N74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="O74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="Q74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="R74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="S74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="T74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="X74">
         <v>-1</v>
       </c>
       <c r="Y74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC74">
         <v>-1</v>
@@ -9682,7 +9682,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9694,76 +9694,76 @@
         <v>45340.125</v>
       </c>
       <c r="F104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>1</v>
       </c>
       <c r="I104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="L104">
         <v>3.75</v>
       </c>
       <c r="M104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="N104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="O104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P104">
+        <v>3.25</v>
+      </c>
+      <c r="Q104">
+        <v>-0.25</v>
+      </c>
+      <c r="R104">
+        <v>1.86</v>
+      </c>
+      <c r="S104">
+        <v>2.04</v>
+      </c>
+      <c r="T104">
         <v>2.75</v>
       </c>
-      <c r="Q104">
-        <v>0</v>
-      </c>
-      <c r="R104">
-        <v>1.8</v>
-      </c>
-      <c r="S104">
-        <v>2.05</v>
-      </c>
-      <c r="T104">
-        <v>3</v>
-      </c>
       <c r="U104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="W104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X104">
         <v>-1</v>
       </c>
       <c r="Y104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AA104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>-0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:29">
@@ -9771,7 +9771,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9783,76 +9783,76 @@
         <v>45340.125</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H105">
         <v>1</v>
       </c>
       <c r="I105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="L105">
         <v>3.75</v>
       </c>
       <c r="M105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="N105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="O105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="Q105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="S105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="T105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="W105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X105">
         <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Z105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC105">
-        <v>0.875</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="106" spans="1:29">
@@ -11462,7 +11462,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11474,76 +11474,76 @@
         <v>45361.125</v>
       </c>
       <c r="F124" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G124" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J124" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="N124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="O124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="P124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="Q124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="R124">
+        <v>2.025</v>
+      </c>
+      <c r="S124">
+        <v>1.825</v>
+      </c>
+      <c r="T124">
+        <v>3</v>
+      </c>
+      <c r="U124">
+        <v>2.05</v>
+      </c>
+      <c r="V124">
         <v>1.8</v>
       </c>
-      <c r="S124">
-        <v>2.05</v>
-      </c>
-      <c r="T124">
-        <v>3.5</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
       <c r="W124">
         <v>-1</v>
       </c>
       <c r="X124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Z124">
         <v>-1</v>
       </c>
       <c r="AA124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AB124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC124">
-        <v>0.925</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="125" spans="1:29">
@@ -11551,7 +11551,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11563,76 +11563,76 @@
         <v>45361.125</v>
       </c>
       <c r="F125" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>1.533</v>
+      </c>
+      <c r="O125">
+        <v>5.25</v>
+      </c>
+      <c r="P125">
+        <v>5</v>
+      </c>
+      <c r="Q125">
+        <v>-1</v>
+      </c>
+      <c r="R125">
+        <v>1.8</v>
+      </c>
+      <c r="S125">
+        <v>2.05</v>
+      </c>
+      <c r="T125">
         <v>3.5</v>
       </c>
-      <c r="M125">
-        <v>2.75</v>
-      </c>
-      <c r="N125">
-        <v>3.4</v>
-      </c>
-      <c r="O125">
-        <v>3.75</v>
-      </c>
-      <c r="P125">
-        <v>2.05</v>
-      </c>
-      <c r="Q125">
-        <v>0.25</v>
-      </c>
-      <c r="R125">
-        <v>2.025</v>
-      </c>
-      <c r="S125">
-        <v>1.825</v>
-      </c>
-      <c r="T125">
-        <v>3</v>
-      </c>
       <c r="U125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
         <v>1.05</v>
       </c>
-      <c r="Z125">
-        <v>-1</v>
-      </c>
-      <c r="AA125">
-        <v>0.825</v>
-      </c>
       <c r="AB125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -14132,7 +14132,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>8096897</v>
+        <v>7127416</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14141,49 +14141,49 @@
         <v>28</v>
       </c>
       <c r="E154" s="2">
-        <v>45402.10416666666</v>
+        <v>45408.28125</v>
       </c>
       <c r="F154" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G154" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K154">
-        <v>3.25</v>
+        <v>2.3</v>
       </c>
       <c r="L154">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="M154">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="N154">
-        <v>3.3</v>
+        <v>2.1</v>
       </c>
       <c r="O154">
         <v>4</v>
       </c>
       <c r="P154">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="Q154">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R154">
-        <v>1.87</v>
+        <v>1.97</v>
       </c>
       <c r="S154">
-        <v>2.03</v>
+        <v>1.93</v>
       </c>
       <c r="T154">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="U154">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V154">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W154">
         <v>0</v>
@@ -14206,7 +14206,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>7127411</v>
+        <v>7127418</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -14215,49 +14215,49 @@
         <v>28</v>
       </c>
       <c r="E155" s="2">
-        <v>45402.1875</v>
+        <v>45409.17708333334</v>
       </c>
       <c r="F155" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G155" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K155">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L155">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="M155">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="N155">
-        <v>1.6</v>
+        <v>3.8</v>
       </c>
       <c r="O155">
-        <v>4.333</v>
+        <v>3.3</v>
       </c>
       <c r="P155">
-        <v>5</v>
+        <v>1.909</v>
       </c>
       <c r="Q155">
-        <v>-1</v>
+        <v>0.5</v>
       </c>
       <c r="R155">
-        <v>2.04</v>
+        <v>1.93</v>
       </c>
       <c r="S155">
-        <v>1.86</v>
+        <v>1.97</v>
       </c>
       <c r="T155">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U155">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="V155">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="W155">
         <v>0</v>
@@ -14280,7 +14280,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>7127415</v>
+        <v>7127419</v>
       </c>
       <c r="C156" t="s">
         <v>28</v>
@@ -14289,49 +14289,49 @@
         <v>28</v>
       </c>
       <c r="E156" s="2">
-        <v>45402.28125</v>
+        <v>45409.17708333334</v>
       </c>
       <c r="F156" t="s">
+        <v>36</v>
+      </c>
+      <c r="G156" t="s">
         <v>31</v>
       </c>
-      <c r="G156" t="s">
-        <v>32</v>
-      </c>
       <c r="K156">
-        <v>3.8</v>
+        <v>1.85</v>
       </c>
       <c r="L156">
+        <v>3.5</v>
+      </c>
+      <c r="M156">
+        <v>3.9</v>
+      </c>
+      <c r="N156">
+        <v>1.75</v>
+      </c>
+      <c r="O156">
+        <v>3.6</v>
+      </c>
+      <c r="P156">
         <v>4.2</v>
       </c>
-      <c r="M156">
-        <v>1.8</v>
-      </c>
-      <c r="N156">
-        <v>4.333</v>
-      </c>
-      <c r="O156">
-        <v>4.2</v>
-      </c>
-      <c r="P156">
-        <v>1.666</v>
-      </c>
       <c r="Q156">
-        <v>0.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R156">
-        <v>2.02</v>
+        <v>2.03</v>
       </c>
       <c r="S156">
-        <v>1.88</v>
+        <v>1.87</v>
       </c>
       <c r="T156">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U156">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V156">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W156">
         <v>0</v>
@@ -14354,7 +14354,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>7127414</v>
+        <v>7127417</v>
       </c>
       <c r="C157" t="s">
         <v>28</v>
@@ -14363,49 +14363,49 @@
         <v>28</v>
       </c>
       <c r="E157" s="2">
-        <v>45403.16666666666</v>
+        <v>45409.28125</v>
       </c>
       <c r="F157" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G157" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K157">
-        <v>2.4</v>
+        <v>2.05</v>
       </c>
       <c r="L157">
-        <v>3.6</v>
+        <v>3.3</v>
       </c>
       <c r="M157">
-        <v>2.625</v>
+        <v>3.4</v>
       </c>
       <c r="N157">
-        <v>2.4</v>
+        <v>1.833</v>
       </c>
       <c r="O157">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="P157">
-        <v>2.7</v>
+        <v>4</v>
       </c>
       <c r="Q157">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="R157">
-        <v>1.84</v>
+        <v>1.86</v>
       </c>
       <c r="S157">
-        <v>2.06</v>
+        <v>2.04</v>
       </c>
       <c r="T157">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U157">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V157">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W157">
         <v>0</v>
@@ -14420,6 +14420,154 @@
         <v>0</v>
       </c>
       <c r="AA157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:29">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>8109525</v>
+      </c>
+      <c r="C158" t="s">
+        <v>28</v>
+      </c>
+      <c r="D158" t="s">
+        <v>28</v>
+      </c>
+      <c r="E158" s="2">
+        <v>45410.08333333334</v>
+      </c>
+      <c r="F158" t="s">
+        <v>32</v>
+      </c>
+      <c r="G158" t="s">
+        <v>34</v>
+      </c>
+      <c r="K158">
+        <v>1.5</v>
+      </c>
+      <c r="L158">
+        <v>3.6</v>
+      </c>
+      <c r="M158">
+        <v>7</v>
+      </c>
+      <c r="N158">
+        <v>1.444</v>
+      </c>
+      <c r="O158">
+        <v>4</v>
+      </c>
+      <c r="P158">
+        <v>7.5</v>
+      </c>
+      <c r="Q158">
+        <v>-1.25</v>
+      </c>
+      <c r="R158">
+        <v>1.9</v>
+      </c>
+      <c r="S158">
+        <v>2</v>
+      </c>
+      <c r="T158">
+        <v>3.5</v>
+      </c>
+      <c r="U158">
+        <v>1.875</v>
+      </c>
+      <c r="V158">
+        <v>1.975</v>
+      </c>
+      <c r="W158">
+        <v>0</v>
+      </c>
+      <c r="X158">
+        <v>0</v>
+      </c>
+      <c r="Y158">
+        <v>0</v>
+      </c>
+      <c r="Z158">
+        <v>0</v>
+      </c>
+      <c r="AA158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:29">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>7127421</v>
+      </c>
+      <c r="C159" t="s">
+        <v>28</v>
+      </c>
+      <c r="D159" t="s">
+        <v>28</v>
+      </c>
+      <c r="E159" s="2">
+        <v>45410.16666666666</v>
+      </c>
+      <c r="F159" t="s">
+        <v>29</v>
+      </c>
+      <c r="G159" t="s">
+        <v>40</v>
+      </c>
+      <c r="K159">
+        <v>1.65</v>
+      </c>
+      <c r="L159">
+        <v>4</v>
+      </c>
+      <c r="M159">
+        <v>4.333</v>
+      </c>
+      <c r="N159">
+        <v>1.4</v>
+      </c>
+      <c r="O159">
+        <v>4.2</v>
+      </c>
+      <c r="P159">
+        <v>7</v>
+      </c>
+      <c r="Q159">
+        <v>-1.25</v>
+      </c>
+      <c r="R159">
+        <v>1.89</v>
+      </c>
+      <c r="S159">
+        <v>2.01</v>
+      </c>
+      <c r="T159">
+        <v>3.5</v>
+      </c>
+      <c r="U159">
+        <v>2.025</v>
+      </c>
+      <c r="V159">
+        <v>1.825</v>
+      </c>
+      <c r="W159">
+        <v>0</v>
+      </c>
+      <c r="X159">
+        <v>0</v>
+      </c>
+      <c r="Y159">
+        <v>0</v>
+      </c>
+      <c r="Z159">
+        <v>0</v>
+      </c>
+      <c r="AA159">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 21-04-2024 às 14:32
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -507,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC159"/>
+  <dimension ref="A1:AC163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10394,7 +10394,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10406,76 +10406,76 @@
         <v>45347.125</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K112">
         <v>1.95</v>
       </c>
       <c r="L112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="N112">
         <v>1.909</v>
       </c>
       <c r="O112">
+        <v>4.2</v>
+      </c>
+      <c r="P112">
         <v>3.6</v>
-      </c>
-      <c r="P112">
-        <v>4</v>
       </c>
       <c r="Q112">
         <v>-0.5</v>
       </c>
       <c r="R112">
+        <v>1.89</v>
+      </c>
+      <c r="S112">
+        <v>2.01</v>
+      </c>
+      <c r="T112">
+        <v>3.5</v>
+      </c>
+      <c r="U112">
+        <v>1.95</v>
+      </c>
+      <c r="V112">
         <v>1.9</v>
       </c>
-      <c r="S112">
-        <v>1.95</v>
-      </c>
-      <c r="T112">
-        <v>2.75</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
       <c r="W112">
         <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
         <v>-1</v>
       </c>
       <c r="AA112">
+        <v>1.01</v>
+      </c>
+      <c r="AB112">
         <v>0.95</v>
       </c>
-      <c r="AB112">
-        <v>-1</v>
-      </c>
       <c r="AC112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:29">
@@ -10483,7 +10483,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10495,76 +10495,76 @@
         <v>45347.125</v>
       </c>
       <c r="F113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K113">
         <v>1.95</v>
       </c>
       <c r="L113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="M113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="N113">
         <v>1.909</v>
       </c>
       <c r="O113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="P113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="Q113">
         <v>-0.5</v>
       </c>
       <c r="R113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="T113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
         <v>-1</v>
       </c>
       <c r="X113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Z113">
         <v>-1</v>
       </c>
       <c r="AA113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AB113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:29">
@@ -14132,7 +14132,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>7127416</v>
+        <v>8096897</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14141,64 +14141,79 @@
         <v>28</v>
       </c>
       <c r="E154" s="2">
-        <v>45408.28125</v>
+        <v>45402.10416666666</v>
       </c>
       <c r="F154" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G154" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+      <c r="I154">
+        <v>2</v>
+      </c>
+      <c r="J154" t="s">
+        <v>41</v>
       </c>
       <c r="K154">
-        <v>2.3</v>
+        <v>3.25</v>
       </c>
       <c r="L154">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="M154">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="N154">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="O154">
         <v>4</v>
       </c>
       <c r="P154">
-        <v>2.75</v>
+        <v>1.95</v>
       </c>
       <c r="Q154">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R154">
-        <v>1.97</v>
+        <v>1.95</v>
       </c>
       <c r="S154">
-        <v>1.93</v>
+        <v>1.95</v>
       </c>
       <c r="T154">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="U154">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V154">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W154">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X154">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y154">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Z154">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA154">
-        <v>0</v>
+        <v>0.95</v>
+      </c>
+      <c r="AB154">
+        <v>-0.5</v>
+      </c>
+      <c r="AC154">
+        <v>0.4625</v>
       </c>
     </row>
     <row r="155" spans="1:29">
@@ -14206,7 +14221,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>7127418</v>
+        <v>7127411</v>
       </c>
       <c r="C155" t="s">
         <v>28</v>
@@ -14215,64 +14230,79 @@
         <v>28</v>
       </c>
       <c r="E155" s="2">
-        <v>45409.17708333334</v>
+        <v>45402.1875</v>
       </c>
       <c r="F155" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G155" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155" t="s">
+        <v>43</v>
       </c>
       <c r="K155">
-        <v>3.6</v>
+        <v>1.65</v>
       </c>
       <c r="L155">
-        <v>3.25</v>
+        <v>4</v>
       </c>
       <c r="M155">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="N155">
-        <v>3.8</v>
+        <v>1.666</v>
       </c>
       <c r="O155">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="P155">
-        <v>1.909</v>
+        <v>4.5</v>
       </c>
       <c r="Q155">
-        <v>0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R155">
-        <v>1.93</v>
+        <v>1.875</v>
       </c>
       <c r="S155">
-        <v>1.97</v>
+        <v>1.975</v>
       </c>
       <c r="T155">
         <v>3</v>
       </c>
       <c r="U155">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V155">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W155">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X155">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="Y155">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z155">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA155">
-        <v>0</v>
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB155">
+        <v>-1</v>
+      </c>
+      <c r="AC155">
+        <v>1.025</v>
       </c>
     </row>
     <row r="156" spans="1:29">
@@ -14280,7 +14310,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>7127419</v>
+        <v>7127415</v>
       </c>
       <c r="C156" t="s">
         <v>28</v>
@@ -14289,64 +14319,79 @@
         <v>28</v>
       </c>
       <c r="E156" s="2">
-        <v>45409.17708333334</v>
+        <v>45402.28125</v>
       </c>
       <c r="F156" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G156" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="H156">
+        <v>1</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156" t="s">
+        <v>42</v>
       </c>
       <c r="K156">
-        <v>1.85</v>
+        <v>3.8</v>
       </c>
       <c r="L156">
+        <v>4.2</v>
+      </c>
+      <c r="M156">
+        <v>1.8</v>
+      </c>
+      <c r="N156">
+        <v>4.333</v>
+      </c>
+      <c r="O156">
+        <v>4.5</v>
+      </c>
+      <c r="P156">
+        <v>1.666</v>
+      </c>
+      <c r="Q156">
+        <v>0.75</v>
+      </c>
+      <c r="R156">
+        <v>2.02</v>
+      </c>
+      <c r="S156">
+        <v>1.88</v>
+      </c>
+      <c r="T156">
         <v>3.5</v>
       </c>
-      <c r="M156">
-        <v>3.9</v>
-      </c>
-      <c r="N156">
-        <v>1.75</v>
-      </c>
-      <c r="O156">
-        <v>3.6</v>
-      </c>
-      <c r="P156">
-        <v>4.2</v>
-      </c>
-      <c r="Q156">
-        <v>-0.75</v>
-      </c>
-      <c r="R156">
-        <v>2.03</v>
-      </c>
-      <c r="S156">
-        <v>1.87</v>
-      </c>
-      <c r="T156">
-        <v>3</v>
-      </c>
       <c r="U156">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V156">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W156">
-        <v>0</v>
+        <v>3.333</v>
       </c>
       <c r="X156">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y156">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Z156">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="AA156">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="AB156">
+        <v>-1</v>
+      </c>
+      <c r="AC156">
+        <v>0.925</v>
       </c>
     </row>
     <row r="157" spans="1:29">
@@ -14354,7 +14399,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>7127417</v>
+        <v>7127414</v>
       </c>
       <c r="C157" t="s">
         <v>28</v>
@@ -14363,64 +14408,79 @@
         <v>28</v>
       </c>
       <c r="E157" s="2">
-        <v>45409.28125</v>
+        <v>45403.16666666666</v>
       </c>
       <c r="F157" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G157" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="H157">
+        <v>3</v>
+      </c>
+      <c r="I157">
+        <v>4</v>
+      </c>
+      <c r="J157" t="s">
+        <v>41</v>
       </c>
       <c r="K157">
-        <v>2.05</v>
+        <v>2.4</v>
       </c>
       <c r="L157">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="M157">
-        <v>3.4</v>
+        <v>2.625</v>
       </c>
       <c r="N157">
-        <v>1.833</v>
+        <v>2.3</v>
       </c>
       <c r="O157">
+        <v>3.75</v>
+      </c>
+      <c r="P157">
+        <v>2.875</v>
+      </c>
+      <c r="Q157">
+        <v>-0.25</v>
+      </c>
+      <c r="R157">
+        <v>2.04</v>
+      </c>
+      <c r="S157">
+        <v>1.86</v>
+      </c>
+      <c r="T157">
         <v>3.5</v>
       </c>
-      <c r="P157">
-        <v>4</v>
-      </c>
-      <c r="Q157">
-        <v>-0.5</v>
-      </c>
-      <c r="R157">
-        <v>1.86</v>
-      </c>
-      <c r="S157">
-        <v>2.04</v>
-      </c>
-      <c r="T157">
-        <v>3</v>
-      </c>
       <c r="U157">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V157">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W157">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X157">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y157">
-        <v>0</v>
+        <v>1.875</v>
       </c>
       <c r="Z157">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA157">
-        <v>0</v>
+        <v>0.8600000000000001</v>
+      </c>
+      <c r="AB157">
+        <v>1</v>
+      </c>
+      <c r="AC157">
+        <v>-1</v>
       </c>
     </row>
     <row r="158" spans="1:29">
@@ -14428,7 +14488,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>8109525</v>
+        <v>7127416</v>
       </c>
       <c r="C158" t="s">
         <v>28</v>
@@ -14437,49 +14497,49 @@
         <v>28</v>
       </c>
       <c r="E158" s="2">
-        <v>45410.08333333334</v>
+        <v>45408.28125</v>
       </c>
       <c r="F158" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G158" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="K158">
-        <v>1.5</v>
+        <v>2.3</v>
       </c>
       <c r="L158">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M158">
-        <v>7</v>
+        <v>2.5</v>
       </c>
       <c r="N158">
-        <v>1.444</v>
+        <v>2.1</v>
       </c>
       <c r="O158">
         <v>4</v>
       </c>
       <c r="P158">
-        <v>7.5</v>
+        <v>2.75</v>
       </c>
       <c r="Q158">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R158">
-        <v>1.9</v>
+        <v>1.97</v>
       </c>
       <c r="S158">
-        <v>2</v>
+        <v>1.93</v>
       </c>
       <c r="T158">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="U158">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V158">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="W158">
         <v>0</v>
@@ -14502,7 +14562,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127421</v>
+        <v>7127418</v>
       </c>
       <c r="C159" t="s">
         <v>28</v>
@@ -14511,49 +14571,49 @@
         <v>28</v>
       </c>
       <c r="E159" s="2">
-        <v>45410.16666666666</v>
+        <v>45409.17708333334</v>
       </c>
       <c r="F159" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K159">
-        <v>1.65</v>
+        <v>3.6</v>
       </c>
       <c r="L159">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="M159">
-        <v>4.333</v>
+        <v>2</v>
       </c>
       <c r="N159">
-        <v>1.4</v>
+        <v>3.8</v>
       </c>
       <c r="O159">
-        <v>4.2</v>
+        <v>3.3</v>
       </c>
       <c r="P159">
-        <v>7</v>
+        <v>1.909</v>
       </c>
       <c r="Q159">
-        <v>-1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R159">
-        <v>1.89</v>
+        <v>1.93</v>
       </c>
       <c r="S159">
-        <v>2.01</v>
+        <v>1.97</v>
       </c>
       <c r="T159">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="U159">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V159">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W159">
         <v>0</v>
@@ -14568,6 +14628,302 @@
         <v>0</v>
       </c>
       <c r="AA159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:29">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>7127419</v>
+      </c>
+      <c r="C160" t="s">
+        <v>28</v>
+      </c>
+      <c r="D160" t="s">
+        <v>28</v>
+      </c>
+      <c r="E160" s="2">
+        <v>45409.17708333334</v>
+      </c>
+      <c r="F160" t="s">
+        <v>36</v>
+      </c>
+      <c r="G160" t="s">
+        <v>31</v>
+      </c>
+      <c r="K160">
+        <v>1.85</v>
+      </c>
+      <c r="L160">
+        <v>3.5</v>
+      </c>
+      <c r="M160">
+        <v>3.9</v>
+      </c>
+      <c r="N160">
+        <v>1.75</v>
+      </c>
+      <c r="O160">
+        <v>3.6</v>
+      </c>
+      <c r="P160">
+        <v>4.2</v>
+      </c>
+      <c r="Q160">
+        <v>-0.75</v>
+      </c>
+      <c r="R160">
+        <v>2.03</v>
+      </c>
+      <c r="S160">
+        <v>1.87</v>
+      </c>
+      <c r="T160">
+        <v>3</v>
+      </c>
+      <c r="U160">
+        <v>1.875</v>
+      </c>
+      <c r="V160">
+        <v>1.975</v>
+      </c>
+      <c r="W160">
+        <v>0</v>
+      </c>
+      <c r="X160">
+        <v>0</v>
+      </c>
+      <c r="Y160">
+        <v>0</v>
+      </c>
+      <c r="Z160">
+        <v>0</v>
+      </c>
+      <c r="AA160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:27">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>7127417</v>
+      </c>
+      <c r="C161" t="s">
+        <v>28</v>
+      </c>
+      <c r="D161" t="s">
+        <v>28</v>
+      </c>
+      <c r="E161" s="2">
+        <v>45409.28125</v>
+      </c>
+      <c r="F161" t="s">
+        <v>38</v>
+      </c>
+      <c r="G161" t="s">
+        <v>33</v>
+      </c>
+      <c r="K161">
+        <v>2.05</v>
+      </c>
+      <c r="L161">
+        <v>3.3</v>
+      </c>
+      <c r="M161">
+        <v>3.4</v>
+      </c>
+      <c r="N161">
+        <v>1.833</v>
+      </c>
+      <c r="O161">
+        <v>3.5</v>
+      </c>
+      <c r="P161">
+        <v>4</v>
+      </c>
+      <c r="Q161">
+        <v>-0.5</v>
+      </c>
+      <c r="R161">
+        <v>1.86</v>
+      </c>
+      <c r="S161">
+        <v>2.04</v>
+      </c>
+      <c r="T161">
+        <v>3</v>
+      </c>
+      <c r="U161">
+        <v>1.925</v>
+      </c>
+      <c r="V161">
+        <v>1.925</v>
+      </c>
+      <c r="W161">
+        <v>0</v>
+      </c>
+      <c r="X161">
+        <v>0</v>
+      </c>
+      <c r="Y161">
+        <v>0</v>
+      </c>
+      <c r="Z161">
+        <v>0</v>
+      </c>
+      <c r="AA161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:27">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>8109525</v>
+      </c>
+      <c r="C162" t="s">
+        <v>28</v>
+      </c>
+      <c r="D162" t="s">
+        <v>28</v>
+      </c>
+      <c r="E162" s="2">
+        <v>45410.08333333334</v>
+      </c>
+      <c r="F162" t="s">
+        <v>32</v>
+      </c>
+      <c r="G162" t="s">
+        <v>34</v>
+      </c>
+      <c r="K162">
+        <v>1.5</v>
+      </c>
+      <c r="L162">
+        <v>3.6</v>
+      </c>
+      <c r="M162">
+        <v>7</v>
+      </c>
+      <c r="N162">
+        <v>1.444</v>
+      </c>
+      <c r="O162">
+        <v>4</v>
+      </c>
+      <c r="P162">
+        <v>7.5</v>
+      </c>
+      <c r="Q162">
+        <v>-1.25</v>
+      </c>
+      <c r="R162">
+        <v>1.9</v>
+      </c>
+      <c r="S162">
+        <v>2</v>
+      </c>
+      <c r="T162">
+        <v>3.5</v>
+      </c>
+      <c r="U162">
+        <v>1.875</v>
+      </c>
+      <c r="V162">
+        <v>1.975</v>
+      </c>
+      <c r="W162">
+        <v>0</v>
+      </c>
+      <c r="X162">
+        <v>0</v>
+      </c>
+      <c r="Y162">
+        <v>0</v>
+      </c>
+      <c r="Z162">
+        <v>0</v>
+      </c>
+      <c r="AA162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:27">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>7127421</v>
+      </c>
+      <c r="C163" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163" t="s">
+        <v>28</v>
+      </c>
+      <c r="E163" s="2">
+        <v>45410.16666666666</v>
+      </c>
+      <c r="F163" t="s">
+        <v>29</v>
+      </c>
+      <c r="G163" t="s">
+        <v>40</v>
+      </c>
+      <c r="K163">
+        <v>1.65</v>
+      </c>
+      <c r="L163">
+        <v>4</v>
+      </c>
+      <c r="M163">
+        <v>4.333</v>
+      </c>
+      <c r="N163">
+        <v>1.4</v>
+      </c>
+      <c r="O163">
+        <v>4.2</v>
+      </c>
+      <c r="P163">
+        <v>7</v>
+      </c>
+      <c r="Q163">
+        <v>-1.25</v>
+      </c>
+      <c r="R163">
+        <v>1.89</v>
+      </c>
+      <c r="S163">
+        <v>2.01</v>
+      </c>
+      <c r="T163">
+        <v>3.5</v>
+      </c>
+      <c r="U163">
+        <v>2.025</v>
+      </c>
+      <c r="V163">
+        <v>1.825</v>
+      </c>
+      <c r="W163">
+        <v>0</v>
+      </c>
+      <c r="X163">
+        <v>0</v>
+      </c>
+      <c r="Y163">
+        <v>0</v>
+      </c>
+      <c r="Z163">
+        <v>0</v>
+      </c>
+      <c r="AA163">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 25-04-2024 às 21:26
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -6722,7 +6722,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>33</v>
@@ -6731,73 +6731,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F73" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>47</v>
+      </c>
+      <c r="J73">
+        <v>1.909</v>
+      </c>
+      <c r="K73">
         <v>4</v>
       </c>
-      <c r="I73" t="s">
-        <v>46</v>
-      </c>
-      <c r="J73">
-        <v>2.45</v>
-      </c>
-      <c r="K73">
-        <v>3.75</v>
-      </c>
       <c r="L73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="M73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="N73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="P73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="R73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="S73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="Z73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB73">
         <v>-1</v>
@@ -6808,7 +6808,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>33</v>
@@ -6817,73 +6817,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F74" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="K74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="L74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="M74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="N74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="P74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="R74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="S74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB74">
         <v>-1</v>
@@ -10076,7 +10076,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>33</v>
@@ -10085,76 +10085,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F112" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10162,7 +10162,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>33</v>
@@ -10171,76 +10171,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F113" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
+        <v>4.2</v>
+      </c>
+      <c r="O113">
         <v>3.6</v>
-      </c>
-      <c r="O113">
-        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
+        <v>1.89</v>
+      </c>
+      <c r="R113">
+        <v>2.01</v>
+      </c>
+      <c r="S113">
+        <v>3.5</v>
+      </c>
+      <c r="T113">
+        <v>1.95</v>
+      </c>
+      <c r="U113">
         <v>1.9</v>
       </c>
-      <c r="R113">
-        <v>1.95</v>
-      </c>
-      <c r="S113">
-        <v>2.75</v>
-      </c>
-      <c r="T113">
-        <v>1.925</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
+        <v>1.01</v>
+      </c>
+      <c r="AA113">
         <v>0.95</v>
       </c>
-      <c r="AA113">
-        <v>-1</v>
-      </c>
       <c r="AB113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -14056,31 +14056,31 @@
         <v>2.5</v>
       </c>
       <c r="M158">
-        <v>2.2</v>
+        <v>2.1</v>
       </c>
       <c r="N158">
         <v>4</v>
       </c>
       <c r="O158">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="P158">
         <v>-0.25</v>
       </c>
       <c r="Q158">
-        <v>1.97</v>
+        <v>1.9</v>
       </c>
       <c r="R158">
-        <v>1.93</v>
+        <v>2</v>
       </c>
       <c r="S158">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="T158">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="U158">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V158">
         <v>0</v>
@@ -14121,31 +14121,31 @@
         <v>2</v>
       </c>
       <c r="M159">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="N159">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O159">
-        <v>1.909</v>
+        <v>1.85</v>
       </c>
       <c r="P159">
         <v>0.5</v>
       </c>
       <c r="Q159">
-        <v>1.99</v>
+        <v>2.02</v>
       </c>
       <c r="R159">
-        <v>1.91</v>
+        <v>1.88</v>
       </c>
       <c r="S159">
         <v>3</v>
       </c>
       <c r="T159">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="U159">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V159">
         <v>0</v>
@@ -14186,31 +14186,31 @@
         <v>3.9</v>
       </c>
       <c r="M160">
-        <v>1.7</v>
+        <v>1.666</v>
       </c>
       <c r="N160">
-        <v>3.8</v>
+        <v>4.333</v>
       </c>
       <c r="O160">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="P160">
         <v>-0.75</v>
       </c>
       <c r="Q160">
-        <v>1.9</v>
+        <v>1.88</v>
       </c>
       <c r="R160">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="S160">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T160">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="U160">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="V160">
         <v>0</v>
@@ -14251,31 +14251,31 @@
         <v>3.4</v>
       </c>
       <c r="M161">
-        <v>1.909</v>
+        <v>1.8</v>
       </c>
       <c r="N161">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
       <c r="O161">
-        <v>4</v>
+        <v>4.2</v>
       </c>
       <c r="P161">
         <v>-0.5</v>
       </c>
       <c r="Q161">
-        <v>1.91</v>
+        <v>1.87</v>
       </c>
       <c r="R161">
-        <v>1.99</v>
+        <v>2.03</v>
       </c>
       <c r="S161">
         <v>3</v>
       </c>
       <c r="T161">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U161">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V161">
         <v>0</v>
@@ -14319,28 +14319,28 @@
         <v>1.4</v>
       </c>
       <c r="N162">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="O162">
-        <v>7.5</v>
+        <v>7</v>
       </c>
       <c r="P162">
         <v>-1.5</v>
       </c>
       <c r="Q162">
-        <v>2.06</v>
+        <v>1.99</v>
       </c>
       <c r="R162">
-        <v>1.84</v>
+        <v>1.91</v>
       </c>
       <c r="S162">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="T162">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U162">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="V162">
         <v>0</v>
@@ -14384,10 +14384,10 @@
         <v>1.444</v>
       </c>
       <c r="N163">
-        <v>4.5</v>
+        <v>5.25</v>
       </c>
       <c r="O163">
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="P163">
         <v>-1.25</v>
@@ -14402,10 +14402,10 @@
         <v>3.5</v>
       </c>
       <c r="T163">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="U163">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="V163">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 27-04-2024 às 11:27
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -510,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB160"/>
+  <dimension ref="A1:AB162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6710,7 +6710,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -6719,73 +6719,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>43</v>
+      </c>
+      <c r="J73">
+        <v>1.909</v>
+      </c>
+      <c r="K73">
         <v>4</v>
       </c>
-      <c r="I73" t="s">
-        <v>42</v>
-      </c>
-      <c r="J73">
-        <v>2.45</v>
-      </c>
-      <c r="K73">
-        <v>3.75</v>
-      </c>
       <c r="L73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="M73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="N73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="P73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="R73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="S73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="Z73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB73">
         <v>-1</v>
@@ -6796,7 +6796,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -6805,73 +6805,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="K74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="L74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="M74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="N74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="P74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="R74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="S74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB74">
         <v>-1</v>
@@ -14105,129 +14105,301 @@
       <c r="A159" s="1">
         <v>157</v>
       </c>
-      <c r="B159" t="s">
-        <v>27</v>
+      <c r="B159">
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
       </c>
       <c r="D159" s="2">
-        <v>45410.08333333334</v>
+        <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F159" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="G159">
+        <v>3</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159" t="s">
+        <v>43</v>
       </c>
       <c r="J159">
-        <v>1.5</v>
+        <v>1.85</v>
       </c>
       <c r="K159">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="L159">
-        <v>7</v>
+        <v>3.9</v>
       </c>
       <c r="M159">
-        <v>1.333</v>
+        <v>1.55</v>
       </c>
       <c r="N159">
-        <v>5.75</v>
+        <v>4.5</v>
       </c>
       <c r="O159">
-        <v>7.5</v>
+        <v>5.25</v>
       </c>
       <c r="P159">
-        <v>-1.75</v>
+        <v>-1</v>
       </c>
       <c r="Q159">
-        <v>2.05</v>
+        <v>1.89</v>
       </c>
       <c r="R159">
-        <v>1.85</v>
+        <v>2.01</v>
       </c>
       <c r="S159">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="T159">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="U159">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="V159">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="W159">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X159">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="Y159">
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="Z159">
+        <v>-1</v>
+      </c>
+      <c r="AA159">
+        <v>-1</v>
+      </c>
+      <c r="AB159">
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:28">
       <c r="A160" s="1">
         <v>158</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160">
+        <v>7127418</v>
+      </c>
+      <c r="C160" t="s">
+        <v>29</v>
+      </c>
+      <c r="D160" s="2">
+        <v>45409.17708333334</v>
+      </c>
+      <c r="E160" t="s">
+        <v>40</v>
+      </c>
+      <c r="F160" t="s">
+        <v>38</v>
+      </c>
+      <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
+        <v>3</v>
+      </c>
+      <c r="I160" t="s">
+        <v>42</v>
+      </c>
+      <c r="J160">
+        <v>3.6</v>
+      </c>
+      <c r="K160">
+        <v>3.25</v>
+      </c>
+      <c r="L160">
+        <v>2</v>
+      </c>
+      <c r="M160">
+        <v>4.2</v>
+      </c>
+      <c r="N160">
+        <v>4</v>
+      </c>
+      <c r="O160">
+        <v>1.75</v>
+      </c>
+      <c r="P160">
+        <v>0.75</v>
+      </c>
+      <c r="Q160">
+        <v>1.85</v>
+      </c>
+      <c r="R160">
+        <v>2</v>
+      </c>
+      <c r="S160">
+        <v>3</v>
+      </c>
+      <c r="T160">
+        <v>1.975</v>
+      </c>
+      <c r="U160">
+        <v>1.875</v>
+      </c>
+      <c r="V160">
+        <v>-1</v>
+      </c>
+      <c r="W160">
+        <v>-1</v>
+      </c>
+      <c r="X160">
+        <v>0.75</v>
+      </c>
+      <c r="Y160">
+        <v>-1</v>
+      </c>
+      <c r="Z160">
+        <v>1</v>
+      </c>
+      <c r="AA160">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB160">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:24">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="B161" t="s">
+        <v>27</v>
+      </c>
+      <c r="C161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D161" s="2">
+        <v>45410.08333333334</v>
+      </c>
+      <c r="E161" t="s">
+        <v>33</v>
+      </c>
+      <c r="F161" t="s">
+        <v>35</v>
+      </c>
+      <c r="J161">
+        <v>1.5</v>
+      </c>
+      <c r="K161">
+        <v>3.6</v>
+      </c>
+      <c r="L161">
+        <v>7</v>
+      </c>
+      <c r="M161">
+        <v>1.333</v>
+      </c>
+      <c r="N161">
+        <v>5.75</v>
+      </c>
+      <c r="O161">
+        <v>7.5</v>
+      </c>
+      <c r="P161">
+        <v>-1.5</v>
+      </c>
+      <c r="Q161">
+        <v>1.85</v>
+      </c>
+      <c r="R161">
+        <v>2.05</v>
+      </c>
+      <c r="S161">
+        <v>3.75</v>
+      </c>
+      <c r="T161">
+        <v>1.85</v>
+      </c>
+      <c r="U161">
+        <v>2</v>
+      </c>
+      <c r="V161">
+        <v>0</v>
+      </c>
+      <c r="W161">
+        <v>0</v>
+      </c>
+      <c r="X161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="B162" t="s">
         <v>28</v>
       </c>
-      <c r="C160" t="s">
-        <v>29</v>
-      </c>
-      <c r="D160" s="2">
+      <c r="C162" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162" s="2">
         <v>45410.16666666666</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E162" t="s">
         <v>30</v>
       </c>
-      <c r="F160" t="s">
+      <c r="F162" t="s">
         <v>41</v>
       </c>
-      <c r="J160">
+      <c r="J162">
         <v>1.65</v>
       </c>
-      <c r="K160">
+      <c r="K162">
         <v>4</v>
       </c>
-      <c r="L160">
+      <c r="L162">
         <v>4.333</v>
       </c>
-      <c r="M160">
-        <v>1.444</v>
-      </c>
-      <c r="N160">
-        <v>5.25</v>
-      </c>
-      <c r="O160">
-        <v>6</v>
-      </c>
-      <c r="P160">
-        <v>-1.25</v>
-      </c>
-      <c r="Q160">
-        <v>1.9</v>
-      </c>
-      <c r="R160">
-        <v>2</v>
-      </c>
-      <c r="S160">
+      <c r="M162">
+        <v>1.363</v>
+      </c>
+      <c r="N162">
+        <v>5.75</v>
+      </c>
+      <c r="O162">
+        <v>7</v>
+      </c>
+      <c r="P162">
+        <v>-1.5</v>
+      </c>
+      <c r="Q162">
+        <v>2.02</v>
+      </c>
+      <c r="R162">
+        <v>1.88</v>
+      </c>
+      <c r="S162">
         <v>3.5</v>
       </c>
-      <c r="T160">
-        <v>1.925</v>
-      </c>
-      <c r="U160">
-        <v>1.925</v>
-      </c>
-      <c r="V160">
+      <c r="T162">
+        <v>1.85</v>
+      </c>
+      <c r="U162">
+        <v>2</v>
+      </c>
+      <c r="V162">
         <v>0</v>
       </c>
-      <c r="W160">
+      <c r="W162">
         <v>0</v>
       </c>
-      <c r="X160">
+      <c r="X162">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 07-05-2024 às 13:23
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -97,10 +97,10 @@
     <t>PL_AhUnder</t>
   </si>
   <si>
-    <t>8155621</t>
+    <t>8182788</t>
   </si>
   <si>
-    <t>8158306</t>
+    <t>8182787</t>
   </si>
   <si>
     <t>Australia ALeague</t>
@@ -510,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB165"/>
+  <dimension ref="A1:AB168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -10064,7 +10064,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10073,76 +10073,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10150,7 +10150,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10159,76 +10159,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
+        <v>4.2</v>
+      </c>
+      <c r="O113">
         <v>3.6</v>
-      </c>
-      <c r="O113">
-        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
+        <v>1.89</v>
+      </c>
+      <c r="R113">
+        <v>2.01</v>
+      </c>
+      <c r="S113">
+        <v>3.5</v>
+      </c>
+      <c r="T113">
+        <v>1.95</v>
+      </c>
+      <c r="U113">
         <v>1.9</v>
       </c>
-      <c r="R113">
-        <v>1.95</v>
-      </c>
-      <c r="S113">
-        <v>2.75</v>
-      </c>
-      <c r="T113">
-        <v>1.925</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
+        <v>1.01</v>
+      </c>
+      <c r="AA113">
         <v>0.95</v>
       </c>
-      <c r="AA113">
-        <v>-1</v>
-      </c>
       <c r="AB113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -14535,129 +14535,387 @@
       <c r="A164" s="1">
         <v>162</v>
       </c>
-      <c r="B164" t="s">
-        <v>27</v>
+      <c r="B164">
+        <v>8135264</v>
       </c>
       <c r="C164" t="s">
         <v>29</v>
       </c>
       <c r="D164" s="2">
-        <v>45416.28125</v>
+        <v>45413.25</v>
       </c>
       <c r="E164" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F164" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G164">
+        <v>2</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+      <c r="I164" t="s">
+        <v>43</v>
       </c>
       <c r="J164">
-        <v>1.909</v>
+        <v>1.666</v>
       </c>
       <c r="K164">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="L164">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M164">
-        <v>1.444</v>
+        <v>1.666</v>
       </c>
       <c r="N164">
-        <v>5</v>
+        <v>4.2</v>
       </c>
       <c r="O164">
-        <v>6.5</v>
+        <v>4.5</v>
       </c>
       <c r="P164">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="Q164">
-        <v>1.87</v>
+        <v>1.85</v>
       </c>
       <c r="R164">
-        <v>2.03</v>
+        <v>2</v>
       </c>
       <c r="S164">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="T164">
+        <v>1.975</v>
+      </c>
+      <c r="U164">
         <v>1.875</v>
       </c>
-      <c r="U164">
-        <v>1.975</v>
-      </c>
       <c r="V164">
-        <v>0</v>
+        <v>0.6659999999999999</v>
       </c>
       <c r="W164">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X164">
-        <v>0</v>
+        <v>-1</v>
+      </c>
+      <c r="Y164">
+        <v>0.8500000000000001</v>
+      </c>
+      <c r="Z164">
+        <v>-1</v>
+      </c>
+      <c r="AA164">
+        <v>-1</v>
+      </c>
+      <c r="AB164">
+        <v>0.875</v>
       </c>
     </row>
     <row r="165" spans="1:28">
       <c r="A165" s="1">
         <v>163</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165">
+        <v>8155621</v>
+      </c>
+      <c r="C165" t="s">
+        <v>29</v>
+      </c>
+      <c r="D165" s="2">
+        <v>45416.28125</v>
+      </c>
+      <c r="E165" t="s">
+        <v>33</v>
+      </c>
+      <c r="F165" t="s">
+        <v>32</v>
+      </c>
+      <c r="G165">
+        <v>4</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+      <c r="I165" t="s">
+        <v>43</v>
+      </c>
+      <c r="J165">
+        <v>1.909</v>
+      </c>
+      <c r="K165">
+        <v>3.5</v>
+      </c>
+      <c r="L165">
+        <v>4</v>
+      </c>
+      <c r="M165">
+        <v>1.5</v>
+      </c>
+      <c r="N165">
+        <v>4.5</v>
+      </c>
+      <c r="O165">
+        <v>5.5</v>
+      </c>
+      <c r="P165">
+        <v>-1.25</v>
+      </c>
+      <c r="Q165">
+        <v>2.06</v>
+      </c>
+      <c r="R165">
+        <v>1.84</v>
+      </c>
+      <c r="S165">
+        <v>3.5</v>
+      </c>
+      <c r="T165">
+        <v>1.975</v>
+      </c>
+      <c r="U165">
+        <v>1.875</v>
+      </c>
+      <c r="V165">
+        <v>0.5</v>
+      </c>
+      <c r="W165">
+        <v>-1</v>
+      </c>
+      <c r="X165">
+        <v>-1</v>
+      </c>
+      <c r="Y165">
+        <v>1.06</v>
+      </c>
+      <c r="Z165">
+        <v>-1</v>
+      </c>
+      <c r="AA165">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AB165">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:28">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>8158306</v>
+      </c>
+      <c r="C166" t="s">
+        <v>29</v>
+      </c>
+      <c r="D166" s="2">
+        <v>45417.16666666666</v>
+      </c>
+      <c r="E166" t="s">
+        <v>39</v>
+      </c>
+      <c r="F166" t="s">
+        <v>30</v>
+      </c>
+      <c r="G166">
+        <v>4</v>
+      </c>
+      <c r="H166">
+        <v>3</v>
+      </c>
+      <c r="I166" t="s">
+        <v>43</v>
+      </c>
+      <c r="J166">
+        <v>2</v>
+      </c>
+      <c r="K166">
+        <v>3.6</v>
+      </c>
+      <c r="L166">
+        <v>3.5</v>
+      </c>
+      <c r="M166">
+        <v>2.6</v>
+      </c>
+      <c r="N166">
+        <v>3.5</v>
+      </c>
+      <c r="O166">
+        <v>2.55</v>
+      </c>
+      <c r="P166">
+        <v>0</v>
+      </c>
+      <c r="Q166">
+        <v>1.925</v>
+      </c>
+      <c r="R166">
+        <v>1.925</v>
+      </c>
+      <c r="S166">
+        <v>2.75</v>
+      </c>
+      <c r="T166">
+        <v>1.95</v>
+      </c>
+      <c r="U166">
+        <v>1.9</v>
+      </c>
+      <c r="V166">
+        <v>1.6</v>
+      </c>
+      <c r="W166">
+        <v>-1</v>
+      </c>
+      <c r="X166">
+        <v>-1</v>
+      </c>
+      <c r="Y166">
+        <v>0.925</v>
+      </c>
+      <c r="Z166">
+        <v>-1</v>
+      </c>
+      <c r="AA166">
+        <v>0.95</v>
+      </c>
+      <c r="AB166">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:28">
+      <c r="A167" s="1">
+        <v>165</v>
+      </c>
+      <c r="B167" t="s">
+        <v>27</v>
+      </c>
+      <c r="C167" t="s">
+        <v>29</v>
+      </c>
+      <c r="D167" s="2">
+        <v>45422.28125</v>
+      </c>
+      <c r="E167" t="s">
+        <v>33</v>
+      </c>
+      <c r="F167" t="s">
+        <v>38</v>
+      </c>
+      <c r="J167">
+        <v>2.2</v>
+      </c>
+      <c r="K167">
+        <v>3.5</v>
+      </c>
+      <c r="L167">
+        <v>3.1</v>
+      </c>
+      <c r="M167">
+        <v>2.05</v>
+      </c>
+      <c r="N167">
+        <v>3.75</v>
+      </c>
+      <c r="O167">
+        <v>3.3</v>
+      </c>
+      <c r="P167">
+        <v>-0.25</v>
+      </c>
+      <c r="Q167">
+        <v>1.84</v>
+      </c>
+      <c r="R167">
+        <v>2.06</v>
+      </c>
+      <c r="S167">
+        <v>2.75</v>
+      </c>
+      <c r="T167">
+        <v>1.825</v>
+      </c>
+      <c r="U167">
+        <v>2.025</v>
+      </c>
+      <c r="V167">
+        <v>0</v>
+      </c>
+      <c r="W167">
+        <v>0</v>
+      </c>
+      <c r="X167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:28">
+      <c r="A168" s="1">
+        <v>166</v>
+      </c>
+      <c r="B168" t="s">
         <v>28</v>
       </c>
-      <c r="C165" t="s">
-        <v>29</v>
-      </c>
-      <c r="D165" s="2">
-        <v>45417.16666666666</v>
-      </c>
-      <c r="E165" t="s">
+      <c r="C168" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168" s="2">
+        <v>45424.125</v>
+      </c>
+      <c r="E168" t="s">
         <v>39</v>
       </c>
-      <c r="F165" t="s">
-        <v>30</v>
-      </c>
-      <c r="J165">
-        <v>2</v>
-      </c>
-      <c r="K165">
+      <c r="F168" t="s">
+        <v>37</v>
+      </c>
+      <c r="J168">
+        <v>1.909</v>
+      </c>
+      <c r="K168">
         <v>3.6</v>
       </c>
-      <c r="L165">
-        <v>3.5</v>
-      </c>
-      <c r="M165">
-        <v>2.45</v>
-      </c>
-      <c r="N165">
-        <v>3.6</v>
-      </c>
-      <c r="O165">
-        <v>2.7</v>
-      </c>
-      <c r="P165">
+      <c r="L168">
+        <v>3.8</v>
+      </c>
+      <c r="M168">
+        <v>1.75</v>
+      </c>
+      <c r="N168">
+        <v>3.75</v>
+      </c>
+      <c r="O168">
+        <v>4.5</v>
+      </c>
+      <c r="P168">
+        <v>-0.75</v>
+      </c>
+      <c r="Q168">
+        <v>2.02</v>
+      </c>
+      <c r="R168">
+        <v>1.88</v>
+      </c>
+      <c r="S168">
+        <v>2.75</v>
+      </c>
+      <c r="T168">
+        <v>1.875</v>
+      </c>
+      <c r="U168">
+        <v>1.975</v>
+      </c>
+      <c r="V168">
         <v>0</v>
       </c>
-      <c r="Q165">
-        <v>1.85</v>
-      </c>
-      <c r="R165">
-        <v>2.05</v>
-      </c>
-      <c r="S165">
-        <v>2.75</v>
-      </c>
-      <c r="T165">
-        <v>1.825</v>
-      </c>
-      <c r="U165">
-        <v>2.025</v>
-      </c>
-      <c r="V165">
+      <c r="W168">
         <v>0</v>
       </c>
-      <c r="W165">
-        <v>0</v>
-      </c>
-      <c r="X165">
+      <c r="X168">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 08-05-2024 às 20:15
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14818,22 +14818,22 @@
         <v>3.1</v>
       </c>
       <c r="M167">
-        <v>2.05</v>
+        <v>2</v>
       </c>
       <c r="N167">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="O167">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="P167">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="Q167">
-        <v>1.84</v>
+        <v>2.02</v>
       </c>
       <c r="R167">
-        <v>2.06</v>
+        <v>1.88</v>
       </c>
       <c r="S167">
         <v>2.75</v>
@@ -14886,10 +14886,10 @@
         <v>1.75</v>
       </c>
       <c r="N168">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="O168">
-        <v>4.5</v>
+        <v>4.333</v>
       </c>
       <c r="P168">
         <v>-0.75</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 09-05-2024 às 19:13
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9376,7 +9376,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -9385,76 +9385,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F104" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I104" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB104">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9462,7 +9462,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -9471,76 +9471,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O105">
+        <v>3.25</v>
+      </c>
+      <c r="P105">
+        <v>-0.25</v>
+      </c>
+      <c r="Q105">
+        <v>1.86</v>
+      </c>
+      <c r="R105">
+        <v>2.04</v>
+      </c>
+      <c r="S105">
         <v>2.75</v>
       </c>
-      <c r="P105">
-        <v>0</v>
-      </c>
-      <c r="Q105">
-        <v>1.8</v>
-      </c>
-      <c r="R105">
-        <v>2.05</v>
-      </c>
-      <c r="S105">
-        <v>3</v>
-      </c>
       <c r="T105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -10064,7 +10064,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10073,76 +10073,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
+        <v>4.2</v>
+      </c>
+      <c r="O112">
         <v>3.6</v>
-      </c>
-      <c r="O112">
-        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
+        <v>1.89</v>
+      </c>
+      <c r="R112">
+        <v>2.01</v>
+      </c>
+      <c r="S112">
+        <v>3.5</v>
+      </c>
+      <c r="T112">
+        <v>1.95</v>
+      </c>
+      <c r="U112">
         <v>1.9</v>
       </c>
-      <c r="R112">
-        <v>1.95</v>
-      </c>
-      <c r="S112">
-        <v>2.75</v>
-      </c>
-      <c r="T112">
-        <v>1.925</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
+        <v>1.01</v>
+      </c>
+      <c r="AA112">
         <v>0.95</v>
       </c>
-      <c r="AA112">
-        <v>-1</v>
-      </c>
       <c r="AB112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10150,7 +10150,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10159,76 +10159,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -11096,7 +11096,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11105,76 +11105,76 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="K124">
+        <v>5</v>
+      </c>
+      <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>1.533</v>
+      </c>
+      <c r="N124">
+        <v>5.25</v>
+      </c>
+      <c r="O124">
+        <v>5</v>
+      </c>
+      <c r="P124">
+        <v>-1</v>
+      </c>
+      <c r="Q124">
+        <v>1.8</v>
+      </c>
+      <c r="R124">
+        <v>2.05</v>
+      </c>
+      <c r="S124">
         <v>3.5</v>
       </c>
-      <c r="L124">
-        <v>2.75</v>
-      </c>
-      <c r="M124">
-        <v>3.4</v>
-      </c>
-      <c r="N124">
-        <v>3.75</v>
-      </c>
-      <c r="O124">
-        <v>2.05</v>
-      </c>
-      <c r="P124">
-        <v>0.25</v>
-      </c>
-      <c r="Q124">
-        <v>2.025</v>
-      </c>
-      <c r="R124">
-        <v>1.825</v>
-      </c>
-      <c r="S124">
-        <v>3</v>
-      </c>
       <c r="T124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="U124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
         <v>-1</v>
       </c>
       <c r="W124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="X124">
+        <v>-1</v>
+      </c>
+      <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
         <v>1.05</v>
       </c>
-      <c r="Y124">
-        <v>-1</v>
-      </c>
-      <c r="Z124">
-        <v>0.825</v>
-      </c>
       <c r="AA124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:28">
@@ -11182,7 +11182,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11191,76 +11191,76 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="K125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="M125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="N125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="O125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="P125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="Q125">
+        <v>2.025</v>
+      </c>
+      <c r="R125">
+        <v>1.825</v>
+      </c>
+      <c r="S125">
+        <v>3</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>1.8</v>
       </c>
-      <c r="R125">
-        <v>2.05</v>
-      </c>
-      <c r="S125">
-        <v>3.5</v>
-      </c>
-      <c r="T125">
-        <v>1.925</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
       <c r="V125">
         <v>-1</v>
       </c>
       <c r="W125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y125">
         <v>-1</v>
       </c>
       <c r="Z125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AA125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:28">
@@ -14818,31 +14818,31 @@
         <v>3.1</v>
       </c>
       <c r="M167">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="N167">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O167">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="P167">
         <v>-0.5</v>
       </c>
       <c r="Q167">
-        <v>2.02</v>
+        <v>2.07</v>
       </c>
       <c r="R167">
-        <v>1.88</v>
+        <v>1.83</v>
       </c>
       <c r="S167">
         <v>2.75</v>
       </c>
       <c r="T167">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="U167">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V167">
         <v>0</v>
@@ -14895,19 +14895,19 @@
         <v>-0.75</v>
       </c>
       <c r="Q168">
-        <v>2.02</v>
+        <v>2.05</v>
       </c>
       <c r="R168">
-        <v>1.88</v>
+        <v>1.85</v>
       </c>
       <c r="S168">
         <v>2.75</v>
       </c>
       <c r="T168">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="U168">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V168">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 14-05-2024 às 01:09
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -97,10 +97,10 @@
     <t>PL_AhUnder</t>
   </si>
   <si>
-    <t>8182788</t>
+    <t>8182994</t>
   </si>
   <si>
-    <t>8182787</t>
+    <t>8182995</t>
   </si>
   <si>
     <t>Australia ALeague</t>
@@ -9376,7 +9376,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -9385,76 +9385,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O104">
+        <v>3.25</v>
+      </c>
+      <c r="P104">
+        <v>-0.25</v>
+      </c>
+      <c r="Q104">
+        <v>1.86</v>
+      </c>
+      <c r="R104">
+        <v>2.04</v>
+      </c>
+      <c r="S104">
         <v>2.75</v>
       </c>
-      <c r="P104">
-        <v>0</v>
-      </c>
-      <c r="Q104">
-        <v>1.8</v>
-      </c>
-      <c r="R104">
-        <v>2.05</v>
-      </c>
-      <c r="S104">
-        <v>3</v>
-      </c>
       <c r="T104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9462,7 +9462,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -9471,76 +9471,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F105" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB105">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -10064,7 +10064,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10073,76 +10073,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10150,7 +10150,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10159,76 +10159,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
+        <v>4.2</v>
+      </c>
+      <c r="O113">
         <v>3.6</v>
-      </c>
-      <c r="O113">
-        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
+        <v>1.89</v>
+      </c>
+      <c r="R113">
+        <v>2.01</v>
+      </c>
+      <c r="S113">
+        <v>3.5</v>
+      </c>
+      <c r="T113">
+        <v>1.95</v>
+      </c>
+      <c r="U113">
         <v>1.9</v>
       </c>
-      <c r="R113">
-        <v>1.95</v>
-      </c>
-      <c r="S113">
-        <v>2.75</v>
-      </c>
-      <c r="T113">
-        <v>1.925</v>
-      </c>
-      <c r="U113">
-        <v>1.925</v>
-      </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
+        <v>1.01</v>
+      </c>
+      <c r="AA113">
         <v>0.95</v>
       </c>
-      <c r="AA113">
-        <v>-1</v>
-      </c>
       <c r="AB113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -11096,7 +11096,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11105,76 +11105,76 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I124" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="K124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="L124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="M124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="N124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="O124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="P124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="Q124">
+        <v>2.025</v>
+      </c>
+      <c r="R124">
+        <v>1.825</v>
+      </c>
+      <c r="S124">
+        <v>3</v>
+      </c>
+      <c r="T124">
+        <v>2.05</v>
+      </c>
+      <c r="U124">
         <v>1.8</v>
       </c>
-      <c r="R124">
-        <v>2.05</v>
-      </c>
-      <c r="S124">
-        <v>3.5</v>
-      </c>
-      <c r="T124">
-        <v>1.925</v>
-      </c>
-      <c r="U124">
-        <v>1.925</v>
-      </c>
       <c r="V124">
         <v>-1</v>
       </c>
       <c r="W124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="X124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y124">
         <v>-1</v>
       </c>
       <c r="Z124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AA124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB124">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:28">
@@ -11182,7 +11182,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11191,76 +11191,76 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I125" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="K125">
+        <v>5</v>
+      </c>
+      <c r="L125">
+        <v>5</v>
+      </c>
+      <c r="M125">
+        <v>1.533</v>
+      </c>
+      <c r="N125">
+        <v>5.25</v>
+      </c>
+      <c r="O125">
+        <v>5</v>
+      </c>
+      <c r="P125">
+        <v>-1</v>
+      </c>
+      <c r="Q125">
+        <v>1.8</v>
+      </c>
+      <c r="R125">
+        <v>2.05</v>
+      </c>
+      <c r="S125">
         <v>3.5</v>
       </c>
-      <c r="L125">
-        <v>2.75</v>
-      </c>
-      <c r="M125">
-        <v>3.4</v>
-      </c>
-      <c r="N125">
-        <v>3.75</v>
-      </c>
-      <c r="O125">
-        <v>2.05</v>
-      </c>
-      <c r="P125">
-        <v>0.25</v>
-      </c>
-      <c r="Q125">
-        <v>2.025</v>
-      </c>
-      <c r="R125">
-        <v>1.825</v>
-      </c>
-      <c r="S125">
-        <v>3</v>
-      </c>
       <c r="T125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="U125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V125">
         <v>-1</v>
       </c>
       <c r="W125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="X125">
+        <v>-1</v>
+      </c>
+      <c r="Y125">
+        <v>-1</v>
+      </c>
+      <c r="Z125">
         <v>1.05</v>
       </c>
-      <c r="Y125">
-        <v>-1</v>
-      </c>
-      <c r="Z125">
-        <v>0.825</v>
-      </c>
       <c r="AA125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB125">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:28">
@@ -14106,7 +14106,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -14115,76 +14115,76 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F159" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I159" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J159">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="K159">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="L159">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M159">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="N159">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="O159">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="P159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Q159">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="R159">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="S159">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="T159">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U159">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V159">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="W159">
         <v>-1</v>
       </c>
       <c r="X159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Y159">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="Z159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA159">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB159">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:28">
@@ -14192,7 +14192,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -14201,76 +14201,76 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F160" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
         <v>3</v>
       </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
       <c r="I160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J160">
+        <v>3.6</v>
+      </c>
+      <c r="K160">
+        <v>3.25</v>
+      </c>
+      <c r="L160">
+        <v>2</v>
+      </c>
+      <c r="M160">
+        <v>4.2</v>
+      </c>
+      <c r="N160">
+        <v>4</v>
+      </c>
+      <c r="O160">
+        <v>1.75</v>
+      </c>
+      <c r="P160">
+        <v>0.75</v>
+      </c>
+      <c r="Q160">
         <v>1.85</v>
       </c>
-      <c r="K160">
-        <v>3.5</v>
-      </c>
-      <c r="L160">
-        <v>3.9</v>
-      </c>
-      <c r="M160">
-        <v>1.55</v>
-      </c>
-      <c r="N160">
-        <v>4.5</v>
-      </c>
-      <c r="O160">
-        <v>5.25</v>
-      </c>
-      <c r="P160">
-        <v>-1</v>
-      </c>
-      <c r="Q160">
-        <v>1.89</v>
-      </c>
       <c r="R160">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="S160">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="T160">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U160">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V160">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="W160">
         <v>-1</v>
       </c>
       <c r="X160">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Y160">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z160">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA160">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB160">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161" spans="1:28">
@@ -14800,49 +14800,49 @@
         <v>29</v>
       </c>
       <c r="D167" s="2">
-        <v>45422.28125</v>
+        <v>45430.14583333334</v>
       </c>
       <c r="E167" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F167" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J167">
-        <v>2.2</v>
+        <v>2.875</v>
       </c>
       <c r="K167">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="L167">
-        <v>3.1</v>
+        <v>2.375</v>
       </c>
       <c r="M167">
-        <v>2.05</v>
+        <v>2.8</v>
       </c>
       <c r="N167">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O167">
-        <v>3.3</v>
+        <v>2.5</v>
       </c>
       <c r="P167">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Q167">
-        <v>2.07</v>
+        <v>2.03</v>
       </c>
       <c r="R167">
-        <v>1.83</v>
+        <v>1.87</v>
       </c>
       <c r="S167">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="T167">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="U167">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V167">
         <v>0</v>
@@ -14865,49 +14865,49 @@
         <v>29</v>
       </c>
       <c r="D168" s="2">
-        <v>45424.125</v>
+        <v>45430.28125</v>
       </c>
       <c r="E168" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F168" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J168">
         <v>1.909</v>
       </c>
       <c r="K168">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L168">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M168">
-        <v>1.75</v>
+        <v>2.3</v>
       </c>
       <c r="N168">
         <v>3.8</v>
       </c>
       <c r="O168">
-        <v>4.333</v>
+        <v>2.8</v>
       </c>
       <c r="P168">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="Q168">
+        <v>2.02</v>
+      </c>
+      <c r="R168">
+        <v>1.88</v>
+      </c>
+      <c r="S168">
+        <v>3</v>
+      </c>
+      <c r="T168">
         <v>2.05</v>
       </c>
-      <c r="R168">
-        <v>1.85</v>
-      </c>
-      <c r="S168">
-        <v>2.75</v>
-      </c>
-      <c r="T168">
-        <v>1.925</v>
-      </c>
       <c r="U168">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V168">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 14-05-2024 às 20:19
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -510,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB168"/>
+  <dimension ref="A1:AB170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6710,7 +6710,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -6719,73 +6719,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="K73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="L73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="M73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="N73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="P73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="R73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="S73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB73">
         <v>-1</v>
@@ -6796,7 +6796,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -6805,73 +6805,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F74" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74" t="s">
+        <v>43</v>
+      </c>
+      <c r="J74">
+        <v>1.909</v>
+      </c>
+      <c r="K74">
         <v>4</v>
       </c>
-      <c r="I74" t="s">
-        <v>42</v>
-      </c>
-      <c r="J74">
-        <v>2.45</v>
-      </c>
-      <c r="K74">
-        <v>3.75</v>
-      </c>
       <c r="L74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="M74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="N74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="P74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="R74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="S74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="Z74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB74">
         <v>-1</v>
@@ -11096,7 +11096,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11105,76 +11105,76 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="K124">
+        <v>5</v>
+      </c>
+      <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>1.533</v>
+      </c>
+      <c r="N124">
+        <v>5.25</v>
+      </c>
+      <c r="O124">
+        <v>5</v>
+      </c>
+      <c r="P124">
+        <v>-1</v>
+      </c>
+      <c r="Q124">
+        <v>1.8</v>
+      </c>
+      <c r="R124">
+        <v>2.05</v>
+      </c>
+      <c r="S124">
         <v>3.5</v>
       </c>
-      <c r="L124">
-        <v>2.75</v>
-      </c>
-      <c r="M124">
-        <v>3.4</v>
-      </c>
-      <c r="N124">
-        <v>3.75</v>
-      </c>
-      <c r="O124">
-        <v>2.05</v>
-      </c>
-      <c r="P124">
-        <v>0.25</v>
-      </c>
-      <c r="Q124">
-        <v>2.025</v>
-      </c>
-      <c r="R124">
-        <v>1.825</v>
-      </c>
-      <c r="S124">
-        <v>3</v>
-      </c>
       <c r="T124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="U124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
         <v>-1</v>
       </c>
       <c r="W124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="X124">
+        <v>-1</v>
+      </c>
+      <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
         <v>1.05</v>
       </c>
-      <c r="Y124">
-        <v>-1</v>
-      </c>
-      <c r="Z124">
-        <v>0.825</v>
-      </c>
       <c r="AA124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:28">
@@ -11182,7 +11182,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11191,76 +11191,76 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="K125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="M125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="N125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="O125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="P125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="Q125">
+        <v>2.025</v>
+      </c>
+      <c r="R125">
+        <v>1.825</v>
+      </c>
+      <c r="S125">
+        <v>3</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>1.8</v>
       </c>
-      <c r="R125">
-        <v>2.05</v>
-      </c>
-      <c r="S125">
-        <v>3.5</v>
-      </c>
-      <c r="T125">
-        <v>1.925</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
       <c r="V125">
         <v>-1</v>
       </c>
       <c r="W125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y125">
         <v>-1</v>
       </c>
       <c r="Z125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AA125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:28">
@@ -14793,129 +14793,301 @@
       <c r="A167" s="1">
         <v>165</v>
       </c>
-      <c r="B167" t="s">
-        <v>27</v>
+      <c r="B167">
+        <v>8182788</v>
       </c>
       <c r="C167" t="s">
         <v>29</v>
       </c>
       <c r="D167" s="2">
-        <v>45430.14583333334</v>
+        <v>45422.28125</v>
       </c>
       <c r="E167" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F167" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="G167">
+        <v>1</v>
+      </c>
+      <c r="H167">
+        <v>2</v>
+      </c>
+      <c r="I167" t="s">
+        <v>42</v>
       </c>
       <c r="J167">
-        <v>2.875</v>
+        <v>2.2</v>
       </c>
       <c r="K167">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="L167">
-        <v>2.375</v>
+        <v>3.1</v>
       </c>
       <c r="M167">
-        <v>2.8</v>
+        <v>2.15</v>
       </c>
       <c r="N167">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="O167">
-        <v>2.5</v>
+        <v>3.2</v>
       </c>
       <c r="P167">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q167">
-        <v>2.03</v>
+        <v>1.925</v>
       </c>
       <c r="R167">
-        <v>1.87</v>
+        <v>1.925</v>
       </c>
       <c r="S167">
         <v>2.5</v>
       </c>
       <c r="T167">
+        <v>2</v>
+      </c>
+      <c r="U167">
         <v>1.85</v>
       </c>
-      <c r="U167">
-        <v>2</v>
-      </c>
       <c r="V167">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="W167">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="X167">
-        <v>0</v>
+        <v>2.2</v>
+      </c>
+      <c r="Y167">
+        <v>-1</v>
+      </c>
+      <c r="Z167">
+        <v>0.925</v>
+      </c>
+      <c r="AA167">
+        <v>1</v>
+      </c>
+      <c r="AB167">
+        <v>-1</v>
       </c>
     </row>
     <row r="168" spans="1:28">
       <c r="A168" s="1">
         <v>166</v>
       </c>
-      <c r="B168" t="s">
-        <v>28</v>
+      <c r="B168">
+        <v>8182787</v>
       </c>
       <c r="C168" t="s">
         <v>29</v>
       </c>
       <c r="D168" s="2">
-        <v>45430.28125</v>
+        <v>45424.125</v>
       </c>
       <c r="E168" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F168" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+      <c r="I168" t="s">
+        <v>44</v>
       </c>
       <c r="J168">
         <v>1.909</v>
       </c>
       <c r="K168">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L168">
+        <v>3.8</v>
+      </c>
+      <c r="M168">
+        <v>2.05</v>
+      </c>
+      <c r="N168">
         <v>3.5</v>
       </c>
-      <c r="M168">
-        <v>2.3</v>
-      </c>
-      <c r="N168">
-        <v>3.8</v>
-      </c>
       <c r="O168">
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="P168">
         <v>-0.25</v>
       </c>
       <c r="Q168">
-        <v>2.02</v>
+        <v>1.8</v>
       </c>
       <c r="R168">
-        <v>1.88</v>
+        <v>2.05</v>
       </c>
       <c r="S168">
+        <v>2.5</v>
+      </c>
+      <c r="T168">
+        <v>1.9</v>
+      </c>
+      <c r="U168">
+        <v>1.95</v>
+      </c>
+      <c r="V168">
+        <v>-1</v>
+      </c>
+      <c r="W168">
+        <v>2.5</v>
+      </c>
+      <c r="X168">
+        <v>-1</v>
+      </c>
+      <c r="Y168">
+        <v>-0.5</v>
+      </c>
+      <c r="Z168">
+        <v>0.5249999999999999</v>
+      </c>
+      <c r="AA168">
+        <v>-1</v>
+      </c>
+      <c r="AB168">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="169" spans="1:28">
+      <c r="A169" s="1">
+        <v>167</v>
+      </c>
+      <c r="B169" t="s">
+        <v>27</v>
+      </c>
+      <c r="C169" t="s">
+        <v>29</v>
+      </c>
+      <c r="D169" s="2">
+        <v>45430.14583333334</v>
+      </c>
+      <c r="E169" t="s">
+        <v>37</v>
+      </c>
+      <c r="F169" t="s">
+        <v>39</v>
+      </c>
+      <c r="J169">
+        <v>2.875</v>
+      </c>
+      <c r="K169">
+        <v>3.4</v>
+      </c>
+      <c r="L169">
+        <v>2.375</v>
+      </c>
+      <c r="M169">
+        <v>2.8</v>
+      </c>
+      <c r="N169">
+        <v>3.4</v>
+      </c>
+      <c r="O169">
+        <v>2.5</v>
+      </c>
+      <c r="P169">
+        <v>0</v>
+      </c>
+      <c r="Q169">
+        <v>2.04</v>
+      </c>
+      <c r="R169">
+        <v>1.86</v>
+      </c>
+      <c r="S169">
+        <v>2.5</v>
+      </c>
+      <c r="T169">
+        <v>1.85</v>
+      </c>
+      <c r="U169">
+        <v>2</v>
+      </c>
+      <c r="V169">
+        <v>0</v>
+      </c>
+      <c r="W169">
+        <v>0</v>
+      </c>
+      <c r="X169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:28">
+      <c r="A170" s="1">
+        <v>168</v>
+      </c>
+      <c r="B170" t="s">
+        <v>28</v>
+      </c>
+      <c r="C170" t="s">
+        <v>29</v>
+      </c>
+      <c r="D170" s="2">
+        <v>45430.28125</v>
+      </c>
+      <c r="E170" t="s">
+        <v>38</v>
+      </c>
+      <c r="F170" t="s">
+        <v>33</v>
+      </c>
+      <c r="J170">
+        <v>1.909</v>
+      </c>
+      <c r="K170">
+        <v>4</v>
+      </c>
+      <c r="L170">
+        <v>3.5</v>
+      </c>
+      <c r="M170">
+        <v>2.25</v>
+      </c>
+      <c r="N170">
+        <v>3.8</v>
+      </c>
+      <c r="O170">
+        <v>2.875</v>
+      </c>
+      <c r="P170">
+        <v>-0.25</v>
+      </c>
+      <c r="Q170">
+        <v>2.01</v>
+      </c>
+      <c r="R170">
+        <v>1.89</v>
+      </c>
+      <c r="S170">
         <v>3</v>
       </c>
-      <c r="T168">
+      <c r="T170">
         <v>2.05</v>
       </c>
-      <c r="U168">
+      <c r="U170">
         <v>1.8</v>
       </c>
-      <c r="V168">
+      <c r="V170">
         <v>0</v>
       </c>
-      <c r="W168">
+      <c r="W170">
         <v>0</v>
       </c>
-      <c r="X168">
+      <c r="X170">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 16-05-2024 às 23:38
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -6710,7 +6710,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -6719,73 +6719,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>43</v>
+      </c>
+      <c r="J73">
+        <v>1.909</v>
+      </c>
+      <c r="K73">
         <v>4</v>
       </c>
-      <c r="I73" t="s">
-        <v>42</v>
-      </c>
-      <c r="J73">
-        <v>2.45</v>
-      </c>
-      <c r="K73">
-        <v>3.75</v>
-      </c>
       <c r="L73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="M73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="N73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="P73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="R73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="S73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="Z73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB73">
         <v>-1</v>
@@ -6796,7 +6796,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -6805,73 +6805,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="K74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="L74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="M74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="N74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="P74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="R74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="S74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB74">
         <v>-1</v>
@@ -9376,7 +9376,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -9385,76 +9385,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F104" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I104" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB104">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9462,7 +9462,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -9471,76 +9471,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O105">
+        <v>3.25</v>
+      </c>
+      <c r="P105">
+        <v>-0.25</v>
+      </c>
+      <c r="Q105">
+        <v>1.86</v>
+      </c>
+      <c r="R105">
+        <v>2.04</v>
+      </c>
+      <c r="S105">
         <v>2.75</v>
       </c>
-      <c r="P105">
-        <v>0</v>
-      </c>
-      <c r="Q105">
-        <v>1.8</v>
-      </c>
-      <c r="R105">
-        <v>2.05</v>
-      </c>
-      <c r="S105">
-        <v>3</v>
-      </c>
       <c r="T105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -14990,22 +14990,22 @@
         <v>2.375</v>
       </c>
       <c r="M169">
-        <v>2.8</v>
+        <v>2.625</v>
       </c>
       <c r="N169">
         <v>3.4</v>
       </c>
       <c r="O169">
-        <v>2.5</v>
+        <v>2.625</v>
       </c>
       <c r="P169">
         <v>0</v>
       </c>
       <c r="Q169">
-        <v>2.04</v>
+        <v>1.95</v>
       </c>
       <c r="R169">
-        <v>1.86</v>
+        <v>1.95</v>
       </c>
       <c r="S169">
         <v>2.5</v>
@@ -15061,25 +15061,25 @@
         <v>3.8</v>
       </c>
       <c r="O170">
-        <v>2.875</v>
+        <v>2.9</v>
       </c>
       <c r="P170">
         <v>-0.25</v>
       </c>
       <c r="Q170">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="R170">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="S170">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="T170">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="U170">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="V170">
         <v>0</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 17-05-2024 às 13:59
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9376,7 +9376,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -9385,76 +9385,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O104">
+        <v>3.25</v>
+      </c>
+      <c r="P104">
+        <v>-0.25</v>
+      </c>
+      <c r="Q104">
+        <v>1.86</v>
+      </c>
+      <c r="R104">
+        <v>2.04</v>
+      </c>
+      <c r="S104">
         <v>2.75</v>
       </c>
-      <c r="P104">
-        <v>0</v>
-      </c>
-      <c r="Q104">
-        <v>1.8</v>
-      </c>
-      <c r="R104">
-        <v>2.05</v>
-      </c>
-      <c r="S104">
-        <v>3</v>
-      </c>
       <c r="T104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9462,7 +9462,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -9471,76 +9471,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F105" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB105">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -10064,7 +10064,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10073,76 +10073,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
+        <v>4.2</v>
+      </c>
+      <c r="O112">
         <v>3.6</v>
-      </c>
-      <c r="O112">
-        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
+        <v>1.89</v>
+      </c>
+      <c r="R112">
+        <v>2.01</v>
+      </c>
+      <c r="S112">
+        <v>3.5</v>
+      </c>
+      <c r="T112">
+        <v>1.95</v>
+      </c>
+      <c r="U112">
         <v>1.9</v>
       </c>
-      <c r="R112">
-        <v>1.95</v>
-      </c>
-      <c r="S112">
-        <v>2.75</v>
-      </c>
-      <c r="T112">
-        <v>1.925</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
+        <v>1.01</v>
+      </c>
+      <c r="AA112">
         <v>0.95</v>
       </c>
-      <c r="AA112">
-        <v>-1</v>
-      </c>
       <c r="AB112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10150,7 +10150,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10159,76 +10159,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -15067,10 +15067,10 @@
         <v>-0.25</v>
       </c>
       <c r="Q170">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="R170">
-        <v>1.9</v>
+        <v>1.88</v>
       </c>
       <c r="S170">
         <v>2.75</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 22-05-2024 às 20:16
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9373,7 +9373,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9382,76 +9382,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F104" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O104">
+        <v>3.25</v>
+      </c>
+      <c r="P104">
+        <v>-0.25</v>
+      </c>
+      <c r="Q104">
+        <v>1.86</v>
+      </c>
+      <c r="R104">
+        <v>2.04</v>
+      </c>
+      <c r="S104">
         <v>2.75</v>
       </c>
-      <c r="P104">
-        <v>0</v>
-      </c>
-      <c r="Q104">
-        <v>1.8</v>
-      </c>
-      <c r="R104">
-        <v>2.05</v>
-      </c>
-      <c r="S104">
-        <v>3</v>
-      </c>
       <c r="T104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9459,7 +9459,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9468,76 +9468,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F105" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I105" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB105">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -10061,7 +10061,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>28</v>
@@ -10070,76 +10070,76 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J112">
         <v>1.95</v>
       </c>
       <c r="K112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="L112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M112">
         <v>1.909</v>
       </c>
       <c r="N112">
+        <v>4.2</v>
+      </c>
+      <c r="O112">
         <v>3.6</v>
-      </c>
-      <c r="O112">
-        <v>4</v>
       </c>
       <c r="P112">
         <v>-0.5</v>
       </c>
       <c r="Q112">
+        <v>1.89</v>
+      </c>
+      <c r="R112">
+        <v>2.01</v>
+      </c>
+      <c r="S112">
+        <v>3.5</v>
+      </c>
+      <c r="T112">
+        <v>1.95</v>
+      </c>
+      <c r="U112">
         <v>1.9</v>
       </c>
-      <c r="R112">
-        <v>1.95</v>
-      </c>
-      <c r="S112">
-        <v>2.75</v>
-      </c>
-      <c r="T112">
-        <v>1.925</v>
-      </c>
-      <c r="U112">
-        <v>1.925</v>
-      </c>
       <c r="V112">
         <v>-1</v>
       </c>
       <c r="W112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y112">
         <v>-1</v>
       </c>
       <c r="Z112">
+        <v>1.01</v>
+      </c>
+      <c r="AA112">
         <v>0.95</v>
       </c>
-      <c r="AA112">
-        <v>-1</v>
-      </c>
       <c r="AB112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:28">
@@ -10147,7 +10147,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>28</v>
@@ -10156,76 +10156,76 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F113" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J113">
         <v>1.95</v>
       </c>
       <c r="K113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="L113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M113">
         <v>1.909</v>
       </c>
       <c r="N113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="O113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="P113">
         <v>-0.5</v>
       </c>
       <c r="Q113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="R113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="S113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="T113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="U113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V113">
         <v>-1</v>
       </c>
       <c r="W113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="X113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y113">
         <v>-1</v>
       </c>
       <c r="Z113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AA113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:28">
@@ -11093,7 +11093,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>28</v>
@@ -11102,76 +11102,76 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="K124">
+        <v>5</v>
+      </c>
+      <c r="L124">
+        <v>5</v>
+      </c>
+      <c r="M124">
+        <v>1.533</v>
+      </c>
+      <c r="N124">
+        <v>5.25</v>
+      </c>
+      <c r="O124">
+        <v>5</v>
+      </c>
+      <c r="P124">
+        <v>-1</v>
+      </c>
+      <c r="Q124">
+        <v>1.8</v>
+      </c>
+      <c r="R124">
+        <v>2.05</v>
+      </c>
+      <c r="S124">
         <v>3.5</v>
       </c>
-      <c r="L124">
-        <v>2.75</v>
-      </c>
-      <c r="M124">
-        <v>3.4</v>
-      </c>
-      <c r="N124">
-        <v>3.75</v>
-      </c>
-      <c r="O124">
-        <v>2.05</v>
-      </c>
-      <c r="P124">
-        <v>0.25</v>
-      </c>
-      <c r="Q124">
-        <v>2.025</v>
-      </c>
-      <c r="R124">
-        <v>1.825</v>
-      </c>
-      <c r="S124">
-        <v>3</v>
-      </c>
       <c r="T124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="U124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V124">
         <v>-1</v>
       </c>
       <c r="W124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="X124">
+        <v>-1</v>
+      </c>
+      <c r="Y124">
+        <v>-1</v>
+      </c>
+      <c r="Z124">
         <v>1.05</v>
       </c>
-      <c r="Y124">
-        <v>-1</v>
-      </c>
-      <c r="Z124">
-        <v>0.825</v>
-      </c>
       <c r="AA124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:28">
@@ -11179,7 +11179,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11188,76 +11188,76 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F125" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="K125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="L125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="M125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="N125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="O125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="P125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="Q125">
+        <v>2.025</v>
+      </c>
+      <c r="R125">
+        <v>1.825</v>
+      </c>
+      <c r="S125">
+        <v>3</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>1.8</v>
       </c>
-      <c r="R125">
-        <v>2.05</v>
-      </c>
-      <c r="S125">
-        <v>3.5</v>
-      </c>
-      <c r="T125">
-        <v>1.925</v>
-      </c>
-      <c r="U125">
-        <v>1.925</v>
-      </c>
       <c r="V125">
         <v>-1</v>
       </c>
       <c r="W125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y125">
         <v>-1</v>
       </c>
       <c r="Z125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AA125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:28">
@@ -15171,10 +15171,10 @@
         <v>-0.25</v>
       </c>
       <c r="Q171">
-        <v>1.9</v>
+        <v>1.89</v>
       </c>
       <c r="R171">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="S171">
         <v>2.5</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 23-05-2024 às 21:10
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9373,7 +9373,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>28</v>
@@ -9382,76 +9382,76 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F104" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I104" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="K104">
         <v>3.75</v>
       </c>
       <c r="L104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="M104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="N104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="O104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="P104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="R104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="S104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="T104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="W104">
         <v>-1</v>
       </c>
       <c r="X104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="Y104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB104">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:28">
@@ -9459,7 +9459,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>28</v>
@@ -9468,76 +9468,76 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F105" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="K105">
         <v>3.75</v>
       </c>
       <c r="L105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="M105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="N105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="O105">
+        <v>3.25</v>
+      </c>
+      <c r="P105">
+        <v>-0.25</v>
+      </c>
+      <c r="Q105">
+        <v>1.86</v>
+      </c>
+      <c r="R105">
+        <v>2.04</v>
+      </c>
+      <c r="S105">
         <v>2.75</v>
       </c>
-      <c r="P105">
-        <v>0</v>
-      </c>
-      <c r="Q105">
-        <v>1.8</v>
-      </c>
-      <c r="R105">
-        <v>2.05</v>
-      </c>
-      <c r="S105">
-        <v>3</v>
-      </c>
       <c r="T105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="W105">
         <v>-1</v>
       </c>
       <c r="X105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Y105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="Z105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:28">
@@ -14103,7 +14103,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>28</v>
@@ -14112,76 +14112,76 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F159" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I159" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J159">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="K159">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="L159">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="M159">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="N159">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="O159">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="P159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Q159">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="R159">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="S159">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="T159">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="U159">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="V159">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="W159">
         <v>-1</v>
       </c>
       <c r="X159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="Y159">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="Z159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AA159">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB159">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:28">
@@ -14189,7 +14189,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C160" t="s">
         <v>28</v>
@@ -14198,76 +14198,76 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F160" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
         <v>3</v>
       </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
       <c r="I160" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J160">
+        <v>3.6</v>
+      </c>
+      <c r="K160">
+        <v>3.25</v>
+      </c>
+      <c r="L160">
+        <v>2</v>
+      </c>
+      <c r="M160">
+        <v>4.2</v>
+      </c>
+      <c r="N160">
+        <v>4</v>
+      </c>
+      <c r="O160">
+        <v>1.75</v>
+      </c>
+      <c r="P160">
+        <v>0.75</v>
+      </c>
+      <c r="Q160">
         <v>1.85</v>
       </c>
-      <c r="K160">
-        <v>3.5</v>
-      </c>
-      <c r="L160">
-        <v>3.9</v>
-      </c>
-      <c r="M160">
-        <v>1.55</v>
-      </c>
-      <c r="N160">
-        <v>4.5</v>
-      </c>
-      <c r="O160">
-        <v>5.25</v>
-      </c>
-      <c r="P160">
-        <v>-1</v>
-      </c>
-      <c r="Q160">
-        <v>1.89</v>
-      </c>
       <c r="R160">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="S160">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="T160">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="U160">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="V160">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="W160">
         <v>-1</v>
       </c>
       <c r="X160">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="Y160">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z160">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AA160">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB160">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161" spans="1:28">
@@ -15159,7 +15159,7 @@
         <v>3</v>
       </c>
       <c r="M171">
-        <v>2.15</v>
+        <v>2.2</v>
       </c>
       <c r="N171">
         <v>3.4</v>
@@ -15171,10 +15171,10 @@
         <v>-0.25</v>
       </c>
       <c r="Q171">
-        <v>1.89</v>
+        <v>1.91</v>
       </c>
       <c r="R171">
-        <v>2.01</v>
+        <v>1.99</v>
       </c>
       <c r="S171">
         <v>2.5</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 27-05-2024 às 07:26
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -504,7 +504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB170"/>
+  <dimension ref="A1:AB171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6704,7 +6704,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
@@ -6713,73 +6713,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F73" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="K73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="L73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="M73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="N73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="O73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="P73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="Q73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="R73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="S73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="T73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="U73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="Y73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB73">
         <v>-1</v>
@@ -6790,7 +6790,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>27</v>
@@ -6799,73 +6799,73 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F74" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74" t="s">
+        <v>41</v>
+      </c>
+      <c r="J74">
+        <v>1.909</v>
+      </c>
+      <c r="K74">
         <v>4</v>
       </c>
-      <c r="I74" t="s">
-        <v>40</v>
-      </c>
-      <c r="J74">
-        <v>2.45</v>
-      </c>
-      <c r="K74">
-        <v>3.75</v>
-      </c>
       <c r="L74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="M74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="N74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="O74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="P74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="R74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="S74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="T74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="U74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="Z74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB74">
         <v>-1</v>
@@ -15125,6 +15125,92 @@
       </c>
       <c r="AB170">
         <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:28">
+      <c r="A171" s="1">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>8233998</v>
+      </c>
+      <c r="C171" t="s">
+        <v>27</v>
+      </c>
+      <c r="D171" s="2">
+        <v>45437.28125</v>
+      </c>
+      <c r="E171" t="s">
+        <v>36</v>
+      </c>
+      <c r="F171" t="s">
+        <v>37</v>
+      </c>
+      <c r="G171">
+        <v>3</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+      <c r="I171" t="s">
+        <v>41</v>
+      </c>
+      <c r="J171">
+        <v>2.3</v>
+      </c>
+      <c r="K171">
+        <v>3.4</v>
+      </c>
+      <c r="L171">
+        <v>3</v>
+      </c>
+      <c r="M171">
+        <v>2.35</v>
+      </c>
+      <c r="N171">
+        <v>3.1</v>
+      </c>
+      <c r="O171">
+        <v>3.25</v>
+      </c>
+      <c r="P171">
+        <v>-0.25</v>
+      </c>
+      <c r="Q171">
+        <v>2.025</v>
+      </c>
+      <c r="R171">
+        <v>1.825</v>
+      </c>
+      <c r="S171">
+        <v>2.25</v>
+      </c>
+      <c r="T171">
+        <v>2.05</v>
+      </c>
+      <c r="U171">
+        <v>1.8</v>
+      </c>
+      <c r="V171">
+        <v>1.35</v>
+      </c>
+      <c r="W171">
+        <v>-1</v>
+      </c>
+      <c r="X171">
+        <v>-1</v>
+      </c>
+      <c r="Y171">
+        <v>1.025</v>
+      </c>
+      <c r="Z171">
+        <v>-1</v>
+      </c>
+      <c r="AA171">
+        <v>1.05</v>
+      </c>
+      <c r="AB171">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 28-05-2024 às 19:13
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>43</v>
+      </c>
+      <c r="L73">
+        <v>1.909</v>
+      </c>
+      <c r="M73">
         <v>4</v>
       </c>
-      <c r="I73">
-        <v>1</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73" t="s">
-        <v>42</v>
-      </c>
-      <c r="L73">
-        <v>2.45</v>
-      </c>
-      <c r="M73">
-        <v>3.75</v>
-      </c>
       <c r="N73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K124" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>5</v>
+      </c>
+      <c r="O124">
+        <v>1.533</v>
+      </c>
+      <c r="P124">
+        <v>5.25</v>
+      </c>
+      <c r="Q124">
+        <v>5</v>
+      </c>
+      <c r="R124">
+        <v>-1</v>
+      </c>
+      <c r="S124">
+        <v>1.8</v>
+      </c>
+      <c r="T124">
+        <v>2.05</v>
+      </c>
+      <c r="U124">
         <v>3.5</v>
       </c>
-      <c r="N124">
-        <v>2.75</v>
-      </c>
-      <c r="O124">
-        <v>3.4</v>
-      </c>
-      <c r="P124">
-        <v>3.75</v>
-      </c>
-      <c r="Q124">
-        <v>2.05</v>
-      </c>
-      <c r="R124">
-        <v>0.25</v>
-      </c>
-      <c r="S124">
-        <v>2.025</v>
-      </c>
-      <c r="T124">
-        <v>1.825</v>
-      </c>
-      <c r="U124">
-        <v>3</v>
-      </c>
       <c r="V124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
+        <v>-1</v>
+      </c>
+      <c r="AB124">
         <v>1.05</v>
       </c>
-      <c r="AA124">
-        <v>-1</v>
-      </c>
-      <c r="AB124">
-        <v>0.825</v>
-      </c>
       <c r="AC124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K125" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S125">
+        <v>2.025</v>
+      </c>
+      <c r="T125">
+        <v>1.825</v>
+      </c>
+      <c r="U125">
+        <v>3</v>
+      </c>
+      <c r="V125">
+        <v>2.05</v>
+      </c>
+      <c r="W125">
         <v>1.8</v>
       </c>
-      <c r="T125">
-        <v>2.05</v>
-      </c>
-      <c r="U125">
-        <v>3.5</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
-      <c r="W125">
-        <v>1.925</v>
-      </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA125">
         <v>-1</v>
       </c>
       <c r="AB125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:30">
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F159" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
         <v>3</v>
       </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
       <c r="I159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L159">
+        <v>3.6</v>
+      </c>
+      <c r="M159">
+        <v>3.25</v>
+      </c>
+      <c r="N159">
+        <v>2</v>
+      </c>
+      <c r="O159">
+        <v>4.2</v>
+      </c>
+      <c r="P159">
+        <v>4</v>
+      </c>
+      <c r="Q159">
+        <v>1.75</v>
+      </c>
+      <c r="R159">
+        <v>0.75</v>
+      </c>
+      <c r="S159">
         <v>1.85</v>
       </c>
-      <c r="M159">
-        <v>3.5</v>
-      </c>
-      <c r="N159">
-        <v>3.9</v>
-      </c>
-      <c r="O159">
-        <v>1.55</v>
-      </c>
-      <c r="P159">
-        <v>4.5</v>
-      </c>
-      <c r="Q159">
-        <v>5.25</v>
-      </c>
-      <c r="R159">
-        <v>-1</v>
-      </c>
-      <c r="S159">
-        <v>1.89</v>
-      </c>
       <c r="T159">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U159">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V159">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W159">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X159">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA159">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB159">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC159">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD159">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F160" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G160">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H160">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I160">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K160" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L160">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M160">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N160">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O160">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P160">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q160">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S160">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T160">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U160">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V160">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W160">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X160">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA160">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB160">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC160">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD160">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 29-05-2024 às 22:54
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K124" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S124">
+        <v>2.025</v>
+      </c>
+      <c r="T124">
+        <v>1.825</v>
+      </c>
+      <c r="U124">
+        <v>3</v>
+      </c>
+      <c r="V124">
+        <v>2.05</v>
+      </c>
+      <c r="W124">
         <v>1.8</v>
       </c>
-      <c r="T124">
-        <v>2.05</v>
-      </c>
-      <c r="U124">
-        <v>3.5</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
-      <c r="W124">
-        <v>1.925</v>
-      </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD124">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K125" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>5</v>
+      </c>
+      <c r="O125">
+        <v>1.533</v>
+      </c>
+      <c r="P125">
+        <v>5.25</v>
+      </c>
+      <c r="Q125">
+        <v>5</v>
+      </c>
+      <c r="R125">
+        <v>-1</v>
+      </c>
+      <c r="S125">
+        <v>1.8</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>3.5</v>
       </c>
-      <c r="N125">
-        <v>2.75</v>
-      </c>
-      <c r="O125">
-        <v>3.4</v>
-      </c>
-      <c r="P125">
-        <v>3.75</v>
-      </c>
-      <c r="Q125">
-        <v>2.05</v>
-      </c>
-      <c r="R125">
-        <v>0.25</v>
-      </c>
-      <c r="S125">
-        <v>2.025</v>
-      </c>
-      <c r="T125">
-        <v>1.825</v>
-      </c>
-      <c r="U125">
-        <v>3</v>
-      </c>
       <c r="V125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
+        <v>-1</v>
+      </c>
+      <c r="AB125">
         <v>1.05</v>
       </c>
-      <c r="AA125">
-        <v>-1</v>
-      </c>
-      <c r="AB125">
-        <v>0.825</v>
-      </c>
       <c r="AC125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD125">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 30-05-2024 às 12:21
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F74" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>43</v>
+      </c>
+      <c r="L74">
+        <v>1.909</v>
+      </c>
+      <c r="M74">
         <v>4</v>
       </c>
-      <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-      <c r="K74" t="s">
-        <v>42</v>
-      </c>
-      <c r="L74">
-        <v>2.45</v>
-      </c>
-      <c r="M74">
-        <v>3.75</v>
-      </c>
       <c r="N74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
+        <v>4.2</v>
+      </c>
+      <c r="Q113">
         <v>3.6</v>
-      </c>
-      <c r="Q113">
-        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
+        <v>1.89</v>
+      </c>
+      <c r="T113">
+        <v>2.01</v>
+      </c>
+      <c r="U113">
+        <v>3.5</v>
+      </c>
+      <c r="V113">
+        <v>1.95</v>
+      </c>
+      <c r="W113">
         <v>1.9</v>
       </c>
-      <c r="T113">
-        <v>1.95</v>
-      </c>
-      <c r="U113">
-        <v>2.75</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
-      <c r="W113">
-        <v>1.925</v>
-      </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
+        <v>1.01</v>
+      </c>
+      <c r="AC113">
         <v>0.95</v>
       </c>
-      <c r="AC113">
-        <v>-1</v>
-      </c>
       <c r="AD113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 01-06-2024 às 01:16
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>43</v>
+      </c>
+      <c r="L73">
+        <v>1.909</v>
+      </c>
+      <c r="M73">
         <v>4</v>
       </c>
-      <c r="I73">
-        <v>1</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73" t="s">
-        <v>42</v>
-      </c>
-      <c r="L73">
-        <v>2.45</v>
-      </c>
-      <c r="M73">
-        <v>3.75</v>
-      </c>
       <c r="N73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
+        <v>4.2</v>
+      </c>
+      <c r="Q112">
         <v>3.6</v>
-      </c>
-      <c r="Q112">
-        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
+        <v>1.89</v>
+      </c>
+      <c r="T112">
+        <v>2.01</v>
+      </c>
+      <c r="U112">
+        <v>3.5</v>
+      </c>
+      <c r="V112">
+        <v>1.95</v>
+      </c>
+      <c r="W112">
         <v>1.9</v>
       </c>
-      <c r="T112">
-        <v>1.95</v>
-      </c>
-      <c r="U112">
-        <v>2.75</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
-      <c r="W112">
-        <v>1.925</v>
-      </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
+        <v>1.01</v>
+      </c>
+      <c r="AC112">
         <v>0.95</v>
       </c>
-      <c r="AC112">
-        <v>-1</v>
-      </c>
       <c r="AD112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 03-06-2024 às 23:01
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F74" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>43</v>
+      </c>
+      <c r="L74">
+        <v>1.909</v>
+      </c>
+      <c r="M74">
         <v>4</v>
       </c>
-      <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-      <c r="K74" t="s">
-        <v>42</v>
-      </c>
-      <c r="L74">
-        <v>2.45</v>
-      </c>
-      <c r="M74">
-        <v>3.75</v>
-      </c>
       <c r="N74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
+        <v>4.2</v>
+      </c>
+      <c r="Q113">
         <v>3.6</v>
-      </c>
-      <c r="Q113">
-        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
+        <v>1.89</v>
+      </c>
+      <c r="T113">
+        <v>2.01</v>
+      </c>
+      <c r="U113">
+        <v>3.5</v>
+      </c>
+      <c r="V113">
+        <v>1.95</v>
+      </c>
+      <c r="W113">
         <v>1.9</v>
       </c>
-      <c r="T113">
-        <v>1.95</v>
-      </c>
-      <c r="U113">
-        <v>2.75</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
-      <c r="W113">
-        <v>1.925</v>
-      </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
+        <v>1.01</v>
+      </c>
+      <c r="AC113">
         <v>0.95</v>
       </c>
-      <c r="AC113">
-        <v>-1</v>
-      </c>
       <c r="AD113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:30">
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K124" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S124">
+        <v>2.025</v>
+      </c>
+      <c r="T124">
+        <v>1.825</v>
+      </c>
+      <c r="U124">
+        <v>3</v>
+      </c>
+      <c r="V124">
+        <v>2.05</v>
+      </c>
+      <c r="W124">
         <v>1.8</v>
       </c>
-      <c r="T124">
-        <v>2.05</v>
-      </c>
-      <c r="U124">
-        <v>3.5</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
-      <c r="W124">
-        <v>1.925</v>
-      </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD124">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K125" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>5</v>
+      </c>
+      <c r="O125">
+        <v>1.533</v>
+      </c>
+      <c r="P125">
+        <v>5.25</v>
+      </c>
+      <c r="Q125">
+        <v>5</v>
+      </c>
+      <c r="R125">
+        <v>-1</v>
+      </c>
+      <c r="S125">
+        <v>1.8</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>3.5</v>
       </c>
-      <c r="N125">
-        <v>2.75</v>
-      </c>
-      <c r="O125">
-        <v>3.4</v>
-      </c>
-      <c r="P125">
-        <v>3.75</v>
-      </c>
-      <c r="Q125">
-        <v>2.05</v>
-      </c>
-      <c r="R125">
-        <v>0.25</v>
-      </c>
-      <c r="S125">
-        <v>2.025</v>
-      </c>
-      <c r="T125">
-        <v>1.825</v>
-      </c>
-      <c r="U125">
-        <v>3</v>
-      </c>
       <c r="V125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
+        <v>-1</v>
+      </c>
+      <c r="AB125">
         <v>1.05</v>
       </c>
-      <c r="AA125">
-        <v>-1</v>
-      </c>
-      <c r="AB125">
-        <v>0.825</v>
-      </c>
       <c r="AC125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD125">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:30">
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F159" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K159" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L159">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M159">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N159">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O159">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P159">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q159">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S159">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T159">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U159">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V159">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W159">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X159">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA159">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC159">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD159">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F160" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
         <v>3</v>
       </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
       <c r="I160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L160">
+        <v>3.6</v>
+      </c>
+      <c r="M160">
+        <v>3.25</v>
+      </c>
+      <c r="N160">
+        <v>2</v>
+      </c>
+      <c r="O160">
+        <v>4.2</v>
+      </c>
+      <c r="P160">
+        <v>4</v>
+      </c>
+      <c r="Q160">
+        <v>1.75</v>
+      </c>
+      <c r="R160">
+        <v>0.75</v>
+      </c>
+      <c r="S160">
         <v>1.85</v>
       </c>
-      <c r="M160">
-        <v>3.5</v>
-      </c>
-      <c r="N160">
-        <v>3.9</v>
-      </c>
-      <c r="O160">
-        <v>1.55</v>
-      </c>
-      <c r="P160">
-        <v>4.5</v>
-      </c>
-      <c r="Q160">
-        <v>5.25</v>
-      </c>
-      <c r="R160">
-        <v>-1</v>
-      </c>
-      <c r="S160">
-        <v>1.89</v>
-      </c>
       <c r="T160">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U160">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V160">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W160">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X160">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA160">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB160">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC160">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD160">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 10-06-2024 às 07:08
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K124" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>5</v>
+      </c>
+      <c r="O124">
+        <v>1.533</v>
+      </c>
+      <c r="P124">
+        <v>5.25</v>
+      </c>
+      <c r="Q124">
+        <v>5</v>
+      </c>
+      <c r="R124">
+        <v>-1</v>
+      </c>
+      <c r="S124">
+        <v>1.8</v>
+      </c>
+      <c r="T124">
+        <v>2.05</v>
+      </c>
+      <c r="U124">
         <v>3.5</v>
       </c>
-      <c r="N124">
-        <v>2.75</v>
-      </c>
-      <c r="O124">
-        <v>3.4</v>
-      </c>
-      <c r="P124">
-        <v>3.75</v>
-      </c>
-      <c r="Q124">
-        <v>2.05</v>
-      </c>
-      <c r="R124">
-        <v>0.25</v>
-      </c>
-      <c r="S124">
-        <v>2.025</v>
-      </c>
-      <c r="T124">
-        <v>1.825</v>
-      </c>
-      <c r="U124">
-        <v>3</v>
-      </c>
       <c r="V124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
+        <v>-1</v>
+      </c>
+      <c r="AB124">
         <v>1.05</v>
       </c>
-      <c r="AA124">
-        <v>-1</v>
-      </c>
-      <c r="AB124">
-        <v>0.825</v>
-      </c>
       <c r="AC124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K125" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S125">
+        <v>2.025</v>
+      </c>
+      <c r="T125">
+        <v>1.825</v>
+      </c>
+      <c r="U125">
+        <v>3</v>
+      </c>
+      <c r="V125">
+        <v>2.05</v>
+      </c>
+      <c r="W125">
         <v>1.8</v>
       </c>
-      <c r="T125">
-        <v>2.05</v>
-      </c>
-      <c r="U125">
-        <v>3.5</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
-      <c r="W125">
-        <v>1.925</v>
-      </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA125">
         <v>-1</v>
       </c>
       <c r="AB125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 10-06-2024 às 21:53
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F159" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
         <v>3</v>
       </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
       <c r="I159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L159">
+        <v>3.6</v>
+      </c>
+      <c r="M159">
+        <v>3.25</v>
+      </c>
+      <c r="N159">
+        <v>2</v>
+      </c>
+      <c r="O159">
+        <v>4.2</v>
+      </c>
+      <c r="P159">
+        <v>4</v>
+      </c>
+      <c r="Q159">
+        <v>1.75</v>
+      </c>
+      <c r="R159">
+        <v>0.75</v>
+      </c>
+      <c r="S159">
         <v>1.85</v>
       </c>
-      <c r="M159">
-        <v>3.5</v>
-      </c>
-      <c r="N159">
-        <v>3.9</v>
-      </c>
-      <c r="O159">
-        <v>1.55</v>
-      </c>
-      <c r="P159">
-        <v>4.5</v>
-      </c>
-      <c r="Q159">
-        <v>5.25</v>
-      </c>
-      <c r="R159">
-        <v>-1</v>
-      </c>
-      <c r="S159">
-        <v>1.89</v>
-      </c>
       <c r="T159">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U159">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V159">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W159">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X159">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA159">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB159">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC159">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD159">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F160" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G160">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H160">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I160">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K160" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L160">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M160">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N160">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O160">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P160">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q160">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S160">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T160">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U160">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V160">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W160">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X160">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA160">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB160">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC160">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD160">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 11-06-2024 às 21:19
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>43</v>
+      </c>
+      <c r="L73">
+        <v>1.909</v>
+      </c>
+      <c r="M73">
         <v>4</v>
       </c>
-      <c r="I73">
-        <v>1</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73" t="s">
-        <v>42</v>
-      </c>
-      <c r="L73">
-        <v>2.45</v>
-      </c>
-      <c r="M73">
-        <v>3.75</v>
-      </c>
       <c r="N73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K124" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S124">
+        <v>2.025</v>
+      </c>
+      <c r="T124">
+        <v>1.825</v>
+      </c>
+      <c r="U124">
+        <v>3</v>
+      </c>
+      <c r="V124">
+        <v>2.05</v>
+      </c>
+      <c r="W124">
         <v>1.8</v>
       </c>
-      <c r="T124">
-        <v>2.05</v>
-      </c>
-      <c r="U124">
-        <v>3.5</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
-      <c r="W124">
-        <v>1.925</v>
-      </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD124">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K125" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>5</v>
+      </c>
+      <c r="O125">
+        <v>1.533</v>
+      </c>
+      <c r="P125">
+        <v>5.25</v>
+      </c>
+      <c r="Q125">
+        <v>5</v>
+      </c>
+      <c r="R125">
+        <v>-1</v>
+      </c>
+      <c r="S125">
+        <v>1.8</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>3.5</v>
       </c>
-      <c r="N125">
-        <v>2.75</v>
-      </c>
-      <c r="O125">
-        <v>3.4</v>
-      </c>
-      <c r="P125">
-        <v>3.75</v>
-      </c>
-      <c r="Q125">
-        <v>2.05</v>
-      </c>
-      <c r="R125">
-        <v>0.25</v>
-      </c>
-      <c r="S125">
-        <v>2.025</v>
-      </c>
-      <c r="T125">
-        <v>1.825</v>
-      </c>
-      <c r="U125">
-        <v>3</v>
-      </c>
       <c r="V125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
+        <v>-1</v>
+      </c>
+      <c r="AB125">
         <v>1.05</v>
       </c>
-      <c r="AA125">
-        <v>-1</v>
-      </c>
-      <c r="AB125">
-        <v>0.825</v>
-      </c>
       <c r="AC125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD125">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:30">
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F159" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K159" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L159">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M159">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N159">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O159">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P159">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q159">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S159">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T159">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U159">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V159">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W159">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X159">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA159">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC159">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD159">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F160" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
         <v>3</v>
       </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
       <c r="I160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L160">
+        <v>3.6</v>
+      </c>
+      <c r="M160">
+        <v>3.25</v>
+      </c>
+      <c r="N160">
+        <v>2</v>
+      </c>
+      <c r="O160">
+        <v>4.2</v>
+      </c>
+      <c r="P160">
+        <v>4</v>
+      </c>
+      <c r="Q160">
+        <v>1.75</v>
+      </c>
+      <c r="R160">
+        <v>0.75</v>
+      </c>
+      <c r="S160">
         <v>1.85</v>
       </c>
-      <c r="M160">
-        <v>3.5</v>
-      </c>
-      <c r="N160">
-        <v>3.9</v>
-      </c>
-      <c r="O160">
-        <v>1.55</v>
-      </c>
-      <c r="P160">
-        <v>4.5</v>
-      </c>
-      <c r="Q160">
-        <v>5.25</v>
-      </c>
-      <c r="R160">
-        <v>-1</v>
-      </c>
-      <c r="S160">
-        <v>1.89</v>
-      </c>
       <c r="T160">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U160">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V160">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W160">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X160">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA160">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB160">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC160">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD160">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 13-06-2024 às 19:35
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K73" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L73">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M73">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N73">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O73">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P73">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q73">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R73">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S73">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T73">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U73">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V73">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W73">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X73">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA73">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC73">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F74" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74" t="s">
+        <v>43</v>
+      </c>
+      <c r="L74">
+        <v>1.909</v>
+      </c>
+      <c r="M74">
         <v>4</v>
       </c>
-      <c r="I74">
-        <v>1</v>
-      </c>
-      <c r="J74">
-        <v>2</v>
-      </c>
-      <c r="K74" t="s">
-        <v>42</v>
-      </c>
-      <c r="L74">
-        <v>2.45</v>
-      </c>
-      <c r="M74">
-        <v>3.75</v>
-      </c>
       <c r="N74">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O74">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P74">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q74">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R74">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S74">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T74">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U74">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W74">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB74">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC74">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
+        <v>4.2</v>
+      </c>
+      <c r="Q112">
         <v>3.6</v>
-      </c>
-      <c r="Q112">
-        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
+        <v>1.89</v>
+      </c>
+      <c r="T112">
+        <v>2.01</v>
+      </c>
+      <c r="U112">
+        <v>3.5</v>
+      </c>
+      <c r="V112">
+        <v>1.95</v>
+      </c>
+      <c r="W112">
         <v>1.9</v>
       </c>
-      <c r="T112">
-        <v>1.95</v>
-      </c>
-      <c r="U112">
-        <v>2.75</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
-      <c r="W112">
-        <v>1.925</v>
-      </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
+        <v>1.01</v>
+      </c>
+      <c r="AC112">
         <v>0.95</v>
       </c>
-      <c r="AC112">
-        <v>-1</v>
-      </c>
       <c r="AD112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:30">
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F159" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
         <v>3</v>
       </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
       <c r="I159">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J159">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K159" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L159">
+        <v>3.6</v>
+      </c>
+      <c r="M159">
+        <v>3.25</v>
+      </c>
+      <c r="N159">
+        <v>2</v>
+      </c>
+      <c r="O159">
+        <v>4.2</v>
+      </c>
+      <c r="P159">
+        <v>4</v>
+      </c>
+      <c r="Q159">
+        <v>1.75</v>
+      </c>
+      <c r="R159">
+        <v>0.75</v>
+      </c>
+      <c r="S159">
         <v>1.85</v>
       </c>
-      <c r="M159">
-        <v>3.5</v>
-      </c>
-      <c r="N159">
-        <v>3.9</v>
-      </c>
-      <c r="O159">
-        <v>1.55</v>
-      </c>
-      <c r="P159">
-        <v>4.5</v>
-      </c>
-      <c r="Q159">
-        <v>5.25</v>
-      </c>
-      <c r="R159">
-        <v>-1</v>
-      </c>
-      <c r="S159">
-        <v>1.89</v>
-      </c>
       <c r="T159">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U159">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V159">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W159">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X159">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA159">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB159">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC159">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD159">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F160" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G160">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H160">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I160">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J160">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K160" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L160">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M160">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N160">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O160">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P160">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q160">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S160">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T160">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U160">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V160">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W160">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X160">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA160">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB160">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC160">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD160">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 14-06-2024 às 20:31
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
+        <v>4.2</v>
+      </c>
+      <c r="Q113">
         <v>3.6</v>
-      </c>
-      <c r="Q113">
-        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
+        <v>1.89</v>
+      </c>
+      <c r="T113">
+        <v>2.01</v>
+      </c>
+      <c r="U113">
+        <v>3.5</v>
+      </c>
+      <c r="V113">
+        <v>1.95</v>
+      </c>
+      <c r="W113">
         <v>1.9</v>
       </c>
-      <c r="T113">
-        <v>1.95</v>
-      </c>
-      <c r="U113">
-        <v>2.75</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
-      <c r="W113">
-        <v>1.925</v>
-      </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
+        <v>1.01</v>
+      </c>
+      <c r="AC113">
         <v>0.95</v>
       </c>
-      <c r="AC113">
-        <v>-1</v>
-      </c>
       <c r="AD113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 15-06-2024 às 21:10
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
+        <v>4.2</v>
+      </c>
+      <c r="Q112">
         <v>3.6</v>
-      </c>
-      <c r="Q112">
-        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
+        <v>1.89</v>
+      </c>
+      <c r="T112">
+        <v>2.01</v>
+      </c>
+      <c r="U112">
+        <v>3.5</v>
+      </c>
+      <c r="V112">
+        <v>1.95</v>
+      </c>
+      <c r="W112">
         <v>1.9</v>
       </c>
-      <c r="T112">
-        <v>1.95</v>
-      </c>
-      <c r="U112">
-        <v>2.75</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
-      <c r="W112">
-        <v>1.925</v>
-      </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
+        <v>1.01</v>
+      </c>
+      <c r="AC112">
         <v>0.95</v>
       </c>
-      <c r="AC112">
-        <v>-1</v>
-      </c>
       <c r="AD112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:30">
@@ -15048,7 +15048,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>7127418</v>
+        <v>7127419</v>
       </c>
       <c r="C159" t="s">
         <v>29</v>
@@ -15057,82 +15057,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E159" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F159" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H159">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I159">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J159">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K159" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L159">
-        <v>3.6</v>
+        <v>1.85</v>
       </c>
       <c r="M159">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="N159">
-        <v>2</v>
+        <v>3.9</v>
       </c>
       <c r="O159">
-        <v>4.2</v>
+        <v>1.55</v>
       </c>
       <c r="P159">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="Q159">
-        <v>1.75</v>
+        <v>5.25</v>
       </c>
       <c r="R159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="S159">
-        <v>1.85</v>
+        <v>1.89</v>
       </c>
       <c r="T159">
-        <v>2</v>
+        <v>2.01</v>
       </c>
       <c r="U159">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="V159">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W159">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X159">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Y159">
         <v>-1</v>
       </c>
       <c r="Z159">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AA159">
-        <v>-1</v>
+        <v>0.8899999999999999</v>
       </c>
       <c r="AB159">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC159">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AD159">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="160" spans="1:30">
@@ -15140,7 +15140,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>7127419</v>
+        <v>7127418</v>
       </c>
       <c r="C160" t="s">
         <v>29</v>
@@ -15149,82 +15149,82 @@
         <v>45409.17708333334</v>
       </c>
       <c r="E160" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F160" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
         <v>3</v>
       </c>
-      <c r="H160">
-        <v>0</v>
-      </c>
       <c r="I160">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J160">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K160" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L160">
+        <v>3.6</v>
+      </c>
+      <c r="M160">
+        <v>3.25</v>
+      </c>
+      <c r="N160">
+        <v>2</v>
+      </c>
+      <c r="O160">
+        <v>4.2</v>
+      </c>
+      <c r="P160">
+        <v>4</v>
+      </c>
+      <c r="Q160">
+        <v>1.75</v>
+      </c>
+      <c r="R160">
+        <v>0.75</v>
+      </c>
+      <c r="S160">
         <v>1.85</v>
       </c>
-      <c r="M160">
-        <v>3.5</v>
-      </c>
-      <c r="N160">
-        <v>3.9</v>
-      </c>
-      <c r="O160">
-        <v>1.55</v>
-      </c>
-      <c r="P160">
-        <v>4.5</v>
-      </c>
-      <c r="Q160">
-        <v>5.25</v>
-      </c>
-      <c r="R160">
-        <v>-1</v>
-      </c>
-      <c r="S160">
-        <v>1.89</v>
-      </c>
       <c r="T160">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="U160">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="V160">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W160">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X160">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Y160">
         <v>-1</v>
       </c>
       <c r="Z160">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AA160">
-        <v>0.8899999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB160">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AC160">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AD160">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="161" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 16-06-2024 às 07:16
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N112">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T112">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U112">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V112">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W112">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z112">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC112">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD112">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F113" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N113">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
+        <v>4.2</v>
+      </c>
+      <c r="Q113">
         <v>3.6</v>
-      </c>
-      <c r="Q113">
-        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
+        <v>1.89</v>
+      </c>
+      <c r="T113">
+        <v>2.01</v>
+      </c>
+      <c r="U113">
+        <v>3.5</v>
+      </c>
+      <c r="V113">
+        <v>1.95</v>
+      </c>
+      <c r="W113">
         <v>1.9</v>
       </c>
-      <c r="T113">
-        <v>1.95</v>
-      </c>
-      <c r="U113">
-        <v>2.75</v>
-      </c>
-      <c r="V113">
-        <v>1.925</v>
-      </c>
-      <c r="W113">
-        <v>1.925</v>
-      </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z113">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
+        <v>1.01</v>
+      </c>
+      <c r="AC113">
         <v>0.95</v>
       </c>
-      <c r="AC113">
-        <v>-1</v>
-      </c>
       <c r="AD113">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114" spans="1:30">
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F124" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H124">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K124" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L124">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M124">
+        <v>5</v>
+      </c>
+      <c r="N124">
+        <v>5</v>
+      </c>
+      <c r="O124">
+        <v>1.533</v>
+      </c>
+      <c r="P124">
+        <v>5.25</v>
+      </c>
+      <c r="Q124">
+        <v>5</v>
+      </c>
+      <c r="R124">
+        <v>-1</v>
+      </c>
+      <c r="S124">
+        <v>1.8</v>
+      </c>
+      <c r="T124">
+        <v>2.05</v>
+      </c>
+      <c r="U124">
         <v>3.5</v>
       </c>
-      <c r="N124">
-        <v>2.75</v>
-      </c>
-      <c r="O124">
-        <v>3.4</v>
-      </c>
-      <c r="P124">
-        <v>3.75</v>
-      </c>
-      <c r="Q124">
-        <v>2.05</v>
-      </c>
-      <c r="R124">
-        <v>0.25</v>
-      </c>
-      <c r="S124">
-        <v>2.025</v>
-      </c>
-      <c r="T124">
-        <v>1.825</v>
-      </c>
-      <c r="U124">
-        <v>3</v>
-      </c>
       <c r="V124">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W124">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z124">
+        <v>-1</v>
+      </c>
+      <c r="AA124">
+        <v>-1</v>
+      </c>
+      <c r="AB124">
         <v>1.05</v>
       </c>
-      <c r="AA124">
-        <v>-1</v>
-      </c>
-      <c r="AB124">
-        <v>0.825</v>
-      </c>
       <c r="AC124">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD124">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K125" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L125">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M125">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N125">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O125">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P125">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q125">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R125">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S125">
+        <v>2.025</v>
+      </c>
+      <c r="T125">
+        <v>1.825</v>
+      </c>
+      <c r="U125">
+        <v>3</v>
+      </c>
+      <c r="V125">
+        <v>2.05</v>
+      </c>
+      <c r="W125">
         <v>1.8</v>
       </c>
-      <c r="T125">
-        <v>2.05</v>
-      </c>
-      <c r="U125">
-        <v>3.5</v>
-      </c>
-      <c r="V125">
-        <v>1.925</v>
-      </c>
-      <c r="W125">
-        <v>1.925</v>
-      </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA125">
         <v>-1</v>
       </c>
       <c r="AB125">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD125">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 17-06-2024 às 21:10
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -7142,7 +7142,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>7646750</v>
+        <v>7646749</v>
       </c>
       <c r="C73" t="s">
         <v>29</v>
@@ -7151,79 +7151,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E73" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F73" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
       <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="K73" t="s">
+        <v>43</v>
+      </c>
+      <c r="L73">
+        <v>1.909</v>
+      </c>
+      <c r="M73">
         <v>4</v>
       </c>
-      <c r="I73">
-        <v>1</v>
-      </c>
-      <c r="J73">
-        <v>2</v>
-      </c>
-      <c r="K73" t="s">
-        <v>42</v>
-      </c>
-      <c r="L73">
-        <v>2.45</v>
-      </c>
-      <c r="M73">
-        <v>3.75</v>
-      </c>
       <c r="N73">
-        <v>2.55</v>
+        <v>3.4</v>
       </c>
       <c r="O73">
-        <v>3.1</v>
+        <v>2.4</v>
       </c>
       <c r="P73">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="Q73">
-        <v>2.05</v>
+        <v>2.6</v>
       </c>
       <c r="R73">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="S73">
-        <v>2</v>
+        <v>1.83</v>
       </c>
       <c r="T73">
-        <v>1.85</v>
+        <v>2.07</v>
       </c>
       <c r="U73">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="V73">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W73">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Y73">
         <v>-1</v>
       </c>
       <c r="Z73">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.8300000000000001</v>
       </c>
       <c r="AB73">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC73">
-        <v>0.925</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AD73">
         <v>-1</v>
@@ -7234,7 +7234,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>7646749</v>
+        <v>7646750</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -7243,79 +7243,79 @@
         <v>45305.23958333334</v>
       </c>
       <c r="E74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F74" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G74">
         <v>3</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L74">
-        <v>1.909</v>
+        <v>2.45</v>
       </c>
       <c r="M74">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="N74">
-        <v>3.4</v>
+        <v>2.55</v>
       </c>
       <c r="O74">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="P74">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="Q74">
-        <v>2.6</v>
+        <v>2.05</v>
       </c>
       <c r="R74">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S74">
-        <v>1.83</v>
+        <v>2</v>
       </c>
       <c r="T74">
-        <v>2.07</v>
+        <v>1.85</v>
       </c>
       <c r="U74">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="V74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W74">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="X74">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
         <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA74">
-        <v>0.8300000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC74">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AD74">
         <v>-1</v>
@@ -9994,7 +9994,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -10003,82 +10003,82 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F104" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I104">
         <v>0</v>
       </c>
       <c r="J104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K104" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L104">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="M104">
         <v>3.75</v>
       </c>
       <c r="N104">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="O104">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="P104">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="Q104">
+        <v>3.25</v>
+      </c>
+      <c r="R104">
+        <v>-0.25</v>
+      </c>
+      <c r="S104">
+        <v>1.86</v>
+      </c>
+      <c r="T104">
+        <v>2.04</v>
+      </c>
+      <c r="U104">
         <v>2.75</v>
       </c>
-      <c r="R104">
-        <v>0</v>
-      </c>
-      <c r="S104">
-        <v>1.8</v>
-      </c>
-      <c r="T104">
-        <v>2.05</v>
-      </c>
-      <c r="U104">
-        <v>3</v>
-      </c>
       <c r="V104">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W104">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X104">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="Y104">
         <v>-1</v>
       </c>
       <c r="Z104">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="AA104">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AB104">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AC104">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD104">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -10086,7 +10086,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -10095,82 +10095,82 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F105" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I105">
         <v>0</v>
       </c>
       <c r="J105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K105" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L105">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="M105">
         <v>3.75</v>
       </c>
       <c r="N105">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="O105">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="P105">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="Q105">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="R105">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="S105">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="T105">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="U105">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="V105">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W105">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X105">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="Y105">
         <v>-1</v>
       </c>
       <c r="Z105">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="AA105">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB105">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AC105">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD105">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -11828,7 +11828,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>7127388</v>
+        <v>7128012</v>
       </c>
       <c r="C124" t="s">
         <v>29</v>
@@ -11837,82 +11837,82 @@
         <v>45361.125</v>
       </c>
       <c r="E124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F124" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I124">
         <v>0</v>
       </c>
       <c r="J124">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K124" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L124">
-        <v>1.5</v>
+        <v>2.4</v>
       </c>
       <c r="M124">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="N124">
-        <v>5</v>
+        <v>2.75</v>
       </c>
       <c r="O124">
-        <v>1.533</v>
+        <v>3.4</v>
       </c>
       <c r="P124">
-        <v>5.25</v>
+        <v>3.75</v>
       </c>
       <c r="Q124">
-        <v>5</v>
+        <v>2.05</v>
       </c>
       <c r="R124">
-        <v>-1</v>
+        <v>0.25</v>
       </c>
       <c r="S124">
+        <v>2.025</v>
+      </c>
+      <c r="T124">
+        <v>1.825</v>
+      </c>
+      <c r="U124">
+        <v>3</v>
+      </c>
+      <c r="V124">
+        <v>2.05</v>
+      </c>
+      <c r="W124">
         <v>1.8</v>
       </c>
-      <c r="T124">
-        <v>2.05</v>
-      </c>
-      <c r="U124">
-        <v>3.5</v>
-      </c>
-      <c r="V124">
-        <v>1.925</v>
-      </c>
-      <c r="W124">
-        <v>1.925</v>
-      </c>
       <c r="X124">
         <v>-1</v>
       </c>
       <c r="Y124">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z124">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA124">
         <v>-1</v>
       </c>
       <c r="AB124">
-        <v>1.05</v>
+        <v>0.825</v>
       </c>
       <c r="AC124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD124">
-        <v>0.925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:30">
@@ -11920,7 +11920,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>7128012</v>
+        <v>7127388</v>
       </c>
       <c r="C125" t="s">
         <v>29</v>
@@ -11929,82 +11929,82 @@
         <v>45361.125</v>
       </c>
       <c r="E125" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I125">
         <v>0</v>
       </c>
       <c r="J125">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K125" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L125">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="M125">
+        <v>5</v>
+      </c>
+      <c r="N125">
+        <v>5</v>
+      </c>
+      <c r="O125">
+        <v>1.533</v>
+      </c>
+      <c r="P125">
+        <v>5.25</v>
+      </c>
+      <c r="Q125">
+        <v>5</v>
+      </c>
+      <c r="R125">
+        <v>-1</v>
+      </c>
+      <c r="S125">
+        <v>1.8</v>
+      </c>
+      <c r="T125">
+        <v>2.05</v>
+      </c>
+      <c r="U125">
         <v>3.5</v>
       </c>
-      <c r="N125">
-        <v>2.75</v>
-      </c>
-      <c r="O125">
-        <v>3.4</v>
-      </c>
-      <c r="P125">
-        <v>3.75</v>
-      </c>
-      <c r="Q125">
-        <v>2.05</v>
-      </c>
-      <c r="R125">
-        <v>0.25</v>
-      </c>
-      <c r="S125">
-        <v>2.025</v>
-      </c>
-      <c r="T125">
-        <v>1.825</v>
-      </c>
-      <c r="U125">
-        <v>3</v>
-      </c>
       <c r="V125">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W125">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="X125">
         <v>-1</v>
       </c>
       <c r="Y125">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z125">
+        <v>-1</v>
+      </c>
+      <c r="AA125">
+        <v>-1</v>
+      </c>
+      <c r="AB125">
         <v>1.05</v>
       </c>
-      <c r="AA125">
-        <v>-1</v>
-      </c>
-      <c r="AB125">
-        <v>0.825</v>
-      </c>
       <c r="AC125">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD125">
-        <v>0</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="126" spans="1:30">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 20-06-2024 às 20:11
</commit_message>
<xml_diff>
--- a/Australia ALeague/Australia ALeague.xlsx
+++ b/Australia ALeague/Australia ALeague.xlsx
@@ -9994,7 +9994,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>7127374</v>
+        <v>7127370</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -10003,82 +10003,82 @@
         <v>45340.125</v>
       </c>
       <c r="E104" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F104" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G104">
         <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I104">
         <v>0</v>
       </c>
       <c r="J104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K104" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L104">
-        <v>1.909</v>
+        <v>2.4</v>
       </c>
       <c r="M104">
         <v>3.75</v>
       </c>
       <c r="N104">
-        <v>3.6</v>
+        <v>2.625</v>
       </c>
       <c r="O104">
-        <v>2.15</v>
+        <v>2.375</v>
       </c>
       <c r="P104">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="Q104">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="R104">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="S104">
-        <v>1.86</v>
+        <v>1.8</v>
       </c>
       <c r="T104">
-        <v>2.04</v>
+        <v>2.05</v>
       </c>
       <c r="U104">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="V104">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="W104">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="X104">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="Y104">
         <v>-1</v>
       </c>
       <c r="Z104">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="AA104">
-        <v>0.8600000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB104">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AC104">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AD104">
-        <v>0.875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:30">
@@ -10086,7 +10086,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>7127370</v>
+        <v>7127374</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -10095,82 +10095,82 @@
         <v>45340.125</v>
       </c>
       <c r="E105" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F105" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G105">
         <v>1</v>
       </c>
       <c r="H105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I105">
         <v>0</v>
       </c>
       <c r="J105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K105" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L105">
-        <v>2.4</v>
+        <v>1.909</v>
       </c>
       <c r="M105">
         <v>3.75</v>
       </c>
       <c r="N105">
-        <v>2.625</v>
+        <v>3.6</v>
       </c>
       <c r="O105">
-        <v>2.375</v>
+        <v>2.15</v>
       </c>
       <c r="P105">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="Q105">
+        <v>3.25</v>
+      </c>
+      <c r="R105">
+        <v>-0.25</v>
+      </c>
+      <c r="S105">
+        <v>1.86</v>
+      </c>
+      <c r="T105">
+        <v>2.04</v>
+      </c>
+      <c r="U105">
         <v>2.75</v>
       </c>
-      <c r="R105">
-        <v>0</v>
-      </c>
-      <c r="S105">
-        <v>1.8</v>
-      </c>
-      <c r="T105">
-        <v>2.05</v>
-      </c>
-      <c r="U105">
-        <v>3</v>
-      </c>
       <c r="V105">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="W105">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="X105">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="Y105">
         <v>-1</v>
       </c>
       <c r="Z105">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="AA105">
-        <v>-1</v>
+        <v>0.8600000000000001</v>
       </c>
       <c r="AB105">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AC105">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AD105">
-        <v>0</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="106" spans="1:30">
@@ -10724,7 +10724,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>7127379</v>
+        <v>7127376</v>
       </c>
       <c r="C112" t="s">
         <v>29</v>
@@ -10733,16 +10733,16 @@
         <v>45347.125</v>
       </c>
       <c r="E112" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I112">
         <v>0</v>
@@ -10751,64 +10751,64 @@
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L112">
         <v>1.95</v>
       </c>
       <c r="M112">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N112">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="O112">
         <v>1.909</v>
       </c>
       <c r="P112">
+        <v>4.2</v>
+      </c>
+      <c r="Q112">
         <v>3.6</v>
-      </c>
-      <c r="Q112">
-        <v>4</v>
       </c>
       <c r="R112">
         <v>-0.5</v>
       </c>
       <c r="S112">
+        <v>1.89</v>
+      </c>
+      <c r="T112">
+        <v>2.01</v>
+      </c>
+      <c r="U112">
+        <v>3.5</v>
+      </c>
+      <c r="V112">
+        <v>1.95</v>
+      </c>
+      <c r="W112">
         <v>1.9</v>
       </c>
-      <c r="T112">
-        <v>1.95</v>
-      </c>
-      <c r="U112">
-        <v>2.75</v>
-      </c>
-      <c r="V112">
-        <v>1.925</v>
-      </c>
-      <c r="W112">
-        <v>1.925</v>
-      </c>
       <c r="X112">
         <v>-1</v>
       </c>
       <c r="Y112">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Z112">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="AA112">
         <v>-1</v>
       </c>
       <c r="AB112">
+        <v>1.01</v>
+      </c>
+      <c r="AC112">
         <v>0.95</v>
       </c>
-      <c r="AC112">
-        <v>-1</v>
-      </c>
       <c r="AD112">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113" spans="1:30">
@@ -10816,7 +10816,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>7127376</v>
+        <v>7127379</v>
       </c>
       <c r="C113" t="s">
         <v>29</v>
@@ -10825,16 +10825,16 @@
         <v>45347.125</v>
       </c>
       <c r="E113" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F113" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H113">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I113">
         <v>0</v>
@@ -10843,64 +10843,64 @@
         <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L113">
         <v>1.95</v>
       </c>
       <c r="M113">
-        <v>4</v>
+        <v>3.6</v>
       </c>
       <c r="N113">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="O113">
         <v>1.909</v>
       </c>
       <c r="P113">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="Q113">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="R113">
         <v>-0.5</v>
       </c>
       <c r="S113">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="T113">
-        <v>2.01</v>
+        <v>1.95</v>
       </c>
       <c r="U113">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="V113">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W113">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="X113">
         <v>-1</v>
       </c>
       <c r="Y113">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Z113">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="AA113">
         <v>-1</v>
       </c>
       <c r="AB113">
-        <v>1.01</v>
+        <v>0.95</v>
       </c>
       <c r="AC113">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AD113">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="114" spans="1:30">

</xml_diff>